<commit_message>
Got rounded buildings to work... sorta... loads of issues remain
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="16260" windowHeight="9000" tabRatio="740" firstSheet="23" activeTab="27"/>
+    <workbookView xWindow="0" yWindow="48" windowWidth="16260" windowHeight="9000" tabRatio="740" firstSheet="24" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" state="hidden" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="Parks" sheetId="33" r:id="rId27"/>
     <sheet name="Cisterns" sheetId="34" r:id="rId28"/>
     <sheet name="Roundabout" sheetId="35" r:id="rId29"/>
+    <sheet name="Circles" sheetId="36" r:id="rId30"/>
   </sheets>
   <definedNames>
     <definedName name="block">Sheet7!$D$5</definedName>
@@ -1144,7 +1145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="31">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1325,6 +1326,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -1461,7 +1480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="228">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1786,6 +1805,14 @@
     <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -24339,7 +24366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BP34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD12" sqref="AD12"/>
     </sheetView>
   </sheetViews>
@@ -26481,7 +26508,7 @@
   <dimension ref="A2:BP52"/>
   <sheetViews>
     <sheetView topLeftCell="Y22" workbookViewId="0">
-      <selection activeCell="BB41" sqref="BB41"/>
+      <selection activeCell="AJ35" sqref="AJ35:AY35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30078,6 +30105,437 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:Q18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" activeCellId="1" sqref="E16:F16 G17:I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="70">
+        <f t="shared" ref="A2:A15" si="0">+A3+1</f>
+        <v>15</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="192"/>
+      <c r="H2" s="192"/>
+      <c r="I2" s="192"/>
+      <c r="J2" s="183"/>
+      <c r="K2" s="183"/>
+      <c r="L2" s="183"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="5"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="70">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="189"/>
+      <c r="F3" s="189"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="219"/>
+      <c r="N3" s="219"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="70">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="189"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="143"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="9"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="70">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="204"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="143"/>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="70">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="204"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="143"/>
+      <c r="Q6" s="9"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="70">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B7" s="223"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="222"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="70">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B8" s="223"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="222"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="70">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="223"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="141"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="222"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="70">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B10" s="224"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="24"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="70">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B11" s="224"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="24"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="70">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B12" s="224"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="24"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="70">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="225"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="9"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="70">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="225"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="9"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="70">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="225"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="221"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="9"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="70">
+        <f>+A17+1</f>
+        <v>1</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="226"/>
+      <c r="F16" s="226"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="221"/>
+      <c r="N16" s="221"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="9"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="70">
+        <v>0</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="227"/>
+      <c r="H17" s="227"/>
+      <c r="I17" s="227"/>
+      <c r="J17" s="220"/>
+      <c r="K17" s="220"/>
+      <c r="L17" s="220"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="15"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B18" s="70">
+        <v>0</v>
+      </c>
+      <c r="C18" s="70">
+        <f>B18+1</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="70">
+        <f t="shared" ref="D18:Q18" si="1">C18+1</f>
+        <v>2</v>
+      </c>
+      <c r="E18" s="70">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F18" s="70">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G18" s="70">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H18" s="70">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I18" s="70">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J18" s="70">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K18" s="70">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="L18" s="70">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M18" s="70">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="N18" s="70">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="O18" s="70">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="P18" s="70">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="Q18" s="70">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -36689,7 +37147,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:N15" ca="1" si="7">IF(AND(MOD(E$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -36709,7 +37167,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -36729,7 +37187,7 @@
       </c>
       <c r="O6">
         <f t="shared" ref="O6:AB15" ca="1" si="8">IF(AND(MOD(O$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -36769,7 +37227,7 @@
       </c>
       <c r="Y6">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -37259,7 +37717,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -37279,7 +37737,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -37299,7 +37757,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -37319,7 +37777,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -37829,7 +38287,7 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:N29" ca="1" si="11">IF(AND(MOD(E$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -37849,7 +38307,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -37869,7 +38327,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -37889,7 +38347,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -38399,7 +38857,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -38419,7 +38877,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -38969,7 +39427,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -38989,7 +39447,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -39009,7 +39467,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -39029,7 +39487,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -39049,7 +39507,7 @@
       </c>
       <c r="Y26">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z26" t="str">
         <f t="shared" ca="1" si="12"/>

</xml_diff>

<commit_message>
v0.55 Theming of city blocks (highrise, midrise, lowrise, big parks, etc.) First pass of roofs (peaks, edges, antennas, air conditioners, etc.)
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="16260" windowHeight="9000" tabRatio="740" firstSheet="4" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="4" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" state="hidden" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="410">
   <si>
     <t>grove</t>
   </si>
@@ -1234,6 +1234,48 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>Floor height</t>
+  </si>
+  <si>
+    <t>Street level</t>
+  </si>
+  <si>
+    <t>Below ground</t>
+  </si>
+  <si>
+    <t>Maximum height</t>
+  </si>
+  <si>
+    <t>Above ground</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Maximum steps</t>
+  </si>
+  <si>
+    <t>Highrise</t>
+  </si>
+  <si>
+    <t>Midrise</t>
+  </si>
+  <si>
+    <t>Lowrise</t>
+  </si>
+  <si>
+    <t>CityCenter</t>
+  </si>
+  <si>
+    <t>Mall</t>
+  </si>
+  <si>
+    <t>Unfinished</t>
+  </si>
+  <si>
+    <t>Antenna</t>
   </si>
 </sst>
 </file>
@@ -16992,13 +17034,17 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AN19"/>
+  <dimension ref="A2:AN32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC20" sqref="AC20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" s="70"/>
@@ -17722,7 +17768,7 @@
       <c r="AL16" s="76"/>
       <c r="AM16" s="78"/>
     </row>
-    <row r="17" spans="23:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="W17" s="70">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -17754,7 +17800,13 @@
       </c>
       <c r="AM17" s="78"/>
     </row>
-    <row r="18" spans="23:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>396</v>
+      </c>
       <c r="W18" s="70">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -17776,9 +17828,116 @@
       <c r="AL18" s="83"/>
       <c r="AM18" s="85"/>
     </row>
-    <row r="19" spans="23:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>397</v>
+      </c>
       <c r="W19" s="70" t="s">
         <v>395</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f>A18*A19</f>
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>127</v>
+      </c>
+      <c r="B21" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f>A21-A20</f>
+        <v>103</v>
+      </c>
+      <c r="B22" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f>A22/A18/A23</f>
+        <v>12.875</v>
+      </c>
+      <c r="B24" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>403</v>
+      </c>
+      <c r="G26">
+        <v>12</v>
+      </c>
+      <c r="H26" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>404</v>
+      </c>
+      <c r="G27">
+        <f>+A26*A23*A18+A20+G26</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -46545,7 +46704,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -46565,7 +46724,7 @@
       </c>
       <c r="O6">
         <f t="shared" ref="O6:AB15" ca="1" si="8">IF(AND(MOD(O$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -46585,7 +46744,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -47095,7 +47254,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -47135,7 +47294,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -47155,7 +47314,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -47685,7 +47844,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -47725,7 +47884,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -48255,7 +48414,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -48275,7 +48434,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -48295,7 +48454,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -48315,7 +48474,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -48825,7 +48984,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -48845,7 +49004,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -48865,7 +49024,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -48885,7 +49044,7 @@
       </c>
       <c r="Y26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z26" t="str">
         <f t="shared" ca="1" si="12"/>

</xml_diff>

<commit_message>
Cleaning up some code
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -17036,8 +17036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AN32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46684,7 +46684,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:N15" ca="1" si="7">IF(AND(MOD(E$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -46744,7 +46744,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -47254,7 +47254,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -47274,7 +47274,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -47294,7 +47294,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -47314,7 +47314,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -47334,7 +47334,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -47824,7 +47824,7 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:N29" ca="1" si="11">IF(AND(MOD(E$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -47844,7 +47844,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -47884,7 +47884,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -48414,7 +48414,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -48434,7 +48434,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -48454,7 +48454,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -48474,7 +48474,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -48964,7 +48964,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -49024,7 +49024,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>

</xml_diff>

<commit_message>
Sigh... GitHub is still acting like a Git! Trying to push the v0.60 changes (including Hax's comment)
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="3" state="hidden" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet6" sheetId="6" state="hidden" r:id="rId2"/>
     <sheet name="Building Nines Circles" sheetId="38" r:id="rId3"/>
     <sheet name="Plat types" sheetId="20" r:id="rId4"/>
@@ -41,14 +41,20 @@
     <sheet name="Roundabout" sheetId="35" r:id="rId32"/>
   </sheets>
   <definedNames>
+    <definedName name="AbsoluteMaximumFloorsBelow">Sheet3!$C$6</definedName>
     <definedName name="block">Sheet7!$D$5</definedName>
+    <definedName name="FloorHeight">Sheet3!$C$3</definedName>
+    <definedName name="FudgeFloorsAbove">Sheet3!$C$5</definedName>
+    <definedName name="FudgeFloorsBelow">Sheet3!$C$4</definedName>
+    <definedName name="RealChunkHeight">Sheet3!$C$2</definedName>
+    <definedName name="StreetLevel">Sheet3!$C$7</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="417">
   <si>
     <t>grove</t>
   </si>
@@ -1278,6 +1284,27 @@
   </si>
   <si>
     <t>Antenna</t>
+  </si>
+  <si>
+    <t>FudgeFloorsBelow</t>
+  </si>
+  <si>
+    <t>FudgeFloorsAbove</t>
+  </si>
+  <si>
+    <t>AbsoluteMaximumFloorsBelow</t>
+  </si>
+  <si>
+    <t>StreetLevel</t>
+  </si>
+  <si>
+    <t>AbsoluteMaximumFloorsAbove</t>
+  </si>
+  <si>
+    <t>FloorHeight</t>
+  </si>
+  <si>
+    <t>RealChunkHeight</t>
   </si>
 </sst>
 </file>
@@ -2576,854 +2603,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AF32"/>
+  <dimension ref="C2:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AQ22" sqref="AQ22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="5"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="5"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="5"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="5"/>
-    </row>
-    <row r="3" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B3" s="10"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="9"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="9"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="9"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="9"/>
-    </row>
-    <row r="4" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B4" s="10"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="9"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="9"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="9"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="9"/>
-    </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B5" s="12"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="24"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="24"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="24"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-      <c r="AC5" s="8"/>
-      <c r="AD5" s="8"/>
-      <c r="AE5" s="8"/>
-      <c r="AF5" s="24"/>
-    </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B6" s="10"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="9"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="9"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="9"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="8"/>
-      <c r="AD6" s="6"/>
-      <c r="AE6" s="6"/>
-      <c r="AF6" s="9"/>
-    </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B7" s="10"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="9"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="9"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="9"/>
-      <c r="Z7" s="10"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="8"/>
-      <c r="AD7" s="6"/>
-      <c r="AE7" s="6"/>
-      <c r="AF7" s="9"/>
-    </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="15"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="15"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="14"/>
-      <c r="AE8" s="14"/>
-      <c r="AF8" s="15"/>
-    </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="5"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="5"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="5"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="4"/>
-      <c r="AD10" s="2"/>
-      <c r="AE10" s="2"/>
-      <c r="AF10" s="5"/>
-    </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B11" s="10"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="9"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="9"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="9"/>
-      <c r="Z11" s="10"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="6"/>
-      <c r="AC11" s="8"/>
-      <c r="AD11" s="6"/>
-      <c r="AE11" s="6"/>
-      <c r="AF11" s="9"/>
-    </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="9"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="9"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="9"/>
-      <c r="Z12" s="10"/>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="8"/>
-      <c r="AD12" s="6"/>
-      <c r="AE12" s="6"/>
-      <c r="AF12" s="9"/>
-    </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="24"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="24"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
-      <c r="X13" s="24"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-      <c r="AC13" s="8"/>
-      <c r="AD13" s="6"/>
-      <c r="AE13" s="6"/>
-      <c r="AF13" s="24"/>
-    </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B14" s="10"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="9"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="9"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="9"/>
-      <c r="Z14" s="10"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="9"/>
-    </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B15" s="10"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="9"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="9"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="6"/>
-      <c r="X15" s="9"/>
-      <c r="Z15" s="10"/>
-      <c r="AA15" s="6"/>
-      <c r="AB15" s="6"/>
-      <c r="AC15" s="6"/>
-      <c r="AD15" s="6"/>
-      <c r="AE15" s="6"/>
-      <c r="AF15" s="9"/>
-    </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="15"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="15"/>
-      <c r="Z16" s="13"/>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="14"/>
-      <c r="AC16" s="21"/>
-      <c r="AD16" s="14"/>
-      <c r="AE16" s="14"/>
-      <c r="AF16" s="15"/>
-    </row>
-    <row r="18" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="5"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="5"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="37"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="4"/>
-      <c r="AD18" s="2"/>
-      <c r="AE18" s="2"/>
-      <c r="AF18" s="5"/>
-    </row>
-    <row r="19" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="9"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="9"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="24"/>
-      <c r="Z19" s="10"/>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="6"/>
-      <c r="AC19" s="8"/>
-      <c r="AD19" s="6"/>
-      <c r="AE19" s="6"/>
-      <c r="AF19" s="9"/>
-    </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B20" s="10"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="9"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="9"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="24"/>
-      <c r="Z20" s="10"/>
-      <c r="AA20" s="6"/>
-      <c r="AB20" s="6"/>
-      <c r="AC20" s="8"/>
-      <c r="AD20" s="6"/>
-      <c r="AE20" s="6"/>
-      <c r="AF20" s="9"/>
-    </row>
-    <row r="21" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="24"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="24"/>
-      <c r="R21" s="12"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6"/>
-      <c r="X21" s="24"/>
-      <c r="Z21" s="12"/>
-      <c r="AA21" s="8"/>
-      <c r="AB21" s="8"/>
-      <c r="AC21" s="8"/>
-      <c r="AD21" s="6"/>
-      <c r="AE21" s="6"/>
-      <c r="AF21" s="24"/>
-    </row>
-    <row r="22" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="9"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="9"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="8"/>
-      <c r="V22" s="6"/>
-      <c r="W22" s="6"/>
-      <c r="X22" s="9"/>
-      <c r="Z22" s="10"/>
-      <c r="AA22" s="6"/>
-      <c r="AB22" s="6"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="6"/>
-      <c r="AE22" s="6"/>
-      <c r="AF22" s="24"/>
-    </row>
-    <row r="23" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="9"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="9"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
-      <c r="X23" s="9"/>
-      <c r="Z23" s="10"/>
-      <c r="AA23" s="6"/>
-      <c r="AB23" s="6"/>
-      <c r="AC23" s="6"/>
-      <c r="AD23" s="6"/>
-      <c r="AE23" s="6"/>
-      <c r="AF23" s="24"/>
-    </row>
-    <row r="24" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B24" s="39"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="15"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="15"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="21"/>
-      <c r="V24" s="14"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="35"/>
-      <c r="Y24" s="36"/>
-      <c r="Z24" s="13"/>
-      <c r="AA24" s="14"/>
-      <c r="AB24" s="14"/>
-      <c r="AC24" s="21"/>
-      <c r="AD24" s="21"/>
-      <c r="AE24" s="21"/>
-      <c r="AF24" s="35"/>
-    </row>
-    <row r="26" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B26" s="1"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="5"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="5"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
-      <c r="X26" s="5"/>
-      <c r="Z26" s="1"/>
-      <c r="AA26" s="2"/>
-      <c r="AB26" s="2"/>
-      <c r="AC26" s="4"/>
-      <c r="AD26" s="2"/>
-      <c r="AE26" s="2"/>
-      <c r="AF26" s="5"/>
-    </row>
-    <row r="27" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B27" s="10"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="9"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="9"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="6"/>
-      <c r="X27" s="9"/>
-      <c r="Z27" s="10"/>
-      <c r="AA27" s="6"/>
-      <c r="AB27" s="6"/>
-      <c r="AC27" s="8"/>
-      <c r="AD27" s="6"/>
-      <c r="AE27" s="6"/>
-      <c r="AF27" s="9"/>
-    </row>
-    <row r="28" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B28" s="10"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="9"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="9"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6"/>
-      <c r="U28" s="6"/>
-      <c r="V28" s="6"/>
-      <c r="W28" s="6"/>
-      <c r="X28" s="9"/>
-      <c r="Z28" s="10"/>
-      <c r="AA28" s="6"/>
-      <c r="AB28" s="6"/>
-      <c r="AC28" s="8"/>
-      <c r="AD28" s="6"/>
-      <c r="AE28" s="6"/>
-      <c r="AF28" s="9"/>
-    </row>
-    <row r="29" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B29" s="12"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="24"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="24"/>
-      <c r="R29" s="12"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="8"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="24"/>
-      <c r="Z29" s="12"/>
-      <c r="AA29" s="8"/>
-      <c r="AB29" s="8"/>
-      <c r="AC29" s="8"/>
-      <c r="AD29" s="6"/>
-      <c r="AE29" s="6"/>
-      <c r="AF29" s="24"/>
-    </row>
-    <row r="30" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B30" s="10"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="9"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="9"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="6"/>
-      <c r="W30" s="6"/>
-      <c r="X30" s="9"/>
-      <c r="Z30" s="10"/>
-      <c r="AA30" s="6"/>
-      <c r="AB30" s="6"/>
-      <c r="AC30" s="8"/>
-      <c r="AD30" s="6"/>
-      <c r="AE30" s="6"/>
-      <c r="AF30" s="9"/>
-    </row>
-    <row r="31" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B31" s="10"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="9"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="9"/>
-      <c r="R31" s="10"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="6"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
-      <c r="X31" s="9"/>
-      <c r="Z31" s="10"/>
-      <c r="AA31" s="6"/>
-      <c r="AB31" s="6"/>
-      <c r="AC31" s="8"/>
-      <c r="AD31" s="6"/>
-      <c r="AE31" s="6"/>
-      <c r="AF31" s="9"/>
-    </row>
-    <row r="32" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B32" s="13"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="15"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
-      <c r="U32" s="21"/>
-      <c r="V32" s="14"/>
-      <c r="W32" s="14"/>
-      <c r="X32" s="15"/>
-      <c r="Z32" s="13"/>
-      <c r="AA32" s="14"/>
-      <c r="AB32" s="14"/>
-      <c r="AC32" s="21"/>
-      <c r="AD32" s="14"/>
-      <c r="AE32" s="14"/>
-      <c r="AF32" s="15"/>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>128</v>
+      </c>
+      <c r="D2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f>FloorHeight * (AbsoluteMaximumFloorsBelow + FudgeFloorsBelow)</f>
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <f>(RealChunkHeight - StreetLevel) / FloorHeight - FudgeFloorsAbove</f>
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <f>MAX(MIN(INT(C14/C10-C11), 4),0)</f>
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <f>INT((RealChunkHeight-C14)/FloorHeight)-C12</f>
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>414</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3917,7 +3211,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:N15" ca="1" si="7">IF(AND(MOD(E$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3937,7 +3231,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3957,7 +3251,7 @@
       </c>
       <c r="O6">
         <f t="shared" ref="O6:AB15" ca="1" si="8">IF(AND(MOD(O$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3977,7 +3271,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4487,7 +3781,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4527,7 +3821,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4547,7 +3841,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4567,7 +3861,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -5057,7 +4351,7 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:N29" ca="1" si="11">IF(AND(MOD(E$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5117,7 +4411,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5137,7 +4431,7 @@
       </c>
       <c r="Y16">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5647,7 +4941,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5667,7 +4961,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -6197,7 +5491,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -6217,7 +5511,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -6237,7 +5531,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -6257,7 +5551,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -6277,7 +5571,7 @@
       </c>
       <c r="Y26">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -43410,7 +42704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BO34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AX3" sqref="AX3:BA4"/>
     </sheetView>
   </sheetViews>
@@ -47087,7 +46381,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Got bridges and tunnels showing up, roughly speaking
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="6" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -39,6 +39,7 @@
     <sheet name="Parks" sheetId="33" r:id="rId30"/>
     <sheet name="Cisterns" sheetId="34" r:id="rId31"/>
     <sheet name="Roundabout" sheetId="35" r:id="rId32"/>
+    <sheet name="Sheet2" sheetId="41" r:id="rId33"/>
   </sheets>
   <definedNames>
     <definedName name="AbsoluteMaximumFloorsBelow">Sheet3!$C$6</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="425">
   <si>
     <t>grove</t>
   </si>
@@ -1306,6 +1307,30 @@
   <si>
     <t>RealChunkHeight</t>
   </si>
+  <si>
+    <t>For each intersection…</t>
+  </si>
+  <si>
+    <t>Is this chunk naturally an intersection?</t>
+  </si>
+  <si>
+    <t>Put roads all around!</t>
+  </si>
+  <si>
+    <t>Are all the surrounding chunks empty OR already a road AND Are the odds in favor of a round-about?</t>
+  </si>
+  <si>
+    <t>Else</t>
+  </si>
+  <si>
+    <t>Put a road here!</t>
+  </si>
+  <si>
+    <t>Put a statue here!</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
 </sst>
 </file>
 
@@ -1774,7 +1799,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="294">
+  <cellXfs count="306">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2195,6 +2220,42 @@
     <xf numFmtId="0" fontId="0" fillId="42" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2605,7 +2666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -3231,7 +3292,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3251,7 +3312,7 @@
       </c>
       <c r="O6">
         <f t="shared" ref="O6:AB15" ca="1" si="8">IF(AND(MOD(O$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3821,7 +3882,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4371,7 +4432,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4391,7 +4452,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4411,7 +4472,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4431,7 +4492,7 @@
       </c>
       <c r="Y16">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4921,7 +4982,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5001,7 +5062,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5511,7 +5572,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5551,7 +5612,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5571,7 +5632,7 @@
       </c>
       <c r="Y26">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -42467,6 +42528,1091 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:AY31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="35" width="2.77734375" style="297"/>
+    <col min="36" max="42" width="2.77734375" style="305"/>
+    <col min="43" max="51" width="2.77734375" style="89"/>
+    <col min="52" max="16384" width="2.77734375" style="297"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B2" s="294"/>
+      <c r="C2" s="295"/>
+      <c r="D2" s="295"/>
+      <c r="E2" s="295"/>
+      <c r="F2" s="295"/>
+      <c r="G2" s="296"/>
+      <c r="H2" s="294"/>
+      <c r="I2" s="295"/>
+      <c r="J2" s="295"/>
+      <c r="K2" s="295"/>
+      <c r="L2" s="295"/>
+      <c r="M2" s="296"/>
+      <c r="N2" s="294"/>
+      <c r="O2" s="295"/>
+      <c r="P2" s="295"/>
+      <c r="Q2" s="295"/>
+      <c r="R2" s="295"/>
+      <c r="S2" s="296"/>
+      <c r="T2" s="294"/>
+      <c r="U2" s="295"/>
+      <c r="V2" s="295"/>
+      <c r="W2" s="295"/>
+      <c r="X2" s="295"/>
+      <c r="Y2" s="296"/>
+      <c r="Z2" s="294"/>
+      <c r="AA2" s="295"/>
+      <c r="AB2" s="295"/>
+      <c r="AC2" s="295"/>
+      <c r="AD2" s="295"/>
+      <c r="AE2" s="296"/>
+      <c r="AK2" s="305" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B3" s="298"/>
+      <c r="C3" s="299"/>
+      <c r="D3" s="300"/>
+      <c r="E3" s="300"/>
+      <c r="F3" s="299"/>
+      <c r="G3" s="301"/>
+      <c r="H3" s="298"/>
+      <c r="I3" s="299"/>
+      <c r="J3" s="300"/>
+      <c r="K3" s="300"/>
+      <c r="L3" s="299"/>
+      <c r="M3" s="301"/>
+      <c r="N3" s="298"/>
+      <c r="O3" s="299"/>
+      <c r="P3" s="300"/>
+      <c r="Q3" s="300"/>
+      <c r="R3" s="299"/>
+      <c r="S3" s="301"/>
+      <c r="T3" s="298"/>
+      <c r="U3" s="299"/>
+      <c r="V3" s="300"/>
+      <c r="W3" s="300"/>
+      <c r="X3" s="299"/>
+      <c r="Y3" s="301"/>
+      <c r="Z3" s="298"/>
+      <c r="AA3" s="299"/>
+      <c r="AB3" s="300"/>
+      <c r="AC3" s="300"/>
+      <c r="AD3" s="299"/>
+      <c r="AE3" s="301"/>
+      <c r="AL3" s="305" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="4" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B4" s="298"/>
+      <c r="C4" s="300"/>
+      <c r="D4" s="300"/>
+      <c r="E4" s="300"/>
+      <c r="F4" s="300"/>
+      <c r="G4" s="301"/>
+      <c r="H4" s="298"/>
+      <c r="I4" s="300"/>
+      <c r="J4" s="300"/>
+      <c r="K4" s="300"/>
+      <c r="L4" s="300"/>
+      <c r="M4" s="301"/>
+      <c r="N4" s="298"/>
+      <c r="O4" s="300"/>
+      <c r="P4" s="300"/>
+      <c r="Q4" s="300"/>
+      <c r="R4" s="300"/>
+      <c r="S4" s="301"/>
+      <c r="T4" s="298"/>
+      <c r="U4" s="300"/>
+      <c r="V4" s="300"/>
+      <c r="W4" s="300"/>
+      <c r="X4" s="300"/>
+      <c r="Y4" s="301"/>
+      <c r="Z4" s="298"/>
+      <c r="AA4" s="300"/>
+      <c r="AB4" s="300"/>
+      <c r="AC4" s="300"/>
+      <c r="AD4" s="300"/>
+      <c r="AE4" s="301"/>
+      <c r="AM4" s="305" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="5" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B5" s="298"/>
+      <c r="C5" s="300"/>
+      <c r="D5" s="300"/>
+      <c r="E5" s="300"/>
+      <c r="F5" s="300"/>
+      <c r="G5" s="301"/>
+      <c r="H5" s="298"/>
+      <c r="I5" s="300"/>
+      <c r="J5" s="300"/>
+      <c r="K5" s="300"/>
+      <c r="L5" s="300"/>
+      <c r="M5" s="301"/>
+      <c r="N5" s="298"/>
+      <c r="O5" s="300"/>
+      <c r="P5" s="300"/>
+      <c r="Q5" s="300"/>
+      <c r="R5" s="300"/>
+      <c r="S5" s="301"/>
+      <c r="T5" s="298"/>
+      <c r="U5" s="300"/>
+      <c r="V5" s="300"/>
+      <c r="W5" s="300"/>
+      <c r="X5" s="300"/>
+      <c r="Y5" s="301"/>
+      <c r="Z5" s="298"/>
+      <c r="AA5" s="300"/>
+      <c r="AB5" s="300"/>
+      <c r="AC5" s="300"/>
+      <c r="AD5" s="300"/>
+      <c r="AE5" s="301"/>
+      <c r="AN5" s="305" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="6" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B6" s="298"/>
+      <c r="C6" s="299"/>
+      <c r="D6" s="300"/>
+      <c r="E6" s="300"/>
+      <c r="F6" s="299"/>
+      <c r="G6" s="301"/>
+      <c r="H6" s="298"/>
+      <c r="I6" s="299" t="s">
+        <v>365</v>
+      </c>
+      <c r="J6" s="300" t="s">
+        <v>365</v>
+      </c>
+      <c r="K6" s="300" t="s">
+        <v>365</v>
+      </c>
+      <c r="L6" s="299" t="s">
+        <v>365</v>
+      </c>
+      <c r="M6" s="301"/>
+      <c r="N6" s="298" t="s">
+        <v>424</v>
+      </c>
+      <c r="O6" s="299" t="s">
+        <v>424</v>
+      </c>
+      <c r="P6" s="300"/>
+      <c r="Q6" s="300"/>
+      <c r="R6" s="299"/>
+      <c r="S6" s="301"/>
+      <c r="T6" s="298"/>
+      <c r="U6" s="299"/>
+      <c r="V6" s="300"/>
+      <c r="W6" s="300"/>
+      <c r="X6" s="299"/>
+      <c r="Y6" s="301"/>
+      <c r="Z6" s="298"/>
+      <c r="AA6" s="299"/>
+      <c r="AB6" s="300"/>
+      <c r="AC6" s="300"/>
+      <c r="AD6" s="299"/>
+      <c r="AE6" s="301"/>
+      <c r="AN6" s="305" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="7" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B7" s="302"/>
+      <c r="C7" s="303"/>
+      <c r="D7" s="303"/>
+      <c r="E7" s="303"/>
+      <c r="F7" s="303"/>
+      <c r="G7" s="304"/>
+      <c r="H7" s="302"/>
+      <c r="I7" s="303"/>
+      <c r="J7" s="303"/>
+      <c r="K7" s="303"/>
+      <c r="L7" s="303" t="s">
+        <v>365</v>
+      </c>
+      <c r="M7" s="304"/>
+      <c r="N7" s="302"/>
+      <c r="O7" s="303" t="s">
+        <v>424</v>
+      </c>
+      <c r="P7" s="303"/>
+      <c r="Q7" s="303"/>
+      <c r="R7" s="303"/>
+      <c r="S7" s="304"/>
+      <c r="T7" s="302"/>
+      <c r="U7" s="303"/>
+      <c r="V7" s="303"/>
+      <c r="W7" s="303"/>
+      <c r="X7" s="303"/>
+      <c r="Y7" s="304"/>
+      <c r="Z7" s="302"/>
+      <c r="AA7" s="303"/>
+      <c r="AB7" s="303"/>
+      <c r="AC7" s="303"/>
+      <c r="AD7" s="303"/>
+      <c r="AE7" s="304"/>
+      <c r="AM7" s="305" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="8" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B8" s="294"/>
+      <c r="C8" s="295"/>
+      <c r="D8" s="295"/>
+      <c r="E8" s="295"/>
+      <c r="F8" s="295"/>
+      <c r="G8" s="296"/>
+      <c r="H8" s="294"/>
+      <c r="I8" s="295"/>
+      <c r="J8" s="295"/>
+      <c r="K8" s="295"/>
+      <c r="L8" s="295" t="s">
+        <v>365</v>
+      </c>
+      <c r="M8" s="296"/>
+      <c r="N8" s="294"/>
+      <c r="O8" s="295" t="s">
+        <v>424</v>
+      </c>
+      <c r="P8" s="295"/>
+      <c r="Q8" s="295"/>
+      <c r="R8" s="295"/>
+      <c r="S8" s="296"/>
+      <c r="T8" s="294"/>
+      <c r="U8" s="295"/>
+      <c r="V8" s="295"/>
+      <c r="W8" s="295"/>
+      <c r="X8" s="295"/>
+      <c r="Y8" s="296"/>
+      <c r="Z8" s="294"/>
+      <c r="AA8" s="295"/>
+      <c r="AB8" s="295"/>
+      <c r="AC8" s="295"/>
+      <c r="AD8" s="295"/>
+      <c r="AE8" s="296"/>
+      <c r="AN8" s="305" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="9" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B9" s="298"/>
+      <c r="C9" s="299"/>
+      <c r="D9" s="300"/>
+      <c r="E9" s="300"/>
+      <c r="F9" s="299"/>
+      <c r="G9" s="301"/>
+      <c r="H9" s="298"/>
+      <c r="I9" s="299" t="s">
+        <v>365</v>
+      </c>
+      <c r="J9" s="300" t="s">
+        <v>365</v>
+      </c>
+      <c r="K9" s="300" t="s">
+        <v>365</v>
+      </c>
+      <c r="L9" s="299" t="s">
+        <v>365</v>
+      </c>
+      <c r="M9" s="301"/>
+      <c r="N9" s="298" t="s">
+        <v>424</v>
+      </c>
+      <c r="O9" s="299" t="s">
+        <v>424</v>
+      </c>
+      <c r="P9" s="300"/>
+      <c r="Q9" s="300"/>
+      <c r="R9" s="299"/>
+      <c r="S9" s="301"/>
+      <c r="T9" s="298"/>
+      <c r="U9" s="299"/>
+      <c r="V9" s="300"/>
+      <c r="W9" s="300"/>
+      <c r="X9" s="299"/>
+      <c r="Y9" s="301"/>
+      <c r="Z9" s="298"/>
+      <c r="AA9" s="299"/>
+      <c r="AB9" s="300"/>
+      <c r="AC9" s="300"/>
+      <c r="AD9" s="299"/>
+      <c r="AE9" s="301"/>
+    </row>
+    <row r="10" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B10" s="298"/>
+      <c r="C10" s="300"/>
+      <c r="D10" s="300"/>
+      <c r="E10" s="300"/>
+      <c r="F10" s="300"/>
+      <c r="G10" s="301"/>
+      <c r="H10" s="298"/>
+      <c r="I10" s="300" t="s">
+        <v>424</v>
+      </c>
+      <c r="J10" s="300"/>
+      <c r="K10" s="300"/>
+      <c r="L10" s="300" t="s">
+        <v>365</v>
+      </c>
+      <c r="M10" s="301"/>
+      <c r="N10" s="298"/>
+      <c r="O10" s="300" t="s">
+        <v>424</v>
+      </c>
+      <c r="P10" s="300"/>
+      <c r="Q10" s="300"/>
+      <c r="R10" s="300"/>
+      <c r="S10" s="301"/>
+      <c r="T10" s="298"/>
+      <c r="U10" s="300"/>
+      <c r="V10" s="300"/>
+      <c r="W10" s="300"/>
+      <c r="X10" s="300"/>
+      <c r="Y10" s="301"/>
+      <c r="Z10" s="298"/>
+      <c r="AA10" s="300"/>
+      <c r="AB10" s="300"/>
+      <c r="AC10" s="300"/>
+      <c r="AD10" s="300"/>
+      <c r="AE10" s="301"/>
+    </row>
+    <row r="11" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B11" s="298"/>
+      <c r="C11" s="300"/>
+      <c r="D11" s="300"/>
+      <c r="E11" s="300"/>
+      <c r="F11" s="300"/>
+      <c r="G11" s="301"/>
+      <c r="H11" s="298"/>
+      <c r="I11" s="300" t="s">
+        <v>424</v>
+      </c>
+      <c r="J11" s="300"/>
+      <c r="K11" s="300"/>
+      <c r="L11" s="300" t="s">
+        <v>365</v>
+      </c>
+      <c r="M11" s="301"/>
+      <c r="N11" s="298"/>
+      <c r="O11" s="300" t="s">
+        <v>424</v>
+      </c>
+      <c r="P11" s="300"/>
+      <c r="Q11" s="300"/>
+      <c r="R11" s="300"/>
+      <c r="S11" s="301"/>
+      <c r="T11" s="298"/>
+      <c r="U11" s="300"/>
+      <c r="V11" s="300"/>
+      <c r="W11" s="300"/>
+      <c r="X11" s="300"/>
+      <c r="Y11" s="301"/>
+      <c r="Z11" s="298"/>
+      <c r="AA11" s="300"/>
+      <c r="AB11" s="300"/>
+      <c r="AC11" s="300"/>
+      <c r="AD11" s="300"/>
+      <c r="AE11" s="301"/>
+    </row>
+    <row r="12" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B12" s="298"/>
+      <c r="C12" s="299"/>
+      <c r="D12" s="300"/>
+      <c r="E12" s="300"/>
+      <c r="F12" s="299"/>
+      <c r="G12" s="301"/>
+      <c r="H12" s="298"/>
+      <c r="I12" s="299" t="s">
+        <v>424</v>
+      </c>
+      <c r="J12" s="300" t="s">
+        <v>424</v>
+      </c>
+      <c r="K12" s="300"/>
+      <c r="L12" s="299" t="s">
+        <v>365</v>
+      </c>
+      <c r="M12" s="301" t="s">
+        <v>365</v>
+      </c>
+      <c r="N12" s="298" t="s">
+        <v>365</v>
+      </c>
+      <c r="O12" s="299" t="s">
+        <v>365</v>
+      </c>
+      <c r="P12" s="300"/>
+      <c r="Q12" s="300" t="s">
+        <v>424</v>
+      </c>
+      <c r="R12" s="299" t="s">
+        <v>424</v>
+      </c>
+      <c r="S12" s="301"/>
+      <c r="T12" s="298"/>
+      <c r="U12" s="299"/>
+      <c r="V12" s="300"/>
+      <c r="W12" s="300"/>
+      <c r="X12" s="299"/>
+      <c r="Y12" s="301"/>
+      <c r="Z12" s="298"/>
+      <c r="AA12" s="299"/>
+      <c r="AB12" s="300"/>
+      <c r="AC12" s="300"/>
+      <c r="AD12" s="299"/>
+      <c r="AE12" s="301"/>
+    </row>
+    <row r="13" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B13" s="302"/>
+      <c r="C13" s="303"/>
+      <c r="D13" s="303"/>
+      <c r="E13" s="303"/>
+      <c r="F13" s="303"/>
+      <c r="G13" s="304"/>
+      <c r="H13" s="302"/>
+      <c r="I13" s="303" t="s">
+        <v>424</v>
+      </c>
+      <c r="J13" s="303"/>
+      <c r="K13" s="303"/>
+      <c r="L13" s="303" t="s">
+        <v>365</v>
+      </c>
+      <c r="M13" s="304"/>
+      <c r="N13" s="302"/>
+      <c r="O13" s="303" t="s">
+        <v>365</v>
+      </c>
+      <c r="P13" s="303"/>
+      <c r="Q13" s="303"/>
+      <c r="R13" s="303"/>
+      <c r="S13" s="304"/>
+      <c r="T13" s="302"/>
+      <c r="U13" s="303"/>
+      <c r="V13" s="303"/>
+      <c r="W13" s="303"/>
+      <c r="X13" s="303"/>
+      <c r="Y13" s="304"/>
+      <c r="Z13" s="302"/>
+      <c r="AA13" s="303"/>
+      <c r="AB13" s="303"/>
+      <c r="AC13" s="303"/>
+      <c r="AD13" s="303"/>
+      <c r="AE13" s="304"/>
+    </row>
+    <row r="14" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B14" s="294"/>
+      <c r="C14" s="295"/>
+      <c r="D14" s="295"/>
+      <c r="E14" s="295"/>
+      <c r="F14" s="295"/>
+      <c r="G14" s="296"/>
+      <c r="H14" s="294"/>
+      <c r="I14" s="295" t="s">
+        <v>424</v>
+      </c>
+      <c r="J14" s="295"/>
+      <c r="K14" s="295"/>
+      <c r="L14" s="295" t="s">
+        <v>365</v>
+      </c>
+      <c r="M14" s="296"/>
+      <c r="N14" s="294"/>
+      <c r="O14" s="295" t="s">
+        <v>365</v>
+      </c>
+      <c r="P14" s="295"/>
+      <c r="Q14" s="295"/>
+      <c r="R14" s="295"/>
+      <c r="S14" s="296"/>
+      <c r="T14" s="294"/>
+      <c r="U14" s="295"/>
+      <c r="V14" s="295"/>
+      <c r="W14" s="295"/>
+      <c r="X14" s="295"/>
+      <c r="Y14" s="296"/>
+      <c r="Z14" s="294"/>
+      <c r="AA14" s="295"/>
+      <c r="AB14" s="295"/>
+      <c r="AC14" s="295"/>
+      <c r="AD14" s="295"/>
+      <c r="AE14" s="296"/>
+    </row>
+    <row r="15" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B15" s="298"/>
+      <c r="C15" s="299"/>
+      <c r="D15" s="300"/>
+      <c r="E15" s="300"/>
+      <c r="F15" s="299"/>
+      <c r="G15" s="301"/>
+      <c r="H15" s="298"/>
+      <c r="I15" s="299" t="s">
+        <v>424</v>
+      </c>
+      <c r="J15" s="300" t="s">
+        <v>424</v>
+      </c>
+      <c r="K15" s="300"/>
+      <c r="L15" s="299" t="s">
+        <v>365</v>
+      </c>
+      <c r="M15" s="301"/>
+      <c r="N15" s="298" t="s">
+        <v>365</v>
+      </c>
+      <c r="O15" s="299" t="s">
+        <v>365</v>
+      </c>
+      <c r="P15" s="300"/>
+      <c r="Q15" s="300"/>
+      <c r="R15" s="299"/>
+      <c r="S15" s="301"/>
+      <c r="T15" s="298"/>
+      <c r="U15" s="299"/>
+      <c r="V15" s="300"/>
+      <c r="W15" s="300"/>
+      <c r="X15" s="299"/>
+      <c r="Y15" s="301"/>
+      <c r="Z15" s="298"/>
+      <c r="AA15" s="299"/>
+      <c r="AB15" s="300"/>
+      <c r="AC15" s="300"/>
+      <c r="AD15" s="299"/>
+      <c r="AE15" s="301"/>
+    </row>
+    <row r="16" spans="2:40" x14ac:dyDescent="0.3">
+      <c r="B16" s="298"/>
+      <c r="C16" s="300"/>
+      <c r="D16" s="300"/>
+      <c r="E16" s="300"/>
+      <c r="F16" s="300"/>
+      <c r="G16" s="301"/>
+      <c r="H16" s="298"/>
+      <c r="I16" s="300"/>
+      <c r="J16" s="300"/>
+      <c r="K16" s="300"/>
+      <c r="L16" s="300"/>
+      <c r="M16" s="301"/>
+      <c r="N16" s="298"/>
+      <c r="O16" s="300"/>
+      <c r="P16" s="300"/>
+      <c r="Q16" s="300"/>
+      <c r="R16" s="300"/>
+      <c r="S16" s="301"/>
+      <c r="T16" s="298"/>
+      <c r="U16" s="300"/>
+      <c r="V16" s="300"/>
+      <c r="W16" s="300"/>
+      <c r="X16" s="300"/>
+      <c r="Y16" s="301"/>
+      <c r="Z16" s="298"/>
+      <c r="AA16" s="300"/>
+      <c r="AB16" s="300"/>
+      <c r="AC16" s="300"/>
+      <c r="AD16" s="300"/>
+      <c r="AE16" s="301"/>
+    </row>
+    <row r="17" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B17" s="298"/>
+      <c r="C17" s="300"/>
+      <c r="D17" s="300"/>
+      <c r="E17" s="300"/>
+      <c r="F17" s="300"/>
+      <c r="G17" s="301"/>
+      <c r="H17" s="298"/>
+      <c r="I17" s="300"/>
+      <c r="J17" s="300"/>
+      <c r="K17" s="300"/>
+      <c r="L17" s="300"/>
+      <c r="M17" s="301"/>
+      <c r="N17" s="298"/>
+      <c r="O17" s="300"/>
+      <c r="P17" s="300"/>
+      <c r="Q17" s="300"/>
+      <c r="R17" s="300"/>
+      <c r="S17" s="301"/>
+      <c r="T17" s="298"/>
+      <c r="U17" s="300"/>
+      <c r="V17" s="300"/>
+      <c r="W17" s="300"/>
+      <c r="X17" s="300"/>
+      <c r="Y17" s="301"/>
+      <c r="Z17" s="298"/>
+      <c r="AA17" s="300"/>
+      <c r="AB17" s="300"/>
+      <c r="AC17" s="300"/>
+      <c r="AD17" s="300"/>
+      <c r="AE17" s="301"/>
+    </row>
+    <row r="18" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B18" s="298"/>
+      <c r="C18" s="299"/>
+      <c r="D18" s="300"/>
+      <c r="E18" s="300"/>
+      <c r="F18" s="299"/>
+      <c r="G18" s="301"/>
+      <c r="H18" s="298"/>
+      <c r="I18" s="299"/>
+      <c r="J18" s="300"/>
+      <c r="K18" s="300"/>
+      <c r="L18" s="299"/>
+      <c r="M18" s="301"/>
+      <c r="N18" s="298"/>
+      <c r="O18" s="299"/>
+      <c r="P18" s="300"/>
+      <c r="Q18" s="300"/>
+      <c r="R18" s="299"/>
+      <c r="S18" s="301"/>
+      <c r="T18" s="298"/>
+      <c r="U18" s="299"/>
+      <c r="V18" s="300"/>
+      <c r="W18" s="300"/>
+      <c r="X18" s="299"/>
+      <c r="Y18" s="301"/>
+      <c r="Z18" s="298"/>
+      <c r="AA18" s="299"/>
+      <c r="AB18" s="300"/>
+      <c r="AC18" s="300"/>
+      <c r="AD18" s="299"/>
+      <c r="AE18" s="301"/>
+    </row>
+    <row r="19" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B19" s="302"/>
+      <c r="C19" s="303"/>
+      <c r="D19" s="303"/>
+      <c r="E19" s="303"/>
+      <c r="F19" s="303"/>
+      <c r="G19" s="304"/>
+      <c r="H19" s="302"/>
+      <c r="I19" s="303"/>
+      <c r="J19" s="303"/>
+      <c r="K19" s="303"/>
+      <c r="L19" s="303"/>
+      <c r="M19" s="304"/>
+      <c r="N19" s="302"/>
+      <c r="O19" s="303"/>
+      <c r="P19" s="303"/>
+      <c r="Q19" s="303"/>
+      <c r="R19" s="303"/>
+      <c r="S19" s="304"/>
+      <c r="T19" s="302"/>
+      <c r="U19" s="303"/>
+      <c r="V19" s="303"/>
+      <c r="W19" s="303"/>
+      <c r="X19" s="303"/>
+      <c r="Y19" s="304"/>
+      <c r="Z19" s="302"/>
+      <c r="AA19" s="303"/>
+      <c r="AB19" s="303"/>
+      <c r="AC19" s="303"/>
+      <c r="AD19" s="303"/>
+      <c r="AE19" s="304"/>
+    </row>
+    <row r="20" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B20" s="294"/>
+      <c r="C20" s="295"/>
+      <c r="D20" s="295"/>
+      <c r="E20" s="295"/>
+      <c r="F20" s="295"/>
+      <c r="G20" s="296"/>
+      <c r="H20" s="294"/>
+      <c r="I20" s="295"/>
+      <c r="J20" s="295"/>
+      <c r="K20" s="295"/>
+      <c r="L20" s="295"/>
+      <c r="M20" s="296"/>
+      <c r="N20" s="294"/>
+      <c r="O20" s="295"/>
+      <c r="P20" s="295"/>
+      <c r="Q20" s="295"/>
+      <c r="R20" s="295"/>
+      <c r="S20" s="296"/>
+      <c r="T20" s="294"/>
+      <c r="U20" s="295"/>
+      <c r="V20" s="295"/>
+      <c r="W20" s="295"/>
+      <c r="X20" s="295"/>
+      <c r="Y20" s="296"/>
+      <c r="Z20" s="294"/>
+      <c r="AA20" s="295"/>
+      <c r="AB20" s="295"/>
+      <c r="AC20" s="295"/>
+      <c r="AD20" s="295"/>
+      <c r="AE20" s="296"/>
+    </row>
+    <row r="21" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B21" s="298"/>
+      <c r="C21" s="299"/>
+      <c r="D21" s="300"/>
+      <c r="E21" s="300"/>
+      <c r="F21" s="299"/>
+      <c r="G21" s="301"/>
+      <c r="H21" s="298"/>
+      <c r="I21" s="299"/>
+      <c r="J21" s="300"/>
+      <c r="K21" s="300"/>
+      <c r="L21" s="299"/>
+      <c r="M21" s="301"/>
+      <c r="N21" s="298"/>
+      <c r="O21" s="299"/>
+      <c r="P21" s="300"/>
+      <c r="Q21" s="300"/>
+      <c r="R21" s="299"/>
+      <c r="S21" s="301"/>
+      <c r="T21" s="298"/>
+      <c r="U21" s="299"/>
+      <c r="V21" s="300"/>
+      <c r="W21" s="300"/>
+      <c r="X21" s="299"/>
+      <c r="Y21" s="301"/>
+      <c r="Z21" s="298"/>
+      <c r="AA21" s="299"/>
+      <c r="AB21" s="300"/>
+      <c r="AC21" s="300"/>
+      <c r="AD21" s="299"/>
+      <c r="AE21" s="301"/>
+    </row>
+    <row r="22" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B22" s="298"/>
+      <c r="C22" s="300"/>
+      <c r="D22" s="300"/>
+      <c r="E22" s="300"/>
+      <c r="F22" s="300"/>
+      <c r="G22" s="301"/>
+      <c r="H22" s="298"/>
+      <c r="I22" s="300"/>
+      <c r="J22" s="300"/>
+      <c r="K22" s="300"/>
+      <c r="L22" s="300"/>
+      <c r="M22" s="301"/>
+      <c r="N22" s="298"/>
+      <c r="O22" s="300"/>
+      <c r="P22" s="300"/>
+      <c r="Q22" s="300"/>
+      <c r="R22" s="300"/>
+      <c r="S22" s="301"/>
+      <c r="T22" s="298"/>
+      <c r="U22" s="300"/>
+      <c r="V22" s="300"/>
+      <c r="W22" s="300"/>
+      <c r="X22" s="300"/>
+      <c r="Y22" s="301"/>
+      <c r="Z22" s="298"/>
+      <c r="AA22" s="300"/>
+      <c r="AB22" s="300"/>
+      <c r="AC22" s="300"/>
+      <c r="AD22" s="300"/>
+      <c r="AE22" s="301"/>
+    </row>
+    <row r="23" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B23" s="298"/>
+      <c r="C23" s="300"/>
+      <c r="D23" s="300"/>
+      <c r="E23" s="300"/>
+      <c r="F23" s="300"/>
+      <c r="G23" s="301"/>
+      <c r="H23" s="298"/>
+      <c r="I23" s="300"/>
+      <c r="J23" s="300"/>
+      <c r="K23" s="300"/>
+      <c r="L23" s="300"/>
+      <c r="M23" s="301"/>
+      <c r="N23" s="298"/>
+      <c r="O23" s="300"/>
+      <c r="P23" s="300"/>
+      <c r="Q23" s="300"/>
+      <c r="R23" s="300"/>
+      <c r="S23" s="301"/>
+      <c r="T23" s="298"/>
+      <c r="U23" s="300"/>
+      <c r="V23" s="300"/>
+      <c r="W23" s="300"/>
+      <c r="X23" s="300"/>
+      <c r="Y23" s="301"/>
+      <c r="Z23" s="298"/>
+      <c r="AA23" s="300"/>
+      <c r="AB23" s="300"/>
+      <c r="AC23" s="300"/>
+      <c r="AD23" s="300"/>
+      <c r="AE23" s="301"/>
+    </row>
+    <row r="24" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B24" s="298"/>
+      <c r="C24" s="299"/>
+      <c r="D24" s="300"/>
+      <c r="E24" s="300"/>
+      <c r="F24" s="299"/>
+      <c r="G24" s="301"/>
+      <c r="H24" s="298"/>
+      <c r="I24" s="299"/>
+      <c r="J24" s="300"/>
+      <c r="K24" s="300"/>
+      <c r="L24" s="299"/>
+      <c r="M24" s="301"/>
+      <c r="N24" s="298"/>
+      <c r="O24" s="299"/>
+      <c r="P24" s="300"/>
+      <c r="Q24" s="300"/>
+      <c r="R24" s="299"/>
+      <c r="S24" s="301"/>
+      <c r="T24" s="298"/>
+      <c r="U24" s="299"/>
+      <c r="V24" s="300"/>
+      <c r="W24" s="300"/>
+      <c r="X24" s="299"/>
+      <c r="Y24" s="301"/>
+      <c r="Z24" s="298"/>
+      <c r="AA24" s="299"/>
+      <c r="AB24" s="300"/>
+      <c r="AC24" s="300"/>
+      <c r="AD24" s="299"/>
+      <c r="AE24" s="301"/>
+    </row>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B25" s="302"/>
+      <c r="C25" s="303"/>
+      <c r="D25" s="303"/>
+      <c r="E25" s="303"/>
+      <c r="F25" s="303"/>
+      <c r="G25" s="304"/>
+      <c r="H25" s="302"/>
+      <c r="I25" s="303"/>
+      <c r="J25" s="303"/>
+      <c r="K25" s="303"/>
+      <c r="L25" s="303"/>
+      <c r="M25" s="304"/>
+      <c r="N25" s="302"/>
+      <c r="O25" s="303"/>
+      <c r="P25" s="303"/>
+      <c r="Q25" s="303"/>
+      <c r="R25" s="303"/>
+      <c r="S25" s="304"/>
+      <c r="T25" s="302"/>
+      <c r="U25" s="303"/>
+      <c r="V25" s="303"/>
+      <c r="W25" s="303"/>
+      <c r="X25" s="303"/>
+      <c r="Y25" s="304"/>
+      <c r="Z25" s="302"/>
+      <c r="AA25" s="303"/>
+      <c r="AB25" s="303"/>
+      <c r="AC25" s="303"/>
+      <c r="AD25" s="303"/>
+      <c r="AE25" s="304"/>
+    </row>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B26" s="294"/>
+      <c r="C26" s="295"/>
+      <c r="D26" s="295"/>
+      <c r="E26" s="295"/>
+      <c r="F26" s="295"/>
+      <c r="G26" s="296"/>
+      <c r="H26" s="294"/>
+      <c r="I26" s="295"/>
+      <c r="J26" s="295"/>
+      <c r="K26" s="295"/>
+      <c r="L26" s="295"/>
+      <c r="M26" s="296"/>
+      <c r="N26" s="294"/>
+      <c r="O26" s="295"/>
+      <c r="P26" s="295"/>
+      <c r="Q26" s="295"/>
+      <c r="R26" s="295"/>
+      <c r="S26" s="296"/>
+      <c r="T26" s="294"/>
+      <c r="U26" s="295"/>
+      <c r="V26" s="295"/>
+      <c r="W26" s="295"/>
+      <c r="X26" s="295"/>
+      <c r="Y26" s="296"/>
+      <c r="Z26" s="294"/>
+      <c r="AA26" s="295"/>
+      <c r="AB26" s="295"/>
+      <c r="AC26" s="295"/>
+      <c r="AD26" s="295"/>
+      <c r="AE26" s="296"/>
+    </row>
+    <row r="27" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B27" s="298"/>
+      <c r="C27" s="299"/>
+      <c r="D27" s="300"/>
+      <c r="E27" s="300"/>
+      <c r="F27" s="299"/>
+      <c r="G27" s="301"/>
+      <c r="H27" s="298"/>
+      <c r="I27" s="299"/>
+      <c r="J27" s="300"/>
+      <c r="K27" s="300"/>
+      <c r="L27" s="299"/>
+      <c r="M27" s="301"/>
+      <c r="N27" s="298"/>
+      <c r="O27" s="299"/>
+      <c r="P27" s="300"/>
+      <c r="Q27" s="300"/>
+      <c r="R27" s="299"/>
+      <c r="S27" s="301"/>
+      <c r="T27" s="298"/>
+      <c r="U27" s="299"/>
+      <c r="V27" s="300"/>
+      <c r="W27" s="300"/>
+      <c r="X27" s="299"/>
+      <c r="Y27" s="301"/>
+      <c r="Z27" s="298"/>
+      <c r="AA27" s="299"/>
+      <c r="AB27" s="300"/>
+      <c r="AC27" s="300"/>
+      <c r="AD27" s="299"/>
+      <c r="AE27" s="301"/>
+    </row>
+    <row r="28" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B28" s="298"/>
+      <c r="C28" s="300"/>
+      <c r="D28" s="300"/>
+      <c r="E28" s="300"/>
+      <c r="F28" s="300"/>
+      <c r="G28" s="301"/>
+      <c r="H28" s="298"/>
+      <c r="I28" s="300"/>
+      <c r="J28" s="300"/>
+      <c r="K28" s="300"/>
+      <c r="L28" s="300"/>
+      <c r="M28" s="301"/>
+      <c r="N28" s="298"/>
+      <c r="O28" s="300"/>
+      <c r="P28" s="300"/>
+      <c r="Q28" s="300"/>
+      <c r="R28" s="300"/>
+      <c r="S28" s="301"/>
+      <c r="T28" s="298"/>
+      <c r="U28" s="300"/>
+      <c r="V28" s="300"/>
+      <c r="W28" s="300"/>
+      <c r="X28" s="300"/>
+      <c r="Y28" s="301"/>
+      <c r="Z28" s="298"/>
+      <c r="AA28" s="300"/>
+      <c r="AB28" s="300"/>
+      <c r="AC28" s="300"/>
+      <c r="AD28" s="300"/>
+      <c r="AE28" s="301"/>
+    </row>
+    <row r="29" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B29" s="298"/>
+      <c r="C29" s="300"/>
+      <c r="D29" s="300"/>
+      <c r="E29" s="300"/>
+      <c r="F29" s="300"/>
+      <c r="G29" s="301"/>
+      <c r="H29" s="298"/>
+      <c r="I29" s="300"/>
+      <c r="J29" s="300"/>
+      <c r="K29" s="300"/>
+      <c r="L29" s="300"/>
+      <c r="M29" s="301"/>
+      <c r="N29" s="298"/>
+      <c r="O29" s="300"/>
+      <c r="P29" s="300"/>
+      <c r="Q29" s="300"/>
+      <c r="R29" s="300"/>
+      <c r="S29" s="301"/>
+      <c r="T29" s="298"/>
+      <c r="U29" s="300"/>
+      <c r="V29" s="300"/>
+      <c r="W29" s="300"/>
+      <c r="X29" s="300"/>
+      <c r="Y29" s="301"/>
+      <c r="Z29" s="298"/>
+      <c r="AA29" s="300"/>
+      <c r="AB29" s="300"/>
+      <c r="AC29" s="300"/>
+      <c r="AD29" s="300"/>
+      <c r="AE29" s="301"/>
+    </row>
+    <row r="30" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B30" s="298"/>
+      <c r="C30" s="299"/>
+      <c r="D30" s="300"/>
+      <c r="E30" s="300"/>
+      <c r="F30" s="299"/>
+      <c r="G30" s="301"/>
+      <c r="H30" s="298"/>
+      <c r="I30" s="299"/>
+      <c r="J30" s="300"/>
+      <c r="K30" s="300"/>
+      <c r="L30" s="299"/>
+      <c r="M30" s="301"/>
+      <c r="N30" s="298"/>
+      <c r="O30" s="299"/>
+      <c r="P30" s="300"/>
+      <c r="Q30" s="300"/>
+      <c r="R30" s="299"/>
+      <c r="S30" s="301"/>
+      <c r="T30" s="298"/>
+      <c r="U30" s="299"/>
+      <c r="V30" s="300"/>
+      <c r="W30" s="300"/>
+      <c r="X30" s="299"/>
+      <c r="Y30" s="301"/>
+      <c r="Z30" s="298"/>
+      <c r="AA30" s="299"/>
+      <c r="AB30" s="300"/>
+      <c r="AC30" s="300"/>
+      <c r="AD30" s="299"/>
+      <c r="AE30" s="301"/>
+    </row>
+    <row r="31" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B31" s="302"/>
+      <c r="C31" s="303"/>
+      <c r="D31" s="303"/>
+      <c r="E31" s="303"/>
+      <c r="F31" s="303"/>
+      <c r="G31" s="304"/>
+      <c r="H31" s="302"/>
+      <c r="I31" s="303"/>
+      <c r="J31" s="303"/>
+      <c r="K31" s="303"/>
+      <c r="L31" s="303"/>
+      <c r="M31" s="304"/>
+      <c r="N31" s="302"/>
+      <c r="O31" s="303"/>
+      <c r="P31" s="303"/>
+      <c r="Q31" s="303"/>
+      <c r="R31" s="303"/>
+      <c r="S31" s="304"/>
+      <c r="T31" s="302"/>
+      <c r="U31" s="303"/>
+      <c r="V31" s="303"/>
+      <c r="W31" s="303"/>
+      <c r="X31" s="303"/>
+      <c r="Y31" s="304"/>
+      <c r="Z31" s="302"/>
+      <c r="AA31" s="303"/>
+      <c r="AB31" s="303"/>
+      <c r="AC31" s="303"/>
+      <c r="AD31" s="303"/>
+      <c r="AE31" s="304"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>

</xml_diff>

<commit_message>
Tunnels and Retainer walls Work! Yea baby! Now for the Bridges... assuming I can find some :-)
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="6" activeTab="32"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="22" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,9 @@
     <sheet name="Parks" sheetId="33" r:id="rId30"/>
     <sheet name="Cisterns" sheetId="34" r:id="rId31"/>
     <sheet name="Roundabout" sheetId="35" r:id="rId32"/>
-    <sheet name="Sheet2" sheetId="41" r:id="rId33"/>
+    <sheet name="Intersections" sheetId="41" r:id="rId33"/>
+    <sheet name="Tunnels" sheetId="42" r:id="rId34"/>
+    <sheet name="Sheet2" sheetId="43" r:id="rId35"/>
   </sheets>
   <definedNames>
     <definedName name="AbsoluteMaximumFloorsBelow">Sheet3!$C$6</definedName>
@@ -55,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="427">
   <si>
     <t>grove</t>
   </si>
@@ -1331,6 +1333,12 @@
   <si>
     <t>f</t>
   </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>X/Z</t>
+  </si>
 </sst>
 </file>
 
@@ -1388,7 +1396,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="43">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1641,6 +1649,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -1799,7 +1813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="306">
+  <cellXfs count="311">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2256,6 +2270,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3272,7 +3291,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:N15" ca="1" si="7">IF(AND(MOD(E$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3292,7 +3311,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3312,7 +3331,7 @@
       </c>
       <c r="O6">
         <f t="shared" ref="O6:AB15" ca="1" si="8">IF(AND(MOD(O$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3352,7 +3371,7 @@
       </c>
       <c r="Y6">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3862,7 +3881,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3882,7 +3901,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3902,7 +3921,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3922,7 +3941,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4412,7 +4431,7 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:N29" ca="1" si="11">IF(AND(MOD(E$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4452,7 +4471,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4472,7 +4491,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4492,7 +4511,7 @@
       </c>
       <c r="Y16">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5062,7 +5081,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5552,7 +5571,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -19721,8 +19740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AN32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X2" sqref="X2:AN2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:AN19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20636,7 +20655,7 @@
   <dimension ref="A1:BS55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AF52" sqref="AF52"/>
+      <selection sqref="A1:R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39162,7 +39181,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BP52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="AI19" sqref="AI19:AI34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -42532,7 +42553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AY31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
@@ -43610,6 +43631,899 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10:W12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="B1" s="70">
+        <v>0</v>
+      </c>
+      <c r="C1" s="70">
+        <f>B1+1</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="70">
+        <f t="shared" ref="D1:Q1" si="0">C1+1</f>
+        <v>2</v>
+      </c>
+      <c r="E1" s="70">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F1" s="70">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G1" s="70">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H1" s="70">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I1" s="70">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J1" s="70">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K1" s="70">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L1" s="70">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M1" s="70">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="N1" s="70">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O1" s="70">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P1" s="70">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q1" s="70">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>394</v>
+      </c>
+      <c r="T1" s="70">
+        <v>0</v>
+      </c>
+      <c r="U1" s="70">
+        <f>T1+1</f>
+        <v>1</v>
+      </c>
+      <c r="V1" s="70">
+        <f t="shared" ref="V1" si="1">U1+1</f>
+        <v>2</v>
+      </c>
+      <c r="W1" s="70">
+        <f t="shared" ref="W1" si="2">V1+1</f>
+        <v>3</v>
+      </c>
+      <c r="X1" s="70">
+        <f t="shared" ref="X1" si="3">W1+1</f>
+        <v>4</v>
+      </c>
+      <c r="Y1" s="70">
+        <f t="shared" ref="Y1" si="4">X1+1</f>
+        <v>5</v>
+      </c>
+      <c r="Z1" s="70">
+        <f t="shared" ref="Z1" si="5">Y1+1</f>
+        <v>6</v>
+      </c>
+      <c r="AA1" s="70">
+        <f t="shared" ref="AA1" si="6">Z1+1</f>
+        <v>7</v>
+      </c>
+      <c r="AB1" s="70">
+        <f t="shared" ref="AB1" si="7">AA1+1</f>
+        <v>8</v>
+      </c>
+      <c r="AC1" s="70">
+        <f t="shared" ref="AC1" si="8">AB1+1</f>
+        <v>9</v>
+      </c>
+      <c r="AD1" s="70">
+        <f t="shared" ref="AD1" si="9">AC1+1</f>
+        <v>10</v>
+      </c>
+      <c r="AE1" s="70">
+        <f t="shared" ref="AE1" si="10">AD1+1</f>
+        <v>11</v>
+      </c>
+      <c r="AF1" s="70">
+        <f t="shared" ref="AF1" si="11">AE1+1</f>
+        <v>12</v>
+      </c>
+      <c r="AG1" s="70">
+        <f t="shared" ref="AG1" si="12">AF1+1</f>
+        <v>13</v>
+      </c>
+      <c r="AH1" s="70">
+        <f t="shared" ref="AH1" si="13">AG1+1</f>
+        <v>14</v>
+      </c>
+      <c r="AI1" s="70">
+        <f t="shared" ref="AI1" si="14">AH1+1</f>
+        <v>15</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A2" s="70">
+        <v>0</v>
+      </c>
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="74"/>
+      <c r="S2" s="70">
+        <f t="shared" ref="S2:S15" si="15">+S3+1</f>
+        <v>15</v>
+      </c>
+      <c r="T2" s="25"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="238"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A3" s="70">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="75"/>
+      <c r="C3" s="76" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" s="76"/>
+      <c r="E3" s="77" t="s">
+        <v>258</v>
+      </c>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76" t="s">
+        <v>242</v>
+      </c>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="77" t="s">
+        <v>257</v>
+      </c>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q3" s="78"/>
+      <c r="S3" s="70">
+        <f t="shared" si="15"/>
+        <v>14</v>
+      </c>
+      <c r="T3" s="16"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="17"/>
+      <c r="AB3" s="17"/>
+      <c r="AC3" s="17"/>
+      <c r="AD3" s="17"/>
+      <c r="AE3" s="17"/>
+      <c r="AF3" s="17"/>
+      <c r="AG3" s="17"/>
+      <c r="AH3" s="17"/>
+      <c r="AI3" s="26"/>
+      <c r="AJ3" s="238"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A4" s="70">
+        <f t="shared" ref="A4:A17" si="16">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="78"/>
+      <c r="S4" s="70">
+        <f t="shared" si="15"/>
+        <v>13</v>
+      </c>
+      <c r="T4" s="16"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="17"/>
+      <c r="AI4" s="26"/>
+      <c r="AJ4" s="238"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A5" s="70">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="79"/>
+      <c r="C5" s="77" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="77"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80" t="s">
+        <v>261</v>
+      </c>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q5" s="81"/>
+      <c r="S5" s="70">
+        <f t="shared" si="15"/>
+        <v>12</v>
+      </c>
+      <c r="T5" s="16"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="26"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A6" s="70">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="76"/>
+      <c r="Q6" s="78"/>
+      <c r="S6" s="70">
+        <f t="shared" si="15"/>
+        <v>11</v>
+      </c>
+      <c r="T6" s="16"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="17"/>
+      <c r="AG6" s="17"/>
+      <c r="AH6" s="17"/>
+      <c r="AI6" s="26"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A7" s="70">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="75"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="76"/>
+      <c r="P7" s="76"/>
+      <c r="Q7" s="78"/>
+      <c r="S7" s="70">
+        <f t="shared" si="15"/>
+        <v>10</v>
+      </c>
+      <c r="T7" s="16"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17"/>
+      <c r="AA7" s="17"/>
+      <c r="AB7" s="17"/>
+      <c r="AC7" s="17"/>
+      <c r="AD7" s="17"/>
+      <c r="AE7" s="17"/>
+      <c r="AF7" s="17"/>
+      <c r="AG7" s="17"/>
+      <c r="AH7" s="17"/>
+      <c r="AI7" s="26"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A8" s="70">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="75"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="76"/>
+      <c r="P8" s="70"/>
+      <c r="Q8" s="78"/>
+      <c r="S8" s="70">
+        <f t="shared" si="15"/>
+        <v>9</v>
+      </c>
+      <c r="T8" s="10"/>
+      <c r="AI8" s="9"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A9" s="70">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="75"/>
+      <c r="C9" s="76" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" s="76"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="76" t="s">
+        <v>245</v>
+      </c>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="80" t="s">
+        <v>260</v>
+      </c>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q9" s="78"/>
+      <c r="S9" s="70">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="T9" s="16"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="121"/>
+      <c r="Z9" s="121"/>
+      <c r="AA9" s="121"/>
+      <c r="AB9" s="121"/>
+      <c r="AC9" s="121"/>
+      <c r="AD9" s="121"/>
+      <c r="AE9" s="17"/>
+      <c r="AF9" s="17"/>
+      <c r="AG9" s="17"/>
+      <c r="AH9" s="17"/>
+      <c r="AI9" s="26"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A10" s="70">
+        <f t="shared" si="16"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="75"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="80" t="s">
+        <v>259</v>
+      </c>
+      <c r="F10" s="76"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="78"/>
+      <c r="S10" s="70">
+        <f t="shared" si="15"/>
+        <v>7</v>
+      </c>
+      <c r="T10" s="16"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="121"/>
+      <c r="X10" s="121"/>
+      <c r="Y10" s="306"/>
+      <c r="Z10" s="306"/>
+      <c r="AA10" s="310"/>
+      <c r="AB10" s="310"/>
+      <c r="AC10" s="306"/>
+      <c r="AD10" s="306"/>
+      <c r="AE10" s="121"/>
+      <c r="AF10" s="121"/>
+      <c r="AG10" s="17"/>
+      <c r="AH10" s="17"/>
+      <c r="AI10" s="26"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A11" s="70">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="75"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="76"/>
+      <c r="P11" s="76"/>
+      <c r="Q11" s="78"/>
+      <c r="S11" s="70">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="T11" s="16"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="121"/>
+      <c r="W11" s="121"/>
+      <c r="X11" s="219"/>
+      <c r="Y11" s="216"/>
+      <c r="Z11" s="219"/>
+      <c r="AA11" s="219"/>
+      <c r="AB11" s="219"/>
+      <c r="AC11" s="219"/>
+      <c r="AD11" s="216"/>
+      <c r="AE11" s="219"/>
+      <c r="AF11" s="121"/>
+      <c r="AG11" s="121"/>
+      <c r="AH11" s="17"/>
+      <c r="AI11" s="26"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A12" s="70">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="76"/>
+      <c r="P12" s="76"/>
+      <c r="Q12" s="78"/>
+      <c r="S12" s="70">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+      <c r="T12" s="16"/>
+      <c r="U12" s="121"/>
+      <c r="V12" s="118"/>
+      <c r="W12" s="307"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="20"/>
+      <c r="AE12" s="20"/>
+      <c r="AF12" s="307"/>
+      <c r="AG12" s="122"/>
+      <c r="AH12" s="121"/>
+      <c r="AI12" s="26"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A13" s="70">
+        <f t="shared" si="16"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="75"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="76"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="76"/>
+      <c r="P13" s="76"/>
+      <c r="Q13" s="78"/>
+      <c r="S13" s="70">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+      <c r="T13" s="16"/>
+      <c r="U13" s="121"/>
+      <c r="V13" s="308"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="17"/>
+      <c r="AB13" s="17"/>
+      <c r="AC13" s="17"/>
+      <c r="AD13" s="17"/>
+      <c r="AE13" s="17"/>
+      <c r="AF13" s="17"/>
+      <c r="AG13" s="309"/>
+      <c r="AH13" s="121"/>
+      <c r="AI13" s="26"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A14" s="70">
+        <f t="shared" si="16"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="79"/>
+      <c r="C14" s="77" t="s">
+        <v>255</v>
+      </c>
+      <c r="D14" s="77"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80" t="s">
+        <v>262</v>
+      </c>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="77"/>
+      <c r="P14" s="77" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q14" s="81"/>
+      <c r="S14" s="70">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="T14" s="120"/>
+      <c r="U14" s="121"/>
+      <c r="V14" s="308"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="17"/>
+      <c r="AF14" s="17"/>
+      <c r="AG14" s="309"/>
+      <c r="AH14" s="121"/>
+      <c r="AI14" s="123"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A15" s="70">
+        <f t="shared" si="16"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="75"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="76"/>
+      <c r="N15" s="77"/>
+      <c r="O15" s="76"/>
+      <c r="P15" s="76"/>
+      <c r="Q15" s="78"/>
+      <c r="S15" s="70">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="T15" s="120"/>
+      <c r="U15" s="219"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="17"/>
+      <c r="AF15" s="17"/>
+      <c r="AG15" s="26"/>
+      <c r="AH15" s="219"/>
+      <c r="AI15" s="123"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A16" s="70">
+        <f t="shared" si="16"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="75"/>
+      <c r="C16" s="76" t="s">
+        <v>247</v>
+      </c>
+      <c r="D16" s="76"/>
+      <c r="E16" s="77" t="s">
+        <v>255</v>
+      </c>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="76"/>
+      <c r="N16" s="77" t="s">
+        <v>256</v>
+      </c>
+      <c r="O16" s="76"/>
+      <c r="P16" s="76" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q16" s="78"/>
+      <c r="S16" s="70">
+        <f>+S17+1</f>
+        <v>1</v>
+      </c>
+      <c r="T16" s="120"/>
+      <c r="U16" s="219"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="17"/>
+      <c r="AF16" s="17"/>
+      <c r="AG16" s="26"/>
+      <c r="AH16" s="219"/>
+      <c r="AI16" s="123"/>
+      <c r="AJ16" s="238"/>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A17" s="70">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="82"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="83"/>
+      <c r="N17" s="84"/>
+      <c r="O17" s="83"/>
+      <c r="P17" s="83"/>
+      <c r="Q17" s="85"/>
+      <c r="S17" s="70">
+        <v>0</v>
+      </c>
+      <c r="T17" s="126"/>
+      <c r="U17" s="218"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+      <c r="AG17" s="33"/>
+      <c r="AH17" s="218"/>
+      <c r="AI17" s="125"/>
+      <c r="AJ17" s="238"/>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A18" s="70" t="s">
+        <v>395</v>
+      </c>
+      <c r="S18" s="70" t="s">
+        <v>425</v>
+      </c>
+      <c r="T18" s="70"/>
+      <c r="U18" s="70"/>
+      <c r="V18" s="70"/>
+      <c r="W18" s="70"/>
+      <c r="X18" s="70"/>
+      <c r="Y18" s="70"/>
+      <c r="Z18" s="70"/>
+      <c r="AA18" s="70"/>
+      <c r="AB18" s="70"/>
+      <c r="AC18" s="70"/>
+      <c r="AD18" s="70"/>
+      <c r="AE18" s="70"/>
+      <c r="AF18" s="70"/>
+      <c r="AG18" s="70"/>
+      <c r="AH18" s="70"/>
+      <c r="AI18" s="70"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="192"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Bridges are starting to work
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="22" activeTab="33"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="22" activeTab="34"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <sheet name="Roundabout" sheetId="35" r:id="rId32"/>
     <sheet name="Intersections" sheetId="41" r:id="rId33"/>
     <sheet name="Tunnels" sheetId="42" r:id="rId34"/>
-    <sheet name="Sheet2" sheetId="43" r:id="rId35"/>
+    <sheet name="Bridge" sheetId="43" r:id="rId35"/>
   </sheets>
   <definedNames>
     <definedName name="AbsoluteMaximumFloorsBelow">Sheet3!$C$6</definedName>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="427">
   <si>
     <t>grove</t>
   </si>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:N15" ca="1" si="7">IF(AND(MOD(E$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3311,7 +3311,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3371,7 +3371,7 @@
       </c>
       <c r="Y6">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3921,7 +3921,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3941,7 +3941,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4431,7 +4431,7 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:N29" ca="1" si="11">IF(AND(MOD(E$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4451,7 +4451,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4491,7 +4491,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4511,7 +4511,7 @@
       </c>
       <c r="Y16">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5001,7 +5001,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5041,7 +5041,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5061,7 +5061,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5611,7 +5611,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -43638,8 +43638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10:W12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44511,19 +44511,1810 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2"/>
+  <dimension ref="A1:BC33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="BK15" sqref="BK15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="192"/>
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B1" s="70">
+        <v>0</v>
+      </c>
+      <c r="C1" s="70">
+        <f>B1+1</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="70">
+        <f t="shared" ref="D1:Q1" si="0">C1+1</f>
+        <v>2</v>
+      </c>
+      <c r="E1" s="70">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F1" s="70">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G1" s="70">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H1" s="70">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I1" s="70">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J1" s="70">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K1" s="70">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L1" s="70">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M1" s="70">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="N1" s="70">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O1" s="70">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P1" s="70">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q1" s="70">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>394</v>
+      </c>
+      <c r="T1" s="70">
+        <v>0</v>
+      </c>
+      <c r="U1" s="70">
+        <f>T1+1</f>
+        <v>1</v>
+      </c>
+      <c r="V1" s="70">
+        <f t="shared" ref="V1:AI1" si="1">U1+1</f>
+        <v>2</v>
+      </c>
+      <c r="W1" s="70">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="X1" s="70">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Y1" s="70">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Z1" s="70">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="AA1" s="70">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="AB1" s="70">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="AC1" s="70">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="AD1" s="70">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="AE1" s="70">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="AF1" s="70">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="AG1" s="70">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="AH1" s="70">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="AI1" s="70">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>426</v>
+      </c>
+      <c r="AM1" s="70">
+        <v>0</v>
+      </c>
+      <c r="AN1" s="70">
+        <f>AM1+1</f>
+        <v>1</v>
+      </c>
+      <c r="AO1" s="70">
+        <f t="shared" ref="AO1" si="2">AN1+1</f>
+        <v>2</v>
+      </c>
+      <c r="AP1" s="70">
+        <f t="shared" ref="AP1" si="3">AO1+1</f>
+        <v>3</v>
+      </c>
+      <c r="AQ1" s="70">
+        <f t="shared" ref="AQ1" si="4">AP1+1</f>
+        <v>4</v>
+      </c>
+      <c r="AR1" s="70">
+        <f t="shared" ref="AR1" si="5">AQ1+1</f>
+        <v>5</v>
+      </c>
+      <c r="AS1" s="70">
+        <f t="shared" ref="AS1" si="6">AR1+1</f>
+        <v>6</v>
+      </c>
+      <c r="AT1" s="70">
+        <f t="shared" ref="AT1" si="7">AS1+1</f>
+        <v>7</v>
+      </c>
+      <c r="AU1" s="70">
+        <f t="shared" ref="AU1" si="8">AT1+1</f>
+        <v>8</v>
+      </c>
+      <c r="AV1" s="70">
+        <f t="shared" ref="AV1" si="9">AU1+1</f>
+        <v>9</v>
+      </c>
+      <c r="AW1" s="70">
+        <f t="shared" ref="AW1" si="10">AV1+1</f>
+        <v>10</v>
+      </c>
+      <c r="AX1" s="70">
+        <f t="shared" ref="AX1" si="11">AW1+1</f>
+        <v>11</v>
+      </c>
+      <c r="AY1" s="70">
+        <f t="shared" ref="AY1" si="12">AX1+1</f>
+        <v>12</v>
+      </c>
+      <c r="AZ1" s="70">
+        <f t="shared" ref="AZ1" si="13">AY1+1</f>
+        <v>13</v>
+      </c>
+      <c r="BA1" s="70">
+        <f t="shared" ref="BA1" si="14">AZ1+1</f>
+        <v>14</v>
+      </c>
+      <c r="BB1" s="70">
+        <f t="shared" ref="BB1" si="15">BA1+1</f>
+        <v>15</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A2" s="70">
+        <v>0</v>
+      </c>
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="74"/>
+      <c r="S2" s="70">
+        <f t="shared" ref="S2:S15" si="16">+S3+1</f>
+        <v>15</v>
+      </c>
+      <c r="T2" s="25"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="238"/>
+      <c r="AL2" s="70">
+        <f t="shared" ref="AL2:AL15" si="17">+AL3+1</f>
+        <v>15</v>
+      </c>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="20"/>
+      <c r="AO2" s="20"/>
+      <c r="AP2" s="20"/>
+      <c r="AQ2" s="20"/>
+      <c r="AR2" s="20"/>
+      <c r="AS2" s="20"/>
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="20"/>
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="20"/>
+      <c r="AY2" s="20"/>
+      <c r="AZ2" s="20"/>
+      <c r="BA2" s="20"/>
+      <c r="BB2" s="31"/>
+      <c r="BC2" s="238"/>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A3" s="70">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="75"/>
+      <c r="C3" s="76" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" s="76"/>
+      <c r="E3" s="77" t="s">
+        <v>258</v>
+      </c>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76" t="s">
+        <v>242</v>
+      </c>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="77" t="s">
+        <v>257</v>
+      </c>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q3" s="78"/>
+      <c r="S3" s="70">
+        <f t="shared" si="16"/>
+        <v>14</v>
+      </c>
+      <c r="T3" s="16"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="17"/>
+      <c r="AB3" s="17"/>
+      <c r="AC3" s="17"/>
+      <c r="AD3" s="17"/>
+      <c r="AE3" s="17"/>
+      <c r="AF3" s="17"/>
+      <c r="AG3" s="17"/>
+      <c r="AH3" s="17"/>
+      <c r="AI3" s="26"/>
+      <c r="AJ3" s="238"/>
+      <c r="AL3" s="70">
+        <f t="shared" si="17"/>
+        <v>14</v>
+      </c>
+      <c r="AM3" s="16"/>
+      <c r="AN3" s="17"/>
+      <c r="AO3" s="17"/>
+      <c r="AP3" s="17"/>
+      <c r="AQ3" s="17"/>
+      <c r="AR3" s="17"/>
+      <c r="AS3" s="17"/>
+      <c r="AT3" s="17"/>
+      <c r="AU3" s="17"/>
+      <c r="AV3" s="17"/>
+      <c r="AW3" s="17"/>
+      <c r="AX3" s="17"/>
+      <c r="AY3" s="17"/>
+      <c r="AZ3" s="17"/>
+      <c r="BA3" s="17"/>
+      <c r="BB3" s="26"/>
+      <c r="BC3" s="238"/>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A4" s="70">
+        <f t="shared" ref="A4:A17" si="18">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="78"/>
+      <c r="S4" s="70">
+        <f t="shared" si="16"/>
+        <v>13</v>
+      </c>
+      <c r="T4" s="16"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="17"/>
+      <c r="AI4" s="26"/>
+      <c r="AJ4" s="238"/>
+      <c r="AL4" s="70">
+        <f t="shared" si="17"/>
+        <v>13</v>
+      </c>
+      <c r="AM4" s="16"/>
+      <c r="AN4" s="17"/>
+      <c r="AO4" s="17"/>
+      <c r="AP4" s="17"/>
+      <c r="AQ4" s="17"/>
+      <c r="AR4" s="17"/>
+      <c r="AS4" s="17"/>
+      <c r="AT4" s="17"/>
+      <c r="AU4" s="17"/>
+      <c r="AV4" s="17"/>
+      <c r="AW4" s="17"/>
+      <c r="AX4" s="17"/>
+      <c r="AY4" s="17"/>
+      <c r="AZ4" s="17"/>
+      <c r="BA4" s="17"/>
+      <c r="BB4" s="26"/>
+      <c r="BC4" s="238"/>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A5" s="70">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="79"/>
+      <c r="C5" s="77" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="77"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80" t="s">
+        <v>261</v>
+      </c>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q5" s="81"/>
+      <c r="S5" s="70">
+        <f t="shared" si="16"/>
+        <v>12</v>
+      </c>
+      <c r="T5" s="120"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="123"/>
+      <c r="AL5" s="70">
+        <f t="shared" si="17"/>
+        <v>12</v>
+      </c>
+      <c r="AM5" s="16"/>
+      <c r="AN5" s="17"/>
+      <c r="AO5" s="17"/>
+      <c r="AP5" s="128"/>
+      <c r="AQ5" s="128"/>
+      <c r="AR5" s="128"/>
+      <c r="AS5" s="128"/>
+      <c r="AT5" s="128"/>
+      <c r="AU5" s="128"/>
+      <c r="AV5" s="128"/>
+      <c r="AW5" s="128"/>
+      <c r="AX5" s="128"/>
+      <c r="AY5" s="128"/>
+      <c r="AZ5" s="17"/>
+      <c r="BA5" s="17"/>
+      <c r="BB5" s="26"/>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A6" s="70">
+        <f t="shared" si="18"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="76"/>
+      <c r="Q6" s="78"/>
+      <c r="S6" s="70">
+        <f t="shared" si="16"/>
+        <v>11</v>
+      </c>
+      <c r="T6" s="120"/>
+      <c r="U6" s="128"/>
+      <c r="V6" s="128"/>
+      <c r="W6" s="128"/>
+      <c r="X6" s="128"/>
+      <c r="Y6" s="128"/>
+      <c r="Z6" s="128"/>
+      <c r="AA6" s="128"/>
+      <c r="AB6" s="128"/>
+      <c r="AC6" s="128"/>
+      <c r="AD6" s="128"/>
+      <c r="AE6" s="128"/>
+      <c r="AF6" s="128"/>
+      <c r="AG6" s="128"/>
+      <c r="AH6" s="128"/>
+      <c r="AI6" s="123"/>
+      <c r="AL6" s="70">
+        <f t="shared" si="17"/>
+        <v>11</v>
+      </c>
+      <c r="AM6" s="127"/>
+      <c r="AN6" s="128"/>
+      <c r="AO6" s="128"/>
+      <c r="AP6" s="128"/>
+      <c r="AQ6" s="121"/>
+      <c r="AR6" s="121"/>
+      <c r="AS6" s="121"/>
+      <c r="AT6" s="121"/>
+      <c r="AU6" s="121"/>
+      <c r="AV6" s="121"/>
+      <c r="AW6" s="121"/>
+      <c r="AX6" s="121"/>
+      <c r="AY6" s="128"/>
+      <c r="AZ6" s="128"/>
+      <c r="BA6" s="128"/>
+      <c r="BB6" s="130"/>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A7" s="70">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="75"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="76"/>
+      <c r="P7" s="76"/>
+      <c r="Q7" s="78"/>
+      <c r="S7" s="70">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="T7" s="120"/>
+      <c r="U7" s="121"/>
+      <c r="V7" s="121"/>
+      <c r="W7" s="121"/>
+      <c r="X7" s="121"/>
+      <c r="Y7" s="121"/>
+      <c r="Z7" s="121"/>
+      <c r="AA7" s="121"/>
+      <c r="AB7" s="121"/>
+      <c r="AC7" s="121"/>
+      <c r="AD7" s="121"/>
+      <c r="AE7" s="121"/>
+      <c r="AF7" s="121"/>
+      <c r="AG7" s="121"/>
+      <c r="AH7" s="121"/>
+      <c r="AI7" s="123"/>
+      <c r="AL7" s="70">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="AM7" s="120"/>
+      <c r="AN7" s="121"/>
+      <c r="AO7" s="121"/>
+      <c r="AP7" s="121"/>
+      <c r="AQ7" s="17"/>
+      <c r="AR7" s="17"/>
+      <c r="AS7" s="17"/>
+      <c r="AT7" s="121"/>
+      <c r="AU7" s="121"/>
+      <c r="AV7" s="17"/>
+      <c r="AW7" s="17"/>
+      <c r="AX7" s="17"/>
+      <c r="AY7" s="121"/>
+      <c r="AZ7" s="121"/>
+      <c r="BA7" s="121"/>
+      <c r="BB7" s="123"/>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A8" s="70">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="75"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="76"/>
+      <c r="P8" s="70"/>
+      <c r="Q8" s="78"/>
+      <c r="S8" s="70">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="T8" s="10"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="121"/>
+      <c r="W8" s="121"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="121"/>
+      <c r="AB8" s="121"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="121"/>
+      <c r="AG8" s="121"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="9"/>
+      <c r="AL8" s="70">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="AM8" s="120"/>
+      <c r="AN8" s="17"/>
+      <c r="AO8" s="17"/>
+      <c r="AP8" s="17"/>
+      <c r="AQ8" s="17"/>
+      <c r="AR8" s="17"/>
+      <c r="AS8" s="17"/>
+      <c r="AT8" s="121"/>
+      <c r="AU8" s="121"/>
+      <c r="AV8" s="17"/>
+      <c r="AW8" s="17"/>
+      <c r="AX8" s="17"/>
+      <c r="AY8" s="17"/>
+      <c r="AZ8" s="17"/>
+      <c r="BA8" s="17"/>
+      <c r="BB8" s="123"/>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A9" s="70">
+        <f t="shared" si="18"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="75"/>
+      <c r="C9" s="76" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" s="76"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="76" t="s">
+        <v>245</v>
+      </c>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="80" t="s">
+        <v>260</v>
+      </c>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q9" s="78"/>
+      <c r="S9" s="70">
+        <f t="shared" si="16"/>
+        <v>8</v>
+      </c>
+      <c r="T9" s="16"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="121"/>
+      <c r="W9" s="121"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17"/>
+      <c r="AA9" s="121"/>
+      <c r="AB9" s="121"/>
+      <c r="AC9" s="17"/>
+      <c r="AD9" s="17"/>
+      <c r="AE9" s="17"/>
+      <c r="AF9" s="121"/>
+      <c r="AG9" s="121"/>
+      <c r="AH9" s="17"/>
+      <c r="AI9" s="26"/>
+      <c r="AL9" s="70">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="AM9" s="120"/>
+      <c r="AN9" s="17"/>
+      <c r="AO9" s="17"/>
+      <c r="AP9" s="17"/>
+      <c r="AQ9" s="17"/>
+      <c r="AR9" s="17"/>
+      <c r="AS9" s="17"/>
+      <c r="AT9" s="121"/>
+      <c r="AU9" s="121"/>
+      <c r="AV9" s="17"/>
+      <c r="AW9" s="17"/>
+      <c r="AX9" s="17"/>
+      <c r="AY9" s="17"/>
+      <c r="AZ9" s="17"/>
+      <c r="BA9" s="17"/>
+      <c r="BB9" s="123"/>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A10" s="70">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="75"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="80" t="s">
+        <v>259</v>
+      </c>
+      <c r="F10" s="76"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="78"/>
+      <c r="S10" s="70">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="T10" s="16"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="121"/>
+      <c r="W10" s="121"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
+      <c r="AA10" s="121"/>
+      <c r="AB10" s="121"/>
+      <c r="AC10" s="17"/>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="17"/>
+      <c r="AF10" s="121"/>
+      <c r="AG10" s="121"/>
+      <c r="AH10" s="17"/>
+      <c r="AI10" s="26"/>
+      <c r="AL10" s="70">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="AM10" s="120"/>
+      <c r="AN10" s="17"/>
+      <c r="AO10" s="17"/>
+      <c r="AP10" s="17"/>
+      <c r="AQ10" s="17"/>
+      <c r="AR10" s="17"/>
+      <c r="AS10" s="17"/>
+      <c r="AT10" s="121"/>
+      <c r="AU10" s="121"/>
+      <c r="AV10" s="17"/>
+      <c r="AW10" s="17"/>
+      <c r="AX10" s="17"/>
+      <c r="AY10" s="17"/>
+      <c r="AZ10" s="17"/>
+      <c r="BA10" s="17"/>
+      <c r="BB10" s="123"/>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A11" s="70">
+        <f t="shared" si="18"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="75"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="76"/>
+      <c r="P11" s="76"/>
+      <c r="Q11" s="78"/>
+      <c r="S11" s="70">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="T11" s="16"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="121"/>
+      <c r="W11" s="121"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="121"/>
+      <c r="AB11" s="121"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="121"/>
+      <c r="AG11" s="121"/>
+      <c r="AH11" s="17"/>
+      <c r="AI11" s="26"/>
+      <c r="AL11" s="70">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="AM11" s="120"/>
+      <c r="AN11" s="17"/>
+      <c r="AO11" s="17"/>
+      <c r="AP11" s="17"/>
+      <c r="AQ11" s="17"/>
+      <c r="AR11" s="17"/>
+      <c r="AS11" s="17"/>
+      <c r="AT11" s="121"/>
+      <c r="AU11" s="121"/>
+      <c r="AV11" s="17"/>
+      <c r="AW11" s="17"/>
+      <c r="AX11" s="17"/>
+      <c r="AY11" s="17"/>
+      <c r="AZ11" s="17"/>
+      <c r="BA11" s="17"/>
+      <c r="BB11" s="123"/>
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A12" s="70">
+        <f t="shared" si="18"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="76"/>
+      <c r="P12" s="76"/>
+      <c r="Q12" s="78"/>
+      <c r="S12" s="70">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="T12" s="16"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="121"/>
+      <c r="W12" s="121"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+      <c r="AA12" s="121"/>
+      <c r="AB12" s="121"/>
+      <c r="AC12" s="17"/>
+      <c r="AD12" s="17"/>
+      <c r="AE12" s="17"/>
+      <c r="AF12" s="121"/>
+      <c r="AG12" s="121"/>
+      <c r="AH12" s="17"/>
+      <c r="AI12" s="26"/>
+      <c r="AL12" s="70">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="AM12" s="120"/>
+      <c r="AN12" s="17"/>
+      <c r="AO12" s="17"/>
+      <c r="AP12" s="17"/>
+      <c r="AQ12" s="17"/>
+      <c r="AR12" s="17"/>
+      <c r="AS12" s="17"/>
+      <c r="AT12" s="121"/>
+      <c r="AU12" s="121"/>
+      <c r="AV12" s="17"/>
+      <c r="AW12" s="17"/>
+      <c r="AX12" s="17"/>
+      <c r="AY12" s="17"/>
+      <c r="AZ12" s="17"/>
+      <c r="BA12" s="17"/>
+      <c r="BB12" s="123"/>
+    </row>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A13" s="70">
+        <f t="shared" si="18"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="75"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="76"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="76"/>
+      <c r="P13" s="76"/>
+      <c r="Q13" s="78"/>
+      <c r="S13" s="70">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="T13" s="16"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="121"/>
+      <c r="W13" s="121"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="121"/>
+      <c r="AB13" s="121"/>
+      <c r="AC13" s="17"/>
+      <c r="AD13" s="17"/>
+      <c r="AE13" s="17"/>
+      <c r="AF13" s="121"/>
+      <c r="AG13" s="121"/>
+      <c r="AH13" s="17"/>
+      <c r="AI13" s="26"/>
+      <c r="AL13" s="70">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="AM13" s="120"/>
+      <c r="AN13" s="17"/>
+      <c r="AO13" s="17"/>
+      <c r="AP13" s="17"/>
+      <c r="AQ13" s="17"/>
+      <c r="AR13" s="17"/>
+      <c r="AS13" s="17"/>
+      <c r="AT13" s="121"/>
+      <c r="AU13" s="121"/>
+      <c r="AV13" s="17"/>
+      <c r="AW13" s="17"/>
+      <c r="AX13" s="17"/>
+      <c r="AY13" s="17"/>
+      <c r="AZ13" s="17"/>
+      <c r="BA13" s="17"/>
+      <c r="BB13" s="123"/>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A14" s="70">
+        <f t="shared" si="18"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="79"/>
+      <c r="C14" s="77" t="s">
+        <v>255</v>
+      </c>
+      <c r="D14" s="77"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80" t="s">
+        <v>262</v>
+      </c>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="77"/>
+      <c r="P14" s="77" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q14" s="81"/>
+      <c r="S14" s="70">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="T14" s="16"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="121"/>
+      <c r="W14" s="121"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="121"/>
+      <c r="AB14" s="121"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="17"/>
+      <c r="AF14" s="121"/>
+      <c r="AG14" s="121"/>
+      <c r="AH14" s="17"/>
+      <c r="AI14" s="26"/>
+      <c r="AL14" s="70">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="AM14" s="120"/>
+      <c r="AN14" s="17"/>
+      <c r="AO14" s="17"/>
+      <c r="AP14" s="17"/>
+      <c r="AQ14" s="17"/>
+      <c r="AR14" s="17"/>
+      <c r="AS14" s="17"/>
+      <c r="AT14" s="121"/>
+      <c r="AU14" s="121"/>
+      <c r="AV14" s="17"/>
+      <c r="AW14" s="17"/>
+      <c r="AX14" s="17"/>
+      <c r="AY14" s="17"/>
+      <c r="AZ14" s="17"/>
+      <c r="BA14" s="17"/>
+      <c r="BB14" s="123"/>
+    </row>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A15" s="70">
+        <f t="shared" si="18"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="75"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="76"/>
+      <c r="N15" s="77"/>
+      <c r="O15" s="76"/>
+      <c r="P15" s="76"/>
+      <c r="Q15" s="78"/>
+      <c r="S15" s="70">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="T15" s="16"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="121"/>
+      <c r="W15" s="121"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="121"/>
+      <c r="AB15" s="121"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="17"/>
+      <c r="AF15" s="121"/>
+      <c r="AG15" s="121"/>
+      <c r="AH15" s="17"/>
+      <c r="AI15" s="26"/>
+      <c r="AL15" s="70">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="AM15" s="120"/>
+      <c r="AN15" s="17"/>
+      <c r="AO15" s="17"/>
+      <c r="AP15" s="17"/>
+      <c r="AQ15" s="17"/>
+      <c r="AR15" s="17"/>
+      <c r="AS15" s="17"/>
+      <c r="AT15" s="121"/>
+      <c r="AU15" s="121"/>
+      <c r="AV15" s="17"/>
+      <c r="AW15" s="17"/>
+      <c r="AX15" s="17"/>
+      <c r="AY15" s="17"/>
+      <c r="AZ15" s="17"/>
+      <c r="BA15" s="17"/>
+      <c r="BB15" s="123"/>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A16" s="70">
+        <f t="shared" si="18"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="75"/>
+      <c r="C16" s="76" t="s">
+        <v>247</v>
+      </c>
+      <c r="D16" s="76"/>
+      <c r="E16" s="77" t="s">
+        <v>255</v>
+      </c>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="76"/>
+      <c r="N16" s="77" t="s">
+        <v>256</v>
+      </c>
+      <c r="O16" s="76"/>
+      <c r="P16" s="76" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q16" s="78"/>
+      <c r="S16" s="70">
+        <f>+S17+1</f>
+        <v>1</v>
+      </c>
+      <c r="T16" s="16"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="121"/>
+      <c r="W16" s="121"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="121"/>
+      <c r="AB16" s="121"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="17"/>
+      <c r="AF16" s="121"/>
+      <c r="AG16" s="121"/>
+      <c r="AH16" s="17"/>
+      <c r="AI16" s="26"/>
+      <c r="AJ16" s="238"/>
+      <c r="AL16" s="70">
+        <f>+AL17+1</f>
+        <v>1</v>
+      </c>
+      <c r="AM16" s="120"/>
+      <c r="AN16" s="17"/>
+      <c r="AO16" s="17"/>
+      <c r="AP16" s="17"/>
+      <c r="AQ16" s="17"/>
+      <c r="AR16" s="17"/>
+      <c r="AS16" s="17"/>
+      <c r="AT16" s="121"/>
+      <c r="AU16" s="121"/>
+      <c r="AV16" s="17"/>
+      <c r="AW16" s="17"/>
+      <c r="AX16" s="17"/>
+      <c r="AY16" s="17"/>
+      <c r="AZ16" s="17"/>
+      <c r="BA16" s="17"/>
+      <c r="BB16" s="123"/>
+      <c r="BC16" s="238"/>
+    </row>
+    <row r="17" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A17" s="70">
+        <f t="shared" si="18"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="82"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="83"/>
+      <c r="N17" s="84"/>
+      <c r="O17" s="83"/>
+      <c r="P17" s="83"/>
+      <c r="Q17" s="85"/>
+      <c r="S17" s="70">
+        <v>0</v>
+      </c>
+      <c r="T17" s="32"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="124"/>
+      <c r="W17" s="124"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="124"/>
+      <c r="AB17" s="124"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="124"/>
+      <c r="AG17" s="124"/>
+      <c r="AH17" s="22"/>
+      <c r="AI17" s="33"/>
+      <c r="AJ17" s="238"/>
+      <c r="AL17" s="70">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="126"/>
+      <c r="AN17" s="22"/>
+      <c r="AO17" s="22"/>
+      <c r="AP17" s="22"/>
+      <c r="AQ17" s="22"/>
+      <c r="AR17" s="22"/>
+      <c r="AS17" s="22"/>
+      <c r="AT17" s="124"/>
+      <c r="AU17" s="124"/>
+      <c r="AV17" s="22"/>
+      <c r="AW17" s="22"/>
+      <c r="AX17" s="22"/>
+      <c r="AY17" s="22"/>
+      <c r="AZ17" s="22"/>
+      <c r="BA17" s="22"/>
+      <c r="BB17" s="125"/>
+      <c r="BC17" s="238"/>
+    </row>
+    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A18" s="70" t="s">
+        <v>395</v>
+      </c>
+      <c r="S18" s="70" t="s">
+        <v>425</v>
+      </c>
+      <c r="T18" s="25"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="20"/>
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="20"/>
+      <c r="AC18" s="20"/>
+      <c r="AD18" s="20"/>
+      <c r="AE18" s="20"/>
+      <c r="AF18" s="20"/>
+      <c r="AG18" s="20"/>
+      <c r="AH18" s="20"/>
+      <c r="AI18" s="31"/>
+      <c r="AL18" s="70" t="s">
+        <v>395</v>
+      </c>
+      <c r="AM18" s="118"/>
+      <c r="AN18" s="20"/>
+      <c r="AO18" s="20"/>
+      <c r="AP18" s="20"/>
+      <c r="AQ18" s="20"/>
+      <c r="AR18" s="20"/>
+      <c r="AS18" s="20"/>
+      <c r="AT18" s="20"/>
+      <c r="AU18" s="20"/>
+      <c r="AV18" s="20"/>
+      <c r="AW18" s="20"/>
+      <c r="AX18" s="20"/>
+      <c r="AY18" s="20"/>
+      <c r="AZ18" s="20"/>
+      <c r="BA18" s="20"/>
+      <c r="BB18" s="122"/>
+    </row>
+    <row r="19" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T19" s="16"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17"/>
+      <c r="AD19" s="17"/>
+      <c r="AE19" s="17"/>
+      <c r="AF19" s="17"/>
+      <c r="AG19" s="17"/>
+      <c r="AH19" s="17"/>
+      <c r="AI19" s="26"/>
+      <c r="AM19" s="120"/>
+      <c r="AN19" s="17"/>
+      <c r="AO19" s="17"/>
+      <c r="AP19" s="17"/>
+      <c r="AQ19" s="17"/>
+      <c r="AR19" s="17"/>
+      <c r="AS19" s="17"/>
+      <c r="AT19" s="17"/>
+      <c r="AU19" s="17"/>
+      <c r="AV19" s="17"/>
+      <c r="AW19" s="17"/>
+      <c r="AX19" s="17"/>
+      <c r="AY19" s="17"/>
+      <c r="AZ19" s="17"/>
+      <c r="BA19" s="17"/>
+      <c r="BB19" s="123"/>
+    </row>
+    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T20" s="16"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="17"/>
+      <c r="Z20" s="17"/>
+      <c r="AA20" s="17"/>
+      <c r="AB20" s="17"/>
+      <c r="AC20" s="17"/>
+      <c r="AD20" s="17"/>
+      <c r="AE20" s="17"/>
+      <c r="AF20" s="17"/>
+      <c r="AG20" s="17"/>
+      <c r="AH20" s="17"/>
+      <c r="AI20" s="26"/>
+      <c r="AM20" s="120"/>
+      <c r="AN20" s="17"/>
+      <c r="AO20" s="17"/>
+      <c r="AP20" s="17"/>
+      <c r="AQ20" s="17"/>
+      <c r="AR20" s="17"/>
+      <c r="AS20" s="17"/>
+      <c r="AT20" s="17"/>
+      <c r="AU20" s="17"/>
+      <c r="AV20" s="17"/>
+      <c r="AW20" s="17"/>
+      <c r="AX20" s="17"/>
+      <c r="AY20" s="17"/>
+      <c r="AZ20" s="17"/>
+      <c r="BA20" s="17"/>
+      <c r="BB20" s="123"/>
+    </row>
+    <row r="21" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T21" s="16"/>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="17"/>
+      <c r="Y21" s="17"/>
+      <c r="Z21" s="17"/>
+      <c r="AA21" s="17"/>
+      <c r="AB21" s="17"/>
+      <c r="AC21" s="17"/>
+      <c r="AD21" s="17"/>
+      <c r="AE21" s="17"/>
+      <c r="AF21" s="17"/>
+      <c r="AG21" s="17"/>
+      <c r="AH21" s="17"/>
+      <c r="AI21" s="26"/>
+      <c r="AM21" s="120"/>
+      <c r="AN21" s="17"/>
+      <c r="AO21" s="17"/>
+      <c r="AP21" s="17"/>
+      <c r="AQ21" s="17"/>
+      <c r="AR21" s="17"/>
+      <c r="AS21" s="17"/>
+      <c r="AT21" s="17"/>
+      <c r="AU21" s="17"/>
+      <c r="AV21" s="17"/>
+      <c r="AW21" s="17"/>
+      <c r="AX21" s="17"/>
+      <c r="AY21" s="17"/>
+      <c r="AZ21" s="17"/>
+      <c r="BA21" s="17"/>
+      <c r="BB21" s="123"/>
+    </row>
+    <row r="22" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T22" s="16"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+      <c r="W22" s="17"/>
+      <c r="X22" s="17"/>
+      <c r="Y22" s="17"/>
+      <c r="Z22" s="17"/>
+      <c r="AA22" s="17"/>
+      <c r="AB22" s="17"/>
+      <c r="AC22" s="17"/>
+      <c r="AD22" s="17"/>
+      <c r="AE22" s="17"/>
+      <c r="AF22" s="17"/>
+      <c r="AG22" s="17"/>
+      <c r="AH22" s="17"/>
+      <c r="AI22" s="26"/>
+      <c r="AM22" s="120"/>
+      <c r="AN22" s="17"/>
+      <c r="AO22" s="17"/>
+      <c r="AP22" s="17"/>
+      <c r="AQ22" s="17"/>
+      <c r="AR22" s="17"/>
+      <c r="AS22" s="17"/>
+      <c r="AT22" s="17"/>
+      <c r="AU22" s="17"/>
+      <c r="AV22" s="17"/>
+      <c r="AW22" s="17"/>
+      <c r="AX22" s="17"/>
+      <c r="AY22" s="17"/>
+      <c r="AZ22" s="17"/>
+      <c r="BA22" s="17"/>
+      <c r="BB22" s="123"/>
+    </row>
+    <row r="23" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T23" s="16"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="17"/>
+      <c r="X23" s="17"/>
+      <c r="Y23" s="17"/>
+      <c r="Z23" s="17"/>
+      <c r="AA23" s="17"/>
+      <c r="AB23" s="17"/>
+      <c r="AC23" s="17"/>
+      <c r="AD23" s="17"/>
+      <c r="AE23" s="17"/>
+      <c r="AF23" s="17"/>
+      <c r="AG23" s="17"/>
+      <c r="AH23" s="17"/>
+      <c r="AI23" s="26"/>
+      <c r="AM23" s="120"/>
+      <c r="AN23" s="17"/>
+      <c r="AO23" s="17"/>
+      <c r="AP23" s="17"/>
+      <c r="AQ23" s="17"/>
+      <c r="AR23" s="17"/>
+      <c r="AS23" s="17"/>
+      <c r="AT23" s="17"/>
+      <c r="AU23" s="17"/>
+      <c r="AV23" s="17"/>
+      <c r="AW23" s="17"/>
+      <c r="AX23" s="17"/>
+      <c r="AY23" s="17"/>
+      <c r="AZ23" s="17"/>
+      <c r="BA23" s="17"/>
+      <c r="BB23" s="123"/>
+    </row>
+    <row r="24" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T24" s="16"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+      <c r="W24" s="17"/>
+      <c r="X24" s="17"/>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="17"/>
+      <c r="AA24" s="17"/>
+      <c r="AB24" s="17"/>
+      <c r="AC24" s="17"/>
+      <c r="AD24" s="17"/>
+      <c r="AE24" s="17"/>
+      <c r="AF24" s="17"/>
+      <c r="AG24" s="17"/>
+      <c r="AH24" s="17"/>
+      <c r="AI24" s="26"/>
+      <c r="AM24" s="120"/>
+      <c r="AN24" s="6"/>
+      <c r="AO24" s="6"/>
+      <c r="AP24" s="6"/>
+      <c r="AQ24" s="6"/>
+      <c r="AR24" s="6"/>
+      <c r="AS24" s="6"/>
+      <c r="AT24" s="6"/>
+      <c r="AU24" s="6"/>
+      <c r="AV24" s="6"/>
+      <c r="AW24" s="6"/>
+      <c r="AX24" s="6"/>
+      <c r="AY24" s="6"/>
+      <c r="AZ24" s="6"/>
+      <c r="BA24" s="6"/>
+      <c r="BB24" s="123"/>
+    </row>
+    <row r="25" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T25" s="16"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="17"/>
+      <c r="AA25" s="17"/>
+      <c r="AB25" s="17"/>
+      <c r="AC25" s="17"/>
+      <c r="AD25" s="17"/>
+      <c r="AE25" s="17"/>
+      <c r="AF25" s="17"/>
+      <c r="AG25" s="17"/>
+      <c r="AH25" s="17"/>
+      <c r="AI25" s="26"/>
+      <c r="AM25" s="120"/>
+      <c r="AN25" s="17"/>
+      <c r="AO25" s="121"/>
+      <c r="AP25" s="121"/>
+      <c r="AQ25" s="17"/>
+      <c r="AR25" s="17"/>
+      <c r="AS25" s="17"/>
+      <c r="AT25" s="121"/>
+      <c r="AU25" s="121"/>
+      <c r="AV25" s="17"/>
+      <c r="AW25" s="17"/>
+      <c r="AX25" s="17"/>
+      <c r="AY25" s="121"/>
+      <c r="AZ25" s="121"/>
+      <c r="BA25" s="17"/>
+      <c r="BB25" s="123"/>
+    </row>
+    <row r="26" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T26" s="16"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+      <c r="Y26" s="17"/>
+      <c r="Z26" s="17"/>
+      <c r="AA26" s="17"/>
+      <c r="AB26" s="17"/>
+      <c r="AC26" s="17"/>
+      <c r="AD26" s="17"/>
+      <c r="AE26" s="17"/>
+      <c r="AF26" s="17"/>
+      <c r="AG26" s="17"/>
+      <c r="AH26" s="17"/>
+      <c r="AI26" s="26"/>
+      <c r="AM26" s="120"/>
+      <c r="AN26" s="17"/>
+      <c r="AO26" s="121"/>
+      <c r="AP26" s="121"/>
+      <c r="AQ26" s="17"/>
+      <c r="AR26" s="17"/>
+      <c r="AS26" s="17"/>
+      <c r="AT26" s="121"/>
+      <c r="AU26" s="121"/>
+      <c r="AV26" s="17"/>
+      <c r="AW26" s="17"/>
+      <c r="AX26" s="17"/>
+      <c r="AY26" s="121"/>
+      <c r="AZ26" s="121"/>
+      <c r="BA26" s="17"/>
+      <c r="BB26" s="123"/>
+    </row>
+    <row r="27" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T27" s="16"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="17"/>
+      <c r="Y27" s="17"/>
+      <c r="Z27" s="17"/>
+      <c r="AA27" s="17"/>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="17"/>
+      <c r="AD27" s="17"/>
+      <c r="AE27" s="17"/>
+      <c r="AF27" s="17"/>
+      <c r="AG27" s="17"/>
+      <c r="AH27" s="17"/>
+      <c r="AI27" s="26"/>
+      <c r="AM27" s="120"/>
+      <c r="AN27" s="17"/>
+      <c r="AO27" s="17"/>
+      <c r="AP27" s="17"/>
+      <c r="AQ27" s="17"/>
+      <c r="AR27" s="17"/>
+      <c r="AS27" s="17"/>
+      <c r="AT27" s="17"/>
+      <c r="AU27" s="17"/>
+      <c r="AV27" s="17"/>
+      <c r="AW27" s="17"/>
+      <c r="AX27" s="17"/>
+      <c r="AY27" s="17"/>
+      <c r="AZ27" s="17"/>
+      <c r="BA27" s="17"/>
+      <c r="BB27" s="123"/>
+    </row>
+    <row r="28" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T28" s="16"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="17"/>
+      <c r="AC28" s="17"/>
+      <c r="AD28" s="17"/>
+      <c r="AE28" s="17"/>
+      <c r="AF28" s="17"/>
+      <c r="AG28" s="17"/>
+      <c r="AH28" s="17"/>
+      <c r="AI28" s="26"/>
+      <c r="AM28" s="120"/>
+      <c r="AN28" s="17"/>
+      <c r="AO28" s="17"/>
+      <c r="AP28" s="17"/>
+      <c r="AQ28" s="17"/>
+      <c r="AR28" s="17"/>
+      <c r="AS28" s="17"/>
+      <c r="AT28" s="17"/>
+      <c r="AU28" s="17"/>
+      <c r="AV28" s="17"/>
+      <c r="AW28" s="17"/>
+      <c r="AX28" s="17"/>
+      <c r="AY28" s="17"/>
+      <c r="AZ28" s="17"/>
+      <c r="BA28" s="17"/>
+      <c r="BB28" s="123"/>
+    </row>
+    <row r="29" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T29" s="16"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="17"/>
+      <c r="X29" s="17"/>
+      <c r="Y29" s="17"/>
+      <c r="Z29" s="17"/>
+      <c r="AA29" s="17"/>
+      <c r="AB29" s="17"/>
+      <c r="AC29" s="17"/>
+      <c r="AD29" s="17"/>
+      <c r="AE29" s="17"/>
+      <c r="AF29" s="17"/>
+      <c r="AG29" s="17"/>
+      <c r="AH29" s="17"/>
+      <c r="AI29" s="26"/>
+      <c r="AM29" s="120"/>
+      <c r="AN29" s="17"/>
+      <c r="AO29" s="17"/>
+      <c r="AP29" s="17"/>
+      <c r="AQ29" s="17"/>
+      <c r="AR29" s="17"/>
+      <c r="AS29" s="17"/>
+      <c r="AT29" s="17"/>
+      <c r="AU29" s="17"/>
+      <c r="AV29" s="17"/>
+      <c r="AW29" s="17"/>
+      <c r="AX29" s="17"/>
+      <c r="AY29" s="17"/>
+      <c r="AZ29" s="17"/>
+      <c r="BA29" s="17"/>
+      <c r="BB29" s="123"/>
+    </row>
+    <row r="30" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T30" s="16"/>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="17"/>
+      <c r="Y30" s="17"/>
+      <c r="Z30" s="17"/>
+      <c r="AA30" s="17"/>
+      <c r="AB30" s="17"/>
+      <c r="AC30" s="17"/>
+      <c r="AD30" s="17"/>
+      <c r="AE30" s="17"/>
+      <c r="AF30" s="17"/>
+      <c r="AG30" s="17"/>
+      <c r="AH30" s="17"/>
+      <c r="AI30" s="26"/>
+      <c r="AM30" s="120"/>
+      <c r="AN30" s="17"/>
+      <c r="AO30" s="17"/>
+      <c r="AP30" s="17"/>
+      <c r="AQ30" s="17"/>
+      <c r="AR30" s="17"/>
+      <c r="AS30" s="17"/>
+      <c r="AT30" s="17"/>
+      <c r="AU30" s="17"/>
+      <c r="AV30" s="17"/>
+      <c r="AW30" s="17"/>
+      <c r="AX30" s="17"/>
+      <c r="AY30" s="17"/>
+      <c r="AZ30" s="17"/>
+      <c r="BA30" s="17"/>
+      <c r="BB30" s="123"/>
+    </row>
+    <row r="31" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T31" s="16"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
+      <c r="AA31" s="17"/>
+      <c r="AB31" s="17"/>
+      <c r="AC31" s="17"/>
+      <c r="AD31" s="17"/>
+      <c r="AE31" s="17"/>
+      <c r="AF31" s="17"/>
+      <c r="AG31" s="17"/>
+      <c r="AH31" s="17"/>
+      <c r="AI31" s="26"/>
+      <c r="AM31" s="120"/>
+      <c r="AN31" s="17"/>
+      <c r="AO31" s="17"/>
+      <c r="AP31" s="17"/>
+      <c r="AQ31" s="17"/>
+      <c r="AR31" s="17"/>
+      <c r="AS31" s="17"/>
+      <c r="AT31" s="17"/>
+      <c r="AU31" s="17"/>
+      <c r="AV31" s="17"/>
+      <c r="AW31" s="17"/>
+      <c r="AX31" s="17"/>
+      <c r="AY31" s="17"/>
+      <c r="AZ31" s="17"/>
+      <c r="BA31" s="17"/>
+      <c r="BB31" s="123"/>
+    </row>
+    <row r="32" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="T32" s="16"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
+      <c r="AA32" s="17"/>
+      <c r="AB32" s="17"/>
+      <c r="AC32" s="17"/>
+      <c r="AD32" s="17"/>
+      <c r="AE32" s="17"/>
+      <c r="AF32" s="17"/>
+      <c r="AG32" s="17"/>
+      <c r="AH32" s="17"/>
+      <c r="AI32" s="26"/>
+      <c r="AM32" s="120"/>
+      <c r="AN32" s="17"/>
+      <c r="AO32" s="17"/>
+      <c r="AP32" s="17"/>
+      <c r="AQ32" s="17"/>
+      <c r="AR32" s="17"/>
+      <c r="AS32" s="17"/>
+      <c r="AT32" s="17"/>
+      <c r="AU32" s="17"/>
+      <c r="AV32" s="17"/>
+      <c r="AW32" s="17"/>
+      <c r="AX32" s="17"/>
+      <c r="AY32" s="17"/>
+      <c r="AZ32" s="17"/>
+      <c r="BA32" s="17"/>
+      <c r="BB32" s="123"/>
+    </row>
+    <row r="33" spans="20:54" x14ac:dyDescent="0.3">
+      <c r="T33" s="32"/>
+      <c r="U33" s="22"/>
+      <c r="V33" s="22"/>
+      <c r="W33" s="22"/>
+      <c r="X33" s="22"/>
+      <c r="Y33" s="22"/>
+      <c r="Z33" s="22"/>
+      <c r="AA33" s="22"/>
+      <c r="AB33" s="22"/>
+      <c r="AC33" s="22"/>
+      <c r="AD33" s="22"/>
+      <c r="AE33" s="22"/>
+      <c r="AF33" s="22"/>
+      <c r="AG33" s="22"/>
+      <c r="AH33" s="22"/>
+      <c r="AI33" s="33"/>
+      <c r="AM33" s="126"/>
+      <c r="AN33" s="22"/>
+      <c r="AO33" s="22"/>
+      <c r="AP33" s="22"/>
+      <c r="AQ33" s="22"/>
+      <c r="AR33" s="22"/>
+      <c r="AS33" s="22"/>
+      <c r="AT33" s="22"/>
+      <c r="AU33" s="22"/>
+      <c r="AV33" s="22"/>
+      <c r="AW33" s="22"/>
+      <c r="AX33" s="22"/>
+      <c r="AY33" s="22"/>
+      <c r="AZ33" s="22"/>
+      <c r="BA33" s="22"/>
+      <c r="BB33" s="125"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Foliage in the natural areas Smooth snow on top of the world Adding residential and rural areas from Conurbation next
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="22" activeTab="34"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="22" activeTab="35"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -42,6 +42,7 @@
     <sheet name="Intersections" sheetId="41" r:id="rId33"/>
     <sheet name="Tunnels" sheetId="42" r:id="rId34"/>
     <sheet name="Bridge" sheetId="43" r:id="rId35"/>
+    <sheet name="Sheet2" sheetId="44" r:id="rId36"/>
   </sheets>
   <definedNames>
     <definedName name="AbsoluteMaximumFloorsBelow">Sheet3!$C$6</definedName>
@@ -3331,7 +3332,7 @@
       </c>
       <c r="O6">
         <f t="shared" ref="O6:AB15" ca="1" si="8">IF(AND(MOD(O$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3351,7 +3352,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3861,7 +3862,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3921,7 +3922,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4431,7 +4432,7 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:N29" ca="1" si="11">IF(AND(MOD(E$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4451,7 +4452,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4491,7 +4492,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4511,7 +4512,7 @@
       </c>
       <c r="Y16">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5001,7 +5002,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5041,7 +5042,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5061,7 +5062,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5081,7 +5082,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5571,7 +5572,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5591,7 +5592,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5631,7 +5632,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5651,7 +5652,7 @@
       </c>
       <c r="Y26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -35967,10 +35968,10 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:BP17"/>
+  <dimension ref="B2:BP34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BU18" sqref="BU18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37030,6 +37031,550 @@
       <c r="BN17" s="147"/>
       <c r="BO17" s="147"/>
       <c r="BP17" s="148"/>
+    </row>
+    <row r="19" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ19" s="144"/>
+      <c r="AK19" s="143"/>
+      <c r="AL19" s="143"/>
+      <c r="AM19" s="143"/>
+      <c r="AN19" s="143"/>
+      <c r="AO19" s="143"/>
+      <c r="AP19" s="194"/>
+      <c r="AQ19" s="131"/>
+      <c r="AR19" s="131"/>
+      <c r="AS19" s="194"/>
+      <c r="AT19" s="143"/>
+      <c r="AU19" s="143"/>
+      <c r="AV19" s="143"/>
+      <c r="AW19" s="143"/>
+      <c r="AX19" s="143"/>
+      <c r="AY19" s="145"/>
+      <c r="BA19" s="144"/>
+      <c r="BB19" s="143"/>
+      <c r="BC19" s="143"/>
+      <c r="BD19" s="143"/>
+      <c r="BE19" s="143"/>
+      <c r="BF19" s="143"/>
+      <c r="BG19" s="194"/>
+      <c r="BH19" s="131"/>
+      <c r="BI19" s="131"/>
+      <c r="BJ19" s="194"/>
+      <c r="BK19" s="143"/>
+      <c r="BL19" s="143"/>
+      <c r="BM19" s="143"/>
+      <c r="BN19" s="143"/>
+      <c r="BO19" s="143"/>
+      <c r="BP19" s="145"/>
+    </row>
+    <row r="20" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ20" s="149"/>
+      <c r="AK20" s="17"/>
+      <c r="AL20" s="17"/>
+      <c r="AM20" s="17"/>
+      <c r="AN20" s="17"/>
+      <c r="AO20" s="17"/>
+      <c r="AP20" s="128"/>
+      <c r="AQ20" s="128"/>
+      <c r="AR20" s="128"/>
+      <c r="AS20" s="128"/>
+      <c r="AT20" s="17"/>
+      <c r="AU20" s="17"/>
+      <c r="AV20" s="17"/>
+      <c r="AW20" s="17"/>
+      <c r="AX20" s="17"/>
+      <c r="AY20" s="150"/>
+      <c r="BA20" s="149"/>
+      <c r="BB20" s="17"/>
+      <c r="BC20" s="17"/>
+      <c r="BD20" s="17"/>
+      <c r="BE20" s="17"/>
+      <c r="BF20" s="17"/>
+      <c r="BG20" s="128"/>
+      <c r="BH20" s="128"/>
+      <c r="BI20" s="128"/>
+      <c r="BJ20" s="128"/>
+      <c r="BK20" s="17"/>
+      <c r="BL20" s="17"/>
+      <c r="BM20" s="17"/>
+      <c r="BN20" s="17"/>
+      <c r="BO20" s="17"/>
+      <c r="BP20" s="150"/>
+    </row>
+    <row r="21" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ21" s="149"/>
+      <c r="AK21" s="17"/>
+      <c r="AL21" s="17"/>
+      <c r="AM21" s="17"/>
+      <c r="AN21" s="17"/>
+      <c r="AO21" s="128"/>
+      <c r="AP21" s="128"/>
+      <c r="AQ21" s="128"/>
+      <c r="AR21" s="128"/>
+      <c r="AS21" s="17"/>
+      <c r="AT21" s="17"/>
+      <c r="AU21" s="17"/>
+      <c r="AV21" s="17"/>
+      <c r="AW21" s="17"/>
+      <c r="AX21" s="17"/>
+      <c r="AY21" s="150"/>
+      <c r="BA21" s="149"/>
+      <c r="BB21" s="17"/>
+      <c r="BC21" s="17"/>
+      <c r="BD21" s="17"/>
+      <c r="BE21" s="17"/>
+      <c r="BF21" s="17"/>
+      <c r="BG21" s="17"/>
+      <c r="BH21" s="128"/>
+      <c r="BI21" s="128"/>
+      <c r="BJ21" s="128"/>
+      <c r="BK21" s="128"/>
+      <c r="BL21" s="17"/>
+      <c r="BM21" s="17"/>
+      <c r="BN21" s="17"/>
+      <c r="BO21" s="17"/>
+      <c r="BP21" s="150"/>
+    </row>
+    <row r="22" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ22" s="149"/>
+      <c r="AK22" s="17"/>
+      <c r="AL22" s="17"/>
+      <c r="AM22" s="17"/>
+      <c r="AN22" s="128"/>
+      <c r="AO22" s="128"/>
+      <c r="AP22" s="128"/>
+      <c r="AQ22" s="128"/>
+      <c r="AR22" s="17"/>
+      <c r="AS22" s="17"/>
+      <c r="AT22" s="17"/>
+      <c r="AU22" s="17"/>
+      <c r="AV22" s="17"/>
+      <c r="AW22" s="17"/>
+      <c r="AX22" s="17"/>
+      <c r="AY22" s="150"/>
+      <c r="BA22" s="149"/>
+      <c r="BB22" s="17"/>
+      <c r="BC22" s="17"/>
+      <c r="BD22" s="17"/>
+      <c r="BE22" s="17"/>
+      <c r="BF22" s="17"/>
+      <c r="BG22" s="17"/>
+      <c r="BH22" s="17"/>
+      <c r="BI22" s="128"/>
+      <c r="BJ22" s="128"/>
+      <c r="BK22" s="128"/>
+      <c r="BL22" s="128"/>
+      <c r="BM22" s="17"/>
+      <c r="BN22" s="17"/>
+      <c r="BO22" s="17"/>
+      <c r="BP22" s="150"/>
+    </row>
+    <row r="23" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ23" s="149"/>
+      <c r="AK23" s="17"/>
+      <c r="AL23" s="17"/>
+      <c r="AM23" s="128"/>
+      <c r="AN23" s="128"/>
+      <c r="AO23" s="128"/>
+      <c r="AP23" s="128"/>
+      <c r="AQ23" s="17"/>
+      <c r="AR23" s="17"/>
+      <c r="AS23" s="17"/>
+      <c r="AT23" s="17"/>
+      <c r="AU23" s="17"/>
+      <c r="AV23" s="17"/>
+      <c r="AW23" s="17"/>
+      <c r="AX23" s="17"/>
+      <c r="AY23" s="150"/>
+      <c r="BA23" s="149"/>
+      <c r="BB23" s="17"/>
+      <c r="BC23" s="17"/>
+      <c r="BD23" s="17"/>
+      <c r="BE23" s="17"/>
+      <c r="BF23" s="17"/>
+      <c r="BG23" s="17"/>
+      <c r="BH23" s="17"/>
+      <c r="BI23" s="17"/>
+      <c r="BJ23" s="128"/>
+      <c r="BK23" s="128"/>
+      <c r="BL23" s="128"/>
+      <c r="BM23" s="128"/>
+      <c r="BN23" s="17"/>
+      <c r="BO23" s="17"/>
+      <c r="BP23" s="150"/>
+    </row>
+    <row r="24" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ24" s="149"/>
+      <c r="AK24" s="17"/>
+      <c r="AL24" s="128"/>
+      <c r="AM24" s="128"/>
+      <c r="AN24" s="128"/>
+      <c r="AO24" s="128"/>
+      <c r="AP24" s="17"/>
+      <c r="AQ24" s="17"/>
+      <c r="AR24" s="17"/>
+      <c r="AS24" s="17"/>
+      <c r="AT24" s="17"/>
+      <c r="AU24" s="17"/>
+      <c r="AV24" s="17"/>
+      <c r="AW24" s="17"/>
+      <c r="AX24" s="17"/>
+      <c r="AY24" s="150"/>
+      <c r="BA24" s="149"/>
+      <c r="BB24" s="17"/>
+      <c r="BC24" s="17"/>
+      <c r="BD24" s="17"/>
+      <c r="BE24" s="17"/>
+      <c r="BF24" s="17"/>
+      <c r="BG24" s="17"/>
+      <c r="BH24" s="17"/>
+      <c r="BI24" s="17"/>
+      <c r="BJ24" s="17"/>
+      <c r="BK24" s="128"/>
+      <c r="BL24" s="128"/>
+      <c r="BM24" s="128"/>
+      <c r="BN24" s="128"/>
+      <c r="BO24" s="17"/>
+      <c r="BP24" s="150"/>
+    </row>
+    <row r="25" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ25" s="196"/>
+      <c r="AK25" s="128"/>
+      <c r="AL25" s="128"/>
+      <c r="AM25" s="128"/>
+      <c r="AN25" s="128"/>
+      <c r="AO25" s="17"/>
+      <c r="AP25" s="17"/>
+      <c r="AQ25" s="17"/>
+      <c r="AR25" s="17"/>
+      <c r="AS25" s="17"/>
+      <c r="AT25" s="17"/>
+      <c r="AU25" s="17"/>
+      <c r="AV25" s="17"/>
+      <c r="AW25" s="17"/>
+      <c r="AX25" s="128"/>
+      <c r="AY25" s="197"/>
+      <c r="BA25" s="196"/>
+      <c r="BB25" s="128"/>
+      <c r="BC25" s="17"/>
+      <c r="BD25" s="17"/>
+      <c r="BE25" s="17"/>
+      <c r="BF25" s="17"/>
+      <c r="BG25" s="17"/>
+      <c r="BH25" s="17"/>
+      <c r="BI25" s="17"/>
+      <c r="BJ25" s="17"/>
+      <c r="BK25" s="17"/>
+      <c r="BL25" s="128"/>
+      <c r="BM25" s="128"/>
+      <c r="BN25" s="128"/>
+      <c r="BO25" s="128"/>
+      <c r="BP25" s="197"/>
+    </row>
+    <row r="26" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ26" s="127"/>
+      <c r="AK26" s="128"/>
+      <c r="AL26" s="128"/>
+      <c r="AM26" s="128"/>
+      <c r="AN26" s="17"/>
+      <c r="AO26" s="17"/>
+      <c r="AP26" s="17"/>
+      <c r="AQ26" s="17"/>
+      <c r="AR26" s="17"/>
+      <c r="AS26" s="17"/>
+      <c r="AT26" s="17"/>
+      <c r="AU26" s="17"/>
+      <c r="AV26" s="17"/>
+      <c r="AW26" s="128"/>
+      <c r="AX26" s="128"/>
+      <c r="AY26" s="130"/>
+      <c r="BA26" s="127"/>
+      <c r="BB26" s="128"/>
+      <c r="BC26" s="128"/>
+      <c r="BD26" s="17"/>
+      <c r="BE26" s="17"/>
+      <c r="BF26" s="17"/>
+      <c r="BG26" s="17"/>
+      <c r="BH26" s="17"/>
+      <c r="BI26" s="17"/>
+      <c r="BJ26" s="17"/>
+      <c r="BK26" s="17"/>
+      <c r="BL26" s="17"/>
+      <c r="BM26" s="128"/>
+      <c r="BN26" s="128"/>
+      <c r="BO26" s="128"/>
+      <c r="BP26" s="130"/>
+    </row>
+    <row r="27" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ27" s="127"/>
+      <c r="AK27" s="128"/>
+      <c r="AL27" s="128"/>
+      <c r="AM27" s="17"/>
+      <c r="AN27" s="17"/>
+      <c r="AO27" s="17"/>
+      <c r="AP27" s="17"/>
+      <c r="AQ27" s="17"/>
+      <c r="AR27" s="17"/>
+      <c r="AS27" s="17"/>
+      <c r="AT27" s="17"/>
+      <c r="AU27" s="17"/>
+      <c r="AV27" s="128"/>
+      <c r="AW27" s="128"/>
+      <c r="AX27" s="128"/>
+      <c r="AY27" s="130"/>
+      <c r="BA27" s="127"/>
+      <c r="BB27" s="128"/>
+      <c r="BC27" s="128"/>
+      <c r="BD27" s="128"/>
+      <c r="BE27" s="17"/>
+      <c r="BF27" s="17"/>
+      <c r="BG27" s="17"/>
+      <c r="BH27" s="17"/>
+      <c r="BI27" s="17"/>
+      <c r="BJ27" s="17"/>
+      <c r="BK27" s="17"/>
+      <c r="BL27" s="17"/>
+      <c r="BM27" s="17"/>
+      <c r="BN27" s="128"/>
+      <c r="BO27" s="128"/>
+      <c r="BP27" s="130"/>
+    </row>
+    <row r="28" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ28" s="196"/>
+      <c r="AK28" s="128"/>
+      <c r="AL28" s="17"/>
+      <c r="AM28" s="17"/>
+      <c r="AN28" s="17"/>
+      <c r="AO28" s="17"/>
+      <c r="AP28" s="17"/>
+      <c r="AQ28" s="17"/>
+      <c r="AR28" s="17"/>
+      <c r="AS28" s="17"/>
+      <c r="AT28" s="17"/>
+      <c r="AU28" s="128"/>
+      <c r="AV28" s="128"/>
+      <c r="AW28" s="128"/>
+      <c r="AX28" s="128"/>
+      <c r="AY28" s="197"/>
+      <c r="BA28" s="196"/>
+      <c r="BB28" s="128"/>
+      <c r="BC28" s="128"/>
+      <c r="BD28" s="128"/>
+      <c r="BE28" s="128"/>
+      <c r="BF28" s="17"/>
+      <c r="BG28" s="17"/>
+      <c r="BH28" s="17"/>
+      <c r="BI28" s="17"/>
+      <c r="BJ28" s="17"/>
+      <c r="BK28" s="17"/>
+      <c r="BL28" s="17"/>
+      <c r="BM28" s="17"/>
+      <c r="BN28" s="17"/>
+      <c r="BO28" s="128"/>
+      <c r="BP28" s="197"/>
+    </row>
+    <row r="29" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ29" s="149"/>
+      <c r="AK29" s="17"/>
+      <c r="AL29" s="17"/>
+      <c r="AM29" s="17"/>
+      <c r="AN29" s="17"/>
+      <c r="AO29" s="17"/>
+      <c r="AP29" s="17"/>
+      <c r="AQ29" s="17"/>
+      <c r="AR29" s="17"/>
+      <c r="AS29" s="17"/>
+      <c r="AT29" s="128"/>
+      <c r="AU29" s="128"/>
+      <c r="AV29" s="128"/>
+      <c r="AW29" s="128"/>
+      <c r="AX29" s="17"/>
+      <c r="AY29" s="150"/>
+      <c r="BA29" s="149"/>
+      <c r="BB29" s="17"/>
+      <c r="BC29" s="128"/>
+      <c r="BD29" s="128"/>
+      <c r="BE29" s="128"/>
+      <c r="BF29" s="128"/>
+      <c r="BG29" s="17"/>
+      <c r="BH29" s="17"/>
+      <c r="BI29" s="17"/>
+      <c r="BJ29" s="17"/>
+      <c r="BK29" s="17"/>
+      <c r="BL29" s="17"/>
+      <c r="BM29" s="17"/>
+      <c r="BN29" s="17"/>
+      <c r="BO29" s="17"/>
+      <c r="BP29" s="150"/>
+    </row>
+    <row r="30" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ30" s="149"/>
+      <c r="AK30" s="17"/>
+      <c r="AL30" s="17"/>
+      <c r="AM30" s="17"/>
+      <c r="AN30" s="17"/>
+      <c r="AO30" s="17"/>
+      <c r="AP30" s="17"/>
+      <c r="AQ30" s="17"/>
+      <c r="AR30" s="17"/>
+      <c r="AS30" s="128"/>
+      <c r="AT30" s="128"/>
+      <c r="AU30" s="128"/>
+      <c r="AV30" s="128"/>
+      <c r="AW30" s="17"/>
+      <c r="AX30" s="17"/>
+      <c r="AY30" s="150"/>
+      <c r="BA30" s="149"/>
+      <c r="BB30" s="17"/>
+      <c r="BC30" s="17"/>
+      <c r="BD30" s="128"/>
+      <c r="BE30" s="128"/>
+      <c r="BF30" s="128"/>
+      <c r="BG30" s="128"/>
+      <c r="BH30" s="17"/>
+      <c r="BI30" s="17"/>
+      <c r="BJ30" s="17"/>
+      <c r="BK30" s="17"/>
+      <c r="BL30" s="17"/>
+      <c r="BM30" s="17"/>
+      <c r="BN30" s="17"/>
+      <c r="BO30" s="17"/>
+      <c r="BP30" s="150"/>
+    </row>
+    <row r="31" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ31" s="149"/>
+      <c r="AK31" s="17"/>
+      <c r="AL31" s="17"/>
+      <c r="AM31" s="17"/>
+      <c r="AN31" s="17"/>
+      <c r="AO31" s="17"/>
+      <c r="AP31" s="17"/>
+      <c r="AQ31" s="17"/>
+      <c r="AR31" s="128"/>
+      <c r="AS31" s="128"/>
+      <c r="AT31" s="128"/>
+      <c r="AU31" s="128"/>
+      <c r="AV31" s="17"/>
+      <c r="AW31" s="17"/>
+      <c r="AX31" s="17"/>
+      <c r="AY31" s="150"/>
+      <c r="BA31" s="149"/>
+      <c r="BB31" s="17"/>
+      <c r="BC31" s="17"/>
+      <c r="BD31" s="17"/>
+      <c r="BE31" s="128"/>
+      <c r="BF31" s="128"/>
+      <c r="BG31" s="128"/>
+      <c r="BH31" s="128"/>
+      <c r="BI31" s="17"/>
+      <c r="BJ31" s="17"/>
+      <c r="BK31" s="17"/>
+      <c r="BL31" s="17"/>
+      <c r="BM31" s="17"/>
+      <c r="BN31" s="17"/>
+      <c r="BO31" s="17"/>
+      <c r="BP31" s="150"/>
+    </row>
+    <row r="32" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="AJ32" s="149"/>
+      <c r="AK32" s="17"/>
+      <c r="AL32" s="17"/>
+      <c r="AM32" s="17"/>
+      <c r="AN32" s="17"/>
+      <c r="AO32" s="17"/>
+      <c r="AP32" s="17"/>
+      <c r="AQ32" s="128"/>
+      <c r="AR32" s="128"/>
+      <c r="AS32" s="128"/>
+      <c r="AT32" s="128"/>
+      <c r="AU32" s="17"/>
+      <c r="AV32" s="17"/>
+      <c r="AW32" s="17"/>
+      <c r="AX32" s="17"/>
+      <c r="AY32" s="150"/>
+      <c r="BA32" s="149"/>
+      <c r="BB32" s="17"/>
+      <c r="BC32" s="17"/>
+      <c r="BD32" s="17"/>
+      <c r="BE32" s="17"/>
+      <c r="BF32" s="128"/>
+      <c r="BG32" s="128"/>
+      <c r="BH32" s="128"/>
+      <c r="BI32" s="128"/>
+      <c r="BJ32" s="17"/>
+      <c r="BK32" s="17"/>
+      <c r="BL32" s="17"/>
+      <c r="BM32" s="17"/>
+      <c r="BN32" s="17"/>
+      <c r="BO32" s="17"/>
+      <c r="BP32" s="150"/>
+    </row>
+    <row r="33" spans="36:68" x14ac:dyDescent="0.3">
+      <c r="AJ33" s="149"/>
+      <c r="AK33" s="17"/>
+      <c r="AL33" s="17"/>
+      <c r="AM33" s="17"/>
+      <c r="AN33" s="17"/>
+      <c r="AO33" s="17"/>
+      <c r="AP33" s="128"/>
+      <c r="AQ33" s="128"/>
+      <c r="AR33" s="128"/>
+      <c r="AS33" s="128"/>
+      <c r="AT33" s="17"/>
+      <c r="AU33" s="17"/>
+      <c r="AV33" s="17"/>
+      <c r="AW33" s="17"/>
+      <c r="AX33" s="17"/>
+      <c r="AY33" s="150"/>
+      <c r="BA33" s="149"/>
+      <c r="BB33" s="17"/>
+      <c r="BC33" s="17"/>
+      <c r="BD33" s="17"/>
+      <c r="BE33" s="17"/>
+      <c r="BF33" s="17"/>
+      <c r="BG33" s="128"/>
+      <c r="BH33" s="128"/>
+      <c r="BI33" s="128"/>
+      <c r="BJ33" s="128"/>
+      <c r="BK33" s="17"/>
+      <c r="BL33" s="17"/>
+      <c r="BM33" s="17"/>
+      <c r="BN33" s="17"/>
+      <c r="BO33" s="17"/>
+      <c r="BP33" s="150"/>
+    </row>
+    <row r="34" spans="36:68" x14ac:dyDescent="0.3">
+      <c r="AJ34" s="146"/>
+      <c r="AK34" s="147"/>
+      <c r="AL34" s="147"/>
+      <c r="AM34" s="147"/>
+      <c r="AN34" s="147"/>
+      <c r="AO34" s="147"/>
+      <c r="AP34" s="195"/>
+      <c r="AQ34" s="129"/>
+      <c r="AR34" s="129"/>
+      <c r="AS34" s="195"/>
+      <c r="AT34" s="147"/>
+      <c r="AU34" s="147"/>
+      <c r="AV34" s="147"/>
+      <c r="AW34" s="147"/>
+      <c r="AX34" s="147"/>
+      <c r="AY34" s="148"/>
+      <c r="BA34" s="146"/>
+      <c r="BB34" s="147"/>
+      <c r="BC34" s="147"/>
+      <c r="BD34" s="147"/>
+      <c r="BE34" s="147"/>
+      <c r="BF34" s="147"/>
+      <c r="BG34" s="195"/>
+      <c r="BH34" s="129"/>
+      <c r="BI34" s="129"/>
+      <c r="BJ34" s="195"/>
+      <c r="BK34" s="147"/>
+      <c r="BL34" s="147"/>
+      <c r="BM34" s="147"/>
+      <c r="BN34" s="147"/>
+      <c r="BO34" s="147"/>
+      <c r="BP34" s="148"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -44513,8 +45058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="BK15" sqref="BK15"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AL14" sqref="AL14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45014,8 +45559,8 @@
         <v>11</v>
       </c>
       <c r="T6" s="120"/>
-      <c r="U6" s="128"/>
-      <c r="V6" s="128"/>
+      <c r="U6" s="219"/>
+      <c r="V6" s="219"/>
       <c r="W6" s="128"/>
       <c r="X6" s="128"/>
       <c r="Y6" s="128"/>
@@ -45026,8 +45571,8 @@
       <c r="AD6" s="128"/>
       <c r="AE6" s="128"/>
       <c r="AF6" s="128"/>
-      <c r="AG6" s="128"/>
-      <c r="AH6" s="128"/>
+      <c r="AG6" s="219"/>
+      <c r="AH6" s="219"/>
       <c r="AI6" s="123"/>
       <c r="AL6" s="70">
         <f t="shared" si="17"/>
@@ -45075,8 +45620,8 @@
         <v>10</v>
       </c>
       <c r="T7" s="120"/>
-      <c r="U7" s="121"/>
-      <c r="V7" s="121"/>
+      <c r="U7" s="219"/>
+      <c r="V7" s="219"/>
       <c r="W7" s="121"/>
       <c r="X7" s="121"/>
       <c r="Y7" s="121"/>
@@ -45087,8 +45632,8 @@
       <c r="AD7" s="121"/>
       <c r="AE7" s="121"/>
       <c r="AF7" s="121"/>
-      <c r="AG7" s="121"/>
-      <c r="AH7" s="121"/>
+      <c r="AG7" s="219"/>
+      <c r="AH7" s="219"/>
       <c r="AI7" s="123"/>
       <c r="AL7" s="70">
         <f t="shared" si="17"/>
@@ -46315,6 +46860,20 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Farms are good! On to houses..
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="22" activeTab="35"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="22" activeTab="34"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -3292,7 +3292,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:N15" ca="1" si="7">IF(AND(MOD(E$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3312,7 +3312,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3352,7 +3352,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3372,7 +3372,7 @@
       </c>
       <c r="Y6">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3882,7 +3882,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3902,7 +3902,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3922,7 +3922,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4432,7 +4432,7 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:N29" ca="1" si="11">IF(AND(MOD(E$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4452,7 +4452,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4472,7 +4472,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4492,7 +4492,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4512,7 +4512,7 @@
       </c>
       <c r="Y16">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5002,7 +5002,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5022,7 +5022,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5042,7 +5042,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5062,7 +5062,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5082,7 +5082,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5572,7 +5572,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5592,7 +5592,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5632,7 +5632,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5652,7 +5652,7 @@
       </c>
       <c r="Y26">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -45058,8 +45058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC33"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AL14" sqref="AL14"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AR12" sqref="AR7:AW12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46867,7 +46867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added option for workinglights
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="22" activeTab="34"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="22" activeTab="35"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="430">
   <si>
     <t>grove</t>
   </si>
@@ -1340,6 +1340,15 @@
   <si>
     <t>X/Z</t>
   </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
 </sst>
 </file>
 
@@ -1814,7 +1823,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="311">
+  <cellXfs count="325">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2276,6 +2285,48 @@
     <xf numFmtId="0" fontId="0" fillId="31" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3312,7 +3363,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3352,7 +3403,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3372,7 +3423,7 @@
       </c>
       <c r="Y6">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3862,7 +3913,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3882,7 +3933,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3902,7 +3953,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3922,7 +3973,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3942,7 +3993,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4452,7 +4503,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4472,7 +4523,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4512,7 +4563,7 @@
       </c>
       <c r="Y16">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5042,7 +5093,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5062,7 +5113,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5082,7 +5133,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5612,7 +5663,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5632,7 +5683,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5652,7 +5703,7 @@
       </c>
       <c r="Y26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -44184,7 +44235,7 @@
   <dimension ref="A1:AJ18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45058,8 +45109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AR12" sqref="AR7:AW12"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AL1" sqref="AL1:BB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46865,15 +46916,479 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="23" max="23" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B1" s="70">
+        <v>0</v>
+      </c>
+      <c r="C1" s="70">
+        <f>B1+1</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="70">
+        <f t="shared" ref="D1:Q1" si="0">C1+1</f>
+        <v>2</v>
+      </c>
+      <c r="E1" s="70">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F1" s="70">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G1" s="70">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H1" s="70">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I1" s="70">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J1" s="70">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K1" s="70">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L1" s="70">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M1" s="70">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="N1" s="70">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O1" s="70">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P1" s="70">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q1" s="70">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="70">
+        <v>0</v>
+      </c>
+      <c r="B2" s="311"/>
+      <c r="C2" s="312"/>
+      <c r="D2" s="312"/>
+      <c r="E2" s="312"/>
+      <c r="F2" s="312"/>
+      <c r="G2" s="312"/>
+      <c r="H2" s="312"/>
+      <c r="I2" s="312"/>
+      <c r="J2" s="312"/>
+      <c r="K2" s="312"/>
+      <c r="L2" s="312"/>
+      <c r="M2" s="312"/>
+      <c r="N2" s="312"/>
+      <c r="O2" s="312"/>
+      <c r="P2" s="312"/>
+      <c r="Q2" s="313"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="70">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="314"/>
+      <c r="C3" s="244"/>
+      <c r="D3" s="244"/>
+      <c r="E3" s="244"/>
+      <c r="F3" s="244"/>
+      <c r="G3" s="244"/>
+      <c r="H3" s="244"/>
+      <c r="I3" s="244"/>
+      <c r="J3" s="244"/>
+      <c r="K3" s="244"/>
+      <c r="L3" s="244"/>
+      <c r="M3" s="244"/>
+      <c r="N3" s="244"/>
+      <c r="O3" s="244"/>
+      <c r="P3" s="244"/>
+      <c r="Q3" s="315"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" s="70">
+        <f t="shared" ref="A4:A17" si="1">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="314"/>
+      <c r="C4" s="244"/>
+      <c r="D4" s="244"/>
+      <c r="E4" s="244"/>
+      <c r="F4" s="244"/>
+      <c r="G4" s="244"/>
+      <c r="H4" s="244"/>
+      <c r="I4" s="244"/>
+      <c r="J4" s="244"/>
+      <c r="K4" s="244"/>
+      <c r="L4" s="244"/>
+      <c r="M4" s="244"/>
+      <c r="N4" s="244"/>
+      <c r="O4" s="244"/>
+      <c r="P4" s="244"/>
+      <c r="Q4" s="315"/>
+      <c r="W4">
+        <v>8</v>
+      </c>
+      <c r="X4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="70">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="314"/>
+      <c r="C5" s="244"/>
+      <c r="D5" s="244"/>
+      <c r="E5" s="244"/>
+      <c r="F5" s="244" t="s">
+        <v>362</v>
+      </c>
+      <c r="G5" s="244"/>
+      <c r="H5" s="244"/>
+      <c r="I5" s="244"/>
+      <c r="J5" s="244"/>
+      <c r="K5" s="244"/>
+      <c r="L5" s="244"/>
+      <c r="M5" s="244"/>
+      <c r="N5" s="244" t="s">
+        <v>361</v>
+      </c>
+      <c r="O5" s="244"/>
+      <c r="P5" s="244"/>
+      <c r="Q5" s="315"/>
+      <c r="W5">
+        <f>W4/2</f>
+        <v>4</v>
+      </c>
+      <c r="X5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" s="70">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="314"/>
+      <c r="C6" s="244"/>
+      <c r="D6" s="244"/>
+      <c r="E6" s="244" t="s">
+        <v>364</v>
+      </c>
+      <c r="F6" s="319"/>
+      <c r="G6" s="320"/>
+      <c r="H6" s="320"/>
+      <c r="I6" s="320"/>
+      <c r="J6" s="320"/>
+      <c r="K6" s="320"/>
+      <c r="L6" s="320"/>
+      <c r="M6" s="320"/>
+      <c r="N6" s="313"/>
+      <c r="O6" s="244"/>
+      <c r="P6" s="244"/>
+      <c r="Q6" s="315"/>
+      <c r="W6">
+        <f>W5</f>
+        <v>4</v>
+      </c>
+      <c r="X6" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" s="70">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="314"/>
+      <c r="C7" s="244"/>
+      <c r="D7" s="244"/>
+      <c r="E7" s="244"/>
+      <c r="F7" s="323"/>
+      <c r="G7" s="244"/>
+      <c r="H7" s="244"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="244"/>
+      <c r="K7" s="244"/>
+      <c r="L7" s="244"/>
+      <c r="M7" s="324"/>
+      <c r="N7" s="315"/>
+      <c r="O7" s="244"/>
+      <c r="P7" s="244"/>
+      <c r="Q7" s="315"/>
+      <c r="W7">
+        <f>Q1+1-W5</f>
+        <v>12</v>
+      </c>
+      <c r="X7" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8" s="70">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="314"/>
+      <c r="C8" s="244"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="244"/>
+      <c r="F8" s="323"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="324"/>
+      <c r="N8" s="315"/>
+      <c r="O8" s="244"/>
+      <c r="P8" s="244"/>
+      <c r="Q8" s="315"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" s="70">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="314"/>
+      <c r="C9" s="244"/>
+      <c r="D9" s="244"/>
+      <c r="E9" s="244"/>
+      <c r="F9" s="323"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="244"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="324"/>
+      <c r="N9" s="315"/>
+      <c r="O9" s="244"/>
+      <c r="P9" s="244"/>
+      <c r="Q9" s="315"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10" s="70">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="314"/>
+      <c r="C10" s="244"/>
+      <c r="D10" s="244"/>
+      <c r="E10" s="244"/>
+      <c r="F10" s="323"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="324"/>
+      <c r="N10" s="315"/>
+      <c r="O10" s="244"/>
+      <c r="P10" s="244"/>
+      <c r="Q10" s="315"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" s="70">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="314"/>
+      <c r="C11" s="244"/>
+      <c r="D11" s="244"/>
+      <c r="E11" s="244"/>
+      <c r="F11" s="323"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="324"/>
+      <c r="N11" s="315"/>
+      <c r="O11" s="244"/>
+      <c r="P11" s="244"/>
+      <c r="Q11" s="315"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12" s="70">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="314"/>
+      <c r="C12" s="244"/>
+      <c r="D12" s="244"/>
+      <c r="E12" s="244"/>
+      <c r="F12" s="323"/>
+      <c r="G12" s="244"/>
+      <c r="H12" s="244"/>
+      <c r="I12" s="244"/>
+      <c r="J12" s="244"/>
+      <c r="K12" s="244"/>
+      <c r="L12" s="244"/>
+      <c r="M12" s="324"/>
+      <c r="N12" s="315"/>
+      <c r="O12" s="244"/>
+      <c r="P12" s="244"/>
+      <c r="Q12" s="315"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13" s="70">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="314"/>
+      <c r="C13" s="244"/>
+      <c r="D13" s="244"/>
+      <c r="E13" s="244"/>
+      <c r="F13" s="323"/>
+      <c r="G13" s="244"/>
+      <c r="H13" s="244"/>
+      <c r="I13" s="244"/>
+      <c r="J13" s="244"/>
+      <c r="K13" s="244"/>
+      <c r="L13" s="244"/>
+      <c r="M13" s="324"/>
+      <c r="N13" s="315"/>
+      <c r="O13" s="244"/>
+      <c r="P13" s="244"/>
+      <c r="Q13" s="315"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A14" s="70">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="314"/>
+      <c r="C14" s="244"/>
+      <c r="D14" s="244"/>
+      <c r="E14" s="244"/>
+      <c r="F14" s="321"/>
+      <c r="G14" s="322"/>
+      <c r="H14" s="322"/>
+      <c r="I14" s="322"/>
+      <c r="J14" s="322"/>
+      <c r="K14" s="322"/>
+      <c r="L14" s="322"/>
+      <c r="M14" s="322"/>
+      <c r="N14" s="318"/>
+      <c r="O14" s="244"/>
+      <c r="P14" s="244"/>
+      <c r="Q14" s="315"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" s="70">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="314"/>
+      <c r="C15" s="244"/>
+      <c r="D15" s="244"/>
+      <c r="E15" s="244" t="s">
+        <v>363</v>
+      </c>
+      <c r="F15" s="244"/>
+      <c r="G15" s="244"/>
+      <c r="H15" s="244"/>
+      <c r="I15" s="244"/>
+      <c r="J15" s="244"/>
+      <c r="K15" s="244"/>
+      <c r="L15" s="244"/>
+      <c r="M15" s="244"/>
+      <c r="N15" s="244"/>
+      <c r="O15" s="244"/>
+      <c r="P15" s="244"/>
+      <c r="Q15" s="315"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A16" s="70">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="314"/>
+      <c r="C16" s="244"/>
+      <c r="D16" s="244"/>
+      <c r="E16" s="244"/>
+      <c r="F16" s="244"/>
+      <c r="G16" s="244"/>
+      <c r="H16" s="244"/>
+      <c r="I16" s="244"/>
+      <c r="J16" s="244"/>
+      <c r="K16" s="244"/>
+      <c r="L16" s="244"/>
+      <c r="M16" s="244"/>
+      <c r="N16" s="244"/>
+      <c r="O16" s="244"/>
+      <c r="P16" s="244"/>
+      <c r="Q16" s="315"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="70">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="316"/>
+      <c r="C17" s="317"/>
+      <c r="D17" s="317"/>
+      <c r="E17" s="317"/>
+      <c r="F17" s="317"/>
+      <c r="G17" s="317"/>
+      <c r="H17" s="317"/>
+      <c r="I17" s="317"/>
+      <c r="J17" s="317"/>
+      <c r="K17" s="317"/>
+      <c r="L17" s="317"/>
+      <c r="M17" s="317"/>
+      <c r="N17" s="317"/>
+      <c r="O17" s="317"/>
+      <c r="P17" s="317"/>
+      <c r="Q17" s="318"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="70" t="s">
+        <v>395</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Oil platforms are back Houses work a LITTLE better but still much to do
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="22" activeTab="35"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" tabRatio="740" firstSheet="31" activeTab="36"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -43,6 +43,7 @@
     <sheet name="Tunnels" sheetId="42" r:id="rId34"/>
     <sheet name="Bridge" sheetId="43" r:id="rId35"/>
     <sheet name="Sheet2" sheetId="44" r:id="rId36"/>
+    <sheet name="Sheet4" sheetId="45" r:id="rId37"/>
   </sheets>
   <definedNames>
     <definedName name="AbsoluteMaximumFloorsBelow">Sheet3!$C$6</definedName>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="433">
   <si>
     <t>grove</t>
   </si>
@@ -1349,6 +1350,15 @@
   <si>
     <t>max</t>
   </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
 </sst>
 </file>
 
@@ -1406,7 +1416,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1665,6 +1675,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -1823,7 +1839,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="325">
+  <cellXfs count="342">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2309,22 +2325,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -3343,7 +3398,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:N15" ca="1" si="7">IF(AND(MOD(E$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3363,7 +3418,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3383,7 +3438,7 @@
       </c>
       <c r="O6">
         <f t="shared" ref="O6:AB15" ca="1" si="8">IF(AND(MOD(O$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3913,7 +3968,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3933,7 +3988,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3993,7 +4048,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4483,7 +4538,7 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:N29" ca="1" si="11">IF(AND(MOD(E$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4523,7 +4578,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4543,7 +4598,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5073,7 +5128,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5133,7 +5188,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5643,7 +5698,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5663,7 +5718,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5683,7 +5738,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5703,7 +5758,7 @@
       </c>
       <c r="Y26">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -46916,10 +46971,10 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:BD30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46927,7 +46982,7 @@
     <col min="23" max="23" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B1" s="70">
         <v>0</v>
       </c>
@@ -46995,7 +47050,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A2" s="70">
         <v>0</v>
       </c>
@@ -47016,7 +47071,7 @@
       <c r="P2" s="312"/>
       <c r="Q2" s="313"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A3" s="70">
         <f>A2+1</f>
         <v>1</v>
@@ -47037,283 +47092,607 @@
       <c r="O3" s="244"/>
       <c r="P3" s="244"/>
       <c r="Q3" s="315"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="S3">
+        <v>8</v>
+      </c>
+      <c r="T3" t="s">
+        <v>252</v>
+      </c>
+      <c r="W3" s="322"/>
+      <c r="X3" s="307"/>
+      <c r="Y3" s="307"/>
+      <c r="Z3" s="307"/>
+      <c r="AA3" s="307"/>
+      <c r="AB3" s="324"/>
+      <c r="AD3" s="322"/>
+      <c r="AE3" s="307"/>
+      <c r="AF3" s="307"/>
+      <c r="AG3" s="307"/>
+      <c r="AH3" s="307"/>
+      <c r="AI3" s="324"/>
+      <c r="AK3" s="322"/>
+      <c r="AL3" s="307"/>
+      <c r="AM3" s="307"/>
+      <c r="AN3" s="307"/>
+      <c r="AO3" s="307"/>
+      <c r="AP3" s="324"/>
+      <c r="AR3" s="322"/>
+      <c r="AS3" s="307"/>
+      <c r="AT3" s="307"/>
+      <c r="AU3" s="307"/>
+      <c r="AV3" s="307"/>
+      <c r="AW3" s="324"/>
+      <c r="AY3" s="322"/>
+      <c r="AZ3" s="307"/>
+      <c r="BA3" s="307"/>
+      <c r="BB3" s="307"/>
+      <c r="BC3" s="307"/>
+      <c r="BD3" s="324"/>
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A4" s="70">
         <f t="shared" ref="A4:A17" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="314"/>
       <c r="C4" s="244"/>
-      <c r="D4" s="244"/>
-      <c r="E4" s="244"/>
-      <c r="F4" s="244"/>
-      <c r="G4" s="244"/>
-      <c r="H4" s="244"/>
-      <c r="I4" s="244"/>
-      <c r="J4" s="244"/>
-      <c r="K4" s="244"/>
-      <c r="L4" s="244"/>
-      <c r="M4" s="244"/>
-      <c r="N4" s="244"/>
+      <c r="D4" s="319"/>
+      <c r="E4" s="320"/>
+      <c r="F4" s="321"/>
+      <c r="G4" s="321"/>
+      <c r="H4" s="320"/>
+      <c r="I4" s="320"/>
+      <c r="J4" s="320"/>
+      <c r="K4" s="321"/>
+      <c r="L4" s="321"/>
+      <c r="M4" s="320"/>
+      <c r="N4" s="319"/>
       <c r="O4" s="244"/>
       <c r="P4" s="244"/>
       <c r="Q4" s="315"/>
-      <c r="W4">
-        <v>8</v>
-      </c>
-      <c r="X4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="S4">
+        <f>S3/2</f>
+        <v>4</v>
+      </c>
+      <c r="T4" t="s">
+        <v>427</v>
+      </c>
+      <c r="W4" s="308"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="326"/>
+      <c r="Z4" s="326"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="309"/>
+      <c r="AD4" s="308"/>
+      <c r="AE4" s="326"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="326"/>
+      <c r="AI4" s="309"/>
+      <c r="AK4" s="308"/>
+      <c r="AL4" s="6"/>
+      <c r="AM4" s="326"/>
+      <c r="AN4" s="326"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="309"/>
+      <c r="AR4" s="308"/>
+      <c r="AS4" s="6"/>
+      <c r="AT4" s="6"/>
+      <c r="AU4" s="6"/>
+      <c r="AV4" s="6"/>
+      <c r="AW4" s="309"/>
+      <c r="AY4" s="308"/>
+      <c r="AZ4" s="6"/>
+      <c r="BA4" s="6"/>
+      <c r="BB4" s="6"/>
+      <c r="BC4" s="6"/>
+      <c r="BD4" s="309"/>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A5" s="70">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B5" s="314"/>
       <c r="C5" s="244"/>
-      <c r="D5" s="244"/>
+      <c r="D5" s="319"/>
       <c r="E5" s="244"/>
-      <c r="F5" s="244" t="s">
-        <v>362</v>
-      </c>
+      <c r="F5" s="244"/>
       <c r="G5" s="244"/>
       <c r="H5" s="244"/>
-      <c r="I5" s="244"/>
+      <c r="I5" s="319"/>
       <c r="J5" s="244"/>
       <c r="K5" s="244"/>
       <c r="L5" s="244"/>
       <c r="M5" s="244"/>
-      <c r="N5" s="244" t="s">
-        <v>361</v>
-      </c>
+      <c r="N5" s="319"/>
       <c r="O5" s="244"/>
       <c r="P5" s="244"/>
       <c r="Q5" s="315"/>
-      <c r="W5">
-        <f>W4/2</f>
+      <c r="S5">
+        <f>S4</f>
         <v>4</v>
       </c>
-      <c r="X5" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="T5" t="s">
+        <v>428</v>
+      </c>
+      <c r="W5" s="308"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="326"/>
+      <c r="Z5" s="326"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="309"/>
+      <c r="AD5" s="308"/>
+      <c r="AE5" s="326"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="326"/>
+      <c r="AI5" s="309"/>
+      <c r="AK5" s="308"/>
+      <c r="AL5" s="326"/>
+      <c r="AM5" s="6"/>
+      <c r="AN5" s="6"/>
+      <c r="AO5" s="6"/>
+      <c r="AP5" s="309"/>
+      <c r="AR5" s="308"/>
+      <c r="AS5" s="6"/>
+      <c r="AT5" s="6"/>
+      <c r="AU5" s="6"/>
+      <c r="AV5" s="6"/>
+      <c r="AW5" s="309"/>
+      <c r="AY5" s="308"/>
+      <c r="AZ5" s="6"/>
+      <c r="BA5" s="6"/>
+      <c r="BB5" s="6"/>
+      <c r="BC5" s="6"/>
+      <c r="BD5" s="309"/>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A6" s="70">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B6" s="314"/>
       <c r="C6" s="244"/>
-      <c r="D6" s="244"/>
-      <c r="E6" s="244" t="s">
-        <v>364</v>
-      </c>
-      <c r="F6" s="319"/>
-      <c r="G6" s="320"/>
-      <c r="H6" s="320"/>
-      <c r="I6" s="320"/>
-      <c r="J6" s="320"/>
-      <c r="K6" s="320"/>
-      <c r="L6" s="320"/>
-      <c r="M6" s="320"/>
-      <c r="N6" s="313"/>
+      <c r="D6" s="321"/>
+      <c r="E6" s="244"/>
+      <c r="F6" s="244"/>
+      <c r="G6" s="244"/>
+      <c r="H6" s="244"/>
+      <c r="I6" s="319"/>
+      <c r="J6" s="244"/>
+      <c r="K6" s="244"/>
+      <c r="L6" s="244"/>
+      <c r="M6" s="244"/>
+      <c r="N6" s="321"/>
       <c r="O6" s="244"/>
       <c r="P6" s="244"/>
       <c r="Q6" s="315"/>
-      <c r="W6">
-        <f>W5</f>
-        <v>4</v>
-      </c>
-      <c r="X6" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="S6">
+        <f>Q1+1-S4</f>
+        <v>12</v>
+      </c>
+      <c r="T6" t="s">
+        <v>429</v>
+      </c>
+      <c r="W6" s="308"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="309"/>
+      <c r="AD6" s="308"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="309"/>
+      <c r="AK6" s="308"/>
+      <c r="AL6" s="326"/>
+      <c r="AM6" s="6"/>
+      <c r="AN6" s="6"/>
+      <c r="AO6" s="6"/>
+      <c r="AP6" s="309"/>
+      <c r="AR6" s="308"/>
+      <c r="AS6" s="6"/>
+      <c r="AT6" s="6"/>
+      <c r="AU6" s="6"/>
+      <c r="AV6" s="6"/>
+      <c r="AW6" s="309"/>
+      <c r="AY6" s="308"/>
+      <c r="AZ6" s="6"/>
+      <c r="BA6" s="6"/>
+      <c r="BB6" s="6"/>
+      <c r="BC6" s="6"/>
+      <c r="BD6" s="309"/>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A7" s="70">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B7" s="314"/>
       <c r="C7" s="244"/>
-      <c r="D7" s="244"/>
+      <c r="D7" s="321"/>
       <c r="E7" s="244"/>
-      <c r="F7" s="323"/>
+      <c r="F7" s="244"/>
       <c r="G7" s="244"/>
       <c r="H7" s="244"/>
-      <c r="I7" s="17"/>
+      <c r="I7" s="142"/>
       <c r="J7" s="244"/>
       <c r="K7" s="244"/>
       <c r="L7" s="244"/>
-      <c r="M7" s="324"/>
-      <c r="N7" s="315"/>
+      <c r="M7" s="244"/>
+      <c r="N7" s="321"/>
       <c r="O7" s="244"/>
       <c r="P7" s="244"/>
       <c r="Q7" s="315"/>
-      <c r="W7">
-        <f>Q1+1-W5</f>
-        <v>12</v>
-      </c>
-      <c r="X7" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W7" s="308"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="309"/>
+      <c r="AD7" s="308"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="309"/>
+      <c r="AK7" s="308"/>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="6"/>
+      <c r="AO7" s="6"/>
+      <c r="AP7" s="309"/>
+      <c r="AR7" s="308"/>
+      <c r="AS7" s="6"/>
+      <c r="AT7" s="6"/>
+      <c r="AU7" s="6"/>
+      <c r="AV7" s="6"/>
+      <c r="AW7" s="309"/>
+      <c r="AY7" s="308"/>
+      <c r="AZ7" s="6"/>
+      <c r="BA7" s="6"/>
+      <c r="BB7" s="6"/>
+      <c r="BC7" s="6"/>
+      <c r="BD7" s="309"/>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A8" s="70">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B8" s="314"/>
       <c r="C8" s="244"/>
-      <c r="D8" s="244"/>
+      <c r="D8" s="319"/>
       <c r="E8" s="244"/>
-      <c r="F8" s="323"/>
+      <c r="F8" s="244"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="I8" s="142"/>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
-      <c r="M8" s="324"/>
-      <c r="N8" s="315"/>
+      <c r="M8" s="244"/>
+      <c r="N8" s="319"/>
       <c r="O8" s="244"/>
       <c r="P8" s="244"/>
       <c r="Q8" s="315"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W8" s="323"/>
+      <c r="X8" s="218"/>
+      <c r="Y8" s="218"/>
+      <c r="Z8" s="218"/>
+      <c r="AA8" s="218"/>
+      <c r="AB8" s="325"/>
+      <c r="AD8" s="323"/>
+      <c r="AE8" s="218"/>
+      <c r="AF8" s="218"/>
+      <c r="AG8" s="218"/>
+      <c r="AH8" s="218"/>
+      <c r="AI8" s="325"/>
+      <c r="AK8" s="323"/>
+      <c r="AL8" s="218"/>
+      <c r="AM8" s="218"/>
+      <c r="AN8" s="218"/>
+      <c r="AO8" s="218"/>
+      <c r="AP8" s="325"/>
+      <c r="AR8" s="323"/>
+      <c r="AS8" s="218"/>
+      <c r="AT8" s="218"/>
+      <c r="AU8" s="218"/>
+      <c r="AV8" s="218"/>
+      <c r="AW8" s="325"/>
+      <c r="AY8" s="323"/>
+      <c r="AZ8" s="218"/>
+      <c r="BA8" s="218"/>
+      <c r="BB8" s="218"/>
+      <c r="BC8" s="218"/>
+      <c r="BD8" s="325"/>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A9" s="70">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B9" s="314"/>
       <c r="C9" s="244"/>
-      <c r="D9" s="244"/>
-      <c r="E9" s="244"/>
-      <c r="F9" s="323"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="244"/>
+      <c r="D9" s="319"/>
+      <c r="E9" s="320"/>
+      <c r="F9" s="320"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="319"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
-      <c r="M9" s="324"/>
-      <c r="N9" s="315"/>
+      <c r="M9" s="244"/>
+      <c r="N9" s="319"/>
       <c r="O9" s="244"/>
       <c r="P9" s="244"/>
       <c r="Q9" s="315"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A10" s="70">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B10" s="314"/>
       <c r="C10" s="244"/>
-      <c r="D10" s="244"/>
+      <c r="D10" s="319"/>
       <c r="E10" s="244"/>
-      <c r="F10" s="323"/>
+      <c r="F10" s="244"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
-      <c r="M10" s="324"/>
-      <c r="N10" s="315"/>
+      <c r="M10" s="244"/>
+      <c r="N10" s="319"/>
       <c r="O10" s="244"/>
       <c r="P10" s="244"/>
       <c r="Q10" s="315"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W10" s="322"/>
+      <c r="X10" s="307"/>
+      <c r="Y10" s="307"/>
+      <c r="Z10" s="307"/>
+      <c r="AA10" s="307"/>
+      <c r="AB10" s="324"/>
+      <c r="AD10" s="322"/>
+      <c r="AE10" s="307"/>
+      <c r="AF10" s="307"/>
+      <c r="AG10" s="307"/>
+      <c r="AH10" s="307"/>
+      <c r="AI10" s="324"/>
+      <c r="AK10" s="322"/>
+      <c r="AL10" s="307"/>
+      <c r="AM10" s="307"/>
+      <c r="AN10" s="307"/>
+      <c r="AO10" s="307"/>
+      <c r="AP10" s="324"/>
+      <c r="AR10" s="322"/>
+      <c r="AS10" s="307"/>
+      <c r="AT10" s="307"/>
+      <c r="AU10" s="307"/>
+      <c r="AV10" s="307"/>
+      <c r="AW10" s="324"/>
+      <c r="AY10" s="322"/>
+      <c r="AZ10" s="307"/>
+      <c r="BA10" s="307"/>
+      <c r="BB10" s="307"/>
+      <c r="BC10" s="307"/>
+      <c r="BD10" s="324"/>
+    </row>
+    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A11" s="70">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B11" s="314"/>
       <c r="C11" s="244"/>
-      <c r="D11" s="244"/>
+      <c r="D11" s="321"/>
       <c r="E11" s="244"/>
-      <c r="F11" s="323"/>
+      <c r="F11" s="244"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
-      <c r="M11" s="324"/>
-      <c r="N11" s="315"/>
+      <c r="M11" s="244"/>
+      <c r="N11" s="321"/>
       <c r="O11" s="244"/>
       <c r="P11" s="244"/>
       <c r="Q11" s="315"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W11" s="308"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="309"/>
+      <c r="AD11" s="308"/>
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="309"/>
+      <c r="AK11" s="308"/>
+      <c r="AL11" s="6"/>
+      <c r="AM11" s="6"/>
+      <c r="AN11" s="6"/>
+      <c r="AO11" s="6"/>
+      <c r="AP11" s="309"/>
+      <c r="AR11" s="308"/>
+      <c r="AS11" s="6"/>
+      <c r="AT11" s="6"/>
+      <c r="AU11" s="6"/>
+      <c r="AV11" s="6"/>
+      <c r="AW11" s="309"/>
+      <c r="AY11" s="308"/>
+      <c r="AZ11" s="6"/>
+      <c r="BA11" s="6"/>
+      <c r="BB11" s="6"/>
+      <c r="BC11" s="6"/>
+      <c r="BD11" s="309"/>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A12" s="70">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B12" s="314"/>
       <c r="C12" s="244"/>
-      <c r="D12" s="244"/>
+      <c r="D12" s="321"/>
       <c r="E12" s="244"/>
-      <c r="F12" s="323"/>
+      <c r="F12" s="244"/>
       <c r="G12" s="244"/>
       <c r="H12" s="244"/>
       <c r="I12" s="244"/>
       <c r="J12" s="244"/>
       <c r="K12" s="244"/>
       <c r="L12" s="244"/>
-      <c r="M12" s="324"/>
-      <c r="N12" s="315"/>
+      <c r="M12" s="244"/>
+      <c r="N12" s="321"/>
       <c r="O12" s="244"/>
       <c r="P12" s="244"/>
       <c r="Q12" s="315"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W12" s="308"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="309"/>
+      <c r="AD12" s="308"/>
+      <c r="AE12" s="6"/>
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="6"/>
+      <c r="AH12" s="6"/>
+      <c r="AI12" s="309"/>
+      <c r="AK12" s="308"/>
+      <c r="AL12" s="6"/>
+      <c r="AM12" s="6"/>
+      <c r="AN12" s="6"/>
+      <c r="AO12" s="6"/>
+      <c r="AP12" s="309"/>
+      <c r="AR12" s="308"/>
+      <c r="AS12" s="6"/>
+      <c r="AT12" s="6"/>
+      <c r="AU12" s="6"/>
+      <c r="AV12" s="6"/>
+      <c r="AW12" s="309"/>
+      <c r="AY12" s="308"/>
+      <c r="AZ12" s="6"/>
+      <c r="BA12" s="6"/>
+      <c r="BB12" s="6"/>
+      <c r="BC12" s="6"/>
+      <c r="BD12" s="309"/>
+    </row>
+    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A13" s="70">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B13" s="314"/>
       <c r="C13" s="244"/>
-      <c r="D13" s="244"/>
+      <c r="D13" s="319"/>
       <c r="E13" s="244"/>
-      <c r="F13" s="323"/>
+      <c r="F13" s="244"/>
       <c r="G13" s="244"/>
       <c r="H13" s="244"/>
       <c r="I13" s="244"/>
       <c r="J13" s="244"/>
       <c r="K13" s="244"/>
       <c r="L13" s="244"/>
-      <c r="M13" s="324"/>
-      <c r="N13" s="315"/>
+      <c r="M13" s="244"/>
+      <c r="N13" s="319"/>
       <c r="O13" s="244"/>
       <c r="P13" s="244"/>
       <c r="Q13" s="315"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W13" s="308"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="309"/>
+      <c r="AD13" s="308"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="6"/>
+      <c r="AG13" s="6"/>
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="309"/>
+      <c r="AK13" s="308"/>
+      <c r="AL13" s="6"/>
+      <c r="AM13" s="6"/>
+      <c r="AN13" s="6"/>
+      <c r="AO13" s="6"/>
+      <c r="AP13" s="309"/>
+      <c r="AR13" s="308"/>
+      <c r="AS13" s="6"/>
+      <c r="AT13" s="6"/>
+      <c r="AU13" s="6"/>
+      <c r="AV13" s="6"/>
+      <c r="AW13" s="309"/>
+      <c r="AY13" s="308"/>
+      <c r="AZ13" s="6"/>
+      <c r="BA13" s="6"/>
+      <c r="BB13" s="6"/>
+      <c r="BC13" s="6"/>
+      <c r="BD13" s="309"/>
+    </row>
+    <row r="14" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A14" s="70">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B14" s="314"/>
       <c r="C14" s="244"/>
-      <c r="D14" s="244"/>
-      <c r="E14" s="244"/>
+      <c r="D14" s="319"/>
+      <c r="E14" s="320"/>
       <c r="F14" s="321"/>
-      <c r="G14" s="322"/>
-      <c r="H14" s="322"/>
-      <c r="I14" s="322"/>
-      <c r="J14" s="322"/>
-      <c r="K14" s="322"/>
-      <c r="L14" s="322"/>
-      <c r="M14" s="322"/>
-      <c r="N14" s="318"/>
+      <c r="G14" s="321"/>
+      <c r="H14" s="320"/>
+      <c r="I14" s="320"/>
+      <c r="J14" s="320"/>
+      <c r="K14" s="321"/>
+      <c r="L14" s="321"/>
+      <c r="M14" s="320"/>
+      <c r="N14" s="319"/>
       <c r="O14" s="244"/>
       <c r="P14" s="244"/>
       <c r="Q14" s="315"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W14" s="308"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="309"/>
+      <c r="AD14" s="308"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="309"/>
+      <c r="AK14" s="308"/>
+      <c r="AL14" s="6"/>
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="6"/>
+      <c r="AP14" s="309"/>
+      <c r="AR14" s="308"/>
+      <c r="AS14" s="6"/>
+      <c r="AT14" s="6"/>
+      <c r="AU14" s="6"/>
+      <c r="AV14" s="6"/>
+      <c r="AW14" s="309"/>
+      <c r="AY14" s="308"/>
+      <c r="AZ14" s="6"/>
+      <c r="BA14" s="6"/>
+      <c r="BB14" s="6"/>
+      <c r="BC14" s="6"/>
+      <c r="BD14" s="309"/>
+    </row>
+    <row r="15" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A15" s="70">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -47321,9 +47700,7 @@
       <c r="B15" s="314"/>
       <c r="C15" s="244"/>
       <c r="D15" s="244"/>
-      <c r="E15" s="244" t="s">
-        <v>363</v>
-      </c>
+      <c r="E15" s="244"/>
       <c r="F15" s="244"/>
       <c r="G15" s="244"/>
       <c r="H15" s="244"/>
@@ -47336,8 +47713,38 @@
       <c r="O15" s="244"/>
       <c r="P15" s="244"/>
       <c r="Q15" s="315"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W15" s="323"/>
+      <c r="X15" s="218"/>
+      <c r="Y15" s="218"/>
+      <c r="Z15" s="218"/>
+      <c r="AA15" s="218"/>
+      <c r="AB15" s="325"/>
+      <c r="AD15" s="323"/>
+      <c r="AE15" s="218"/>
+      <c r="AF15" s="218"/>
+      <c r="AG15" s="218"/>
+      <c r="AH15" s="218"/>
+      <c r="AI15" s="325"/>
+      <c r="AK15" s="323"/>
+      <c r="AL15" s="218"/>
+      <c r="AM15" s="218"/>
+      <c r="AN15" s="218"/>
+      <c r="AO15" s="218"/>
+      <c r="AP15" s="325"/>
+      <c r="AR15" s="323"/>
+      <c r="AS15" s="218"/>
+      <c r="AT15" s="218"/>
+      <c r="AU15" s="218"/>
+      <c r="AV15" s="218"/>
+      <c r="AW15" s="325"/>
+      <c r="AY15" s="323"/>
+      <c r="AZ15" s="218"/>
+      <c r="BA15" s="218"/>
+      <c r="BB15" s="218"/>
+      <c r="BC15" s="218"/>
+      <c r="BD15" s="325"/>
+    </row>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A16" s="70">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -47359,7 +47766,7 @@
       <c r="P16" s="244"/>
       <c r="Q16" s="315"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A17" s="70">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -47380,15 +47787,2560 @@
       <c r="O17" s="317"/>
       <c r="P17" s="317"/>
       <c r="Q17" s="318"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="W17" s="322"/>
+      <c r="X17" s="307"/>
+      <c r="Y17" s="307"/>
+      <c r="Z17" s="307"/>
+      <c r="AA17" s="307"/>
+      <c r="AB17" s="324"/>
+      <c r="AD17" s="322"/>
+      <c r="AE17" s="307"/>
+      <c r="AF17" s="307"/>
+      <c r="AG17" s="307"/>
+      <c r="AH17" s="307"/>
+      <c r="AI17" s="324"/>
+      <c r="AK17" s="322"/>
+      <c r="AL17" s="307"/>
+      <c r="AM17" s="307"/>
+      <c r="AN17" s="307"/>
+      <c r="AO17" s="307"/>
+      <c r="AP17" s="324"/>
+      <c r="AR17" s="322"/>
+      <c r="AS17" s="307"/>
+      <c r="AT17" s="307"/>
+      <c r="AU17" s="307"/>
+      <c r="AV17" s="307"/>
+      <c r="AW17" s="324"/>
+      <c r="AY17" s="322"/>
+      <c r="AZ17" s="307"/>
+      <c r="BA17" s="307"/>
+      <c r="BB17" s="307"/>
+      <c r="BC17" s="307"/>
+      <c r="BD17" s="324"/>
+    </row>
+    <row r="18" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A18" s="70" t="s">
         <v>395</v>
+      </c>
+      <c r="W18" s="308"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="309"/>
+      <c r="AD18" s="308"/>
+      <c r="AE18" s="6"/>
+      <c r="AF18" s="6"/>
+      <c r="AG18" s="6"/>
+      <c r="AH18" s="6"/>
+      <c r="AI18" s="309"/>
+      <c r="AK18" s="308"/>
+      <c r="AL18" s="6"/>
+      <c r="AM18" s="6"/>
+      <c r="AN18" s="6"/>
+      <c r="AO18" s="6"/>
+      <c r="AP18" s="309"/>
+      <c r="AR18" s="308"/>
+      <c r="AS18" s="6"/>
+      <c r="AT18" s="6"/>
+      <c r="AU18" s="6"/>
+      <c r="AV18" s="6"/>
+      <c r="AW18" s="309"/>
+      <c r="AY18" s="308"/>
+      <c r="AZ18" s="6"/>
+      <c r="BA18" s="6"/>
+      <c r="BB18" s="6"/>
+      <c r="BC18" s="6"/>
+      <c r="BD18" s="309"/>
+    </row>
+    <row r="19" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="W19" s="308"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="309"/>
+      <c r="AD19" s="308"/>
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="6"/>
+      <c r="AG19" s="6"/>
+      <c r="AH19" s="6"/>
+      <c r="AI19" s="309"/>
+      <c r="AK19" s="308"/>
+      <c r="AL19" s="6"/>
+      <c r="AM19" s="6"/>
+      <c r="AN19" s="6"/>
+      <c r="AO19" s="6"/>
+      <c r="AP19" s="309"/>
+      <c r="AR19" s="308"/>
+      <c r="AS19" s="6"/>
+      <c r="AT19" s="6"/>
+      <c r="AU19" s="6"/>
+      <c r="AV19" s="6"/>
+      <c r="AW19" s="309"/>
+      <c r="AY19" s="308"/>
+      <c r="AZ19" s="6"/>
+      <c r="BA19" s="6"/>
+      <c r="BB19" s="6"/>
+      <c r="BC19" s="6"/>
+      <c r="BD19" s="309"/>
+    </row>
+    <row r="20" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="5"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="5"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="W20" s="308"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="309"/>
+      <c r="AD20" s="308"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="6"/>
+      <c r="AH20" s="6"/>
+      <c r="AI20" s="309"/>
+      <c r="AK20" s="308"/>
+      <c r="AL20" s="6"/>
+      <c r="AM20" s="6"/>
+      <c r="AN20" s="6"/>
+      <c r="AO20" s="6"/>
+      <c r="AP20" s="309"/>
+      <c r="AR20" s="308"/>
+      <c r="AS20" s="6"/>
+      <c r="AT20" s="6"/>
+      <c r="AU20" s="6"/>
+      <c r="AV20" s="6"/>
+      <c r="AW20" s="309"/>
+      <c r="AY20" s="308"/>
+      <c r="AZ20" s="6"/>
+      <c r="BA20" s="6"/>
+      <c r="BB20" s="6"/>
+      <c r="BC20" s="6"/>
+      <c r="BD20" s="309"/>
+    </row>
+    <row r="21" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="C21" s="13"/>
+      <c r="D21" s="15"/>
+      <c r="F21" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="L21" s="13"/>
+      <c r="M21" s="15"/>
+      <c r="W21" s="308"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="309"/>
+      <c r="AD21" s="308"/>
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="6"/>
+      <c r="AG21" s="6"/>
+      <c r="AH21" s="6"/>
+      <c r="AI21" s="309"/>
+      <c r="AK21" s="308"/>
+      <c r="AL21" s="6"/>
+      <c r="AM21" s="6"/>
+      <c r="AN21" s="6"/>
+      <c r="AO21" s="6"/>
+      <c r="AP21" s="309"/>
+      <c r="AR21" s="308"/>
+      <c r="AS21" s="6"/>
+      <c r="AT21" s="6"/>
+      <c r="AU21" s="6"/>
+      <c r="AV21" s="6"/>
+      <c r="AW21" s="309"/>
+      <c r="AY21" s="308"/>
+      <c r="AZ21" s="6"/>
+      <c r="BA21" s="6"/>
+      <c r="BB21" s="6"/>
+      <c r="BC21" s="6"/>
+      <c r="BD21" s="309"/>
+    </row>
+    <row r="22" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="W22" s="323"/>
+      <c r="X22" s="218"/>
+      <c r="Y22" s="218"/>
+      <c r="Z22" s="218"/>
+      <c r="AA22" s="218"/>
+      <c r="AB22" s="325"/>
+      <c r="AD22" s="323"/>
+      <c r="AE22" s="218"/>
+      <c r="AF22" s="218"/>
+      <c r="AG22" s="218"/>
+      <c r="AH22" s="218"/>
+      <c r="AI22" s="325"/>
+      <c r="AK22" s="323"/>
+      <c r="AL22" s="218"/>
+      <c r="AM22" s="218"/>
+      <c r="AN22" s="218"/>
+      <c r="AO22" s="218"/>
+      <c r="AP22" s="325"/>
+      <c r="AR22" s="323"/>
+      <c r="AS22" s="218"/>
+      <c r="AT22" s="218"/>
+      <c r="AU22" s="218"/>
+      <c r="AV22" s="218"/>
+      <c r="AW22" s="325"/>
+      <c r="AY22" s="323"/>
+      <c r="AZ22" s="218"/>
+      <c r="BA22" s="218"/>
+      <c r="BB22" s="218"/>
+      <c r="BC22" s="218"/>
+      <c r="BD22" s="325"/>
+    </row>
+    <row r="23" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="F23" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="C24" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="F24" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="L24" s="13"/>
+      <c r="M24" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="W24" s="322"/>
+      <c r="X24" s="307"/>
+      <c r="Y24" s="307"/>
+      <c r="Z24" s="307"/>
+      <c r="AA24" s="307"/>
+      <c r="AB24" s="324"/>
+      <c r="AD24" s="322"/>
+      <c r="AE24" s="307"/>
+      <c r="AF24" s="307"/>
+      <c r="AG24" s="307"/>
+      <c r="AH24" s="307"/>
+      <c r="AI24" s="324"/>
+      <c r="AK24" s="322"/>
+      <c r="AL24" s="307"/>
+      <c r="AM24" s="307"/>
+      <c r="AN24" s="307"/>
+      <c r="AO24" s="307"/>
+      <c r="AP24" s="324"/>
+      <c r="AR24" s="322"/>
+      <c r="AS24" s="307"/>
+      <c r="AT24" s="307"/>
+      <c r="AU24" s="307"/>
+      <c r="AV24" s="307"/>
+      <c r="AW24" s="324"/>
+      <c r="AY24" s="322"/>
+      <c r="AZ24" s="307"/>
+      <c r="BA24" s="307"/>
+      <c r="BB24" s="307"/>
+      <c r="BC24" s="307"/>
+      <c r="BD24" s="324"/>
+    </row>
+    <row r="25" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="W25" s="308"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="309"/>
+      <c r="AD25" s="308"/>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="6"/>
+      <c r="AG25" s="6"/>
+      <c r="AH25" s="6"/>
+      <c r="AI25" s="309"/>
+      <c r="AK25" s="308"/>
+      <c r="AL25" s="6"/>
+      <c r="AM25" s="6"/>
+      <c r="AN25" s="6"/>
+      <c r="AO25" s="6"/>
+      <c r="AP25" s="309"/>
+      <c r="AR25" s="308"/>
+      <c r="AS25" s="6"/>
+      <c r="AT25" s="6"/>
+      <c r="AU25" s="6"/>
+      <c r="AV25" s="6"/>
+      <c r="AW25" s="309"/>
+      <c r="AY25" s="308"/>
+      <c r="AZ25" s="6"/>
+      <c r="BA25" s="6"/>
+      <c r="BB25" s="6"/>
+      <c r="BC25" s="6"/>
+      <c r="BD25" s="309"/>
+    </row>
+    <row r="26" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="C26" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="F26" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="W26" s="308"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="309"/>
+      <c r="AD26" s="308"/>
+      <c r="AE26" s="6"/>
+      <c r="AF26" s="6"/>
+      <c r="AG26" s="6"/>
+      <c r="AH26" s="6"/>
+      <c r="AI26" s="309"/>
+      <c r="AK26" s="308"/>
+      <c r="AL26" s="6"/>
+      <c r="AM26" s="6"/>
+      <c r="AN26" s="6"/>
+      <c r="AO26" s="6"/>
+      <c r="AP26" s="309"/>
+      <c r="AR26" s="308"/>
+      <c r="AS26" s="6"/>
+      <c r="AT26" s="6"/>
+      <c r="AU26" s="6"/>
+      <c r="AV26" s="6"/>
+      <c r="AW26" s="309"/>
+      <c r="AY26" s="308"/>
+      <c r="AZ26" s="6"/>
+      <c r="BA26" s="6"/>
+      <c r="BB26" s="6"/>
+      <c r="BC26" s="6"/>
+      <c r="BD26" s="309"/>
+    </row>
+    <row r="27" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="C27" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>431</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="G27" s="15"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="M27" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="W27" s="308"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="309"/>
+      <c r="AD27" s="308"/>
+      <c r="AE27" s="6"/>
+      <c r="AF27" s="6"/>
+      <c r="AG27" s="6"/>
+      <c r="AH27" s="6"/>
+      <c r="AI27" s="309"/>
+      <c r="AK27" s="308"/>
+      <c r="AL27" s="6"/>
+      <c r="AM27" s="6"/>
+      <c r="AN27" s="6"/>
+      <c r="AO27" s="6"/>
+      <c r="AP27" s="309"/>
+      <c r="AR27" s="308"/>
+      <c r="AS27" s="6"/>
+      <c r="AT27" s="6"/>
+      <c r="AU27" s="6"/>
+      <c r="AV27" s="6"/>
+      <c r="AW27" s="309"/>
+      <c r="AY27" s="308"/>
+      <c r="AZ27" s="6"/>
+      <c r="BA27" s="6"/>
+      <c r="BB27" s="6"/>
+      <c r="BC27" s="6"/>
+      <c r="BD27" s="309"/>
+    </row>
+    <row r="28" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="W28" s="308"/>
+      <c r="X28" s="6"/>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="309"/>
+      <c r="AD28" s="308"/>
+      <c r="AE28" s="6"/>
+      <c r="AF28" s="6"/>
+      <c r="AG28" s="6"/>
+      <c r="AH28" s="6"/>
+      <c r="AI28" s="309"/>
+      <c r="AK28" s="308"/>
+      <c r="AL28" s="6"/>
+      <c r="AM28" s="6"/>
+      <c r="AN28" s="6"/>
+      <c r="AO28" s="6"/>
+      <c r="AP28" s="309"/>
+      <c r="AR28" s="308"/>
+      <c r="AS28" s="6"/>
+      <c r="AT28" s="6"/>
+      <c r="AU28" s="6"/>
+      <c r="AV28" s="6"/>
+      <c r="AW28" s="309"/>
+      <c r="AY28" s="308"/>
+      <c r="AZ28" s="6"/>
+      <c r="BA28" s="6"/>
+      <c r="BB28" s="6"/>
+      <c r="BC28" s="6"/>
+      <c r="BD28" s="309"/>
+    </row>
+    <row r="29" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G29" s="205"/>
+      <c r="I29" s="204"/>
+      <c r="J29" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="W29" s="323"/>
+      <c r="X29" s="218"/>
+      <c r="Y29" s="218"/>
+      <c r="Z29" s="218"/>
+      <c r="AA29" s="218"/>
+      <c r="AB29" s="325"/>
+      <c r="AD29" s="323"/>
+      <c r="AE29" s="218"/>
+      <c r="AF29" s="218"/>
+      <c r="AG29" s="218"/>
+      <c r="AH29" s="218"/>
+      <c r="AI29" s="325"/>
+      <c r="AK29" s="323"/>
+      <c r="AL29" s="218"/>
+      <c r="AM29" s="218"/>
+      <c r="AN29" s="218"/>
+      <c r="AO29" s="218"/>
+      <c r="AP29" s="325"/>
+      <c r="AR29" s="323"/>
+      <c r="AS29" s="218"/>
+      <c r="AT29" s="218"/>
+      <c r="AU29" s="218"/>
+      <c r="AV29" s="218"/>
+      <c r="AW29" s="325"/>
+      <c r="AY29" s="323"/>
+      <c r="AZ29" s="218"/>
+      <c r="BA29" s="218"/>
+      <c r="BB29" s="218"/>
+      <c r="BC29" s="218"/>
+      <c r="BD29" s="325"/>
+    </row>
+    <row r="30" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="C30" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="D30" s="207"/>
+      <c r="F30" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="L30" s="206"/>
+      <c r="M30" s="15" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="AT39" sqref="AT39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B1" s="70">
+        <v>0</v>
+      </c>
+      <c r="C1" s="70">
+        <f>B1+1</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="70">
+        <f t="shared" ref="D1:Q1" si="0">C1+1</f>
+        <v>2</v>
+      </c>
+      <c r="E1" s="70">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F1" s="70">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G1" s="70">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H1" s="70">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I1" s="70">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J1" s="70">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K1" s="70">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L1" s="70">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M1" s="70">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="N1" s="70">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O1" s="70">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P1" s="70">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q1" s="70">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="T1" s="70">
+        <v>0</v>
+      </c>
+      <c r="U1" s="70">
+        <f>T1+1</f>
+        <v>1</v>
+      </c>
+      <c r="V1" s="70">
+        <f t="shared" ref="V1:AI1" si="1">U1+1</f>
+        <v>2</v>
+      </c>
+      <c r="W1" s="70">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="X1" s="70">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Y1" s="70">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Z1" s="70">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="AA1" s="70">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="AB1" s="70">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="AC1" s="70">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="AD1" s="70">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="AE1" s="70">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="AF1" s="70">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="AG1" s="70">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="AH1" s="70">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="AI1" s="70">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A2" s="70">
+        <v>0</v>
+      </c>
+      <c r="B2" s="311"/>
+      <c r="C2" s="312"/>
+      <c r="D2" s="312"/>
+      <c r="E2" s="312"/>
+      <c r="F2" s="312"/>
+      <c r="G2" s="312"/>
+      <c r="H2" s="312"/>
+      <c r="I2" s="312"/>
+      <c r="J2" s="312"/>
+      <c r="K2" s="312"/>
+      <c r="L2" s="312"/>
+      <c r="M2" s="312"/>
+      <c r="N2" s="312"/>
+      <c r="O2" s="312"/>
+      <c r="P2" s="312"/>
+      <c r="Q2" s="313"/>
+      <c r="S2" s="70">
+        <v>0</v>
+      </c>
+      <c r="T2" s="328"/>
+      <c r="U2" s="335"/>
+      <c r="V2" s="335"/>
+      <c r="W2" s="335"/>
+      <c r="X2" s="335"/>
+      <c r="Y2" s="335"/>
+      <c r="Z2" s="335"/>
+      <c r="AA2" s="335"/>
+      <c r="AB2" s="335"/>
+      <c r="AC2" s="335"/>
+      <c r="AD2" s="335"/>
+      <c r="AE2" s="335"/>
+      <c r="AF2" s="335"/>
+      <c r="AG2" s="335"/>
+      <c r="AH2" s="335"/>
+      <c r="AI2" s="333"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A3" s="70">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="314"/>
+      <c r="C3" s="244"/>
+      <c r="D3" s="244"/>
+      <c r="E3" s="244"/>
+      <c r="F3" s="244"/>
+      <c r="G3" s="244"/>
+      <c r="H3" s="244"/>
+      <c r="I3" s="244"/>
+      <c r="J3" s="244"/>
+      <c r="K3" s="244"/>
+      <c r="L3" s="244"/>
+      <c r="M3" s="244"/>
+      <c r="N3" s="244"/>
+      <c r="O3" s="244"/>
+      <c r="P3" s="244"/>
+      <c r="Q3" s="315"/>
+      <c r="S3" s="70">
+        <f>S2+1</f>
+        <v>1</v>
+      </c>
+      <c r="T3" s="329"/>
+      <c r="U3" s="327"/>
+      <c r="V3" s="327"/>
+      <c r="W3" s="327"/>
+      <c r="X3" s="327"/>
+      <c r="Y3" s="327"/>
+      <c r="Z3" s="327"/>
+      <c r="AA3" s="327"/>
+      <c r="AB3" s="327"/>
+      <c r="AC3" s="327"/>
+      <c r="AD3" s="327"/>
+      <c r="AE3" s="327"/>
+      <c r="AF3" s="327"/>
+      <c r="AG3" s="327"/>
+      <c r="AH3" s="327"/>
+      <c r="AI3" s="334"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A4" s="70">
+        <f t="shared" ref="A4:A17" si="2">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="314"/>
+      <c r="C4" s="244"/>
+      <c r="D4" s="336"/>
+      <c r="E4" s="336"/>
+      <c r="F4" s="327"/>
+      <c r="G4" s="327"/>
+      <c r="H4" s="244"/>
+      <c r="I4" s="244"/>
+      <c r="J4" s="244"/>
+      <c r="K4" s="244"/>
+      <c r="L4" s="244"/>
+      <c r="M4" s="244"/>
+      <c r="N4" s="336"/>
+      <c r="O4" s="336"/>
+      <c r="P4" s="244"/>
+      <c r="Q4" s="315"/>
+      <c r="S4" s="70">
+        <f t="shared" ref="S4:S17" si="3">S3+1</f>
+        <v>2</v>
+      </c>
+      <c r="T4" s="329"/>
+      <c r="U4" s="327"/>
+      <c r="V4" s="336"/>
+      <c r="W4" s="336"/>
+      <c r="X4" s="327"/>
+      <c r="Y4" s="327"/>
+      <c r="Z4" s="327"/>
+      <c r="AA4" s="327"/>
+      <c r="AB4" s="327"/>
+      <c r="AC4" s="327"/>
+      <c r="AD4" s="327"/>
+      <c r="AE4" s="327"/>
+      <c r="AF4" s="336"/>
+      <c r="AG4" s="336"/>
+      <c r="AH4" s="327"/>
+      <c r="AI4" s="334"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A5" s="70">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="314"/>
+      <c r="C5" s="244"/>
+      <c r="D5" s="336"/>
+      <c r="E5" s="336"/>
+      <c r="F5" s="327"/>
+      <c r="G5" s="327"/>
+      <c r="H5" s="244"/>
+      <c r="I5" s="244"/>
+      <c r="J5" s="244"/>
+      <c r="K5" s="244"/>
+      <c r="L5" s="244"/>
+      <c r="M5" s="244"/>
+      <c r="N5" s="336"/>
+      <c r="O5" s="336"/>
+      <c r="P5" s="244"/>
+      <c r="Q5" s="315"/>
+      <c r="S5" s="70">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="T5" s="329"/>
+      <c r="U5" s="327"/>
+      <c r="V5" s="336"/>
+      <c r="W5" s="336"/>
+      <c r="X5" s="327"/>
+      <c r="Y5" s="327"/>
+      <c r="Z5" s="327"/>
+      <c r="AA5" s="327"/>
+      <c r="AB5" s="327"/>
+      <c r="AC5" s="327"/>
+      <c r="AD5" s="327"/>
+      <c r="AE5" s="327"/>
+      <c r="AF5" s="336"/>
+      <c r="AG5" s="336"/>
+      <c r="AH5" s="327"/>
+      <c r="AI5" s="334"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A6" s="70">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="314"/>
+      <c r="C6" s="244"/>
+      <c r="D6" s="327"/>
+      <c r="E6" s="339"/>
+      <c r="F6" s="327"/>
+      <c r="G6" s="327"/>
+      <c r="H6" s="244"/>
+      <c r="I6" s="244"/>
+      <c r="J6" s="244"/>
+      <c r="K6" s="244"/>
+      <c r="L6" s="244"/>
+      <c r="M6" s="244"/>
+      <c r="N6" s="244"/>
+      <c r="O6" s="244"/>
+      <c r="P6" s="244"/>
+      <c r="Q6" s="315"/>
+      <c r="S6" s="70">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="T6" s="329"/>
+      <c r="U6" s="327"/>
+      <c r="V6" s="327"/>
+      <c r="W6" s="339"/>
+      <c r="X6" s="327"/>
+      <c r="Y6" s="327"/>
+      <c r="Z6" s="327"/>
+      <c r="AA6" s="327"/>
+      <c r="AB6" s="327"/>
+      <c r="AC6" s="327"/>
+      <c r="AD6" s="327"/>
+      <c r="AE6" s="327"/>
+      <c r="AF6" s="327"/>
+      <c r="AG6" s="327"/>
+      <c r="AH6" s="327"/>
+      <c r="AI6" s="334"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A7" s="70">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="314"/>
+      <c r="C7" s="244"/>
+      <c r="D7" s="327"/>
+      <c r="E7" s="327"/>
+      <c r="F7" s="327"/>
+      <c r="G7" s="327"/>
+      <c r="H7" s="244"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="244"/>
+      <c r="K7" s="244"/>
+      <c r="L7" s="244"/>
+      <c r="M7" s="244"/>
+      <c r="N7" s="244"/>
+      <c r="O7" s="244"/>
+      <c r="P7" s="244"/>
+      <c r="Q7" s="315"/>
+      <c r="S7" s="70">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="T7" s="329"/>
+      <c r="U7" s="327"/>
+      <c r="V7" s="327"/>
+      <c r="W7" s="327"/>
+      <c r="X7" s="327"/>
+      <c r="Y7" s="327"/>
+      <c r="Z7" s="327"/>
+      <c r="AA7" s="128"/>
+      <c r="AB7" s="327"/>
+      <c r="AC7" s="327"/>
+      <c r="AD7" s="327"/>
+      <c r="AE7" s="327"/>
+      <c r="AF7" s="327"/>
+      <c r="AG7" s="327"/>
+      <c r="AH7" s="327"/>
+      <c r="AI7" s="334"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A8" s="70">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="314"/>
+      <c r="C8" s="244"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="244"/>
+      <c r="F8" s="244"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="244"/>
+      <c r="N8" s="244"/>
+      <c r="O8" s="244"/>
+      <c r="P8" s="244"/>
+      <c r="Q8" s="315"/>
+      <c r="S8" s="70">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="T8" s="329"/>
+      <c r="U8" s="327"/>
+      <c r="V8" s="327"/>
+      <c r="W8" s="327"/>
+      <c r="X8" s="327"/>
+      <c r="Y8" s="128"/>
+      <c r="Z8" s="162"/>
+      <c r="AA8" s="162"/>
+      <c r="AB8" s="162"/>
+      <c r="AC8" s="162"/>
+      <c r="AD8" s="128"/>
+      <c r="AE8" s="327"/>
+      <c r="AF8" s="327"/>
+      <c r="AG8" s="327"/>
+      <c r="AH8" s="327"/>
+      <c r="AI8" s="334"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A9" s="70">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="314"/>
+      <c r="C9" s="244"/>
+      <c r="D9" s="244"/>
+      <c r="E9" s="244"/>
+      <c r="F9" s="244"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="244"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="244"/>
+      <c r="N9" s="244"/>
+      <c r="O9" s="244"/>
+      <c r="P9" s="244"/>
+      <c r="Q9" s="315"/>
+      <c r="S9" s="70">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="T9" s="329"/>
+      <c r="U9" s="327"/>
+      <c r="V9" s="327"/>
+      <c r="W9" s="327"/>
+      <c r="X9" s="327"/>
+      <c r="Y9" s="128"/>
+      <c r="Z9" s="162"/>
+      <c r="AA9" s="244"/>
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="162"/>
+      <c r="AD9" s="128"/>
+      <c r="AE9" s="327"/>
+      <c r="AF9" s="327"/>
+      <c r="AG9" s="327"/>
+      <c r="AH9" s="327"/>
+      <c r="AI9" s="334"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A10" s="70">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="314"/>
+      <c r="C10" s="244"/>
+      <c r="D10" s="244"/>
+      <c r="E10" s="244"/>
+      <c r="F10" s="244"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="201"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="244"/>
+      <c r="N10" s="244"/>
+      <c r="O10" s="244"/>
+      <c r="P10" s="244"/>
+      <c r="Q10" s="315"/>
+      <c r="S10" s="70">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="T10" s="329"/>
+      <c r="U10" s="327"/>
+      <c r="V10" s="327"/>
+      <c r="W10" s="327"/>
+      <c r="X10" s="327"/>
+      <c r="Y10" s="128"/>
+      <c r="Z10" s="162"/>
+      <c r="AA10" s="17"/>
+      <c r="AB10" s="201"/>
+      <c r="AC10" s="162"/>
+      <c r="AD10" s="128"/>
+      <c r="AE10" s="327"/>
+      <c r="AF10" s="327"/>
+      <c r="AG10" s="327"/>
+      <c r="AH10" s="327"/>
+      <c r="AI10" s="334"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A11" s="70">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="314"/>
+      <c r="C11" s="244"/>
+      <c r="D11" s="244"/>
+      <c r="E11" s="244"/>
+      <c r="F11" s="244"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="244"/>
+      <c r="N11" s="244"/>
+      <c r="O11" s="244"/>
+      <c r="P11" s="244"/>
+      <c r="Q11" s="315"/>
+      <c r="S11" s="70">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="T11" s="329"/>
+      <c r="U11" s="327"/>
+      <c r="V11" s="327"/>
+      <c r="W11" s="327"/>
+      <c r="X11" s="327"/>
+      <c r="Y11" s="128"/>
+      <c r="Z11" s="162"/>
+      <c r="AA11" s="162"/>
+      <c r="AB11" s="162"/>
+      <c r="AC11" s="162"/>
+      <c r="AD11" s="128"/>
+      <c r="AE11" s="327"/>
+      <c r="AF11" s="327"/>
+      <c r="AG11" s="327"/>
+      <c r="AH11" s="327"/>
+      <c r="AI11" s="334"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A12" s="70">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="314"/>
+      <c r="C12" s="244"/>
+      <c r="D12" s="244"/>
+      <c r="E12" s="244"/>
+      <c r="F12" s="244"/>
+      <c r="G12" s="244"/>
+      <c r="H12" s="244"/>
+      <c r="I12" s="244"/>
+      <c r="J12" s="244"/>
+      <c r="K12" s="244"/>
+      <c r="L12" s="327"/>
+      <c r="M12" s="327"/>
+      <c r="N12" s="327"/>
+      <c r="O12" s="327"/>
+      <c r="P12" s="244"/>
+      <c r="Q12" s="315"/>
+      <c r="S12" s="70">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="T12" s="329"/>
+      <c r="U12" s="327"/>
+      <c r="V12" s="327"/>
+      <c r="W12" s="327"/>
+      <c r="X12" s="327"/>
+      <c r="Y12" s="327"/>
+      <c r="Z12" s="327"/>
+      <c r="AA12" s="327"/>
+      <c r="AB12" s="327"/>
+      <c r="AC12" s="327"/>
+      <c r="AD12" s="327"/>
+      <c r="AE12" s="327"/>
+      <c r="AF12" s="327"/>
+      <c r="AG12" s="327"/>
+      <c r="AH12" s="327"/>
+      <c r="AI12" s="334"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A13" s="70">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="314"/>
+      <c r="C13" s="244"/>
+      <c r="D13" s="244"/>
+      <c r="E13" s="244"/>
+      <c r="F13" s="244"/>
+      <c r="G13" s="244"/>
+      <c r="H13" s="244"/>
+      <c r="I13" s="244"/>
+      <c r="J13" s="244"/>
+      <c r="K13" s="244"/>
+      <c r="L13" s="327"/>
+      <c r="M13" s="327"/>
+      <c r="N13" s="339"/>
+      <c r="O13" s="327"/>
+      <c r="P13" s="244"/>
+      <c r="Q13" s="315"/>
+      <c r="S13" s="70">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="T13" s="329"/>
+      <c r="U13" s="327"/>
+      <c r="V13" s="327"/>
+      <c r="W13" s="327"/>
+      <c r="X13" s="327"/>
+      <c r="Y13" s="327"/>
+      <c r="Z13" s="327"/>
+      <c r="AA13" s="327"/>
+      <c r="AB13" s="327"/>
+      <c r="AC13" s="327"/>
+      <c r="AD13" s="327"/>
+      <c r="AE13" s="327"/>
+      <c r="AF13" s="339"/>
+      <c r="AG13" s="327"/>
+      <c r="AH13" s="327"/>
+      <c r="AI13" s="334"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A14" s="70">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="314"/>
+      <c r="C14" s="244"/>
+      <c r="D14" s="336"/>
+      <c r="E14" s="336"/>
+      <c r="F14" s="244"/>
+      <c r="G14" s="244"/>
+      <c r="H14" s="244"/>
+      <c r="I14" s="244"/>
+      <c r="J14" s="244"/>
+      <c r="K14" s="244"/>
+      <c r="L14" s="327"/>
+      <c r="M14" s="327"/>
+      <c r="N14" s="336"/>
+      <c r="O14" s="336"/>
+      <c r="P14" s="244"/>
+      <c r="Q14" s="315"/>
+      <c r="S14" s="70">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="T14" s="329"/>
+      <c r="U14" s="327"/>
+      <c r="V14" s="336"/>
+      <c r="W14" s="336"/>
+      <c r="X14" s="327"/>
+      <c r="Y14" s="327"/>
+      <c r="Z14" s="327"/>
+      <c r="AA14" s="327"/>
+      <c r="AB14" s="327"/>
+      <c r="AC14" s="327"/>
+      <c r="AD14" s="327"/>
+      <c r="AE14" s="327"/>
+      <c r="AF14" s="336"/>
+      <c r="AG14" s="336"/>
+      <c r="AH14" s="327"/>
+      <c r="AI14" s="334"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A15" s="70">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="314"/>
+      <c r="C15" s="244"/>
+      <c r="D15" s="336"/>
+      <c r="E15" s="336"/>
+      <c r="F15" s="244"/>
+      <c r="G15" s="244"/>
+      <c r="H15" s="244"/>
+      <c r="I15" s="244"/>
+      <c r="J15" s="244"/>
+      <c r="K15" s="244"/>
+      <c r="L15" s="327"/>
+      <c r="M15" s="327"/>
+      <c r="N15" s="336"/>
+      <c r="O15" s="336"/>
+      <c r="P15" s="244"/>
+      <c r="Q15" s="315"/>
+      <c r="S15" s="70">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="T15" s="329"/>
+      <c r="U15" s="327"/>
+      <c r="V15" s="336"/>
+      <c r="W15" s="336"/>
+      <c r="X15" s="327"/>
+      <c r="Y15" s="327"/>
+      <c r="Z15" s="327"/>
+      <c r="AA15" s="327"/>
+      <c r="AB15" s="327"/>
+      <c r="AC15" s="327"/>
+      <c r="AD15" s="327"/>
+      <c r="AE15" s="327"/>
+      <c r="AF15" s="336"/>
+      <c r="AG15" s="336"/>
+      <c r="AH15" s="327"/>
+      <c r="AI15" s="334"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A16" s="70">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="314"/>
+      <c r="C16" s="244"/>
+      <c r="D16" s="244"/>
+      <c r="E16" s="244"/>
+      <c r="F16" s="244"/>
+      <c r="G16" s="244"/>
+      <c r="H16" s="244"/>
+      <c r="I16" s="244"/>
+      <c r="J16" s="244"/>
+      <c r="K16" s="244"/>
+      <c r="L16" s="244"/>
+      <c r="M16" s="244"/>
+      <c r="N16" s="244"/>
+      <c r="O16" s="244"/>
+      <c r="P16" s="244"/>
+      <c r="Q16" s="315"/>
+      <c r="S16" s="70">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="T16" s="329"/>
+      <c r="U16" s="327"/>
+      <c r="V16" s="327"/>
+      <c r="W16" s="327"/>
+      <c r="X16" s="327"/>
+      <c r="Y16" s="327"/>
+      <c r="Z16" s="327"/>
+      <c r="AA16" s="327"/>
+      <c r="AB16" s="327"/>
+      <c r="AC16" s="327"/>
+      <c r="AD16" s="327"/>
+      <c r="AE16" s="327"/>
+      <c r="AF16" s="327"/>
+      <c r="AG16" s="327"/>
+      <c r="AH16" s="327"/>
+      <c r="AI16" s="334"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A17" s="70">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="316"/>
+      <c r="C17" s="317"/>
+      <c r="D17" s="317"/>
+      <c r="E17" s="317"/>
+      <c r="F17" s="317"/>
+      <c r="G17" s="317"/>
+      <c r="H17" s="317"/>
+      <c r="I17" s="317"/>
+      <c r="J17" s="317"/>
+      <c r="K17" s="317"/>
+      <c r="L17" s="317"/>
+      <c r="M17" s="317"/>
+      <c r="N17" s="317"/>
+      <c r="O17" s="317"/>
+      <c r="P17" s="317"/>
+      <c r="Q17" s="318"/>
+      <c r="S17" s="70">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="T17" s="330"/>
+      <c r="U17" s="331"/>
+      <c r="V17" s="331"/>
+      <c r="W17" s="331"/>
+      <c r="X17" s="331"/>
+      <c r="Y17" s="331"/>
+      <c r="Z17" s="331"/>
+      <c r="AA17" s="331"/>
+      <c r="AB17" s="331"/>
+      <c r="AC17" s="331"/>
+      <c r="AD17" s="331"/>
+      <c r="AE17" s="331"/>
+      <c r="AF17" s="331"/>
+      <c r="AG17" s="331"/>
+      <c r="AH17" s="331"/>
+      <c r="AI17" s="332"/>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B19" s="70">
+        <v>0</v>
+      </c>
+      <c r="C19" s="70">
+        <f>B19+1</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="70">
+        <f t="shared" ref="D19" si="4">C19+1</f>
+        <v>2</v>
+      </c>
+      <c r="E19" s="70">
+        <f t="shared" ref="E19" si="5">D19+1</f>
+        <v>3</v>
+      </c>
+      <c r="F19" s="70">
+        <f t="shared" ref="F19" si="6">E19+1</f>
+        <v>4</v>
+      </c>
+      <c r="G19" s="70">
+        <f t="shared" ref="G19" si="7">F19+1</f>
+        <v>5</v>
+      </c>
+      <c r="H19" s="70">
+        <f t="shared" ref="H19" si="8">G19+1</f>
+        <v>6</v>
+      </c>
+      <c r="I19" s="70">
+        <f t="shared" ref="I19" si="9">H19+1</f>
+        <v>7</v>
+      </c>
+      <c r="J19" s="70">
+        <f t="shared" ref="J19" si="10">I19+1</f>
+        <v>8</v>
+      </c>
+      <c r="K19" s="70">
+        <f t="shared" ref="K19" si="11">J19+1</f>
+        <v>9</v>
+      </c>
+      <c r="L19" s="70">
+        <f t="shared" ref="L19" si="12">K19+1</f>
+        <v>10</v>
+      </c>
+      <c r="M19" s="70">
+        <f t="shared" ref="M19" si="13">L19+1</f>
+        <v>11</v>
+      </c>
+      <c r="N19" s="70">
+        <f t="shared" ref="N19" si="14">M19+1</f>
+        <v>12</v>
+      </c>
+      <c r="O19" s="70">
+        <f t="shared" ref="O19" si="15">N19+1</f>
+        <v>13</v>
+      </c>
+      <c r="P19" s="70">
+        <f t="shared" ref="P19" si="16">O19+1</f>
+        <v>14</v>
+      </c>
+      <c r="Q19" s="70">
+        <f t="shared" ref="Q19" si="17">P19+1</f>
+        <v>15</v>
+      </c>
+      <c r="T19" s="70">
+        <v>0</v>
+      </c>
+      <c r="U19" s="70">
+        <f>T19+1</f>
+        <v>1</v>
+      </c>
+      <c r="V19" s="70">
+        <f t="shared" ref="V19" si="18">U19+1</f>
+        <v>2</v>
+      </c>
+      <c r="W19" s="70">
+        <f t="shared" ref="W19" si="19">V19+1</f>
+        <v>3</v>
+      </c>
+      <c r="X19" s="70">
+        <f t="shared" ref="X19" si="20">W19+1</f>
+        <v>4</v>
+      </c>
+      <c r="Y19" s="70">
+        <f t="shared" ref="Y19" si="21">X19+1</f>
+        <v>5</v>
+      </c>
+      <c r="Z19" s="70">
+        <f t="shared" ref="Z19" si="22">Y19+1</f>
+        <v>6</v>
+      </c>
+      <c r="AA19" s="70">
+        <f t="shared" ref="AA19" si="23">Z19+1</f>
+        <v>7</v>
+      </c>
+      <c r="AB19" s="70">
+        <f t="shared" ref="AB19" si="24">AA19+1</f>
+        <v>8</v>
+      </c>
+      <c r="AC19" s="70">
+        <f t="shared" ref="AC19" si="25">AB19+1</f>
+        <v>9</v>
+      </c>
+      <c r="AD19" s="70">
+        <f t="shared" ref="AD19" si="26">AC19+1</f>
+        <v>10</v>
+      </c>
+      <c r="AE19" s="70">
+        <f t="shared" ref="AE19" si="27">AD19+1</f>
+        <v>11</v>
+      </c>
+      <c r="AF19" s="70">
+        <f t="shared" ref="AF19" si="28">AE19+1</f>
+        <v>12</v>
+      </c>
+      <c r="AG19" s="70">
+        <f t="shared" ref="AG19" si="29">AF19+1</f>
+        <v>13</v>
+      </c>
+      <c r="AH19" s="70">
+        <f t="shared" ref="AH19" si="30">AG19+1</f>
+        <v>14</v>
+      </c>
+      <c r="AI19" s="70">
+        <f t="shared" ref="AI19" si="31">AH19+1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A20" s="70">
+        <v>0</v>
+      </c>
+      <c r="B20" s="328"/>
+      <c r="C20" s="335"/>
+      <c r="D20" s="335"/>
+      <c r="E20" s="335"/>
+      <c r="F20" s="335"/>
+      <c r="G20" s="335"/>
+      <c r="H20" s="335"/>
+      <c r="I20" s="335"/>
+      <c r="J20" s="335"/>
+      <c r="K20" s="335"/>
+      <c r="L20" s="335"/>
+      <c r="M20" s="335"/>
+      <c r="N20" s="335"/>
+      <c r="O20" s="335"/>
+      <c r="P20" s="335"/>
+      <c r="Q20" s="333"/>
+      <c r="S20" s="70">
+        <v>0</v>
+      </c>
+      <c r="T20" s="311"/>
+      <c r="U20" s="312"/>
+      <c r="V20" s="312"/>
+      <c r="W20" s="312"/>
+      <c r="X20" s="312"/>
+      <c r="Y20" s="312"/>
+      <c r="Z20" s="312"/>
+      <c r="AA20" s="312"/>
+      <c r="AB20" s="312"/>
+      <c r="AC20" s="312"/>
+      <c r="AD20" s="312"/>
+      <c r="AE20" s="312"/>
+      <c r="AF20" s="312"/>
+      <c r="AG20" s="312"/>
+      <c r="AH20" s="312"/>
+      <c r="AI20" s="313"/>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A21" s="70">
+        <f>A20+1</f>
+        <v>1</v>
+      </c>
+      <c r="B21" s="329"/>
+      <c r="C21" s="327"/>
+      <c r="D21" s="327"/>
+      <c r="E21" s="327"/>
+      <c r="F21" s="327"/>
+      <c r="G21" s="327"/>
+      <c r="H21" s="327"/>
+      <c r="I21" s="327"/>
+      <c r="J21" s="327"/>
+      <c r="K21" s="327"/>
+      <c r="L21" s="327"/>
+      <c r="M21" s="327"/>
+      <c r="N21" s="327"/>
+      <c r="O21" s="327"/>
+      <c r="P21" s="327"/>
+      <c r="Q21" s="334"/>
+      <c r="S21" s="70">
+        <f>S20+1</f>
+        <v>1</v>
+      </c>
+      <c r="T21" s="314"/>
+      <c r="U21" s="244"/>
+      <c r="V21" s="244"/>
+      <c r="W21" s="244"/>
+      <c r="X21" s="244"/>
+      <c r="Y21" s="338"/>
+      <c r="AA21" s="338"/>
+      <c r="AB21" s="244"/>
+      <c r="AC21" s="338"/>
+      <c r="AD21" s="34"/>
+      <c r="AE21" s="338"/>
+      <c r="AG21" s="244"/>
+      <c r="AH21" s="244"/>
+      <c r="AI21" s="315"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A22" s="70">
+        <f t="shared" ref="A22:A35" si="32">A21+1</f>
+        <v>2</v>
+      </c>
+      <c r="B22" s="329"/>
+      <c r="C22" s="327"/>
+      <c r="D22" s="336"/>
+      <c r="E22" s="336"/>
+      <c r="F22" s="327"/>
+      <c r="G22" s="327"/>
+      <c r="H22" s="327"/>
+      <c r="I22" s="327"/>
+      <c r="J22" s="327"/>
+      <c r="K22" s="327"/>
+      <c r="L22" s="327"/>
+      <c r="M22" s="327"/>
+      <c r="N22" s="336"/>
+      <c r="O22" s="336"/>
+      <c r="P22" s="327"/>
+      <c r="Q22" s="334"/>
+      <c r="S22" s="70">
+        <f t="shared" ref="S22:S35" si="33">S21+1</f>
+        <v>2</v>
+      </c>
+      <c r="T22" s="314"/>
+      <c r="U22" s="244"/>
+      <c r="V22" s="336"/>
+      <c r="W22" s="336"/>
+      <c r="X22" s="337"/>
+      <c r="Y22" s="337"/>
+      <c r="Z22" s="337"/>
+      <c r="AA22" s="337"/>
+      <c r="AB22" s="337"/>
+      <c r="AC22" s="337"/>
+      <c r="AD22" s="337"/>
+      <c r="AE22" s="337"/>
+      <c r="AF22" s="337"/>
+      <c r="AG22" s="336"/>
+      <c r="AH22" s="244"/>
+      <c r="AI22" s="315"/>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A23" s="70">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+      <c r="B23" s="329"/>
+      <c r="C23" s="327"/>
+      <c r="D23" s="336"/>
+      <c r="E23" s="336"/>
+      <c r="F23" s="327"/>
+      <c r="G23" s="327"/>
+      <c r="H23" s="327"/>
+      <c r="I23" s="327"/>
+      <c r="J23" s="327"/>
+      <c r="K23" s="327"/>
+      <c r="L23" s="327"/>
+      <c r="M23" s="327"/>
+      <c r="N23" s="336"/>
+      <c r="O23" s="336"/>
+      <c r="P23" s="327"/>
+      <c r="Q23" s="334"/>
+      <c r="S23" s="70">
+        <f t="shared" si="33"/>
+        <v>3</v>
+      </c>
+      <c r="T23" s="314"/>
+      <c r="U23" s="244"/>
+      <c r="V23" s="336"/>
+      <c r="W23" s="336"/>
+      <c r="X23" s="327"/>
+      <c r="Y23" s="327"/>
+      <c r="Z23" s="327"/>
+      <c r="AA23" s="327"/>
+      <c r="AB23" s="327"/>
+      <c r="AC23" s="327"/>
+      <c r="AD23" s="327"/>
+      <c r="AE23" s="327"/>
+      <c r="AF23" s="327"/>
+      <c r="AG23" s="337"/>
+      <c r="AH23" s="244"/>
+      <c r="AI23" s="315"/>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A24" s="70">
+        <f t="shared" si="32"/>
+        <v>4</v>
+      </c>
+      <c r="B24" s="329"/>
+      <c r="C24" s="327"/>
+      <c r="D24" s="327"/>
+      <c r="E24" s="339"/>
+      <c r="F24" s="327"/>
+      <c r="G24" s="327"/>
+      <c r="H24" s="327"/>
+      <c r="I24" s="327"/>
+      <c r="J24" s="327"/>
+      <c r="K24" s="327"/>
+      <c r="L24" s="327"/>
+      <c r="M24" s="327"/>
+      <c r="N24" s="327"/>
+      <c r="O24" s="327"/>
+      <c r="P24" s="327"/>
+      <c r="Q24" s="334"/>
+      <c r="S24" s="70">
+        <f t="shared" si="33"/>
+        <v>4</v>
+      </c>
+      <c r="T24" s="314"/>
+      <c r="U24" s="244"/>
+      <c r="V24" s="337"/>
+      <c r="W24" s="339"/>
+      <c r="X24" s="327"/>
+      <c r="Y24" s="327"/>
+      <c r="Z24" s="327"/>
+      <c r="AA24" s="327"/>
+      <c r="AB24" s="327"/>
+      <c r="AC24" s="327"/>
+      <c r="AD24" s="327"/>
+      <c r="AE24" s="327"/>
+      <c r="AF24" s="327"/>
+      <c r="AG24" s="337"/>
+      <c r="AH24" s="244"/>
+      <c r="AI24" s="315"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A25" s="70">
+        <f t="shared" si="32"/>
+        <v>5</v>
+      </c>
+      <c r="B25" s="329"/>
+      <c r="C25" s="327"/>
+      <c r="D25" s="327"/>
+      <c r="E25" s="327"/>
+      <c r="F25" s="327"/>
+      <c r="G25" s="327"/>
+      <c r="H25" s="327"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="327"/>
+      <c r="K25" s="327"/>
+      <c r="L25" s="327"/>
+      <c r="M25" s="327"/>
+      <c r="N25" s="327"/>
+      <c r="O25" s="327"/>
+      <c r="P25" s="327"/>
+      <c r="Q25" s="334"/>
+      <c r="S25" s="70">
+        <f t="shared" si="33"/>
+        <v>5</v>
+      </c>
+      <c r="T25" s="314"/>
+      <c r="U25" s="244"/>
+      <c r="V25" s="337"/>
+      <c r="W25" s="327"/>
+      <c r="X25" s="327"/>
+      <c r="Y25" s="327"/>
+      <c r="Z25" s="327"/>
+      <c r="AA25" s="128"/>
+      <c r="AB25" s="327"/>
+      <c r="AC25" s="327"/>
+      <c r="AD25" s="327"/>
+      <c r="AE25" s="327"/>
+      <c r="AF25" s="327"/>
+      <c r="AG25" s="337"/>
+      <c r="AH25" s="244"/>
+      <c r="AI25" s="315"/>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A26" s="70">
+        <f t="shared" si="32"/>
+        <v>6</v>
+      </c>
+      <c r="B26" s="329"/>
+      <c r="C26" s="327"/>
+      <c r="D26" s="327"/>
+      <c r="E26" s="327"/>
+      <c r="F26" s="327"/>
+      <c r="G26" s="128"/>
+      <c r="H26" s="162"/>
+      <c r="I26" s="162"/>
+      <c r="J26" s="162"/>
+      <c r="K26" s="162"/>
+      <c r="L26" s="128"/>
+      <c r="M26" s="327"/>
+      <c r="N26" s="327"/>
+      <c r="O26" s="327"/>
+      <c r="P26" s="327"/>
+      <c r="Q26" s="334"/>
+      <c r="S26" s="70">
+        <f t="shared" si="33"/>
+        <v>6</v>
+      </c>
+      <c r="T26" s="314"/>
+      <c r="U26" s="244"/>
+      <c r="V26" s="337"/>
+      <c r="W26" s="327"/>
+      <c r="X26" s="327"/>
+      <c r="Y26" s="128"/>
+      <c r="Z26" s="162"/>
+      <c r="AA26" s="162"/>
+      <c r="AB26" s="162"/>
+      <c r="AC26" s="340"/>
+      <c r="AD26" s="128"/>
+      <c r="AE26" s="327"/>
+      <c r="AF26" s="327"/>
+      <c r="AG26" s="337"/>
+      <c r="AH26" s="244"/>
+      <c r="AI26" s="315"/>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A27" s="70">
+        <f t="shared" si="32"/>
+        <v>7</v>
+      </c>
+      <c r="B27" s="329"/>
+      <c r="C27" s="327"/>
+      <c r="D27" s="327"/>
+      <c r="E27" s="327"/>
+      <c r="F27" s="327"/>
+      <c r="G27" s="128"/>
+      <c r="H27" s="162"/>
+      <c r="I27" s="244"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="162"/>
+      <c r="L27" s="128"/>
+      <c r="M27" s="327"/>
+      <c r="N27" s="327"/>
+      <c r="O27" s="327"/>
+      <c r="P27" s="327"/>
+      <c r="Q27" s="334"/>
+      <c r="S27" s="70">
+        <f t="shared" si="33"/>
+        <v>7</v>
+      </c>
+      <c r="T27" s="314"/>
+      <c r="U27" s="244"/>
+      <c r="V27" s="337"/>
+      <c r="W27" s="327"/>
+      <c r="X27" s="327"/>
+      <c r="Y27" s="128"/>
+      <c r="Z27" s="162"/>
+      <c r="AA27" s="244"/>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="162"/>
+      <c r="AD27" s="128"/>
+      <c r="AE27" s="327"/>
+      <c r="AF27" s="327"/>
+      <c r="AG27" s="337"/>
+      <c r="AH27" s="244"/>
+      <c r="AI27" s="315"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A28" s="70">
+        <f t="shared" si="32"/>
+        <v>8</v>
+      </c>
+      <c r="B28" s="329"/>
+      <c r="C28" s="327"/>
+      <c r="D28" s="327"/>
+      <c r="E28" s="327"/>
+      <c r="F28" s="327"/>
+      <c r="G28" s="128"/>
+      <c r="H28" s="162"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="201"/>
+      <c r="K28" s="162"/>
+      <c r="L28" s="128"/>
+      <c r="M28" s="327"/>
+      <c r="N28" s="327"/>
+      <c r="O28" s="327"/>
+      <c r="P28" s="327"/>
+      <c r="Q28" s="334"/>
+      <c r="S28" s="70">
+        <f t="shared" si="33"/>
+        <v>8</v>
+      </c>
+      <c r="T28" s="314"/>
+      <c r="U28" s="244"/>
+      <c r="V28" s="337"/>
+      <c r="W28" s="327"/>
+      <c r="X28" s="327"/>
+      <c r="Y28" s="128"/>
+      <c r="Z28" s="162"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="201"/>
+      <c r="AC28" s="162"/>
+      <c r="AD28" s="128"/>
+      <c r="AE28" s="327"/>
+      <c r="AF28" s="327"/>
+      <c r="AG28" s="337"/>
+      <c r="AH28" s="244"/>
+      <c r="AI28" s="315"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A29" s="70">
+        <f t="shared" si="32"/>
+        <v>9</v>
+      </c>
+      <c r="B29" s="329"/>
+      <c r="C29" s="327"/>
+      <c r="D29" s="327"/>
+      <c r="E29" s="327"/>
+      <c r="F29" s="327"/>
+      <c r="G29" s="128"/>
+      <c r="H29" s="162"/>
+      <c r="I29" s="162"/>
+      <c r="J29" s="162"/>
+      <c r="K29" s="162"/>
+      <c r="L29" s="128"/>
+      <c r="M29" s="327"/>
+      <c r="N29" s="327"/>
+      <c r="O29" s="327"/>
+      <c r="P29" s="327"/>
+      <c r="Q29" s="334"/>
+      <c r="S29" s="70">
+        <f t="shared" si="33"/>
+        <v>9</v>
+      </c>
+      <c r="T29" s="314"/>
+      <c r="U29" s="244"/>
+      <c r="V29" s="337"/>
+      <c r="W29" s="327"/>
+      <c r="X29" s="327"/>
+      <c r="Y29" s="128"/>
+      <c r="Z29" s="340"/>
+      <c r="AA29" s="162"/>
+      <c r="AB29" s="162"/>
+      <c r="AC29" s="162"/>
+      <c r="AD29" s="128"/>
+      <c r="AE29" s="327"/>
+      <c r="AF29" s="327"/>
+      <c r="AG29" s="337"/>
+      <c r="AH29" s="34"/>
+      <c r="AI29" s="315"/>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A30" s="70">
+        <f t="shared" si="32"/>
+        <v>10</v>
+      </c>
+      <c r="B30" s="329"/>
+      <c r="C30" s="327"/>
+      <c r="D30" s="327"/>
+      <c r="E30" s="327"/>
+      <c r="F30" s="327"/>
+      <c r="G30" s="327"/>
+      <c r="H30" s="327"/>
+      <c r="I30" s="327"/>
+      <c r="J30" s="327"/>
+      <c r="K30" s="327"/>
+      <c r="L30" s="327"/>
+      <c r="M30" s="327"/>
+      <c r="N30" s="327"/>
+      <c r="O30" s="327"/>
+      <c r="P30" s="327"/>
+      <c r="Q30" s="334"/>
+      <c r="S30" s="70">
+        <f t="shared" si="33"/>
+        <v>10</v>
+      </c>
+      <c r="T30" s="314"/>
+      <c r="U30" s="244"/>
+      <c r="V30" s="337"/>
+      <c r="W30" s="327"/>
+      <c r="X30" s="327"/>
+      <c r="Y30" s="327"/>
+      <c r="Z30" s="327"/>
+      <c r="AA30" s="327"/>
+      <c r="AB30" s="327"/>
+      <c r="AC30" s="327"/>
+      <c r="AD30" s="327"/>
+      <c r="AE30" s="327"/>
+      <c r="AF30" s="327"/>
+      <c r="AG30" s="337"/>
+      <c r="AH30" s="244"/>
+      <c r="AI30" s="315"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A31" s="70">
+        <f t="shared" si="32"/>
+        <v>11</v>
+      </c>
+      <c r="B31" s="329"/>
+      <c r="C31" s="327"/>
+      <c r="D31" s="327"/>
+      <c r="E31" s="327"/>
+      <c r="F31" s="327"/>
+      <c r="G31" s="327"/>
+      <c r="H31" s="327"/>
+      <c r="I31" s="327"/>
+      <c r="J31" s="327"/>
+      <c r="K31" s="327"/>
+      <c r="L31" s="327"/>
+      <c r="M31" s="327"/>
+      <c r="N31" s="339"/>
+      <c r="O31" s="327"/>
+      <c r="P31" s="327"/>
+      <c r="Q31" s="334"/>
+      <c r="S31" s="70">
+        <f t="shared" si="33"/>
+        <v>11</v>
+      </c>
+      <c r="T31" s="314"/>
+      <c r="U31" s="244"/>
+      <c r="V31" s="337"/>
+      <c r="W31" s="327"/>
+      <c r="X31" s="327"/>
+      <c r="Y31" s="327"/>
+      <c r="Z31" s="327"/>
+      <c r="AA31" s="327"/>
+      <c r="AB31" s="327"/>
+      <c r="AC31" s="327"/>
+      <c r="AD31" s="327"/>
+      <c r="AE31" s="327"/>
+      <c r="AF31" s="339"/>
+      <c r="AG31" s="337"/>
+      <c r="AH31" s="244"/>
+      <c r="AI31" s="315"/>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A32" s="70">
+        <f t="shared" si="32"/>
+        <v>12</v>
+      </c>
+      <c r="B32" s="329"/>
+      <c r="C32" s="327"/>
+      <c r="D32" s="336"/>
+      <c r="E32" s="336"/>
+      <c r="F32" s="327"/>
+      <c r="G32" s="327"/>
+      <c r="H32" s="327"/>
+      <c r="I32" s="327"/>
+      <c r="J32" s="327"/>
+      <c r="K32" s="327"/>
+      <c r="L32" s="327"/>
+      <c r="M32" s="327"/>
+      <c r="N32" s="336"/>
+      <c r="O32" s="336"/>
+      <c r="P32" s="327"/>
+      <c r="Q32" s="334"/>
+      <c r="S32" s="70">
+        <f t="shared" si="33"/>
+        <v>12</v>
+      </c>
+      <c r="T32" s="314"/>
+      <c r="U32" s="244"/>
+      <c r="V32" s="337"/>
+      <c r="W32" s="327"/>
+      <c r="X32" s="327"/>
+      <c r="Y32" s="327"/>
+      <c r="Z32" s="327"/>
+      <c r="AA32" s="327"/>
+      <c r="AB32" s="327"/>
+      <c r="AC32" s="327"/>
+      <c r="AD32" s="327"/>
+      <c r="AE32" s="327"/>
+      <c r="AF32" s="336"/>
+      <c r="AG32" s="336"/>
+      <c r="AH32" s="244"/>
+      <c r="AI32" s="315"/>
+    </row>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A33" s="70">
+        <f t="shared" si="32"/>
+        <v>13</v>
+      </c>
+      <c r="B33" s="329"/>
+      <c r="C33" s="327"/>
+      <c r="D33" s="336"/>
+      <c r="E33" s="336"/>
+      <c r="F33" s="327"/>
+      <c r="G33" s="327"/>
+      <c r="H33" s="327"/>
+      <c r="I33" s="327"/>
+      <c r="J33" s="327"/>
+      <c r="K33" s="327"/>
+      <c r="L33" s="327"/>
+      <c r="M33" s="327"/>
+      <c r="N33" s="336"/>
+      <c r="O33" s="336"/>
+      <c r="P33" s="327"/>
+      <c r="Q33" s="334"/>
+      <c r="S33" s="70">
+        <f t="shared" si="33"/>
+        <v>13</v>
+      </c>
+      <c r="T33" s="314"/>
+      <c r="U33" s="244"/>
+      <c r="V33" s="336"/>
+      <c r="W33" s="337"/>
+      <c r="X33" s="337"/>
+      <c r="Y33" s="337"/>
+      <c r="Z33" s="337"/>
+      <c r="AA33" s="337"/>
+      <c r="AB33" s="337"/>
+      <c r="AC33" s="337"/>
+      <c r="AD33" s="337"/>
+      <c r="AE33" s="337"/>
+      <c r="AF33" s="336"/>
+      <c r="AG33" s="336"/>
+      <c r="AH33" s="244"/>
+      <c r="AI33" s="315"/>
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A34" s="70">
+        <f t="shared" si="32"/>
+        <v>14</v>
+      </c>
+      <c r="B34" s="329"/>
+      <c r="C34" s="327"/>
+      <c r="D34" s="327"/>
+      <c r="E34" s="327"/>
+      <c r="F34" s="327"/>
+      <c r="G34" s="327"/>
+      <c r="H34" s="327"/>
+      <c r="I34" s="327"/>
+      <c r="J34" s="327"/>
+      <c r="K34" s="327"/>
+      <c r="L34" s="327"/>
+      <c r="M34" s="327"/>
+      <c r="N34" s="327"/>
+      <c r="O34" s="327"/>
+      <c r="P34" s="327"/>
+      <c r="Q34" s="334"/>
+      <c r="S34" s="70">
+        <f t="shared" si="33"/>
+        <v>14</v>
+      </c>
+      <c r="T34" s="314"/>
+      <c r="U34" s="244"/>
+      <c r="V34" s="244"/>
+      <c r="W34" s="244"/>
+      <c r="X34" s="244"/>
+      <c r="Y34" s="244"/>
+      <c r="Z34" s="244"/>
+      <c r="AA34" s="244"/>
+      <c r="AB34" s="244"/>
+      <c r="AC34" s="244"/>
+      <c r="AD34" s="244"/>
+      <c r="AE34" s="244"/>
+      <c r="AF34" s="244"/>
+      <c r="AG34" s="244"/>
+      <c r="AH34" s="244"/>
+      <c r="AI34" s="315"/>
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A35" s="70">
+        <f t="shared" si="32"/>
+        <v>15</v>
+      </c>
+      <c r="B35" s="330"/>
+      <c r="C35" s="331"/>
+      <c r="D35" s="331"/>
+      <c r="E35" s="331"/>
+      <c r="F35" s="331"/>
+      <c r="G35" s="331"/>
+      <c r="H35" s="331"/>
+      <c r="I35" s="331"/>
+      <c r="J35" s="331"/>
+      <c r="K35" s="331"/>
+      <c r="L35" s="331"/>
+      <c r="M35" s="331"/>
+      <c r="N35" s="331"/>
+      <c r="O35" s="331"/>
+      <c r="P35" s="331"/>
+      <c r="Q35" s="332"/>
+      <c r="S35" s="70">
+        <f t="shared" si="33"/>
+        <v>15</v>
+      </c>
+      <c r="T35" s="316"/>
+      <c r="U35" s="317"/>
+      <c r="V35" s="317"/>
+      <c r="W35" s="317"/>
+      <c r="X35" s="317"/>
+      <c r="Y35" s="317"/>
+      <c r="Z35" s="317"/>
+      <c r="AA35" s="317"/>
+      <c r="AB35" s="317"/>
+      <c r="AC35" s="317"/>
+      <c r="AD35" s="317"/>
+      <c r="AE35" s="317"/>
+      <c r="AF35" s="317"/>
+      <c r="AG35" s="317"/>
+      <c r="AH35" s="317"/>
+      <c r="AI35" s="318"/>
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="T37" s="70">
+        <v>0</v>
+      </c>
+      <c r="U37" s="70">
+        <f>T37+1</f>
+        <v>1</v>
+      </c>
+      <c r="V37" s="70">
+        <f t="shared" ref="V37" si="34">U37+1</f>
+        <v>2</v>
+      </c>
+      <c r="W37" s="70">
+        <f t="shared" ref="W37" si="35">V37+1</f>
+        <v>3</v>
+      </c>
+      <c r="X37" s="70">
+        <f t="shared" ref="X37" si="36">W37+1</f>
+        <v>4</v>
+      </c>
+      <c r="Y37" s="70">
+        <f t="shared" ref="Y37" si="37">X37+1</f>
+        <v>5</v>
+      </c>
+      <c r="Z37" s="70">
+        <f t="shared" ref="Z37" si="38">Y37+1</f>
+        <v>6</v>
+      </c>
+      <c r="AA37" s="70">
+        <f t="shared" ref="AA37" si="39">Z37+1</f>
+        <v>7</v>
+      </c>
+      <c r="AB37" s="70">
+        <f t="shared" ref="AB37" si="40">AA37+1</f>
+        <v>8</v>
+      </c>
+      <c r="AC37" s="70">
+        <f t="shared" ref="AC37" si="41">AB37+1</f>
+        <v>9</v>
+      </c>
+      <c r="AD37" s="70">
+        <f t="shared" ref="AD37" si="42">AC37+1</f>
+        <v>10</v>
+      </c>
+      <c r="AE37" s="70">
+        <f t="shared" ref="AE37" si="43">AD37+1</f>
+        <v>11</v>
+      </c>
+      <c r="AF37" s="70">
+        <f t="shared" ref="AF37" si="44">AE37+1</f>
+        <v>12</v>
+      </c>
+      <c r="AG37" s="70">
+        <f t="shared" ref="AG37" si="45">AF37+1</f>
+        <v>13</v>
+      </c>
+      <c r="AH37" s="70">
+        <f t="shared" ref="AH37" si="46">AG37+1</f>
+        <v>14</v>
+      </c>
+      <c r="AI37" s="70">
+        <f t="shared" ref="AI37" si="47">AH37+1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="S38" s="70">
+        <v>0</v>
+      </c>
+      <c r="T38" s="311"/>
+      <c r="U38" s="312"/>
+      <c r="V38" s="312"/>
+      <c r="W38" s="312"/>
+      <c r="X38" s="312"/>
+      <c r="Y38" s="312"/>
+      <c r="Z38" s="312"/>
+      <c r="AA38" s="312"/>
+      <c r="AB38" s="312"/>
+      <c r="AC38" s="312"/>
+      <c r="AD38" s="312"/>
+      <c r="AE38" s="312"/>
+      <c r="AF38" s="312"/>
+      <c r="AG38" s="312"/>
+      <c r="AH38" s="312"/>
+      <c r="AI38" s="313"/>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="S39" s="70">
+        <f>S38+1</f>
+        <v>1</v>
+      </c>
+      <c r="T39" s="314"/>
+      <c r="U39" s="244"/>
+      <c r="V39" s="244"/>
+      <c r="W39" s="244"/>
+      <c r="X39" s="244"/>
+      <c r="Y39" s="244"/>
+      <c r="Z39" s="244"/>
+      <c r="AA39" s="34"/>
+      <c r="AB39" s="244"/>
+      <c r="AC39" s="244"/>
+      <c r="AD39" s="244"/>
+      <c r="AE39" s="34"/>
+      <c r="AF39" s="244"/>
+      <c r="AG39" s="244"/>
+      <c r="AH39" s="244"/>
+      <c r="AI39" s="315"/>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="S40" s="70">
+        <f t="shared" ref="S40:S53" si="48">S39+1</f>
+        <v>2</v>
+      </c>
+      <c r="T40" s="314"/>
+      <c r="U40" s="244"/>
+      <c r="V40" s="336"/>
+      <c r="W40" s="336"/>
+      <c r="X40" s="244"/>
+      <c r="Y40" s="244"/>
+      <c r="Z40" s="244"/>
+      <c r="AA40" s="244"/>
+      <c r="AB40" s="244"/>
+      <c r="AC40" s="244"/>
+      <c r="AD40" s="244"/>
+      <c r="AE40" s="244"/>
+      <c r="AF40" s="244"/>
+      <c r="AG40" s="244"/>
+      <c r="AH40" s="244"/>
+      <c r="AI40" s="315"/>
+    </row>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="S41" s="70">
+        <f t="shared" si="48"/>
+        <v>3</v>
+      </c>
+      <c r="T41" s="314"/>
+      <c r="U41" s="244"/>
+      <c r="V41" s="336"/>
+      <c r="W41" s="336"/>
+      <c r="X41" s="244"/>
+      <c r="Y41" s="244"/>
+      <c r="Z41" s="244"/>
+      <c r="AA41" s="244"/>
+      <c r="AB41" s="244"/>
+      <c r="AC41" s="244"/>
+      <c r="AD41" s="244"/>
+      <c r="AE41" s="244"/>
+      <c r="AF41" s="244"/>
+      <c r="AG41" s="244"/>
+      <c r="AH41" s="244"/>
+      <c r="AI41" s="315"/>
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="S42" s="70">
+        <f t="shared" si="48"/>
+        <v>4</v>
+      </c>
+      <c r="T42" s="314"/>
+      <c r="U42" s="244"/>
+      <c r="V42" s="244"/>
+      <c r="W42" s="339"/>
+      <c r="X42" s="244"/>
+      <c r="Y42" s="244"/>
+      <c r="Z42" s="244"/>
+      <c r="AA42" s="244"/>
+      <c r="AB42" s="244"/>
+      <c r="AC42" s="244"/>
+      <c r="AD42" s="244"/>
+      <c r="AE42" s="244"/>
+      <c r="AF42" s="244"/>
+      <c r="AG42" s="244"/>
+      <c r="AH42" s="244"/>
+      <c r="AI42" s="315"/>
+    </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="S43" s="70">
+        <f t="shared" si="48"/>
+        <v>5</v>
+      </c>
+      <c r="T43" s="314"/>
+      <c r="U43" s="244"/>
+      <c r="V43" s="244"/>
+      <c r="W43" s="244"/>
+      <c r="X43" s="244"/>
+      <c r="Y43" s="244"/>
+      <c r="Z43" s="244"/>
+      <c r="AA43" s="17"/>
+      <c r="AB43" s="244"/>
+      <c r="AC43" s="244"/>
+      <c r="AD43" s="244"/>
+      <c r="AE43" s="244"/>
+      <c r="AF43" s="244"/>
+      <c r="AG43" s="244"/>
+      <c r="AH43" s="244"/>
+      <c r="AI43" s="315"/>
+    </row>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="S44" s="70">
+        <f t="shared" si="48"/>
+        <v>6</v>
+      </c>
+      <c r="T44" s="314"/>
+      <c r="U44" s="244"/>
+      <c r="V44" s="244"/>
+      <c r="W44" s="244"/>
+      <c r="X44" s="244"/>
+      <c r="Y44" s="17"/>
+      <c r="Z44" s="17"/>
+      <c r="AA44" s="17"/>
+      <c r="AB44" s="17"/>
+      <c r="AC44" s="340"/>
+      <c r="AD44" s="162"/>
+      <c r="AE44" s="337"/>
+      <c r="AF44" s="337"/>
+      <c r="AG44" s="337"/>
+      <c r="AH44" s="244"/>
+      <c r="AI44" s="315"/>
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="S45" s="70">
+        <f t="shared" si="48"/>
+        <v>7</v>
+      </c>
+      <c r="T45" s="314"/>
+      <c r="U45" s="244"/>
+      <c r="V45" s="244"/>
+      <c r="W45" s="244"/>
+      <c r="X45" s="244"/>
+      <c r="Y45" s="17"/>
+      <c r="Z45" s="17"/>
+      <c r="AA45" s="341"/>
+      <c r="AB45" s="140"/>
+      <c r="AC45" s="128"/>
+      <c r="AD45" s="128"/>
+      <c r="AE45" s="327"/>
+      <c r="AF45" s="327"/>
+      <c r="AG45" s="337"/>
+      <c r="AH45" s="244"/>
+      <c r="AI45" s="315"/>
+    </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="S46" s="70">
+        <f t="shared" si="48"/>
+        <v>8</v>
+      </c>
+      <c r="T46" s="314"/>
+      <c r="U46" s="244"/>
+      <c r="V46" s="244"/>
+      <c r="W46" s="244"/>
+      <c r="X46" s="244"/>
+      <c r="Y46" s="17"/>
+      <c r="Z46" s="17"/>
+      <c r="AA46" s="140"/>
+      <c r="AB46" s="201"/>
+      <c r="AC46" s="128"/>
+      <c r="AD46" s="128"/>
+      <c r="AE46" s="327"/>
+      <c r="AF46" s="327"/>
+      <c r="AG46" s="337"/>
+      <c r="AH46" s="244"/>
+      <c r="AI46" s="315"/>
+    </row>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="S47" s="70">
+        <f t="shared" si="48"/>
+        <v>9</v>
+      </c>
+      <c r="T47" s="314"/>
+      <c r="U47" s="244"/>
+      <c r="V47" s="244"/>
+      <c r="W47" s="244"/>
+      <c r="X47" s="244"/>
+      <c r="Y47" s="17"/>
+      <c r="Z47" s="340"/>
+      <c r="AA47" s="128"/>
+      <c r="AB47" s="128"/>
+      <c r="AC47" s="128"/>
+      <c r="AD47" s="128"/>
+      <c r="AE47" s="327"/>
+      <c r="AF47" s="327"/>
+      <c r="AG47" s="337"/>
+      <c r="AH47" s="34"/>
+      <c r="AI47" s="315"/>
+    </row>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="S48" s="70">
+        <f t="shared" si="48"/>
+        <v>10</v>
+      </c>
+      <c r="T48" s="314"/>
+      <c r="U48" s="244"/>
+      <c r="V48" s="244"/>
+      <c r="W48" s="244"/>
+      <c r="X48" s="244"/>
+      <c r="Y48" s="244"/>
+      <c r="Z48" s="337"/>
+      <c r="AA48" s="327"/>
+      <c r="AB48" s="327"/>
+      <c r="AC48" s="327"/>
+      <c r="AD48" s="327"/>
+      <c r="AE48" s="327"/>
+      <c r="AF48" s="327"/>
+      <c r="AG48" s="337"/>
+      <c r="AH48" s="244"/>
+      <c r="AI48" s="315"/>
+    </row>
+    <row r="49" spans="19:35" x14ac:dyDescent="0.3">
+      <c r="S49" s="70">
+        <f t="shared" si="48"/>
+        <v>11</v>
+      </c>
+      <c r="T49" s="314"/>
+      <c r="U49" s="244"/>
+      <c r="V49" s="244"/>
+      <c r="W49" s="244"/>
+      <c r="X49" s="244"/>
+      <c r="Y49" s="244"/>
+      <c r="Z49" s="337"/>
+      <c r="AA49" s="327"/>
+      <c r="AB49" s="327"/>
+      <c r="AC49" s="327"/>
+      <c r="AD49" s="327"/>
+      <c r="AE49" s="327"/>
+      <c r="AF49" s="339"/>
+      <c r="AG49" s="337"/>
+      <c r="AH49" s="244"/>
+      <c r="AI49" s="315"/>
+    </row>
+    <row r="50" spans="19:35" x14ac:dyDescent="0.3">
+      <c r="S50" s="70">
+        <f t="shared" si="48"/>
+        <v>12</v>
+      </c>
+      <c r="T50" s="314"/>
+      <c r="U50" s="244"/>
+      <c r="V50" s="244"/>
+      <c r="W50" s="244"/>
+      <c r="X50" s="244"/>
+      <c r="Y50" s="244"/>
+      <c r="Z50" s="337"/>
+      <c r="AA50" s="327"/>
+      <c r="AB50" s="327"/>
+      <c r="AC50" s="327"/>
+      <c r="AD50" s="327"/>
+      <c r="AE50" s="327"/>
+      <c r="AF50" s="336"/>
+      <c r="AG50" s="336"/>
+      <c r="AH50" s="244"/>
+      <c r="AI50" s="315"/>
+    </row>
+    <row r="51" spans="19:35" x14ac:dyDescent="0.3">
+      <c r="S51" s="70">
+        <f t="shared" si="48"/>
+        <v>13</v>
+      </c>
+      <c r="T51" s="314"/>
+      <c r="U51" s="244"/>
+      <c r="V51" s="244"/>
+      <c r="W51" s="244"/>
+      <c r="X51" s="244"/>
+      <c r="Y51" s="244"/>
+      <c r="Z51" s="337"/>
+      <c r="AA51" s="337"/>
+      <c r="AB51" s="337"/>
+      <c r="AC51" s="337"/>
+      <c r="AD51" s="337"/>
+      <c r="AE51" s="337"/>
+      <c r="AF51" s="336"/>
+      <c r="AG51" s="336"/>
+      <c r="AH51" s="244"/>
+      <c r="AI51" s="315"/>
+    </row>
+    <row r="52" spans="19:35" x14ac:dyDescent="0.3">
+      <c r="S52" s="70">
+        <f t="shared" si="48"/>
+        <v>14</v>
+      </c>
+      <c r="T52" s="314"/>
+      <c r="U52" s="244"/>
+      <c r="V52" s="244"/>
+      <c r="W52" s="244"/>
+      <c r="X52" s="244"/>
+      <c r="Y52" s="244"/>
+      <c r="Z52" s="244"/>
+      <c r="AA52" s="244"/>
+      <c r="AB52" s="244"/>
+      <c r="AC52" s="244"/>
+      <c r="AD52" s="244"/>
+      <c r="AE52" s="244"/>
+      <c r="AF52" s="244"/>
+      <c r="AG52" s="244"/>
+      <c r="AH52" s="244"/>
+      <c r="AI52" s="315"/>
+    </row>
+    <row r="53" spans="19:35" x14ac:dyDescent="0.3">
+      <c r="S53" s="70">
+        <f t="shared" si="48"/>
+        <v>15</v>
+      </c>
+      <c r="T53" s="316"/>
+      <c r="U53" s="317"/>
+      <c r="V53" s="317"/>
+      <c r="W53" s="317"/>
+      <c r="X53" s="317"/>
+      <c r="Y53" s="317"/>
+      <c r="Z53" s="317"/>
+      <c r="AA53" s="317"/>
+      <c r="AB53" s="317"/>
+      <c r="AC53" s="317"/>
+      <c r="AD53" s="317"/>
+      <c r="AE53" s="317"/>
+      <c r="AF53" s="317"/>
+      <c r="AG53" s="317"/>
+      <c r="AH53" s="317"/>
+      <c r="AI53" s="318"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Now with simple underground facilities... mind you they are hard to find
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="31" activeTab="38"/>
+    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="31" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -44,8 +44,9 @@
     <sheet name="Bridge" sheetId="43" r:id="rId35"/>
     <sheet name="House" sheetId="44" r:id="rId36"/>
     <sheet name="Drilling Platform" sheetId="45" r:id="rId37"/>
-    <sheet name="Mineshafts" sheetId="46" r:id="rId38"/>
-    <sheet name="Sheet4" sheetId="47" r:id="rId39"/>
+    <sheet name="Mineshafts, thoughts" sheetId="46" state="hidden" r:id="rId38"/>
+    <sheet name="Mineshafts" sheetId="47" r:id="rId39"/>
+    <sheet name="Bunkers" sheetId="48" r:id="rId40"/>
   </sheets>
   <definedNames>
     <definedName name="AbsoluteMaximumFloorsBelow">Sheet3!$C$6</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="433">
   <si>
     <t>grove</t>
   </si>
@@ -1890,7 +1891,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="374">
+  <cellXfs count="385">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2497,6 +2498,39 @@
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3533,7 +3567,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3553,7 +3587,7 @@
       </c>
       <c r="O6">
         <f t="shared" ref="O6:AB15" ca="1" si="8">IF(AND(MOD(O$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3593,7 +3627,7 @@
       </c>
       <c r="Y6">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4123,7 +4157,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4143,7 +4177,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4163,7 +4197,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4653,7 +4687,7 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:N29" ca="1" si="11">IF(AND(MOD(E$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4673,7 +4707,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4713,7 +4747,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5223,7 +5257,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5243,7 +5277,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5263,7 +5297,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5283,7 +5317,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5303,7 +5337,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5793,7 +5827,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5813,7 +5847,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5833,7 +5867,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5853,7 +5887,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -50463,7 +50497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:Q35"/>
     </sheetView>
   </sheetViews>
@@ -52432,8 +52466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CL37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="BA26" sqref="BA26"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -56532,6 +56566,1260 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A1" s="242"/>
+      <c r="B1" s="70">
+        <v>0</v>
+      </c>
+      <c r="C1" s="70">
+        <f>B1+1</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="70">
+        <f t="shared" ref="D1:Q1" si="0">C1+1</f>
+        <v>2</v>
+      </c>
+      <c r="E1" s="70">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F1" s="70">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G1" s="70">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H1" s="70">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I1" s="70">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J1" s="70">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K1" s="70">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L1" s="70">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M1" s="70">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="N1" s="70">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O1" s="70">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P1" s="70">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q1" s="70">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="R1" s="242" t="s">
+        <v>394</v>
+      </c>
+      <c r="T1" s="242"/>
+      <c r="U1" s="70">
+        <v>0</v>
+      </c>
+      <c r="V1" s="70">
+        <f>U1+1</f>
+        <v>1</v>
+      </c>
+      <c r="W1" s="70">
+        <f t="shared" ref="W1" si="1">V1+1</f>
+        <v>2</v>
+      </c>
+      <c r="X1" s="70">
+        <f t="shared" ref="X1" si="2">W1+1</f>
+        <v>3</v>
+      </c>
+      <c r="Y1" s="70">
+        <f t="shared" ref="Y1" si="3">X1+1</f>
+        <v>4</v>
+      </c>
+      <c r="Z1" s="70">
+        <f t="shared" ref="Z1" si="4">Y1+1</f>
+        <v>5</v>
+      </c>
+      <c r="AA1" s="70">
+        <f t="shared" ref="AA1" si="5">Z1+1</f>
+        <v>6</v>
+      </c>
+      <c r="AB1" s="70">
+        <f t="shared" ref="AB1" si="6">AA1+1</f>
+        <v>7</v>
+      </c>
+      <c r="AC1" s="70">
+        <f t="shared" ref="AC1" si="7">AB1+1</f>
+        <v>8</v>
+      </c>
+      <c r="AD1" s="70">
+        <f t="shared" ref="AD1" si="8">AC1+1</f>
+        <v>9</v>
+      </c>
+      <c r="AE1" s="70">
+        <f t="shared" ref="AE1" si="9">AD1+1</f>
+        <v>10</v>
+      </c>
+      <c r="AF1" s="70">
+        <f t="shared" ref="AF1" si="10">AE1+1</f>
+        <v>11</v>
+      </c>
+      <c r="AG1" s="70">
+        <f t="shared" ref="AG1" si="11">AF1+1</f>
+        <v>12</v>
+      </c>
+      <c r="AH1" s="70">
+        <f t="shared" ref="AH1" si="12">AG1+1</f>
+        <v>13</v>
+      </c>
+      <c r="AI1" s="70">
+        <f t="shared" ref="AI1" si="13">AH1+1</f>
+        <v>14</v>
+      </c>
+      <c r="AJ1" s="70">
+        <f t="shared" ref="AJ1" si="14">AI1+1</f>
+        <v>15</v>
+      </c>
+      <c r="AK1" s="242" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A2" s="70">
+        <v>0</v>
+      </c>
+      <c r="B2" s="378"/>
+      <c r="C2" s="348"/>
+      <c r="D2" s="312"/>
+      <c r="E2" s="312"/>
+      <c r="F2" s="312"/>
+      <c r="G2" s="312"/>
+      <c r="H2" s="374"/>
+      <c r="I2" s="357"/>
+      <c r="J2" s="357"/>
+      <c r="K2" s="374"/>
+      <c r="L2" s="312"/>
+      <c r="M2" s="312"/>
+      <c r="N2" s="312"/>
+      <c r="O2" s="312"/>
+      <c r="P2" s="348"/>
+      <c r="Q2" s="377"/>
+      <c r="T2" s="70">
+        <v>0</v>
+      </c>
+      <c r="U2" s="381"/>
+      <c r="V2" s="356"/>
+      <c r="W2" s="356"/>
+      <c r="X2" s="356"/>
+      <c r="Y2" s="356"/>
+      <c r="Z2" s="356"/>
+      <c r="AA2" s="356"/>
+      <c r="AB2" s="356"/>
+      <c r="AC2" s="356"/>
+      <c r="AD2" s="356"/>
+      <c r="AE2" s="356"/>
+      <c r="AF2" s="356"/>
+      <c r="AG2" s="356"/>
+      <c r="AH2" s="356"/>
+      <c r="AI2" s="356"/>
+      <c r="AJ2" s="379"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A3" s="70">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="382"/>
+      <c r="C3" s="244"/>
+      <c r="D3" s="244"/>
+      <c r="E3" s="244"/>
+      <c r="F3" s="244"/>
+      <c r="G3" s="244"/>
+      <c r="H3" s="384"/>
+      <c r="I3" s="342"/>
+      <c r="J3" s="342"/>
+      <c r="K3" s="384"/>
+      <c r="L3" s="244"/>
+      <c r="M3" s="244"/>
+      <c r="N3" s="244"/>
+      <c r="O3" s="244"/>
+      <c r="P3" s="244"/>
+      <c r="Q3" s="380"/>
+      <c r="T3" s="70">
+        <f>T2+1</f>
+        <v>1</v>
+      </c>
+      <c r="U3" s="382"/>
+      <c r="V3" s="239"/>
+      <c r="W3" s="239"/>
+      <c r="X3" s="239"/>
+      <c r="Y3" s="239"/>
+      <c r="Z3" s="239"/>
+      <c r="AA3" s="239"/>
+      <c r="AB3" s="239"/>
+      <c r="AC3" s="239"/>
+      <c r="AD3" s="239"/>
+      <c r="AE3" s="239"/>
+      <c r="AF3" s="239"/>
+      <c r="AG3" s="239"/>
+      <c r="AH3" s="239"/>
+      <c r="AI3" s="239"/>
+      <c r="AJ3" s="380"/>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A4" s="70">
+        <f t="shared" ref="A4:A17" si="15">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="314"/>
+      <c r="C4" s="244"/>
+      <c r="D4" s="342"/>
+      <c r="E4" s="342"/>
+      <c r="F4" s="342"/>
+      <c r="G4" s="342"/>
+      <c r="H4" s="342"/>
+      <c r="I4" s="319"/>
+      <c r="J4" s="319"/>
+      <c r="K4" s="342"/>
+      <c r="L4" s="342"/>
+      <c r="M4" s="342"/>
+      <c r="N4" s="342"/>
+      <c r="O4" s="342"/>
+      <c r="P4" s="244"/>
+      <c r="Q4" s="315"/>
+      <c r="T4" s="70">
+        <f t="shared" ref="T4:T17" si="16">T3+1</f>
+        <v>2</v>
+      </c>
+      <c r="U4" s="343"/>
+      <c r="V4" s="327"/>
+      <c r="W4" s="244"/>
+      <c r="X4" s="244"/>
+      <c r="Y4" s="244"/>
+      <c r="Z4" s="244"/>
+      <c r="AA4" s="244"/>
+      <c r="AB4" s="244"/>
+      <c r="AC4" s="244"/>
+      <c r="AD4" s="244"/>
+      <c r="AE4" s="244"/>
+      <c r="AF4" s="244"/>
+      <c r="AG4" s="244"/>
+      <c r="AH4" s="244"/>
+      <c r="AI4" s="327"/>
+      <c r="AJ4" s="344"/>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A5" s="70">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="314"/>
+      <c r="C5" s="244"/>
+      <c r="D5" s="342"/>
+      <c r="E5" s="319"/>
+      <c r="F5" s="319"/>
+      <c r="G5" s="319"/>
+      <c r="H5" s="319"/>
+      <c r="I5" s="319"/>
+      <c r="J5" s="319"/>
+      <c r="K5" s="319"/>
+      <c r="L5" s="319"/>
+      <c r="M5" s="319"/>
+      <c r="N5" s="319"/>
+      <c r="O5" s="342"/>
+      <c r="P5" s="244"/>
+      <c r="Q5" s="315"/>
+      <c r="T5" s="70">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="U5" s="343"/>
+      <c r="V5" s="327"/>
+      <c r="W5" s="244"/>
+      <c r="X5" s="244"/>
+      <c r="Y5" s="244"/>
+      <c r="Z5" s="244"/>
+      <c r="AA5" s="244"/>
+      <c r="AB5" s="244"/>
+      <c r="AC5" s="244"/>
+      <c r="AD5" s="244"/>
+      <c r="AE5" s="244"/>
+      <c r="AF5" s="244"/>
+      <c r="AG5" s="244"/>
+      <c r="AH5" s="244"/>
+      <c r="AI5" s="327"/>
+      <c r="AJ5" s="344"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A6" s="70">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="314"/>
+      <c r="C6" s="244"/>
+      <c r="D6" s="342"/>
+      <c r="E6" s="319"/>
+      <c r="F6" s="320"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="320"/>
+      <c r="N6" s="319"/>
+      <c r="O6" s="342"/>
+      <c r="P6" s="244"/>
+      <c r="Q6" s="315"/>
+      <c r="T6" s="70">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="U6" s="343"/>
+      <c r="V6" s="327"/>
+      <c r="W6" s="244"/>
+      <c r="X6" s="244"/>
+      <c r="Y6" s="244"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="244"/>
+      <c r="AG6" s="244"/>
+      <c r="AH6" s="244"/>
+      <c r="AI6" s="327"/>
+      <c r="AJ6" s="344"/>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A7" s="70">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="314"/>
+      <c r="C7" s="244"/>
+      <c r="D7" s="342"/>
+      <c r="E7" s="319"/>
+      <c r="F7" s="320"/>
+      <c r="G7" s="142"/>
+      <c r="H7" s="142"/>
+      <c r="I7" s="319"/>
+      <c r="J7" s="142"/>
+      <c r="K7" s="142"/>
+      <c r="L7" s="142"/>
+      <c r="M7" s="320"/>
+      <c r="N7" s="319"/>
+      <c r="O7" s="342"/>
+      <c r="P7" s="244"/>
+      <c r="Q7" s="315"/>
+      <c r="T7" s="70">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="U7" s="343"/>
+      <c r="V7" s="327"/>
+      <c r="W7" s="244"/>
+      <c r="X7" s="244"/>
+      <c r="Y7" s="244"/>
+      <c r="Z7" s="17"/>
+      <c r="AA7" s="17"/>
+      <c r="AB7" s="244"/>
+      <c r="AC7" s="17"/>
+      <c r="AD7" s="17"/>
+      <c r="AE7" s="17"/>
+      <c r="AF7" s="244"/>
+      <c r="AG7" s="244"/>
+      <c r="AH7" s="244"/>
+      <c r="AI7" s="327"/>
+      <c r="AJ7" s="344"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A8" s="70">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="376"/>
+      <c r="C8" s="384"/>
+      <c r="D8" s="342"/>
+      <c r="E8" s="319"/>
+      <c r="F8" s="320"/>
+      <c r="G8" s="142"/>
+      <c r="H8" s="142"/>
+      <c r="I8" s="142"/>
+      <c r="J8" s="142"/>
+      <c r="K8" s="142"/>
+      <c r="L8" s="142"/>
+      <c r="M8" s="320"/>
+      <c r="N8" s="319"/>
+      <c r="O8" s="342"/>
+      <c r="P8" s="384"/>
+      <c r="Q8" s="375"/>
+      <c r="T8" s="70">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="U8" s="343"/>
+      <c r="V8" s="327"/>
+      <c r="W8" s="244"/>
+      <c r="X8" s="244"/>
+      <c r="Y8" s="244"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="17"/>
+      <c r="AF8" s="244"/>
+      <c r="AG8" s="244"/>
+      <c r="AH8" s="244"/>
+      <c r="AI8" s="327"/>
+      <c r="AJ8" s="344"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A9" s="70">
+        <f t="shared" si="15"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="308"/>
+      <c r="C9" s="219"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="142"/>
+      <c r="H9" s="142"/>
+      <c r="I9" s="142"/>
+      <c r="J9" s="142"/>
+      <c r="K9" s="142"/>
+      <c r="L9" s="142"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="142"/>
+      <c r="O9" s="142"/>
+      <c r="P9" s="219"/>
+      <c r="Q9" s="309"/>
+      <c r="T9" s="70">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="U9" s="127"/>
+      <c r="V9" s="128"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17"/>
+      <c r="AA9" s="17"/>
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="17"/>
+      <c r="AD9" s="17"/>
+      <c r="AE9" s="17"/>
+      <c r="AF9" s="17"/>
+      <c r="AG9" s="17"/>
+      <c r="AH9" s="17"/>
+      <c r="AI9" s="128"/>
+      <c r="AJ9" s="130"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A10" s="70">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="383"/>
+      <c r="C10" s="342"/>
+      <c r="D10" s="319"/>
+      <c r="E10" s="319"/>
+      <c r="F10" s="320"/>
+      <c r="G10" s="142"/>
+      <c r="H10" s="142"/>
+      <c r="I10" s="142"/>
+      <c r="J10" s="142"/>
+      <c r="K10" s="142"/>
+      <c r="L10" s="142"/>
+      <c r="M10" s="320"/>
+      <c r="N10" s="319"/>
+      <c r="O10" s="319"/>
+      <c r="P10" s="342"/>
+      <c r="Q10" s="352"/>
+      <c r="T10" s="70">
+        <f t="shared" si="16"/>
+        <v>8</v>
+      </c>
+      <c r="U10" s="343"/>
+      <c r="V10" s="327"/>
+      <c r="W10" s="244"/>
+      <c r="X10" s="244"/>
+      <c r="Y10" s="244"/>
+      <c r="Z10" s="17"/>
+      <c r="AA10" s="17"/>
+      <c r="AB10" s="17"/>
+      <c r="AC10" s="17"/>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="17"/>
+      <c r="AF10" s="244"/>
+      <c r="AG10" s="244"/>
+      <c r="AH10" s="244"/>
+      <c r="AI10" s="327"/>
+      <c r="AJ10" s="344"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A11" s="70">
+        <f t="shared" si="15"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="376"/>
+      <c r="C11" s="384"/>
+      <c r="D11" s="219"/>
+      <c r="E11" s="142"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="142"/>
+      <c r="H11" s="142"/>
+      <c r="I11" s="142"/>
+      <c r="J11" s="142"/>
+      <c r="K11" s="142"/>
+      <c r="L11" s="142"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="142"/>
+      <c r="O11" s="219"/>
+      <c r="P11" s="384"/>
+      <c r="Q11" s="375"/>
+      <c r="T11" s="70">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="U11" s="343"/>
+      <c r="V11" s="327"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="17"/>
+      <c r="AG11" s="17"/>
+      <c r="AH11" s="17"/>
+      <c r="AI11" s="327"/>
+      <c r="AJ11" s="344"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A12" s="70">
+        <f t="shared" si="15"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="314"/>
+      <c r="C12" s="244"/>
+      <c r="D12" s="342"/>
+      <c r="E12" s="319"/>
+      <c r="F12" s="320"/>
+      <c r="G12" s="319"/>
+      <c r="H12" s="319"/>
+      <c r="I12" s="319"/>
+      <c r="J12" s="319"/>
+      <c r="K12" s="319"/>
+      <c r="L12" s="319"/>
+      <c r="M12" s="320"/>
+      <c r="N12" s="319"/>
+      <c r="O12" s="342"/>
+      <c r="P12" s="244"/>
+      <c r="Q12" s="315"/>
+      <c r="T12" s="70">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="U12" s="343"/>
+      <c r="V12" s="327"/>
+      <c r="W12" s="244"/>
+      <c r="X12" s="244"/>
+      <c r="Y12" s="244"/>
+      <c r="Z12" s="244"/>
+      <c r="AA12" s="244"/>
+      <c r="AB12" s="244"/>
+      <c r="AC12" s="244"/>
+      <c r="AD12" s="244"/>
+      <c r="AE12" s="244"/>
+      <c r="AF12" s="244"/>
+      <c r="AG12" s="244"/>
+      <c r="AH12" s="244"/>
+      <c r="AI12" s="327"/>
+      <c r="AJ12" s="344"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A13" s="70">
+        <f t="shared" si="15"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="314"/>
+      <c r="C13" s="244"/>
+      <c r="D13" s="342"/>
+      <c r="E13" s="319"/>
+      <c r="F13" s="320"/>
+      <c r="G13" s="320"/>
+      <c r="H13" s="320"/>
+      <c r="I13" s="320"/>
+      <c r="J13" s="320"/>
+      <c r="K13" s="320"/>
+      <c r="L13" s="320"/>
+      <c r="M13" s="320"/>
+      <c r="N13" s="319"/>
+      <c r="O13" s="342"/>
+      <c r="P13" s="244"/>
+      <c r="Q13" s="315"/>
+      <c r="T13" s="70">
+        <f t="shared" si="16"/>
+        <v>11</v>
+      </c>
+      <c r="U13" s="343"/>
+      <c r="V13" s="327"/>
+      <c r="W13" s="244"/>
+      <c r="X13" s="244"/>
+      <c r="Y13" s="244"/>
+      <c r="Z13" s="244"/>
+      <c r="AA13" s="244"/>
+      <c r="AB13" s="244"/>
+      <c r="AC13" s="244"/>
+      <c r="AD13" s="244"/>
+      <c r="AE13" s="244"/>
+      <c r="AF13" s="244"/>
+      <c r="AG13" s="244"/>
+      <c r="AH13" s="244"/>
+      <c r="AI13" s="327"/>
+      <c r="AJ13" s="344"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A14" s="70">
+        <f t="shared" si="15"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="314"/>
+      <c r="C14" s="244"/>
+      <c r="D14" s="342"/>
+      <c r="E14" s="319"/>
+      <c r="F14" s="319"/>
+      <c r="G14" s="319"/>
+      <c r="H14" s="319"/>
+      <c r="I14" s="319"/>
+      <c r="J14" s="319"/>
+      <c r="K14" s="319"/>
+      <c r="L14" s="319"/>
+      <c r="M14" s="319"/>
+      <c r="N14" s="319"/>
+      <c r="O14" s="342"/>
+      <c r="P14" s="244"/>
+      <c r="Q14" s="315"/>
+      <c r="T14" s="70">
+        <f t="shared" si="16"/>
+        <v>12</v>
+      </c>
+      <c r="U14" s="343"/>
+      <c r="V14" s="327"/>
+      <c r="W14" s="244"/>
+      <c r="X14" s="244"/>
+      <c r="Y14" s="244"/>
+      <c r="Z14" s="244"/>
+      <c r="AA14" s="244"/>
+      <c r="AB14" s="244"/>
+      <c r="AC14" s="244"/>
+      <c r="AD14" s="244"/>
+      <c r="AE14" s="244"/>
+      <c r="AF14" s="244"/>
+      <c r="AG14" s="244"/>
+      <c r="AH14" s="244"/>
+      <c r="AI14" s="327"/>
+      <c r="AJ14" s="344"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A15" s="70">
+        <f t="shared" si="15"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="314"/>
+      <c r="C15" s="244"/>
+      <c r="D15" s="342"/>
+      <c r="E15" s="342"/>
+      <c r="F15" s="342"/>
+      <c r="G15" s="342"/>
+      <c r="H15" s="342"/>
+      <c r="I15" s="319"/>
+      <c r="J15" s="319"/>
+      <c r="K15" s="342"/>
+      <c r="L15" s="342"/>
+      <c r="M15" s="342"/>
+      <c r="N15" s="342"/>
+      <c r="O15" s="342"/>
+      <c r="P15" s="244"/>
+      <c r="Q15" s="315"/>
+      <c r="T15" s="70">
+        <f t="shared" si="16"/>
+        <v>13</v>
+      </c>
+      <c r="U15" s="343"/>
+      <c r="V15" s="327"/>
+      <c r="W15" s="244"/>
+      <c r="X15" s="244"/>
+      <c r="Y15" s="244"/>
+      <c r="Z15" s="244"/>
+      <c r="AA15" s="244"/>
+      <c r="AB15" s="244"/>
+      <c r="AC15" s="244"/>
+      <c r="AD15" s="244"/>
+      <c r="AE15" s="244"/>
+      <c r="AF15" s="244"/>
+      <c r="AG15" s="244"/>
+      <c r="AH15" s="244"/>
+      <c r="AI15" s="327"/>
+      <c r="AJ15" s="344"/>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A16" s="70">
+        <f t="shared" si="15"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="120"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="244"/>
+      <c r="E16" s="244"/>
+      <c r="F16" s="244"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="226"/>
+      <c r="I16" s="219"/>
+      <c r="J16" s="219"/>
+      <c r="K16" s="226"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="244"/>
+      <c r="N16" s="244"/>
+      <c r="O16" s="244"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="123"/>
+      <c r="T16" s="70">
+        <f t="shared" si="16"/>
+        <v>14</v>
+      </c>
+      <c r="U16" s="120"/>
+      <c r="V16" s="121"/>
+      <c r="W16" s="239"/>
+      <c r="X16" s="239"/>
+      <c r="Y16" s="239"/>
+      <c r="Z16" s="121"/>
+      <c r="AA16" s="121"/>
+      <c r="AB16" s="121"/>
+      <c r="AC16" s="121"/>
+      <c r="AD16" s="121"/>
+      <c r="AE16" s="121"/>
+      <c r="AF16" s="239"/>
+      <c r="AG16" s="239"/>
+      <c r="AH16" s="239"/>
+      <c r="AI16" s="121"/>
+      <c r="AJ16" s="123"/>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A17" s="70">
+        <f t="shared" si="15"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="206"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="358"/>
+      <c r="I17" s="218"/>
+      <c r="J17" s="218"/>
+      <c r="K17" s="358"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="129"/>
+      <c r="Q17" s="207"/>
+      <c r="T17" s="70">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="U17" s="126"/>
+      <c r="V17" s="124"/>
+      <c r="W17" s="124"/>
+      <c r="X17" s="124"/>
+      <c r="Y17" s="124"/>
+      <c r="Z17" s="124"/>
+      <c r="AA17" s="124"/>
+      <c r="AB17" s="124"/>
+      <c r="AC17" s="124"/>
+      <c r="AD17" s="124"/>
+      <c r="AE17" s="124"/>
+      <c r="AF17" s="124"/>
+      <c r="AG17" s="124"/>
+      <c r="AH17" s="124"/>
+      <c r="AI17" s="124"/>
+      <c r="AJ17" s="125"/>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A18" s="242" t="s">
+        <v>395</v>
+      </c>
+      <c r="T18" s="242" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A20" s="242"/>
+      <c r="B20" s="70">
+        <v>0</v>
+      </c>
+      <c r="C20" s="70">
+        <f>B20+1</f>
+        <v>1</v>
+      </c>
+      <c r="D20" s="70">
+        <f t="shared" ref="D20" si="17">C20+1</f>
+        <v>2</v>
+      </c>
+      <c r="E20" s="70">
+        <f t="shared" ref="E20" si="18">D20+1</f>
+        <v>3</v>
+      </c>
+      <c r="F20" s="70">
+        <f t="shared" ref="F20" si="19">E20+1</f>
+        <v>4</v>
+      </c>
+      <c r="G20" s="70">
+        <f t="shared" ref="G20" si="20">F20+1</f>
+        <v>5</v>
+      </c>
+      <c r="H20" s="70">
+        <f t="shared" ref="H20" si="21">G20+1</f>
+        <v>6</v>
+      </c>
+      <c r="I20" s="70">
+        <f t="shared" ref="I20" si="22">H20+1</f>
+        <v>7</v>
+      </c>
+      <c r="J20" s="70">
+        <f t="shared" ref="J20" si="23">I20+1</f>
+        <v>8</v>
+      </c>
+      <c r="K20" s="70">
+        <f t="shared" ref="K20" si="24">J20+1</f>
+        <v>9</v>
+      </c>
+      <c r="L20" s="70">
+        <f t="shared" ref="L20" si="25">K20+1</f>
+        <v>10</v>
+      </c>
+      <c r="M20" s="70">
+        <f t="shared" ref="M20" si="26">L20+1</f>
+        <v>11</v>
+      </c>
+      <c r="N20" s="70">
+        <f t="shared" ref="N20" si="27">M20+1</f>
+        <v>12</v>
+      </c>
+      <c r="O20" s="70">
+        <f t="shared" ref="O20" si="28">N20+1</f>
+        <v>13</v>
+      </c>
+      <c r="P20" s="70">
+        <f t="shared" ref="P20" si="29">O20+1</f>
+        <v>14</v>
+      </c>
+      <c r="Q20" s="70">
+        <f t="shared" ref="Q20" si="30">P20+1</f>
+        <v>15</v>
+      </c>
+      <c r="R20" s="242" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A21" s="70">
+        <v>0</v>
+      </c>
+      <c r="B21" s="381"/>
+      <c r="C21" s="356"/>
+      <c r="D21" s="312"/>
+      <c r="E21" s="312"/>
+      <c r="F21" s="312"/>
+      <c r="G21" s="312"/>
+      <c r="H21" s="312"/>
+      <c r="I21" s="357"/>
+      <c r="J21" s="357"/>
+      <c r="K21" s="312"/>
+      <c r="L21" s="312"/>
+      <c r="M21" s="312"/>
+      <c r="N21" s="312"/>
+      <c r="O21" s="312"/>
+      <c r="P21" s="356"/>
+      <c r="Q21" s="379"/>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A22" s="70">
+        <f>A21+1</f>
+        <v>1</v>
+      </c>
+      <c r="B22" s="382"/>
+      <c r="C22" s="244"/>
+      <c r="D22" s="244"/>
+      <c r="E22" s="244"/>
+      <c r="F22" s="244"/>
+      <c r="G22" s="244"/>
+      <c r="H22" s="244"/>
+      <c r="I22" s="342"/>
+      <c r="J22" s="342"/>
+      <c r="K22" s="244"/>
+      <c r="L22" s="244"/>
+      <c r="M22" s="244"/>
+      <c r="N22" s="244"/>
+      <c r="O22" s="244"/>
+      <c r="P22" s="244"/>
+      <c r="Q22" s="380"/>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A23" s="70">
+        <f t="shared" ref="A23:A36" si="31">A22+1</f>
+        <v>2</v>
+      </c>
+      <c r="B23" s="314"/>
+      <c r="C23" s="244"/>
+      <c r="D23" s="319"/>
+      <c r="E23" s="319"/>
+      <c r="F23" s="319"/>
+      <c r="G23" s="319"/>
+      <c r="H23" s="319"/>
+      <c r="I23" s="319"/>
+      <c r="J23" s="319"/>
+      <c r="K23" s="319"/>
+      <c r="L23" s="319"/>
+      <c r="M23" s="319"/>
+      <c r="N23" s="319"/>
+      <c r="O23" s="319"/>
+      <c r="P23" s="244"/>
+      <c r="Q23" s="315"/>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A24" s="70">
+        <f t="shared" si="31"/>
+        <v>3</v>
+      </c>
+      <c r="B24" s="314"/>
+      <c r="C24" s="244"/>
+      <c r="D24" s="319"/>
+      <c r="E24" s="319"/>
+      <c r="F24" s="319"/>
+      <c r="G24" s="319"/>
+      <c r="H24" s="319"/>
+      <c r="I24" s="319"/>
+      <c r="J24" s="319"/>
+      <c r="K24" s="319"/>
+      <c r="L24" s="319"/>
+      <c r="M24" s="319"/>
+      <c r="N24" s="319"/>
+      <c r="O24" s="319"/>
+      <c r="P24" s="244"/>
+      <c r="Q24" s="315"/>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A25" s="70">
+        <f t="shared" si="31"/>
+        <v>4</v>
+      </c>
+      <c r="B25" s="314"/>
+      <c r="C25" s="244"/>
+      <c r="D25" s="319"/>
+      <c r="E25" s="319"/>
+      <c r="F25" s="320"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="142"/>
+      <c r="I25" s="142"/>
+      <c r="J25" s="142"/>
+      <c r="K25" s="142"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="320"/>
+      <c r="N25" s="319"/>
+      <c r="O25" s="319"/>
+      <c r="P25" s="244"/>
+      <c r="Q25" s="315"/>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A26" s="70">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="B26" s="314"/>
+      <c r="C26" s="244"/>
+      <c r="D26" s="319"/>
+      <c r="E26" s="319"/>
+      <c r="F26" s="320"/>
+      <c r="G26" s="142"/>
+      <c r="H26" s="142"/>
+      <c r="I26" s="319"/>
+      <c r="J26" s="142"/>
+      <c r="K26" s="142"/>
+      <c r="L26" s="142"/>
+      <c r="M26" s="320"/>
+      <c r="N26" s="319"/>
+      <c r="O26" s="319"/>
+      <c r="P26" s="244"/>
+      <c r="Q26" s="315"/>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A27" s="70">
+        <f t="shared" si="31"/>
+        <v>6</v>
+      </c>
+      <c r="B27" s="314"/>
+      <c r="C27" s="244"/>
+      <c r="D27" s="319"/>
+      <c r="E27" s="319"/>
+      <c r="F27" s="319"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="142"/>
+      <c r="I27" s="142"/>
+      <c r="J27" s="142"/>
+      <c r="K27" s="142"/>
+      <c r="L27" s="142"/>
+      <c r="M27" s="319"/>
+      <c r="N27" s="319"/>
+      <c r="O27" s="319"/>
+      <c r="P27" s="244"/>
+      <c r="Q27" s="315"/>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A28" s="70">
+        <f t="shared" si="31"/>
+        <v>7</v>
+      </c>
+      <c r="B28" s="308"/>
+      <c r="C28" s="219"/>
+      <c r="D28" s="142"/>
+      <c r="E28" s="142"/>
+      <c r="F28" s="142"/>
+      <c r="G28" s="142"/>
+      <c r="H28" s="142"/>
+      <c r="I28" s="142"/>
+      <c r="J28" s="142"/>
+      <c r="K28" s="142"/>
+      <c r="L28" s="142"/>
+      <c r="M28" s="142"/>
+      <c r="N28" s="142"/>
+      <c r="O28" s="142"/>
+      <c r="P28" s="219"/>
+      <c r="Q28" s="309"/>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A29" s="70">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="B29" s="383"/>
+      <c r="C29" s="342"/>
+      <c r="D29" s="319"/>
+      <c r="E29" s="319"/>
+      <c r="F29" s="319"/>
+      <c r="G29" s="142"/>
+      <c r="H29" s="142"/>
+      <c r="I29" s="142"/>
+      <c r="J29" s="142"/>
+      <c r="K29" s="142"/>
+      <c r="L29" s="142"/>
+      <c r="M29" s="319"/>
+      <c r="N29" s="319"/>
+      <c r="O29" s="319"/>
+      <c r="P29" s="342"/>
+      <c r="Q29" s="352"/>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A30" s="70">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="B30" s="314"/>
+      <c r="C30" s="244"/>
+      <c r="D30" s="142"/>
+      <c r="E30" s="142"/>
+      <c r="F30" s="142"/>
+      <c r="G30" s="142"/>
+      <c r="H30" s="142"/>
+      <c r="I30" s="142"/>
+      <c r="J30" s="142"/>
+      <c r="K30" s="142"/>
+      <c r="L30" s="142"/>
+      <c r="M30" s="142"/>
+      <c r="N30" s="142"/>
+      <c r="O30" s="142"/>
+      <c r="P30" s="244"/>
+      <c r="Q30" s="315"/>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A31" s="70">
+        <f t="shared" si="31"/>
+        <v>10</v>
+      </c>
+      <c r="B31" s="314"/>
+      <c r="C31" s="244"/>
+      <c r="D31" s="319"/>
+      <c r="E31" s="319"/>
+      <c r="F31" s="320"/>
+      <c r="G31" s="319"/>
+      <c r="H31" s="319"/>
+      <c r="I31" s="319"/>
+      <c r="J31" s="319"/>
+      <c r="K31" s="319"/>
+      <c r="L31" s="319"/>
+      <c r="M31" s="320"/>
+      <c r="N31" s="319"/>
+      <c r="O31" s="319"/>
+      <c r="P31" s="244"/>
+      <c r="Q31" s="315"/>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A32" s="70">
+        <f t="shared" si="31"/>
+        <v>11</v>
+      </c>
+      <c r="B32" s="314"/>
+      <c r="C32" s="244"/>
+      <c r="D32" s="319"/>
+      <c r="E32" s="319"/>
+      <c r="F32" s="320"/>
+      <c r="G32" s="320"/>
+      <c r="H32" s="319"/>
+      <c r="I32" s="319"/>
+      <c r="J32" s="319"/>
+      <c r="K32" s="319"/>
+      <c r="L32" s="320"/>
+      <c r="M32" s="320"/>
+      <c r="N32" s="319"/>
+      <c r="O32" s="319"/>
+      <c r="P32" s="244"/>
+      <c r="Q32" s="315"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33" s="70">
+        <f t="shared" si="31"/>
+        <v>12</v>
+      </c>
+      <c r="B33" s="314"/>
+      <c r="C33" s="244"/>
+      <c r="D33" s="319"/>
+      <c r="E33" s="319"/>
+      <c r="F33" s="319"/>
+      <c r="G33" s="319"/>
+      <c r="H33" s="319"/>
+      <c r="I33" s="319"/>
+      <c r="J33" s="319"/>
+      <c r="K33" s="319"/>
+      <c r="L33" s="319"/>
+      <c r="M33" s="319"/>
+      <c r="N33" s="319"/>
+      <c r="O33" s="319"/>
+      <c r="P33" s="244"/>
+      <c r="Q33" s="315"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" s="70">
+        <f t="shared" si="31"/>
+        <v>13</v>
+      </c>
+      <c r="B34" s="314"/>
+      <c r="C34" s="244"/>
+      <c r="D34" s="319"/>
+      <c r="E34" s="319"/>
+      <c r="F34" s="319"/>
+      <c r="G34" s="319"/>
+      <c r="H34" s="319"/>
+      <c r="I34" s="319"/>
+      <c r="J34" s="319"/>
+      <c r="K34" s="319"/>
+      <c r="L34" s="319"/>
+      <c r="M34" s="319"/>
+      <c r="N34" s="319"/>
+      <c r="O34" s="319"/>
+      <c r="P34" s="244"/>
+      <c r="Q34" s="315"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" s="70">
+        <f t="shared" si="31"/>
+        <v>14</v>
+      </c>
+      <c r="B35" s="120"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="244"/>
+      <c r="E35" s="244"/>
+      <c r="F35" s="244"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="219"/>
+      <c r="J35" s="219"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="244"/>
+      <c r="N35" s="244"/>
+      <c r="O35" s="244"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="123"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" s="70">
+        <f t="shared" si="31"/>
+        <v>15</v>
+      </c>
+      <c r="B36" s="126"/>
+      <c r="C36" s="124"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="218"/>
+      <c r="J36" s="218"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="124"/>
+      <c r="Q36" s="125"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" s="242" t="s">
+        <v>395</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added one more bunker building style Added potential lava and water below the bunker buildings Changed over to stone for "springs" under the buildings due to potential fires with the new potential of lava... mind you it was pretty having all that wool burn :-)
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="433">
   <si>
     <t>grove</t>
   </si>
@@ -3594,7 +3594,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3614,7 +3614,7 @@
       </c>
       <c r="O6">
         <f t="shared" ref="O6:AB15" ca="1" si="8">IF(AND(MOD(O$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3634,7 +3634,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3654,7 +3654,7 @@
       </c>
       <c r="Y6">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4144,7 +4144,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4184,7 +4184,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4224,7 +4224,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4754,7 +4754,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5284,7 +5284,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5324,7 +5324,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5344,7 +5344,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5364,7 +5364,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5854,7 +5854,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5874,7 +5874,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5894,7 +5894,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5914,7 +5914,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -56629,10 +56629,10 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK56"/>
+  <dimension ref="A1:BV56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="AD48" sqref="AD48"/>
+    <sheetView tabSelected="1" topLeftCell="AL19" workbookViewId="0">
+      <selection activeCell="AP24" sqref="AP24:AY24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57409,7 +57409,7 @@
       <c r="AI16" s="121"/>
       <c r="AJ16" s="123"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A17" s="70">
         <f t="shared" si="15"/>
         <v>15</v>
@@ -57451,7 +57451,7 @@
       <c r="AI17" s="124"/>
       <c r="AJ17" s="125"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A18" s="242" t="s">
         <v>395</v>
       </c>
@@ -57459,7 +57459,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A20" s="242"/>
       <c r="B20" s="70">
         <v>0</v>
@@ -57591,8 +57591,142 @@
         <f t="shared" ref="AJ20" si="44">AI20+1</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL20" s="242"/>
+      <c r="AM20" s="70">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="70">
+        <f>AM20+1</f>
+        <v>1</v>
+      </c>
+      <c r="AO20" s="70">
+        <f t="shared" ref="AO20" si="45">AN20+1</f>
+        <v>2</v>
+      </c>
+      <c r="AP20" s="70">
+        <f t="shared" ref="AP20" si="46">AO20+1</f>
+        <v>3</v>
+      </c>
+      <c r="AQ20" s="70">
+        <f t="shared" ref="AQ20" si="47">AP20+1</f>
+        <v>4</v>
+      </c>
+      <c r="AR20" s="70">
+        <f t="shared" ref="AR20" si="48">AQ20+1</f>
+        <v>5</v>
+      </c>
+      <c r="AS20" s="70">
+        <f t="shared" ref="AS20" si="49">AR20+1</f>
+        <v>6</v>
+      </c>
+      <c r="AT20" s="70">
+        <f t="shared" ref="AT20" si="50">AS20+1</f>
+        <v>7</v>
+      </c>
+      <c r="AU20" s="70">
+        <f t="shared" ref="AU20" si="51">AT20+1</f>
+        <v>8</v>
+      </c>
+      <c r="AV20" s="70">
+        <f t="shared" ref="AV20" si="52">AU20+1</f>
+        <v>9</v>
+      </c>
+      <c r="AW20" s="70">
+        <f t="shared" ref="AW20" si="53">AV20+1</f>
+        <v>10</v>
+      </c>
+      <c r="AX20" s="70">
+        <f t="shared" ref="AX20" si="54">AW20+1</f>
+        <v>11</v>
+      </c>
+      <c r="AY20" s="70">
+        <f t="shared" ref="AY20" si="55">AX20+1</f>
+        <v>12</v>
+      </c>
+      <c r="AZ20" s="70">
+        <f t="shared" ref="AZ20" si="56">AY20+1</f>
+        <v>13</v>
+      </c>
+      <c r="BA20" s="70">
+        <f t="shared" ref="BA20" si="57">AZ20+1</f>
+        <v>14</v>
+      </c>
+      <c r="BB20" s="70">
+        <f t="shared" ref="BB20" si="58">BA20+1</f>
+        <v>15</v>
+      </c>
+      <c r="BC20" s="242" t="s">
+        <v>394</v>
+      </c>
+      <c r="BE20" s="242"/>
+      <c r="BF20" s="70">
+        <v>0</v>
+      </c>
+      <c r="BG20" s="70">
+        <f>BF20+1</f>
+        <v>1</v>
+      </c>
+      <c r="BH20" s="70">
+        <f t="shared" ref="BH20" si="59">BG20+1</f>
+        <v>2</v>
+      </c>
+      <c r="BI20" s="70">
+        <f t="shared" ref="BI20" si="60">BH20+1</f>
+        <v>3</v>
+      </c>
+      <c r="BJ20" s="70">
+        <f t="shared" ref="BJ20" si="61">BI20+1</f>
+        <v>4</v>
+      </c>
+      <c r="BK20" s="70">
+        <f t="shared" ref="BK20" si="62">BJ20+1</f>
+        <v>5</v>
+      </c>
+      <c r="BL20" s="70">
+        <f t="shared" ref="BL20" si="63">BK20+1</f>
+        <v>6</v>
+      </c>
+      <c r="BM20" s="70">
+        <f t="shared" ref="BM20" si="64">BL20+1</f>
+        <v>7</v>
+      </c>
+      <c r="BN20" s="70">
+        <f t="shared" ref="BN20" si="65">BM20+1</f>
+        <v>8</v>
+      </c>
+      <c r="BO20" s="70">
+        <f t="shared" ref="BO20" si="66">BN20+1</f>
+        <v>9</v>
+      </c>
+      <c r="BP20" s="70">
+        <f t="shared" ref="BP20" si="67">BO20+1</f>
+        <v>10</v>
+      </c>
+      <c r="BQ20" s="70">
+        <f t="shared" ref="BQ20" si="68">BP20+1</f>
+        <v>11</v>
+      </c>
+      <c r="BR20" s="70">
+        <f t="shared" ref="BR20" si="69">BQ20+1</f>
+        <v>12</v>
+      </c>
+      <c r="BS20" s="70">
+        <f t="shared" ref="BS20" si="70">BR20+1</f>
+        <v>13</v>
+      </c>
+      <c r="BT20" s="70">
+        <f t="shared" ref="BT20" si="71">BS20+1</f>
+        <v>14</v>
+      </c>
+      <c r="BU20" s="70">
+        <f t="shared" ref="BU20" si="72">BT20+1</f>
+        <v>15</v>
+      </c>
+      <c r="BV20" s="242" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="21" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A21" s="70">
         <v>0</v>
       </c>
@@ -57631,8 +57765,46 @@
       <c r="AH21" s="312"/>
       <c r="AI21" s="356"/>
       <c r="AJ21" s="379"/>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL21" s="70">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="381"/>
+      <c r="AN21" s="356"/>
+      <c r="AO21" s="312"/>
+      <c r="AP21" s="312"/>
+      <c r="AQ21" s="312"/>
+      <c r="AR21" s="312"/>
+      <c r="AS21" s="312"/>
+      <c r="AT21" s="357"/>
+      <c r="AU21" s="357"/>
+      <c r="AV21" s="312"/>
+      <c r="AW21" s="312"/>
+      <c r="AX21" s="312"/>
+      <c r="AY21" s="312"/>
+      <c r="AZ21" s="312"/>
+      <c r="BA21" s="356"/>
+      <c r="BB21" s="379"/>
+      <c r="BE21" s="70">
+        <v>0</v>
+      </c>
+      <c r="BF21" s="381"/>
+      <c r="BG21" s="356"/>
+      <c r="BH21" s="312"/>
+      <c r="BI21" s="312"/>
+      <c r="BJ21" s="312"/>
+      <c r="BK21" s="312"/>
+      <c r="BL21" s="312"/>
+      <c r="BM21" s="357"/>
+      <c r="BN21" s="357"/>
+      <c r="BO21" s="312"/>
+      <c r="BP21" s="312"/>
+      <c r="BQ21" s="312"/>
+      <c r="BR21" s="312"/>
+      <c r="BS21" s="312"/>
+      <c r="BT21" s="356"/>
+      <c r="BU21" s="379"/>
+    </row>
+    <row r="22" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A22" s="70">
         <f>A21+1</f>
         <v>1</v>
@@ -57677,10 +57849,58 @@
       <c r="AH22" s="244"/>
       <c r="AI22" s="244"/>
       <c r="AJ22" s="380"/>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL22" s="70">
+        <f>AL21+1</f>
+        <v>1</v>
+      </c>
+      <c r="AM22" s="382"/>
+      <c r="AN22" s="244"/>
+      <c r="AO22" s="244"/>
+      <c r="AP22" s="244"/>
+      <c r="AQ22" s="244" t="s">
+        <v>362</v>
+      </c>
+      <c r="AR22" s="244"/>
+      <c r="AS22" s="244"/>
+      <c r="AT22" s="342"/>
+      <c r="AU22" s="342"/>
+      <c r="AV22" s="244"/>
+      <c r="AW22" s="244"/>
+      <c r="AX22" s="244"/>
+      <c r="AY22" s="244" t="s">
+        <v>361</v>
+      </c>
+      <c r="AZ22" s="244"/>
+      <c r="BA22" s="244"/>
+      <c r="BB22" s="380"/>
+      <c r="BE22" s="70">
+        <f>BE21+1</f>
+        <v>1</v>
+      </c>
+      <c r="BF22" s="382"/>
+      <c r="BG22" s="244"/>
+      <c r="BH22" s="244"/>
+      <c r="BI22" s="244"/>
+      <c r="BJ22" s="244" t="s">
+        <v>362</v>
+      </c>
+      <c r="BK22" s="244"/>
+      <c r="BL22" s="244"/>
+      <c r="BM22" s="342"/>
+      <c r="BN22" s="342"/>
+      <c r="BO22" s="244"/>
+      <c r="BP22" s="244"/>
+      <c r="BQ22" s="244"/>
+      <c r="BR22" s="244" t="s">
+        <v>361</v>
+      </c>
+      <c r="BS22" s="244"/>
+      <c r="BT22" s="244"/>
+      <c r="BU22" s="380"/>
+    </row>
+    <row r="23" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A23" s="70">
-        <f t="shared" ref="A23:A36" si="45">A22+1</f>
+        <f t="shared" ref="A23:A36" si="73">A22+1</f>
         <v>2</v>
       </c>
       <c r="B23" s="314"/>
@@ -57700,7 +57920,7 @@
       <c r="P23" s="244"/>
       <c r="Q23" s="315"/>
       <c r="T23" s="70">
-        <f t="shared" ref="T23:T36" si="46">T22+1</f>
+        <f t="shared" ref="T23:T36" si="74">T22+1</f>
         <v>2</v>
       </c>
       <c r="U23" s="314"/>
@@ -57719,10 +57939,50 @@
       <c r="AH23" s="319"/>
       <c r="AI23" s="244"/>
       <c r="AJ23" s="315"/>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL23" s="70">
+        <f t="shared" ref="AL23:AL36" si="75">AL22+1</f>
+        <v>2</v>
+      </c>
+      <c r="AM23" s="314"/>
+      <c r="AN23" s="244"/>
+      <c r="AO23" s="319"/>
+      <c r="AP23" s="319"/>
+      <c r="AQ23" s="319"/>
+      <c r="AR23" s="319"/>
+      <c r="AS23" s="319"/>
+      <c r="AT23" s="319"/>
+      <c r="AU23" s="319"/>
+      <c r="AV23" s="319"/>
+      <c r="AW23" s="319"/>
+      <c r="AX23" s="319"/>
+      <c r="AY23" s="319"/>
+      <c r="AZ23" s="319"/>
+      <c r="BA23" s="244"/>
+      <c r="BB23" s="315"/>
+      <c r="BE23" s="70">
+        <f t="shared" ref="BE23:BE36" si="76">BE22+1</f>
+        <v>2</v>
+      </c>
+      <c r="BF23" s="314"/>
+      <c r="BG23" s="244"/>
+      <c r="BH23" s="319"/>
+      <c r="BI23" s="319"/>
+      <c r="BJ23" s="319"/>
+      <c r="BK23" s="319"/>
+      <c r="BL23" s="319"/>
+      <c r="BM23" s="319"/>
+      <c r="BN23" s="319"/>
+      <c r="BO23" s="319"/>
+      <c r="BP23" s="319"/>
+      <c r="BQ23" s="319"/>
+      <c r="BR23" s="319"/>
+      <c r="BS23" s="319"/>
+      <c r="BT23" s="244"/>
+      <c r="BU23" s="315"/>
+    </row>
+    <row r="24" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A24" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>3</v>
       </c>
       <c r="B24" s="314"/>
@@ -57742,7 +58002,7 @@
       <c r="P24" s="244"/>
       <c r="Q24" s="315"/>
       <c r="T24" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>3</v>
       </c>
       <c r="U24" s="314"/>
@@ -57761,10 +58021,50 @@
       <c r="AH24" s="319"/>
       <c r="AI24" s="244"/>
       <c r="AJ24" s="315"/>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL24" s="70">
+        <f t="shared" si="75"/>
+        <v>3</v>
+      </c>
+      <c r="AM24" s="314"/>
+      <c r="AN24" s="244"/>
+      <c r="AO24" s="319"/>
+      <c r="AP24" s="319"/>
+      <c r="AQ24" s="320"/>
+      <c r="AR24" s="319"/>
+      <c r="AS24" s="320"/>
+      <c r="AT24" s="319"/>
+      <c r="AU24" s="320"/>
+      <c r="AV24" s="319"/>
+      <c r="AW24" s="320"/>
+      <c r="AX24" s="319"/>
+      <c r="AY24" s="320"/>
+      <c r="AZ24" s="319"/>
+      <c r="BA24" s="244"/>
+      <c r="BB24" s="315"/>
+      <c r="BE24" s="70">
+        <f t="shared" si="76"/>
+        <v>3</v>
+      </c>
+      <c r="BF24" s="314"/>
+      <c r="BG24" s="244"/>
+      <c r="BH24" s="319"/>
+      <c r="BI24" s="319"/>
+      <c r="BJ24" s="319"/>
+      <c r="BK24" s="319"/>
+      <c r="BL24" s="319"/>
+      <c r="BM24" s="319"/>
+      <c r="BN24" s="319"/>
+      <c r="BO24" s="319"/>
+      <c r="BP24" s="319"/>
+      <c r="BQ24" s="319"/>
+      <c r="BR24" s="319"/>
+      <c r="BS24" s="319"/>
+      <c r="BT24" s="244"/>
+      <c r="BU24" s="315"/>
+    </row>
+    <row r="25" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A25" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>4</v>
       </c>
       <c r="B25" s="314"/>
@@ -57786,7 +58086,7 @@
       <c r="P25" s="244"/>
       <c r="Q25" s="315"/>
       <c r="T25" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>4</v>
       </c>
       <c r="U25" s="314"/>
@@ -57805,10 +58105,54 @@
       <c r="AH25" s="319"/>
       <c r="AI25" s="244"/>
       <c r="AJ25" s="315"/>
-    </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL25" s="70">
+        <f t="shared" si="75"/>
+        <v>4</v>
+      </c>
+      <c r="AM25" s="314"/>
+      <c r="AN25" s="244" t="s">
+        <v>364</v>
+      </c>
+      <c r="AO25" s="319"/>
+      <c r="AP25" s="320"/>
+      <c r="AQ25" s="320"/>
+      <c r="AR25" s="8"/>
+      <c r="AS25" s="8"/>
+      <c r="AT25" s="8"/>
+      <c r="AU25" s="8"/>
+      <c r="AV25" s="8"/>
+      <c r="AW25" s="8"/>
+      <c r="AX25" s="320"/>
+      <c r="AY25" s="319"/>
+      <c r="AZ25" s="319"/>
+      <c r="BA25" s="244"/>
+      <c r="BB25" s="315"/>
+      <c r="BE25" s="70">
+        <f t="shared" si="76"/>
+        <v>4</v>
+      </c>
+      <c r="BF25" s="314"/>
+      <c r="BG25" s="244" t="s">
+        <v>364</v>
+      </c>
+      <c r="BH25" s="319"/>
+      <c r="BI25" s="319"/>
+      <c r="BJ25" s="319"/>
+      <c r="BK25" s="142"/>
+      <c r="BL25" s="142"/>
+      <c r="BM25" s="142"/>
+      <c r="BN25" s="142"/>
+      <c r="BO25" s="142"/>
+      <c r="BP25" s="142"/>
+      <c r="BQ25" s="319"/>
+      <c r="BR25" s="319"/>
+      <c r="BS25" s="319"/>
+      <c r="BT25" s="244"/>
+      <c r="BU25" s="315"/>
+    </row>
+    <row r="26" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A26" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>5</v>
       </c>
       <c r="B26" s="314"/>
@@ -57828,7 +58172,7 @@
       <c r="P26" s="244"/>
       <c r="Q26" s="315"/>
       <c r="T26" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>5</v>
       </c>
       <c r="U26" s="314"/>
@@ -57847,10 +58191,50 @@
       <c r="AH26" s="319"/>
       <c r="AI26" s="244"/>
       <c r="AJ26" s="315"/>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL26" s="70">
+        <f t="shared" si="75"/>
+        <v>5</v>
+      </c>
+      <c r="AM26" s="314"/>
+      <c r="AN26" s="244"/>
+      <c r="AO26" s="319"/>
+      <c r="AP26" s="319"/>
+      <c r="AQ26" s="320"/>
+      <c r="AR26" s="142"/>
+      <c r="AS26" s="142"/>
+      <c r="AT26" s="319"/>
+      <c r="AU26" s="142"/>
+      <c r="AV26" s="142"/>
+      <c r="AW26" s="142"/>
+      <c r="AX26" s="320"/>
+      <c r="AY26" s="320"/>
+      <c r="AZ26" s="319"/>
+      <c r="BA26" s="244"/>
+      <c r="BB26" s="315"/>
+      <c r="BE26" s="70">
+        <f t="shared" si="76"/>
+        <v>5</v>
+      </c>
+      <c r="BF26" s="314"/>
+      <c r="BG26" s="244"/>
+      <c r="BH26" s="319"/>
+      <c r="BI26" s="319"/>
+      <c r="BJ26" s="319"/>
+      <c r="BK26" s="8"/>
+      <c r="BL26" s="8"/>
+      <c r="BM26" s="320"/>
+      <c r="BN26" s="8"/>
+      <c r="BO26" s="8"/>
+      <c r="BP26" s="8"/>
+      <c r="BQ26" s="319"/>
+      <c r="BR26" s="319"/>
+      <c r="BS26" s="319"/>
+      <c r="BT26" s="244"/>
+      <c r="BU26" s="315"/>
+    </row>
+    <row r="27" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A27" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>6</v>
       </c>
       <c r="B27" s="314"/>
@@ -57870,7 +58254,7 @@
       <c r="P27" s="244"/>
       <c r="Q27" s="315"/>
       <c r="T27" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>6</v>
       </c>
       <c r="U27" s="314"/>
@@ -57889,10 +58273,50 @@
       <c r="AH27" s="319"/>
       <c r="AI27" s="244"/>
       <c r="AJ27" s="315"/>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL27" s="70">
+        <f t="shared" si="75"/>
+        <v>6</v>
+      </c>
+      <c r="AM27" s="314"/>
+      <c r="AN27" s="244"/>
+      <c r="AO27" s="319"/>
+      <c r="AP27" s="320"/>
+      <c r="AQ27" s="320"/>
+      <c r="AR27" s="142"/>
+      <c r="AS27" s="142"/>
+      <c r="AT27" s="142"/>
+      <c r="AU27" s="142"/>
+      <c r="AV27" s="142"/>
+      <c r="AW27" s="142"/>
+      <c r="AX27" s="320"/>
+      <c r="AY27" s="319"/>
+      <c r="AZ27" s="319"/>
+      <c r="BA27" s="244"/>
+      <c r="BB27" s="315"/>
+      <c r="BE27" s="70">
+        <f t="shared" si="76"/>
+        <v>6</v>
+      </c>
+      <c r="BF27" s="314"/>
+      <c r="BG27" s="244"/>
+      <c r="BH27" s="319"/>
+      <c r="BI27" s="319"/>
+      <c r="BJ27" s="319"/>
+      <c r="BK27" s="8"/>
+      <c r="BL27" s="142"/>
+      <c r="BM27" s="142"/>
+      <c r="BN27" s="142"/>
+      <c r="BO27" s="142"/>
+      <c r="BP27" s="8"/>
+      <c r="BQ27" s="319"/>
+      <c r="BR27" s="319"/>
+      <c r="BS27" s="319"/>
+      <c r="BT27" s="244"/>
+      <c r="BU27" s="315"/>
+    </row>
+    <row r="28" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A28" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>7</v>
       </c>
       <c r="B28" s="308"/>
@@ -57912,7 +58336,7 @@
       <c r="P28" s="219"/>
       <c r="Q28" s="309"/>
       <c r="T28" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>7</v>
       </c>
       <c r="U28" s="308"/>
@@ -57931,10 +58355,50 @@
       <c r="AH28" s="142"/>
       <c r="AI28" s="219"/>
       <c r="AJ28" s="309"/>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL28" s="70">
+        <f t="shared" si="75"/>
+        <v>7</v>
+      </c>
+      <c r="AM28" s="308"/>
+      <c r="AN28" s="219"/>
+      <c r="AO28" s="142"/>
+      <c r="AP28" s="142"/>
+      <c r="AQ28" s="8"/>
+      <c r="AR28" s="142"/>
+      <c r="AS28" s="142"/>
+      <c r="AT28" s="142"/>
+      <c r="AU28" s="142"/>
+      <c r="AV28" s="142"/>
+      <c r="AW28" s="142"/>
+      <c r="AX28" s="8"/>
+      <c r="AY28" s="8"/>
+      <c r="AZ28" s="142"/>
+      <c r="BA28" s="219"/>
+      <c r="BB28" s="309"/>
+      <c r="BE28" s="70">
+        <f t="shared" si="76"/>
+        <v>7</v>
+      </c>
+      <c r="BF28" s="308"/>
+      <c r="BG28" s="219"/>
+      <c r="BH28" s="142"/>
+      <c r="BI28" s="142"/>
+      <c r="BJ28" s="142"/>
+      <c r="BK28" s="8"/>
+      <c r="BL28" s="142"/>
+      <c r="BM28" s="142"/>
+      <c r="BN28" s="142"/>
+      <c r="BO28" s="142"/>
+      <c r="BP28" s="8"/>
+      <c r="BQ28" s="142"/>
+      <c r="BR28" s="142"/>
+      <c r="BS28" s="142"/>
+      <c r="BT28" s="219"/>
+      <c r="BU28" s="309"/>
+    </row>
+    <row r="29" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A29" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>8</v>
       </c>
       <c r="B29" s="383"/>
@@ -57954,7 +58418,7 @@
       <c r="P29" s="342"/>
       <c r="Q29" s="352"/>
       <c r="T29" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>8</v>
       </c>
       <c r="U29" s="383"/>
@@ -57973,10 +58437,50 @@
       <c r="AH29" s="319"/>
       <c r="AI29" s="342"/>
       <c r="AJ29" s="352"/>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL29" s="70">
+        <f t="shared" si="75"/>
+        <v>8</v>
+      </c>
+      <c r="AM29" s="383"/>
+      <c r="AN29" s="342"/>
+      <c r="AO29" s="319"/>
+      <c r="AP29" s="320"/>
+      <c r="AQ29" s="320"/>
+      <c r="AR29" s="142"/>
+      <c r="AS29" s="142"/>
+      <c r="AT29" s="142"/>
+      <c r="AU29" s="142"/>
+      <c r="AV29" s="142"/>
+      <c r="AW29" s="142"/>
+      <c r="AX29" s="320"/>
+      <c r="AY29" s="319"/>
+      <c r="AZ29" s="319"/>
+      <c r="BA29" s="342"/>
+      <c r="BB29" s="352"/>
+      <c r="BE29" s="70">
+        <f t="shared" si="76"/>
+        <v>8</v>
+      </c>
+      <c r="BF29" s="383"/>
+      <c r="BG29" s="342"/>
+      <c r="BH29" s="319"/>
+      <c r="BI29" s="319"/>
+      <c r="BJ29" s="319"/>
+      <c r="BK29" s="8"/>
+      <c r="BL29" s="142"/>
+      <c r="BM29" s="142"/>
+      <c r="BN29" s="142"/>
+      <c r="BO29" s="142"/>
+      <c r="BP29" s="8"/>
+      <c r="BQ29" s="319"/>
+      <c r="BR29" s="319"/>
+      <c r="BS29" s="319"/>
+      <c r="BT29" s="342"/>
+      <c r="BU29" s="352"/>
+    </row>
+    <row r="30" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A30" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>9</v>
       </c>
       <c r="B30" s="314"/>
@@ -57996,7 +58500,7 @@
       <c r="P30" s="244"/>
       <c r="Q30" s="315"/>
       <c r="T30" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>9</v>
       </c>
       <c r="U30" s="314"/>
@@ -58015,10 +58519,50 @@
       <c r="AH30" s="142"/>
       <c r="AI30" s="244"/>
       <c r="AJ30" s="315"/>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL30" s="70">
+        <f t="shared" si="75"/>
+        <v>9</v>
+      </c>
+      <c r="AM30" s="314"/>
+      <c r="AN30" s="244"/>
+      <c r="AO30" s="142"/>
+      <c r="AP30" s="142"/>
+      <c r="AQ30" s="8"/>
+      <c r="AR30" s="142"/>
+      <c r="AS30" s="142"/>
+      <c r="AT30" s="142"/>
+      <c r="AU30" s="142"/>
+      <c r="AV30" s="142"/>
+      <c r="AW30" s="142"/>
+      <c r="AX30" s="8"/>
+      <c r="AY30" s="8"/>
+      <c r="AZ30" s="142"/>
+      <c r="BA30" s="244"/>
+      <c r="BB30" s="315"/>
+      <c r="BE30" s="70">
+        <f t="shared" si="76"/>
+        <v>9</v>
+      </c>
+      <c r="BF30" s="314"/>
+      <c r="BG30" s="244"/>
+      <c r="BH30" s="142"/>
+      <c r="BI30" s="142"/>
+      <c r="BJ30" s="142"/>
+      <c r="BK30" s="8"/>
+      <c r="BL30" s="142"/>
+      <c r="BM30" s="142"/>
+      <c r="BN30" s="142"/>
+      <c r="BO30" s="142"/>
+      <c r="BP30" s="8"/>
+      <c r="BQ30" s="142"/>
+      <c r="BR30" s="142"/>
+      <c r="BS30" s="142"/>
+      <c r="BT30" s="244"/>
+      <c r="BU30" s="315"/>
+    </row>
+    <row r="31" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A31" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>10</v>
       </c>
       <c r="B31" s="314"/>
@@ -58038,7 +58582,7 @@
       <c r="P31" s="244"/>
       <c r="Q31" s="315"/>
       <c r="T31" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>10</v>
       </c>
       <c r="U31" s="314"/>
@@ -58057,10 +58601,50 @@
       <c r="AH31" s="319"/>
       <c r="AI31" s="244"/>
       <c r="AJ31" s="315"/>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL31" s="70">
+        <f t="shared" si="75"/>
+        <v>10</v>
+      </c>
+      <c r="AM31" s="314"/>
+      <c r="AN31" s="244"/>
+      <c r="AO31" s="319"/>
+      <c r="AP31" s="320"/>
+      <c r="AQ31" s="320"/>
+      <c r="AR31" s="319"/>
+      <c r="AS31" s="319"/>
+      <c r="AT31" s="319"/>
+      <c r="AU31" s="319"/>
+      <c r="AV31" s="319"/>
+      <c r="AW31" s="319"/>
+      <c r="AX31" s="320"/>
+      <c r="AY31" s="319"/>
+      <c r="AZ31" s="319"/>
+      <c r="BA31" s="244"/>
+      <c r="BB31" s="315"/>
+      <c r="BE31" s="70">
+        <f t="shared" si="76"/>
+        <v>10</v>
+      </c>
+      <c r="BF31" s="314"/>
+      <c r="BG31" s="244"/>
+      <c r="BH31" s="319"/>
+      <c r="BI31" s="319"/>
+      <c r="BJ31" s="319"/>
+      <c r="BK31" s="320"/>
+      <c r="BL31" s="320"/>
+      <c r="BM31" s="320"/>
+      <c r="BN31" s="320"/>
+      <c r="BO31" s="320"/>
+      <c r="BP31" s="320"/>
+      <c r="BQ31" s="319"/>
+      <c r="BR31" s="319"/>
+      <c r="BS31" s="319"/>
+      <c r="BT31" s="244"/>
+      <c r="BU31" s="315"/>
+    </row>
+    <row r="32" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A32" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>11</v>
       </c>
       <c r="B32" s="314"/>
@@ -58080,7 +58664,7 @@
       <c r="P32" s="244"/>
       <c r="Q32" s="315"/>
       <c r="T32" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>11</v>
       </c>
       <c r="U32" s="314"/>
@@ -58099,10 +58683,50 @@
       <c r="AH32" s="319"/>
       <c r="AI32" s="244"/>
       <c r="AJ32" s="315"/>
-    </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AL32" s="70">
+        <f t="shared" si="75"/>
+        <v>11</v>
+      </c>
+      <c r="AM32" s="314"/>
+      <c r="AN32" s="244"/>
+      <c r="AO32" s="319"/>
+      <c r="AP32" s="319"/>
+      <c r="AQ32" s="320"/>
+      <c r="AR32" s="320"/>
+      <c r="AS32" s="320"/>
+      <c r="AT32" s="320"/>
+      <c r="AU32" s="320"/>
+      <c r="AV32" s="320"/>
+      <c r="AW32" s="320"/>
+      <c r="AX32" s="320"/>
+      <c r="AY32" s="320"/>
+      <c r="AZ32" s="319"/>
+      <c r="BA32" s="244"/>
+      <c r="BB32" s="315"/>
+      <c r="BE32" s="70">
+        <f t="shared" si="76"/>
+        <v>11</v>
+      </c>
+      <c r="BF32" s="314"/>
+      <c r="BG32" s="244"/>
+      <c r="BH32" s="319"/>
+      <c r="BI32" s="319"/>
+      <c r="BJ32" s="319"/>
+      <c r="BK32" s="319"/>
+      <c r="BL32" s="319"/>
+      <c r="BM32" s="319"/>
+      <c r="BN32" s="319"/>
+      <c r="BO32" s="319"/>
+      <c r="BP32" s="319"/>
+      <c r="BQ32" s="319"/>
+      <c r="BR32" s="319"/>
+      <c r="BS32" s="319"/>
+      <c r="BT32" s="244"/>
+      <c r="BU32" s="315"/>
+    </row>
+    <row r="33" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A33" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>12</v>
       </c>
       <c r="B33" s="314"/>
@@ -58124,7 +58748,7 @@
       <c r="P33" s="244"/>
       <c r="Q33" s="315"/>
       <c r="T33" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>12</v>
       </c>
       <c r="U33" s="314"/>
@@ -58143,10 +58767,54 @@
       <c r="AH33" s="319"/>
       <c r="AI33" s="244"/>
       <c r="AJ33" s="315"/>
-    </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AL33" s="70">
+        <f t="shared" si="75"/>
+        <v>12</v>
+      </c>
+      <c r="AM33" s="314"/>
+      <c r="AN33" s="244" t="s">
+        <v>363</v>
+      </c>
+      <c r="AO33" s="319"/>
+      <c r="AP33" s="320"/>
+      <c r="AQ33" s="319"/>
+      <c r="AR33" s="320"/>
+      <c r="AS33" s="319"/>
+      <c r="AT33" s="320"/>
+      <c r="AU33" s="319"/>
+      <c r="AV33" s="320"/>
+      <c r="AW33" s="319"/>
+      <c r="AX33" s="320"/>
+      <c r="AY33" s="319"/>
+      <c r="AZ33" s="319"/>
+      <c r="BA33" s="244"/>
+      <c r="BB33" s="315"/>
+      <c r="BE33" s="70">
+        <f t="shared" si="76"/>
+        <v>12</v>
+      </c>
+      <c r="BF33" s="314"/>
+      <c r="BG33" s="244" t="s">
+        <v>363</v>
+      </c>
+      <c r="BH33" s="319"/>
+      <c r="BI33" s="319"/>
+      <c r="BJ33" s="319"/>
+      <c r="BK33" s="319"/>
+      <c r="BL33" s="319"/>
+      <c r="BM33" s="319"/>
+      <c r="BN33" s="319"/>
+      <c r="BO33" s="319"/>
+      <c r="BP33" s="319"/>
+      <c r="BQ33" s="319"/>
+      <c r="BR33" s="319"/>
+      <c r="BS33" s="319"/>
+      <c r="BT33" s="244"/>
+      <c r="BU33" s="315"/>
+    </row>
+    <row r="34" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A34" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>13</v>
       </c>
       <c r="B34" s="314"/>
@@ -58166,7 +58834,7 @@
       <c r="P34" s="244"/>
       <c r="Q34" s="315"/>
       <c r="T34" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>13</v>
       </c>
       <c r="U34" s="314"/>
@@ -58185,10 +58853,50 @@
       <c r="AH34" s="319"/>
       <c r="AI34" s="244"/>
       <c r="AJ34" s="315"/>
-    </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AL34" s="70">
+        <f t="shared" si="75"/>
+        <v>13</v>
+      </c>
+      <c r="AM34" s="314"/>
+      <c r="AN34" s="244"/>
+      <c r="AO34" s="319"/>
+      <c r="AP34" s="319"/>
+      <c r="AQ34" s="319"/>
+      <c r="AR34" s="319"/>
+      <c r="AS34" s="319"/>
+      <c r="AT34" s="319"/>
+      <c r="AU34" s="319"/>
+      <c r="AV34" s="319"/>
+      <c r="AW34" s="319"/>
+      <c r="AX34" s="319"/>
+      <c r="AY34" s="319"/>
+      <c r="AZ34" s="319"/>
+      <c r="BA34" s="244"/>
+      <c r="BB34" s="315"/>
+      <c r="BE34" s="70">
+        <f t="shared" si="76"/>
+        <v>13</v>
+      </c>
+      <c r="BF34" s="314"/>
+      <c r="BG34" s="244"/>
+      <c r="BH34" s="319"/>
+      <c r="BI34" s="319"/>
+      <c r="BJ34" s="319"/>
+      <c r="BK34" s="319"/>
+      <c r="BL34" s="319"/>
+      <c r="BM34" s="319"/>
+      <c r="BN34" s="319"/>
+      <c r="BO34" s="319"/>
+      <c r="BP34" s="319"/>
+      <c r="BQ34" s="319"/>
+      <c r="BR34" s="319"/>
+      <c r="BS34" s="319"/>
+      <c r="BT34" s="244"/>
+      <c r="BU34" s="315"/>
+    </row>
+    <row r="35" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A35" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>14</v>
       </c>
       <c r="B35" s="120"/>
@@ -58208,7 +58916,7 @@
       <c r="P35" s="17"/>
       <c r="Q35" s="123"/>
       <c r="T35" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>14</v>
       </c>
       <c r="U35" s="120"/>
@@ -58227,10 +58935,50 @@
       <c r="AH35" s="244"/>
       <c r="AI35" s="17"/>
       <c r="AJ35" s="123"/>
-    </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AL35" s="70">
+        <f t="shared" si="75"/>
+        <v>14</v>
+      </c>
+      <c r="AM35" s="120"/>
+      <c r="AN35" s="17"/>
+      <c r="AO35" s="244"/>
+      <c r="AP35" s="244"/>
+      <c r="AQ35" s="244"/>
+      <c r="AR35" s="17"/>
+      <c r="AS35" s="17"/>
+      <c r="AT35" s="219"/>
+      <c r="AU35" s="219"/>
+      <c r="AV35" s="17"/>
+      <c r="AW35" s="17"/>
+      <c r="AX35" s="244"/>
+      <c r="AY35" s="244"/>
+      <c r="AZ35" s="244"/>
+      <c r="BA35" s="17"/>
+      <c r="BB35" s="123"/>
+      <c r="BE35" s="70">
+        <f t="shared" si="76"/>
+        <v>14</v>
+      </c>
+      <c r="BF35" s="120"/>
+      <c r="BG35" s="17"/>
+      <c r="BH35" s="244"/>
+      <c r="BI35" s="244"/>
+      <c r="BJ35" s="244"/>
+      <c r="BK35" s="17"/>
+      <c r="BL35" s="17"/>
+      <c r="BM35" s="219"/>
+      <c r="BN35" s="219"/>
+      <c r="BO35" s="17"/>
+      <c r="BP35" s="17"/>
+      <c r="BQ35" s="244"/>
+      <c r="BR35" s="244"/>
+      <c r="BS35" s="244"/>
+      <c r="BT35" s="17"/>
+      <c r="BU35" s="123"/>
+    </row>
+    <row r="36" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A36" s="70">
-        <f t="shared" si="45"/>
+        <f t="shared" si="73"/>
         <v>15</v>
       </c>
       <c r="B36" s="126"/>
@@ -58250,7 +58998,7 @@
       <c r="P36" s="124"/>
       <c r="Q36" s="125"/>
       <c r="T36" s="70">
-        <f t="shared" si="46"/>
+        <f t="shared" si="74"/>
         <v>15</v>
       </c>
       <c r="U36" s="126"/>
@@ -58269,13 +59017,59 @@
       <c r="AH36" s="22"/>
       <c r="AI36" s="124"/>
       <c r="AJ36" s="125"/>
-    </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AL36" s="70">
+        <f t="shared" si="75"/>
+        <v>15</v>
+      </c>
+      <c r="AM36" s="126"/>
+      <c r="AN36" s="124"/>
+      <c r="AO36" s="22"/>
+      <c r="AP36" s="22"/>
+      <c r="AQ36" s="22"/>
+      <c r="AR36" s="22"/>
+      <c r="AS36" s="22"/>
+      <c r="AT36" s="218"/>
+      <c r="AU36" s="218"/>
+      <c r="AV36" s="22"/>
+      <c r="AW36" s="22"/>
+      <c r="AX36" s="22"/>
+      <c r="AY36" s="22"/>
+      <c r="AZ36" s="22"/>
+      <c r="BA36" s="124"/>
+      <c r="BB36" s="125"/>
+      <c r="BE36" s="70">
+        <f t="shared" si="76"/>
+        <v>15</v>
+      </c>
+      <c r="BF36" s="126"/>
+      <c r="BG36" s="124"/>
+      <c r="BH36" s="22"/>
+      <c r="BI36" s="22"/>
+      <c r="BJ36" s="22"/>
+      <c r="BK36" s="22"/>
+      <c r="BL36" s="22"/>
+      <c r="BM36" s="218"/>
+      <c r="BN36" s="218"/>
+      <c r="BO36" s="22"/>
+      <c r="BP36" s="22"/>
+      <c r="BQ36" s="22"/>
+      <c r="BR36" s="22"/>
+      <c r="BS36" s="22"/>
+      <c r="BT36" s="124"/>
+      <c r="BU36" s="125"/>
+    </row>
+    <row r="37" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A37" s="242" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AL37" s="242" t="s">
+        <v>395</v>
+      </c>
+      <c r="BE37" s="242" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="39" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A39" s="242"/>
       <c r="B39" s="70">
         <v>0</v>
@@ -58285,59 +59079,59 @@
         <v>1</v>
       </c>
       <c r="D39" s="70">
-        <f t="shared" ref="D39" si="47">C39+1</f>
+        <f t="shared" ref="D39" si="77">C39+1</f>
         <v>2</v>
       </c>
       <c r="E39" s="70">
-        <f t="shared" ref="E39" si="48">D39+1</f>
+        <f t="shared" ref="E39" si="78">D39+1</f>
         <v>3</v>
       </c>
       <c r="F39" s="70">
-        <f t="shared" ref="F39" si="49">E39+1</f>
+        <f t="shared" ref="F39" si="79">E39+1</f>
         <v>4</v>
       </c>
       <c r="G39" s="70">
-        <f t="shared" ref="G39" si="50">F39+1</f>
+        <f t="shared" ref="G39" si="80">F39+1</f>
         <v>5</v>
       </c>
       <c r="H39" s="70">
-        <f t="shared" ref="H39" si="51">G39+1</f>
+        <f t="shared" ref="H39" si="81">G39+1</f>
         <v>6</v>
       </c>
       <c r="I39" s="70">
-        <f t="shared" ref="I39" si="52">H39+1</f>
+        <f t="shared" ref="I39" si="82">H39+1</f>
         <v>7</v>
       </c>
       <c r="J39" s="70">
-        <f t="shared" ref="J39" si="53">I39+1</f>
+        <f t="shared" ref="J39" si="83">I39+1</f>
         <v>8</v>
       </c>
       <c r="K39" s="70">
-        <f t="shared" ref="K39" si="54">J39+1</f>
+        <f t="shared" ref="K39" si="84">J39+1</f>
         <v>9</v>
       </c>
       <c r="L39" s="70">
-        <f t="shared" ref="L39" si="55">K39+1</f>
+        <f t="shared" ref="L39" si="85">K39+1</f>
         <v>10</v>
       </c>
       <c r="M39" s="70">
-        <f t="shared" ref="M39" si="56">L39+1</f>
+        <f t="shared" ref="M39" si="86">L39+1</f>
         <v>11</v>
       </c>
       <c r="N39" s="70">
-        <f t="shared" ref="N39" si="57">M39+1</f>
+        <f t="shared" ref="N39" si="87">M39+1</f>
         <v>12</v>
       </c>
       <c r="O39" s="70">
-        <f t="shared" ref="O39" si="58">N39+1</f>
+        <f t="shared" ref="O39" si="88">N39+1</f>
         <v>13</v>
       </c>
       <c r="P39" s="70">
-        <f t="shared" ref="P39" si="59">O39+1</f>
+        <f t="shared" ref="P39" si="89">O39+1</f>
         <v>14</v>
       </c>
       <c r="Q39" s="70">
-        <f t="shared" ref="Q39" si="60">P39+1</f>
+        <f t="shared" ref="Q39" si="90">P39+1</f>
         <v>15</v>
       </c>
       <c r="R39" s="242" t="s">
@@ -58352,66 +59146,66 @@
         <v>1</v>
       </c>
       <c r="W39" s="70">
-        <f t="shared" ref="W39" si="61">V39+1</f>
+        <f t="shared" ref="W39" si="91">V39+1</f>
         <v>2</v>
       </c>
       <c r="X39" s="70">
-        <f t="shared" ref="X39" si="62">W39+1</f>
+        <f t="shared" ref="X39" si="92">W39+1</f>
         <v>3</v>
       </c>
       <c r="Y39" s="70">
-        <f t="shared" ref="Y39" si="63">X39+1</f>
+        <f t="shared" ref="Y39" si="93">X39+1</f>
         <v>4</v>
       </c>
       <c r="Z39" s="70">
-        <f t="shared" ref="Z39" si="64">Y39+1</f>
+        <f t="shared" ref="Z39" si="94">Y39+1</f>
         <v>5</v>
       </c>
       <c r="AA39" s="70">
-        <f t="shared" ref="AA39" si="65">Z39+1</f>
+        <f t="shared" ref="AA39" si="95">Z39+1</f>
         <v>6</v>
       </c>
       <c r="AB39" s="70">
-        <f t="shared" ref="AB39" si="66">AA39+1</f>
+        <f t="shared" ref="AB39" si="96">AA39+1</f>
         <v>7</v>
       </c>
       <c r="AC39" s="70">
-        <f t="shared" ref="AC39" si="67">AB39+1</f>
+        <f t="shared" ref="AC39" si="97">AB39+1</f>
         <v>8</v>
       </c>
       <c r="AD39" s="70">
-        <f t="shared" ref="AD39" si="68">AC39+1</f>
+        <f t="shared" ref="AD39" si="98">AC39+1</f>
         <v>9</v>
       </c>
       <c r="AE39" s="70">
-        <f t="shared" ref="AE39" si="69">AD39+1</f>
+        <f t="shared" ref="AE39" si="99">AD39+1</f>
         <v>10</v>
       </c>
       <c r="AF39" s="70">
-        <f t="shared" ref="AF39" si="70">AE39+1</f>
+        <f t="shared" ref="AF39" si="100">AE39+1</f>
         <v>11</v>
       </c>
       <c r="AG39" s="70">
-        <f t="shared" ref="AG39" si="71">AF39+1</f>
+        <f t="shared" ref="AG39" si="101">AF39+1</f>
         <v>12</v>
       </c>
       <c r="AH39" s="70">
-        <f t="shared" ref="AH39" si="72">AG39+1</f>
+        <f t="shared" ref="AH39" si="102">AG39+1</f>
         <v>13</v>
       </c>
       <c r="AI39" s="70">
-        <f t="shared" ref="AI39" si="73">AH39+1</f>
+        <f t="shared" ref="AI39" si="103">AH39+1</f>
         <v>14</v>
       </c>
       <c r="AJ39" s="70">
-        <f t="shared" ref="AJ39" si="74">AI39+1</f>
+        <f t="shared" ref="AJ39" si="104">AI39+1</f>
         <v>15</v>
       </c>
       <c r="AK39" s="242" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A40" s="70">
         <v>0</v>
       </c>
@@ -58451,7 +59245,7 @@
       <c r="AI40" s="356"/>
       <c r="AJ40" s="379"/>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A41" s="70">
         <f>A40+1</f>
         <v>1</v>
@@ -58493,9 +59287,9 @@
       <c r="AI41" s="244"/>
       <c r="AJ41" s="380"/>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A42" s="70">
-        <f t="shared" ref="A42:A55" si="75">A41+1</f>
+        <f t="shared" ref="A42:A55" si="105">A41+1</f>
         <v>2</v>
       </c>
       <c r="B42" s="314"/>
@@ -58515,7 +59309,7 @@
       <c r="P42" s="244"/>
       <c r="Q42" s="315"/>
       <c r="T42" s="70">
-        <f t="shared" ref="T42:T55" si="76">T41+1</f>
+        <f t="shared" ref="T42:T55" si="106">T41+1</f>
         <v>2</v>
       </c>
       <c r="U42" s="314"/>
@@ -58535,9 +59329,9 @@
       <c r="AI42" s="244"/>
       <c r="AJ42" s="315"/>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A43" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>3</v>
       </c>
       <c r="B43" s="314"/>
@@ -58557,7 +59351,7 @@
       <c r="P43" s="244"/>
       <c r="Q43" s="315"/>
       <c r="T43" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>3</v>
       </c>
       <c r="U43" s="314"/>
@@ -58577,9 +59371,9 @@
       <c r="AI43" s="244"/>
       <c r="AJ43" s="315"/>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A44" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>4</v>
       </c>
       <c r="B44" s="314"/>
@@ -58599,7 +59393,7 @@
       <c r="P44" s="244"/>
       <c r="Q44" s="315"/>
       <c r="T44" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>4</v>
       </c>
       <c r="U44" s="314"/>
@@ -58619,9 +59413,9 @@
       <c r="AI44" s="244"/>
       <c r="AJ44" s="315"/>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A45" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>5</v>
       </c>
       <c r="B45" s="314"/>
@@ -58641,7 +59435,7 @@
       <c r="P45" s="244"/>
       <c r="Q45" s="315"/>
       <c r="T45" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>5</v>
       </c>
       <c r="U45" s="314"/>
@@ -58661,9 +59455,9 @@
       <c r="AI45" s="244"/>
       <c r="AJ45" s="315"/>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A46" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>6</v>
       </c>
       <c r="B46" s="314"/>
@@ -58683,7 +59477,7 @@
       <c r="P46" s="244"/>
       <c r="Q46" s="315"/>
       <c r="T46" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>6</v>
       </c>
       <c r="U46" s="314"/>
@@ -58703,9 +59497,9 @@
       <c r="AI46" s="244"/>
       <c r="AJ46" s="315"/>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A47" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>7</v>
       </c>
       <c r="B47" s="308"/>
@@ -58725,7 +59519,7 @@
       <c r="P47" s="219"/>
       <c r="Q47" s="309"/>
       <c r="T47" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>7</v>
       </c>
       <c r="U47" s="308"/>
@@ -58745,9 +59539,9 @@
       <c r="AI47" s="219"/>
       <c r="AJ47" s="309"/>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A48" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>8</v>
       </c>
       <c r="B48" s="383"/>
@@ -58767,7 +59561,7 @@
       <c r="P48" s="342"/>
       <c r="Q48" s="352"/>
       <c r="T48" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>8</v>
       </c>
       <c r="U48" s="383"/>
@@ -58789,7 +59583,7 @@
     </row>
     <row r="49" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A49" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>9</v>
       </c>
       <c r="B49" s="314"/>
@@ -58809,7 +59603,7 @@
       <c r="P49" s="244"/>
       <c r="Q49" s="315"/>
       <c r="T49" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>9</v>
       </c>
       <c r="U49" s="314"/>
@@ -58831,7 +59625,7 @@
     </row>
     <row r="50" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A50" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>10</v>
       </c>
       <c r="B50" s="314"/>
@@ -58851,7 +59645,7 @@
       <c r="P50" s="244"/>
       <c r="Q50" s="315"/>
       <c r="T50" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>10</v>
       </c>
       <c r="U50" s="314"/>
@@ -58873,7 +59667,7 @@
     </row>
     <row r="51" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A51" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>11</v>
       </c>
       <c r="B51" s="314"/>
@@ -58893,7 +59687,7 @@
       <c r="P51" s="244"/>
       <c r="Q51" s="315"/>
       <c r="T51" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>11</v>
       </c>
       <c r="U51" s="314"/>
@@ -58915,7 +59709,7 @@
     </row>
     <row r="52" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A52" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>12</v>
       </c>
       <c r="B52" s="314"/>
@@ -58935,7 +59729,7 @@
       <c r="P52" s="244"/>
       <c r="Q52" s="315"/>
       <c r="T52" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>12</v>
       </c>
       <c r="U52" s="314"/>
@@ -58957,7 +59751,7 @@
     </row>
     <row r="53" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A53" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>13</v>
       </c>
       <c r="B53" s="314"/>
@@ -58977,7 +59771,7 @@
       <c r="P53" s="244"/>
       <c r="Q53" s="315"/>
       <c r="T53" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>13</v>
       </c>
       <c r="U53" s="314"/>
@@ -58999,7 +59793,7 @@
     </row>
     <row r="54" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A54" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>14</v>
       </c>
       <c r="B54" s="120"/>
@@ -59019,7 +59813,7 @@
       <c r="P54" s="17"/>
       <c r="Q54" s="123"/>
       <c r="T54" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>14</v>
       </c>
       <c r="U54" s="120"/>
@@ -59041,7 +59835,7 @@
     </row>
     <row r="55" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A55" s="70">
-        <f t="shared" si="75"/>
+        <f t="shared" si="105"/>
         <v>15</v>
       </c>
       <c r="B55" s="126"/>
@@ -59061,7 +59855,7 @@
       <c r="P55" s="124"/>
       <c r="Q55" s="125"/>
       <c r="T55" s="70">
-        <f t="shared" si="76"/>
+        <f t="shared" si="106"/>
         <v>15</v>
       </c>
       <c r="U55" s="126"/>

</xml_diff>

<commit_message>
Bunkers now have tricks and treats, still need more interiors Sewers have been debugged Added in the beginnings of PhatLoot Nearing release time, incremented the version to 1.00
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="20" activeTab="40"/>
+    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="29" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <sheet name="Mineshafts, thoughts" sheetId="46" state="hidden" r:id="rId38"/>
     <sheet name="Mineshafts" sheetId="47" r:id="rId39"/>
     <sheet name="Bunkers" sheetId="48" r:id="rId40"/>
-    <sheet name="Sheet2" sheetId="49" r:id="rId41"/>
+    <sheet name="Sewers2" sheetId="49" r:id="rId41"/>
   </sheets>
   <definedNames>
     <definedName name="AbsoluteMaximumFloorsBelow">Sheet3!$C$6</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="441">
   <si>
     <t>grove</t>
   </si>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3695,7 +3695,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="Y6">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4205,7 +4205,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4225,7 +4225,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4265,7 +4265,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4795,7 +4795,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4835,7 +4835,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4855,7 +4855,7 @@
       </c>
       <c r="Y16">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5345,7 +5345,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5365,7 +5365,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5405,7 +5405,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5425,7 +5425,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5935,7 +5935,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5975,7 +5975,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5995,7 +5995,7 @@
       </c>
       <c r="Y26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -53194,8 +53194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CL37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:R18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="AO28" sqref="AO28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53534,10 +53534,10 @@
       <c r="F2" s="312"/>
       <c r="G2" s="312"/>
       <c r="H2" s="312"/>
-      <c r="I2" s="348"/>
-      <c r="J2" s="355"/>
-      <c r="K2" s="355"/>
-      <c r="L2" s="348"/>
+      <c r="I2" s="312"/>
+      <c r="J2" s="312"/>
+      <c r="K2" s="312"/>
+      <c r="L2" s="312"/>
       <c r="M2" s="312"/>
       <c r="N2" s="312"/>
       <c r="O2" s="312"/>
@@ -53637,10 +53637,10 @@
       <c r="F3" s="244"/>
       <c r="G3" s="244"/>
       <c r="H3" s="244"/>
-      <c r="I3" s="327"/>
-      <c r="J3" s="346"/>
-      <c r="K3" s="346"/>
-      <c r="L3" s="327"/>
+      <c r="I3" s="244"/>
+      <c r="J3" s="244"/>
+      <c r="K3" s="244"/>
+      <c r="L3" s="244"/>
       <c r="M3" s="244"/>
       <c r="N3" s="244"/>
       <c r="O3" s="244"/>
@@ -53743,10 +53743,10 @@
       <c r="F4" s="244"/>
       <c r="G4" s="244"/>
       <c r="H4" s="244"/>
-      <c r="I4" s="327"/>
-      <c r="J4" s="342"/>
-      <c r="K4" s="342"/>
-      <c r="L4" s="327"/>
+      <c r="I4" s="244"/>
+      <c r="J4" s="244"/>
+      <c r="K4" s="244"/>
+      <c r="L4" s="244"/>
       <c r="M4" s="244"/>
       <c r="N4" s="244"/>
       <c r="O4" s="244"/>
@@ -53849,10 +53849,10 @@
       <c r="F5" s="244"/>
       <c r="G5" s="244"/>
       <c r="H5" s="244"/>
-      <c r="I5" s="327"/>
-      <c r="J5" s="346"/>
-      <c r="K5" s="346"/>
-      <c r="L5" s="327"/>
+      <c r="I5" s="244"/>
+      <c r="J5" s="244"/>
+      <c r="K5" s="244"/>
+      <c r="L5" s="244"/>
       <c r="M5" s="244"/>
       <c r="N5" s="244"/>
       <c r="O5" s="244"/>
@@ -53955,10 +53955,10 @@
       <c r="F6" s="244"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="353"/>
-      <c r="K6" s="353"/>
-      <c r="L6" s="128"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
       <c r="M6" s="244"/>
       <c r="N6" s="244"/>
       <c r="O6" s="244"/>
@@ -54054,12 +54054,12 @@
       <c r="D7" s="244"/>
       <c r="E7" s="244"/>
       <c r="F7" s="244"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="128"/>
-      <c r="I7" s="327"/>
-      <c r="J7" s="219"/>
-      <c r="K7" s="219"/>
-      <c r="L7" s="128"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="244"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
       <c r="M7" s="244"/>
       <c r="N7" s="244"/>
       <c r="O7" s="244"/>
@@ -54158,12 +54158,12 @@
       <c r="D8" s="244"/>
       <c r="E8" s="244"/>
       <c r="F8" s="244"/>
-      <c r="G8" s="128"/>
-      <c r="H8" s="201"/>
-      <c r="I8" s="353"/>
-      <c r="J8" s="353"/>
-      <c r="K8" s="353"/>
-      <c r="L8" s="128"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
       <c r="M8" s="244"/>
       <c r="N8" s="244"/>
       <c r="O8" s="244"/>
@@ -54179,10 +54179,10 @@
       <c r="W8" s="128"/>
       <c r="X8" s="128"/>
       <c r="Y8" s="128"/>
-      <c r="Z8" s="353"/>
+      <c r="Z8" s="128"/>
       <c r="AA8" s="353"/>
       <c r="AB8" s="353"/>
-      <c r="AC8" s="353"/>
+      <c r="AC8" s="128"/>
       <c r="AD8" s="128"/>
       <c r="AE8" s="128"/>
       <c r="AF8" s="128"/>
@@ -54259,22 +54259,22 @@
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="B9" s="127"/>
-      <c r="C9" s="128"/>
-      <c r="D9" s="128"/>
-      <c r="E9" s="128"/>
-      <c r="F9" s="128"/>
-      <c r="G9" s="128"/>
-      <c r="H9" s="353"/>
-      <c r="I9" s="353"/>
-      <c r="J9" s="353"/>
-      <c r="K9" s="353"/>
-      <c r="L9" s="353"/>
-      <c r="M9" s="128"/>
-      <c r="N9" s="128"/>
-      <c r="O9" s="128"/>
-      <c r="P9" s="128"/>
-      <c r="Q9" s="130"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="26"/>
       <c r="S9" s="70">
         <f t="shared" si="8"/>
         <v>7</v>
@@ -54365,22 +54365,22 @@
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="B10" s="345"/>
-      <c r="C10" s="346"/>
-      <c r="D10" s="342"/>
-      <c r="E10" s="346"/>
-      <c r="F10" s="346"/>
-      <c r="G10" s="219"/>
-      <c r="H10" s="353"/>
-      <c r="I10" s="353"/>
-      <c r="J10" s="353"/>
-      <c r="K10" s="353"/>
-      <c r="L10" s="353"/>
-      <c r="M10" s="346"/>
-      <c r="N10" s="342"/>
-      <c r="O10" s="346"/>
-      <c r="P10" s="346"/>
-      <c r="Q10" s="352"/>
+      <c r="B10" s="314"/>
+      <c r="C10" s="244"/>
+      <c r="D10" s="244"/>
+      <c r="E10" s="244"/>
+      <c r="F10" s="244"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="244"/>
+      <c r="N10" s="244"/>
+      <c r="O10" s="244"/>
+      <c r="P10" s="244"/>
+      <c r="Q10" s="315"/>
       <c r="S10" s="70">
         <f t="shared" si="8"/>
         <v>8</v>
@@ -54471,22 +54471,22 @@
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="B11" s="345"/>
-      <c r="C11" s="346"/>
-      <c r="D11" s="219"/>
-      <c r="E11" s="353"/>
-      <c r="F11" s="353"/>
-      <c r="G11" s="219"/>
-      <c r="H11" s="353"/>
-      <c r="I11" s="353"/>
-      <c r="J11" s="353"/>
-      <c r="K11" s="353"/>
-      <c r="L11" s="353"/>
-      <c r="M11" s="353"/>
-      <c r="N11" s="219"/>
-      <c r="O11" s="353"/>
-      <c r="P11" s="346"/>
-      <c r="Q11" s="352"/>
+      <c r="B11" s="314"/>
+      <c r="C11" s="244"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="244"/>
+      <c r="Q11" s="315"/>
       <c r="S11" s="70">
         <f t="shared" si="8"/>
         <v>9</v>
@@ -54497,10 +54497,10 @@
       <c r="W11" s="327"/>
       <c r="X11" s="327"/>
       <c r="Y11" s="327"/>
-      <c r="Z11" s="346"/>
+      <c r="Z11" s="327"/>
       <c r="AA11" s="346"/>
       <c r="AB11" s="346"/>
-      <c r="AC11" s="346"/>
+      <c r="AC11" s="327"/>
       <c r="AD11" s="327"/>
       <c r="AE11" s="327"/>
       <c r="AF11" s="327"/>
@@ -54577,22 +54577,22 @@
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="B12" s="343"/>
-      <c r="C12" s="327"/>
-      <c r="D12" s="327"/>
-      <c r="E12" s="327"/>
-      <c r="F12" s="327"/>
-      <c r="G12" s="327"/>
-      <c r="H12" s="327"/>
-      <c r="I12" s="346"/>
-      <c r="J12" s="346"/>
-      <c r="K12" s="346"/>
-      <c r="L12" s="346"/>
-      <c r="M12" s="327"/>
-      <c r="N12" s="327"/>
-      <c r="O12" s="327"/>
-      <c r="P12" s="327"/>
-      <c r="Q12" s="344"/>
+      <c r="B12" s="314"/>
+      <c r="C12" s="244"/>
+      <c r="D12" s="244"/>
+      <c r="E12" s="244"/>
+      <c r="F12" s="244"/>
+      <c r="G12" s="244"/>
+      <c r="H12" s="244"/>
+      <c r="I12" s="244"/>
+      <c r="J12" s="244"/>
+      <c r="K12" s="244"/>
+      <c r="L12" s="244"/>
+      <c r="M12" s="244"/>
+      <c r="N12" s="244"/>
+      <c r="O12" s="244"/>
+      <c r="P12" s="244"/>
+      <c r="Q12" s="315"/>
       <c r="S12" s="70">
         <f t="shared" si="8"/>
         <v>10</v>
@@ -54685,10 +54685,10 @@
       <c r="F13" s="244"/>
       <c r="G13" s="244"/>
       <c r="H13" s="244"/>
-      <c r="I13" s="327"/>
-      <c r="J13" s="346"/>
-      <c r="K13" s="346"/>
-      <c r="L13" s="327"/>
+      <c r="I13" s="244"/>
+      <c r="J13" s="244"/>
+      <c r="K13" s="244"/>
+      <c r="L13" s="244"/>
       <c r="M13" s="244"/>
       <c r="N13" s="244"/>
       <c r="O13" s="244"/>
@@ -54780,10 +54780,10 @@
       <c r="F14" s="244"/>
       <c r="G14" s="244"/>
       <c r="H14" s="244"/>
-      <c r="I14" s="327"/>
-      <c r="J14" s="342"/>
-      <c r="K14" s="342"/>
-      <c r="L14" s="327"/>
+      <c r="I14" s="244"/>
+      <c r="J14" s="244"/>
+      <c r="K14" s="244"/>
+      <c r="L14" s="244"/>
       <c r="M14" s="244"/>
       <c r="N14" s="244"/>
       <c r="O14" s="244"/>
@@ -54883,10 +54883,10 @@
       <c r="F15" s="244"/>
       <c r="G15" s="244"/>
       <c r="H15" s="244"/>
-      <c r="I15" s="327"/>
-      <c r="J15" s="346"/>
-      <c r="K15" s="346"/>
-      <c r="L15" s="327"/>
+      <c r="I15" s="244"/>
+      <c r="J15" s="244"/>
+      <c r="K15" s="244"/>
+      <c r="L15" s="244"/>
       <c r="M15" s="244"/>
       <c r="N15" s="244"/>
       <c r="O15" s="244"/>
@@ -54986,10 +54986,10 @@
       <c r="F16" s="244"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
-      <c r="I16" s="128"/>
-      <c r="J16" s="353"/>
-      <c r="K16" s="353"/>
-      <c r="L16" s="128"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
       <c r="M16" s="244"/>
       <c r="N16" s="244"/>
       <c r="O16" s="244"/>
@@ -55089,10 +55089,10 @@
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
-      <c r="I17" s="129"/>
-      <c r="J17" s="218"/>
-      <c r="K17" s="218"/>
-      <c r="L17" s="129"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
       <c r="M17" s="22"/>
       <c r="N17" s="22"/>
       <c r="O17" s="22"/>
@@ -55530,11 +55530,11 @@
       <c r="E21" s="312"/>
       <c r="F21" s="312"/>
       <c r="G21" s="312"/>
-      <c r="H21" s="348"/>
-      <c r="I21" s="355"/>
-      <c r="J21" s="355"/>
-      <c r="K21" s="348"/>
-      <c r="L21" s="2"/>
+      <c r="H21" s="312"/>
+      <c r="I21" s="312"/>
+      <c r="J21" s="312"/>
+      <c r="K21" s="312"/>
+      <c r="L21" s="20"/>
       <c r="M21" s="312"/>
       <c r="N21" s="312"/>
       <c r="O21" s="312"/>
@@ -55631,10 +55631,10 @@
       <c r="E22" s="244"/>
       <c r="F22" s="244"/>
       <c r="G22" s="244"/>
-      <c r="H22" s="327"/>
-      <c r="I22" s="342"/>
-      <c r="J22" s="342"/>
-      <c r="K22" s="327"/>
+      <c r="H22" s="244"/>
+      <c r="I22" s="244"/>
+      <c r="J22" s="244"/>
+      <c r="K22" s="244"/>
       <c r="L22" s="244"/>
       <c r="M22" s="244"/>
       <c r="N22" s="244"/>
@@ -55734,16 +55734,16 @@
       <c r="E23" s="244"/>
       <c r="F23" s="244"/>
       <c r="G23" s="244"/>
-      <c r="H23" s="327"/>
-      <c r="I23" s="346"/>
-      <c r="J23" s="346"/>
-      <c r="K23" s="327"/>
+      <c r="H23" s="244"/>
+      <c r="I23" s="244"/>
+      <c r="J23" s="244"/>
+      <c r="K23" s="244"/>
       <c r="L23" s="244"/>
       <c r="M23" s="244"/>
       <c r="N23" s="244"/>
       <c r="O23" s="244"/>
       <c r="P23" s="244"/>
-      <c r="Q23" s="9"/>
+      <c r="Q23" s="26"/>
       <c r="S23" s="70">
         <f t="shared" ref="S23:S36" si="16">S22+1</f>
         <v>2</v>
@@ -55837,16 +55837,16 @@
       <c r="E24" s="244"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
-      <c r="H24" s="128"/>
-      <c r="I24" s="353"/>
-      <c r="J24" s="353"/>
-      <c r="K24" s="128"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
       <c r="L24" s="244"/>
       <c r="M24" s="244"/>
       <c r="N24" s="244"/>
       <c r="O24" s="244"/>
       <c r="P24" s="244"/>
-      <c r="Q24" s="9"/>
+      <c r="Q24" s="26"/>
       <c r="S24" s="70">
         <f t="shared" si="16"/>
         <v>3</v>
@@ -55936,18 +55936,18 @@
       <c r="C25" s="244"/>
       <c r="D25" s="244"/>
       <c r="E25" s="244"/>
-      <c r="F25" s="128"/>
-      <c r="G25" s="128"/>
-      <c r="H25" s="327"/>
-      <c r="I25" s="219"/>
-      <c r="J25" s="219"/>
-      <c r="K25" s="128"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="244"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
       <c r="L25" s="244"/>
       <c r="M25" s="244"/>
       <c r="N25" s="244"/>
       <c r="O25" s="244"/>
       <c r="P25" s="244"/>
-      <c r="Q25" s="9"/>
+      <c r="Q25" s="26"/>
       <c r="S25" s="70">
         <f t="shared" si="16"/>
         <v>4</v>
@@ -56037,18 +56037,18 @@
       <c r="C26" s="244"/>
       <c r="D26" s="244"/>
       <c r="E26" s="244"/>
-      <c r="F26" s="128"/>
-      <c r="G26" s="201"/>
-      <c r="H26" s="353"/>
-      <c r="I26" s="353"/>
-      <c r="J26" s="353"/>
-      <c r="K26" s="128"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
       <c r="L26" s="244"/>
       <c r="M26" s="244"/>
       <c r="N26" s="244"/>
       <c r="O26" s="244"/>
       <c r="P26" s="244"/>
-      <c r="Q26" s="9"/>
+      <c r="Q26" s="26"/>
       <c r="S26" s="70">
         <f t="shared" si="16"/>
         <v>5</v>
@@ -56139,22 +56139,22 @@
         <f t="shared" si="15"/>
         <v>6</v>
       </c>
-      <c r="B27" s="127"/>
-      <c r="C27" s="128"/>
-      <c r="D27" s="128"/>
-      <c r="E27" s="128"/>
-      <c r="F27" s="128"/>
-      <c r="G27" s="353"/>
-      <c r="H27" s="353"/>
-      <c r="I27" s="353"/>
-      <c r="J27" s="353"/>
-      <c r="K27" s="353"/>
-      <c r="L27" s="128"/>
-      <c r="M27" s="128"/>
-      <c r="N27" s="128"/>
-      <c r="O27" s="128"/>
-      <c r="P27" s="128"/>
-      <c r="Q27" s="130"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="26"/>
       <c r="S27" s="70">
         <f t="shared" si="16"/>
         <v>6</v>
@@ -56165,10 +56165,10 @@
       <c r="W27" s="128"/>
       <c r="X27" s="128"/>
       <c r="Y27" s="128"/>
-      <c r="Z27" s="353"/>
+      <c r="Z27" s="128"/>
       <c r="AA27" s="353"/>
       <c r="AB27" s="353"/>
-      <c r="AC27" s="353"/>
+      <c r="AC27" s="128"/>
       <c r="AD27" s="128"/>
       <c r="AE27" s="128"/>
       <c r="AF27" s="128"/>
@@ -56245,22 +56245,22 @@
         <f t="shared" si="15"/>
         <v>7</v>
       </c>
-      <c r="B28" s="345"/>
-      <c r="C28" s="342"/>
-      <c r="D28" s="346"/>
-      <c r="E28" s="346"/>
-      <c r="F28" s="219"/>
-      <c r="G28" s="353"/>
-      <c r="H28" s="353"/>
-      <c r="I28" s="353"/>
-      <c r="J28" s="353"/>
-      <c r="K28" s="353"/>
-      <c r="L28" s="346"/>
-      <c r="M28" s="342"/>
-      <c r="N28" s="346"/>
-      <c r="O28" s="346"/>
-      <c r="P28" s="342"/>
-      <c r="Q28" s="347"/>
+      <c r="B28" s="314"/>
+      <c r="C28" s="244"/>
+      <c r="D28" s="244"/>
+      <c r="E28" s="244"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="244"/>
+      <c r="M28" s="244"/>
+      <c r="N28" s="244"/>
+      <c r="O28" s="244"/>
+      <c r="P28" s="244"/>
+      <c r="Q28" s="315"/>
       <c r="S28" s="70">
         <f t="shared" si="16"/>
         <v>7</v>
@@ -56351,22 +56351,22 @@
         <f t="shared" si="15"/>
         <v>8</v>
       </c>
-      <c r="B29" s="345"/>
-      <c r="C29" s="219"/>
-      <c r="D29" s="353"/>
-      <c r="E29" s="353"/>
-      <c r="F29" s="219"/>
-      <c r="G29" s="353"/>
-      <c r="H29" s="353"/>
-      <c r="I29" s="353"/>
-      <c r="J29" s="353"/>
-      <c r="K29" s="353"/>
-      <c r="L29" s="353"/>
-      <c r="M29" s="219"/>
-      <c r="N29" s="353"/>
-      <c r="O29" s="346"/>
-      <c r="P29" s="342"/>
-      <c r="Q29" s="347"/>
+      <c r="B29" s="314"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="244"/>
+      <c r="P29" s="244"/>
+      <c r="Q29" s="315"/>
       <c r="S29" s="70">
         <f t="shared" si="16"/>
         <v>8</v>
@@ -56457,22 +56457,22 @@
         <f t="shared" si="15"/>
         <v>9</v>
       </c>
-      <c r="B30" s="343"/>
-      <c r="C30" s="327"/>
-      <c r="D30" s="327"/>
-      <c r="E30" s="327"/>
-      <c r="F30" s="327"/>
-      <c r="G30" s="327"/>
-      <c r="H30" s="346"/>
-      <c r="I30" s="346"/>
-      <c r="J30" s="346"/>
-      <c r="K30" s="346"/>
-      <c r="L30" s="327"/>
-      <c r="M30" s="327"/>
-      <c r="N30" s="327"/>
-      <c r="O30" s="327"/>
-      <c r="P30" s="327"/>
-      <c r="Q30" s="344"/>
+      <c r="B30" s="314"/>
+      <c r="C30" s="244"/>
+      <c r="D30" s="244"/>
+      <c r="E30" s="244"/>
+      <c r="F30" s="244"/>
+      <c r="G30" s="244"/>
+      <c r="H30" s="244"/>
+      <c r="I30" s="244"/>
+      <c r="J30" s="244"/>
+      <c r="K30" s="244"/>
+      <c r="L30" s="244"/>
+      <c r="M30" s="244"/>
+      <c r="N30" s="244"/>
+      <c r="O30" s="244"/>
+      <c r="P30" s="244"/>
+      <c r="Q30" s="315"/>
       <c r="S30" s="70">
         <f t="shared" si="16"/>
         <v>9</v>
@@ -56483,10 +56483,10 @@
       <c r="W30" s="327"/>
       <c r="X30" s="327"/>
       <c r="Y30" s="327"/>
-      <c r="Z30" s="346"/>
+      <c r="Z30" s="327"/>
       <c r="AA30" s="346"/>
       <c r="AB30" s="346"/>
-      <c r="AC30" s="346"/>
+      <c r="AC30" s="327"/>
       <c r="AD30" s="327"/>
       <c r="AE30" s="327"/>
       <c r="AF30" s="327"/>
@@ -56561,22 +56561,22 @@
         <f t="shared" si="15"/>
         <v>10</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="244"/>
       <c r="D31" s="244"/>
       <c r="E31" s="244"/>
       <c r="F31" s="244"/>
       <c r="G31" s="244"/>
-      <c r="H31" s="327"/>
-      <c r="I31" s="346"/>
-      <c r="J31" s="346"/>
-      <c r="K31" s="327"/>
+      <c r="H31" s="244"/>
+      <c r="I31" s="244"/>
+      <c r="J31" s="244"/>
+      <c r="K31" s="244"/>
       <c r="L31" s="244"/>
       <c r="M31" s="244"/>
       <c r="N31" s="244"/>
       <c r="O31" s="244"/>
       <c r="P31" s="244"/>
-      <c r="Q31" s="9"/>
+      <c r="Q31" s="26"/>
       <c r="S31" s="70">
         <f t="shared" si="16"/>
         <v>10</v>
@@ -56671,16 +56671,16 @@
       <c r="E32" s="244"/>
       <c r="F32" s="244"/>
       <c r="G32" s="244"/>
-      <c r="H32" s="327"/>
-      <c r="I32" s="342"/>
-      <c r="J32" s="342"/>
-      <c r="K32" s="327"/>
+      <c r="H32" s="244"/>
+      <c r="I32" s="244"/>
+      <c r="J32" s="244"/>
+      <c r="K32" s="244"/>
       <c r="L32" s="244"/>
       <c r="M32" s="244"/>
       <c r="N32" s="244"/>
       <c r="O32" s="244"/>
       <c r="P32" s="244"/>
-      <c r="Q32" s="9"/>
+      <c r="Q32" s="26"/>
       <c r="S32" s="70">
         <f t="shared" si="16"/>
         <v>11</v>
@@ -56777,16 +56777,16 @@
       <c r="E33" s="244"/>
       <c r="F33" s="244"/>
       <c r="G33" s="244"/>
-      <c r="H33" s="327"/>
-      <c r="I33" s="346"/>
-      <c r="J33" s="346"/>
-      <c r="K33" s="327"/>
+      <c r="H33" s="244"/>
+      <c r="I33" s="244"/>
+      <c r="J33" s="244"/>
+      <c r="K33" s="244"/>
       <c r="L33" s="244"/>
       <c r="M33" s="244"/>
       <c r="N33" s="244"/>
       <c r="O33" s="244"/>
       <c r="P33" s="244"/>
-      <c r="Q33" s="9"/>
+      <c r="Q33" s="26"/>
       <c r="S33" s="70">
         <f t="shared" si="16"/>
         <v>12</v>
@@ -56881,16 +56881,16 @@
       <c r="E34" s="244"/>
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
-      <c r="H34" s="128"/>
-      <c r="I34" s="353"/>
-      <c r="J34" s="353"/>
-      <c r="K34" s="128"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
       <c r="L34" s="244"/>
       <c r="M34" s="244"/>
       <c r="N34" s="244"/>
       <c r="O34" s="17"/>
       <c r="P34" s="17"/>
-      <c r="Q34" s="9"/>
+      <c r="Q34" s="26"/>
       <c r="S34" s="70">
         <f t="shared" si="16"/>
         <v>13</v>
@@ -56947,16 +56947,16 @@
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
-      <c r="H35" s="128"/>
-      <c r="I35" s="219"/>
-      <c r="J35" s="219"/>
-      <c r="K35" s="128"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
       <c r="L35" s="17"/>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
       <c r="O35" s="17"/>
       <c r="P35" s="17"/>
-      <c r="Q35" s="9"/>
+      <c r="Q35" s="26"/>
       <c r="S35" s="70">
         <f t="shared" si="16"/>
         <v>14</v>
@@ -57009,20 +57009,20 @@
       </c>
       <c r="B36" s="32"/>
       <c r="C36" s="22"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="350"/>
-      <c r="I36" s="354"/>
-      <c r="J36" s="354"/>
-      <c r="K36" s="350"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="15"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="317"/>
+      <c r="I36" s="317"/>
+      <c r="J36" s="317"/>
+      <c r="K36" s="317"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="33"/>
       <c r="S36" s="70">
         <f t="shared" si="16"/>
         <v>15</v>
@@ -57301,8 +57301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BV56"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:R37"/>
+    <sheetView tabSelected="1" topLeftCell="AB19" workbookViewId="0">
+      <selection activeCell="AR26" sqref="AR26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -59874,6 +59874,73 @@
       <c r="AK39" s="242" t="s">
         <v>394</v>
       </c>
+      <c r="AL39" s="242"/>
+      <c r="AM39" s="70">
+        <v>0</v>
+      </c>
+      <c r="AN39" s="70">
+        <f t="shared" ref="AN39" si="14">AM39+1</f>
+        <v>1</v>
+      </c>
+      <c r="AO39" s="70">
+        <f t="shared" ref="AO39" si="15">AN39+1</f>
+        <v>2</v>
+      </c>
+      <c r="AP39" s="70">
+        <f t="shared" ref="AP39" si="16">AO39+1</f>
+        <v>3</v>
+      </c>
+      <c r="AQ39" s="70">
+        <f t="shared" ref="AQ39" si="17">AP39+1</f>
+        <v>4</v>
+      </c>
+      <c r="AR39" s="70">
+        <f t="shared" ref="AR39" si="18">AQ39+1</f>
+        <v>5</v>
+      </c>
+      <c r="AS39" s="70">
+        <f t="shared" ref="AS39" si="19">AR39+1</f>
+        <v>6</v>
+      </c>
+      <c r="AT39" s="70">
+        <f t="shared" ref="AT39" si="20">AS39+1</f>
+        <v>7</v>
+      </c>
+      <c r="AU39" s="70">
+        <f t="shared" ref="AU39" si="21">AT39+1</f>
+        <v>8</v>
+      </c>
+      <c r="AV39" s="70">
+        <f t="shared" ref="AV39" si="22">AU39+1</f>
+        <v>9</v>
+      </c>
+      <c r="AW39" s="70">
+        <f t="shared" ref="AW39" si="23">AV39+1</f>
+        <v>10</v>
+      </c>
+      <c r="AX39" s="70">
+        <f t="shared" ref="AX39" si="24">AW39+1</f>
+        <v>11</v>
+      </c>
+      <c r="AY39" s="70">
+        <f t="shared" ref="AY39" si="25">AX39+1</f>
+        <v>12</v>
+      </c>
+      <c r="AZ39" s="70">
+        <f t="shared" ref="AZ39" si="26">AY39+1</f>
+        <v>13</v>
+      </c>
+      <c r="BA39" s="70">
+        <f t="shared" ref="BA39" si="27">AZ39+1</f>
+        <v>14</v>
+      </c>
+      <c r="BB39" s="70">
+        <f t="shared" ref="BB39" si="28">BA39+1</f>
+        <v>15</v>
+      </c>
+      <c r="BC39" s="242" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="40" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A40" s="70">
@@ -59914,6 +59981,25 @@
       <c r="AH40" s="312"/>
       <c r="AI40" s="356"/>
       <c r="AJ40" s="379"/>
+      <c r="AL40" s="70">
+        <v>0</v>
+      </c>
+      <c r="AM40" s="381"/>
+      <c r="AN40" s="356"/>
+      <c r="AO40" s="312"/>
+      <c r="AP40" s="312"/>
+      <c r="AQ40" s="312"/>
+      <c r="AR40" s="312"/>
+      <c r="AS40" s="312"/>
+      <c r="AT40" s="357"/>
+      <c r="AU40" s="357"/>
+      <c r="AV40" s="312"/>
+      <c r="AW40" s="312"/>
+      <c r="AX40" s="312"/>
+      <c r="AY40" s="312"/>
+      <c r="AZ40" s="312"/>
+      <c r="BA40" s="356"/>
+      <c r="BB40" s="379"/>
     </row>
     <row r="41" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A41" s="70">
@@ -59956,10 +60042,30 @@
       <c r="AH41" s="244"/>
       <c r="AI41" s="244"/>
       <c r="AJ41" s="380"/>
+      <c r="AL41" s="70">
+        <f>AL40+1</f>
+        <v>1</v>
+      </c>
+      <c r="AM41" s="382"/>
+      <c r="AN41" s="244"/>
+      <c r="AO41" s="244"/>
+      <c r="AP41" s="244"/>
+      <c r="AQ41" s="244"/>
+      <c r="AR41" s="244"/>
+      <c r="AS41" s="320"/>
+      <c r="AT41" s="319"/>
+      <c r="AU41" s="319"/>
+      <c r="AV41" s="320"/>
+      <c r="AW41" s="244"/>
+      <c r="AX41" s="244"/>
+      <c r="AY41" s="244"/>
+      <c r="AZ41" s="244"/>
+      <c r="BA41" s="244"/>
+      <c r="BB41" s="380"/>
     </row>
     <row r="42" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A42" s="70">
-        <f t="shared" ref="A42:A55" si="14">A41+1</f>
+        <f t="shared" ref="A42:A55" si="29">A41+1</f>
         <v>2</v>
       </c>
       <c r="B42" s="314"/>
@@ -59979,7 +60085,7 @@
       <c r="P42" s="244"/>
       <c r="Q42" s="315"/>
       <c r="T42" s="70">
-        <f t="shared" ref="T42:T55" si="15">T41+1</f>
+        <f t="shared" ref="T42:T55" si="30">T41+1</f>
         <v>2</v>
       </c>
       <c r="U42" s="314"/>
@@ -59998,10 +60104,30 @@
       <c r="AH42" s="319"/>
       <c r="AI42" s="244"/>
       <c r="AJ42" s="315"/>
+      <c r="AL42" s="70">
+        <f t="shared" ref="AL42:AL55" si="31">AL41+1</f>
+        <v>2</v>
+      </c>
+      <c r="AM42" s="314"/>
+      <c r="AN42" s="244"/>
+      <c r="AO42" s="244"/>
+      <c r="AP42" s="320"/>
+      <c r="AQ42" s="320"/>
+      <c r="AR42" s="320"/>
+      <c r="AS42" s="342"/>
+      <c r="AT42" s="342"/>
+      <c r="AU42" s="342"/>
+      <c r="AV42" s="342"/>
+      <c r="AW42" s="320"/>
+      <c r="AX42" s="342"/>
+      <c r="AY42" s="342"/>
+      <c r="AZ42" s="342"/>
+      <c r="BA42" s="244"/>
+      <c r="BB42" s="315"/>
     </row>
     <row r="43" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A43" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>3</v>
       </c>
       <c r="B43" s="314"/>
@@ -60021,7 +60147,7 @@
       <c r="P43" s="244"/>
       <c r="Q43" s="315"/>
       <c r="T43" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
       <c r="U43" s="314"/>
@@ -60040,10 +60166,30 @@
       <c r="AH43" s="342"/>
       <c r="AI43" s="244"/>
       <c r="AJ43" s="315"/>
+      <c r="AL43" s="70">
+        <f t="shared" si="31"/>
+        <v>3</v>
+      </c>
+      <c r="AM43" s="314"/>
+      <c r="AN43" s="244"/>
+      <c r="AO43" s="320"/>
+      <c r="AP43" s="342"/>
+      <c r="AQ43" s="342"/>
+      <c r="AR43" s="346"/>
+      <c r="AS43" s="342"/>
+      <c r="AT43" s="342"/>
+      <c r="AU43" s="342"/>
+      <c r="AV43" s="342"/>
+      <c r="AW43" s="320"/>
+      <c r="AX43" s="342"/>
+      <c r="AY43" s="342"/>
+      <c r="AZ43" s="342"/>
+      <c r="BA43" s="244"/>
+      <c r="BB43" s="315"/>
     </row>
     <row r="44" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A44" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>4</v>
       </c>
       <c r="B44" s="314"/>
@@ -60063,7 +60209,7 @@
       <c r="P44" s="244"/>
       <c r="Q44" s="315"/>
       <c r="T44" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>4</v>
       </c>
       <c r="U44" s="314"/>
@@ -60082,10 +60228,30 @@
       <c r="AH44" s="342"/>
       <c r="AI44" s="244"/>
       <c r="AJ44" s="315"/>
+      <c r="AL44" s="70">
+        <f t="shared" si="31"/>
+        <v>4</v>
+      </c>
+      <c r="AM44" s="314"/>
+      <c r="AN44" s="244"/>
+      <c r="AO44" s="320"/>
+      <c r="AP44" s="342"/>
+      <c r="AQ44" s="342"/>
+      <c r="AR44" s="353"/>
+      <c r="AS44" s="219"/>
+      <c r="AT44" s="219"/>
+      <c r="AU44" s="219"/>
+      <c r="AV44" s="219"/>
+      <c r="AW44" s="8"/>
+      <c r="AX44" s="342"/>
+      <c r="AY44" s="342"/>
+      <c r="AZ44" s="342"/>
+      <c r="BA44" s="244"/>
+      <c r="BB44" s="315"/>
     </row>
     <row r="45" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A45" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>5</v>
       </c>
       <c r="B45" s="314"/>
@@ -60105,7 +60271,7 @@
       <c r="P45" s="244"/>
       <c r="Q45" s="315"/>
       <c r="T45" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>5</v>
       </c>
       <c r="U45" s="314"/>
@@ -60124,10 +60290,30 @@
       <c r="AH45" s="342"/>
       <c r="AI45" s="244"/>
       <c r="AJ45" s="315"/>
+      <c r="AL45" s="70">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="AM45" s="314"/>
+      <c r="AN45" s="244"/>
+      <c r="AO45" s="320"/>
+      <c r="AP45" s="346"/>
+      <c r="AQ45" s="346"/>
+      <c r="AR45" s="142"/>
+      <c r="AS45" s="142"/>
+      <c r="AT45" s="319"/>
+      <c r="AU45" s="142"/>
+      <c r="AV45" s="142"/>
+      <c r="AW45" s="142"/>
+      <c r="AX45" s="342"/>
+      <c r="AY45" s="342"/>
+      <c r="AZ45" s="342"/>
+      <c r="BA45" s="244"/>
+      <c r="BB45" s="315"/>
     </row>
     <row r="46" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A46" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="B46" s="314"/>
@@ -60147,7 +60333,7 @@
       <c r="P46" s="244"/>
       <c r="Q46" s="315"/>
       <c r="T46" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>6</v>
       </c>
       <c r="U46" s="314"/>
@@ -60166,10 +60352,30 @@
       <c r="AH46" s="319"/>
       <c r="AI46" s="244"/>
       <c r="AJ46" s="315"/>
+      <c r="AL46" s="70">
+        <f t="shared" si="31"/>
+        <v>6</v>
+      </c>
+      <c r="AM46" s="314"/>
+      <c r="AN46" s="320"/>
+      <c r="AO46" s="342"/>
+      <c r="AP46" s="342"/>
+      <c r="AQ46" s="342"/>
+      <c r="AR46" s="142"/>
+      <c r="AS46" s="7"/>
+      <c r="AT46" s="187"/>
+      <c r="AU46" s="390"/>
+      <c r="AV46" s="7"/>
+      <c r="AW46" s="142"/>
+      <c r="AX46" s="342"/>
+      <c r="AY46" s="342"/>
+      <c r="AZ46" s="342"/>
+      <c r="BA46" s="244"/>
+      <c r="BB46" s="315"/>
     </row>
     <row r="47" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A47" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>7</v>
       </c>
       <c r="B47" s="308"/>
@@ -60189,7 +60395,7 @@
       <c r="P47" s="219"/>
       <c r="Q47" s="309"/>
       <c r="T47" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>7</v>
       </c>
       <c r="U47" s="308"/>
@@ -60208,10 +60414,30 @@
       <c r="AH47" s="142"/>
       <c r="AI47" s="219"/>
       <c r="AJ47" s="309"/>
+      <c r="AL47" s="70">
+        <f t="shared" si="31"/>
+        <v>7</v>
+      </c>
+      <c r="AM47" s="308"/>
+      <c r="AN47" s="142"/>
+      <c r="AO47" s="219"/>
+      <c r="AP47" s="219"/>
+      <c r="AQ47" s="219"/>
+      <c r="AR47" s="142"/>
+      <c r="AS47" s="390"/>
+      <c r="AT47" s="219"/>
+      <c r="AU47" s="219"/>
+      <c r="AV47" s="187"/>
+      <c r="AW47" s="142"/>
+      <c r="AX47" s="219"/>
+      <c r="AY47" s="219"/>
+      <c r="AZ47" s="219"/>
+      <c r="BA47" s="219"/>
+      <c r="BB47" s="309"/>
     </row>
     <row r="48" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A48" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>8</v>
       </c>
       <c r="B48" s="383"/>
@@ -60231,7 +60457,7 @@
       <c r="P48" s="342"/>
       <c r="Q48" s="352"/>
       <c r="T48" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>8</v>
       </c>
       <c r="U48" s="383"/>
@@ -60250,10 +60476,30 @@
       <c r="AH48" s="319"/>
       <c r="AI48" s="342"/>
       <c r="AJ48" s="352"/>
-    </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL48" s="70">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="AM48" s="383"/>
+      <c r="AN48" s="319"/>
+      <c r="AO48" s="342"/>
+      <c r="AP48" s="342"/>
+      <c r="AQ48" s="342"/>
+      <c r="AR48" s="142"/>
+      <c r="AS48" s="187"/>
+      <c r="AT48" s="219"/>
+      <c r="AU48" s="219"/>
+      <c r="AV48" s="390"/>
+      <c r="AW48" s="142"/>
+      <c r="AX48" s="342"/>
+      <c r="AY48" s="342"/>
+      <c r="AZ48" s="342"/>
+      <c r="BA48" s="342"/>
+      <c r="BB48" s="352"/>
+    </row>
+    <row r="49" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A49" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>9</v>
       </c>
       <c r="B49" s="314"/>
@@ -60273,7 +60519,7 @@
       <c r="P49" s="244"/>
       <c r="Q49" s="315"/>
       <c r="T49" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>9</v>
       </c>
       <c r="U49" s="314"/>
@@ -60292,10 +60538,30 @@
       <c r="AH49" s="142"/>
       <c r="AI49" s="244"/>
       <c r="AJ49" s="315"/>
-    </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL49" s="70">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="AM49" s="314"/>
+      <c r="AN49" s="320"/>
+      <c r="AO49" s="219"/>
+      <c r="AP49" s="219"/>
+      <c r="AQ49" s="219"/>
+      <c r="AR49" s="142"/>
+      <c r="AS49" s="7"/>
+      <c r="AT49" s="390"/>
+      <c r="AU49" s="187"/>
+      <c r="AV49" s="7"/>
+      <c r="AW49" s="142"/>
+      <c r="AX49" s="219"/>
+      <c r="AY49" s="219"/>
+      <c r="AZ49" s="219"/>
+      <c r="BA49" s="244"/>
+      <c r="BB49" s="315"/>
+    </row>
+    <row r="50" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A50" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>10</v>
       </c>
       <c r="B50" s="314"/>
@@ -60315,7 +60581,7 @@
       <c r="P50" s="244"/>
       <c r="Q50" s="315"/>
       <c r="T50" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>10</v>
       </c>
       <c r="U50" s="314"/>
@@ -60334,10 +60600,30 @@
       <c r="AH50" s="342"/>
       <c r="AI50" s="244"/>
       <c r="AJ50" s="315"/>
-    </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL50" s="70">
+        <f t="shared" si="31"/>
+        <v>10</v>
+      </c>
+      <c r="AM50" s="314"/>
+      <c r="AN50" s="244"/>
+      <c r="AO50" s="320"/>
+      <c r="AP50" s="320"/>
+      <c r="AQ50" s="320"/>
+      <c r="AR50" s="319"/>
+      <c r="AS50" s="319"/>
+      <c r="AT50" s="319"/>
+      <c r="AU50" s="319"/>
+      <c r="AV50" s="319"/>
+      <c r="AW50" s="319"/>
+      <c r="AX50" s="342"/>
+      <c r="AY50" s="342"/>
+      <c r="AZ50" s="342"/>
+      <c r="BA50" s="244"/>
+      <c r="BB50" s="315"/>
+    </row>
+    <row r="51" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A51" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>11</v>
       </c>
       <c r="B51" s="314"/>
@@ -60357,7 +60643,7 @@
       <c r="P51" s="244"/>
       <c r="Q51" s="315"/>
       <c r="T51" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>11</v>
       </c>
       <c r="U51" s="314"/>
@@ -60376,10 +60662,30 @@
       <c r="AH51" s="342"/>
       <c r="AI51" s="244"/>
       <c r="AJ51" s="315"/>
-    </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL51" s="70">
+        <f t="shared" si="31"/>
+        <v>11</v>
+      </c>
+      <c r="AM51" s="314"/>
+      <c r="AN51" s="244"/>
+      <c r="AO51" s="342"/>
+      <c r="AP51" s="342"/>
+      <c r="AQ51" s="342"/>
+      <c r="AR51" s="342"/>
+      <c r="AS51" s="342"/>
+      <c r="AT51" s="342"/>
+      <c r="AU51" s="342"/>
+      <c r="AV51" s="342"/>
+      <c r="AW51" s="342"/>
+      <c r="AX51" s="342"/>
+      <c r="AY51" s="342"/>
+      <c r="AZ51" s="342"/>
+      <c r="BA51" s="244"/>
+      <c r="BB51" s="315"/>
+    </row>
+    <row r="52" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A52" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>12</v>
       </c>
       <c r="B52" s="314"/>
@@ -60399,7 +60705,7 @@
       <c r="P52" s="244"/>
       <c r="Q52" s="315"/>
       <c r="T52" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="U52" s="314"/>
@@ -60418,10 +60724,30 @@
       <c r="AH52" s="342"/>
       <c r="AI52" s="244"/>
       <c r="AJ52" s="315"/>
-    </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL52" s="70">
+        <f t="shared" si="31"/>
+        <v>12</v>
+      </c>
+      <c r="AM52" s="314"/>
+      <c r="AN52" s="244"/>
+      <c r="AO52" s="342"/>
+      <c r="AP52" s="342"/>
+      <c r="AQ52" s="342"/>
+      <c r="AR52" s="342"/>
+      <c r="AS52" s="342"/>
+      <c r="AT52" s="342"/>
+      <c r="AU52" s="342"/>
+      <c r="AV52" s="342"/>
+      <c r="AW52" s="342"/>
+      <c r="AX52" s="342"/>
+      <c r="AY52" s="342"/>
+      <c r="AZ52" s="342"/>
+      <c r="BA52" s="244"/>
+      <c r="BB52" s="315"/>
+    </row>
+    <row r="53" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A53" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>13</v>
       </c>
       <c r="B53" s="314"/>
@@ -60441,7 +60767,7 @@
       <c r="P53" s="244"/>
       <c r="Q53" s="315"/>
       <c r="T53" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>13</v>
       </c>
       <c r="U53" s="314"/>
@@ -60460,10 +60786,30 @@
       <c r="AH53" s="319"/>
       <c r="AI53" s="244"/>
       <c r="AJ53" s="315"/>
-    </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL53" s="70">
+        <f t="shared" si="31"/>
+        <v>13</v>
+      </c>
+      <c r="AM53" s="314"/>
+      <c r="AN53" s="244"/>
+      <c r="AO53" s="342"/>
+      <c r="AP53" s="342"/>
+      <c r="AQ53" s="342"/>
+      <c r="AR53" s="342"/>
+      <c r="AS53" s="342"/>
+      <c r="AT53" s="342"/>
+      <c r="AU53" s="342"/>
+      <c r="AV53" s="342"/>
+      <c r="AW53" s="342"/>
+      <c r="AX53" s="342"/>
+      <c r="AY53" s="342"/>
+      <c r="AZ53" s="342"/>
+      <c r="BA53" s="244"/>
+      <c r="BB53" s="315"/>
+    </row>
+    <row r="54" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A54" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>14</v>
       </c>
       <c r="B54" s="120"/>
@@ -60483,7 +60829,7 @@
       <c r="P54" s="17"/>
       <c r="Q54" s="123"/>
       <c r="T54" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>14</v>
       </c>
       <c r="U54" s="120"/>
@@ -60502,10 +60848,30 @@
       <c r="AH54" s="244"/>
       <c r="AI54" s="17"/>
       <c r="AJ54" s="123"/>
-    </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL54" s="70">
+        <f t="shared" si="31"/>
+        <v>14</v>
+      </c>
+      <c r="AM54" s="120"/>
+      <c r="AN54" s="17"/>
+      <c r="AO54" s="244"/>
+      <c r="AP54" s="244"/>
+      <c r="AQ54" s="244"/>
+      <c r="AR54" s="17"/>
+      <c r="AS54" s="17"/>
+      <c r="AT54" s="219"/>
+      <c r="AU54" s="219"/>
+      <c r="AV54" s="17"/>
+      <c r="AW54" s="17"/>
+      <c r="AX54" s="244"/>
+      <c r="AY54" s="244"/>
+      <c r="AZ54" s="244"/>
+      <c r="BA54" s="17"/>
+      <c r="BB54" s="123"/>
+    </row>
+    <row r="55" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A55" s="70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>15</v>
       </c>
       <c r="B55" s="126"/>
@@ -60525,7 +60891,7 @@
       <c r="P55" s="124"/>
       <c r="Q55" s="125"/>
       <c r="T55" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>15</v>
       </c>
       <c r="U55" s="126"/>
@@ -60544,12 +60910,35 @@
       <c r="AH55" s="22"/>
       <c r="AI55" s="124"/>
       <c r="AJ55" s="125"/>
-    </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AL55" s="70">
+        <f t="shared" si="31"/>
+        <v>15</v>
+      </c>
+      <c r="AM55" s="126"/>
+      <c r="AN55" s="124"/>
+      <c r="AO55" s="22"/>
+      <c r="AP55" s="22"/>
+      <c r="AQ55" s="22"/>
+      <c r="AR55" s="22"/>
+      <c r="AS55" s="22"/>
+      <c r="AT55" s="218"/>
+      <c r="AU55" s="218"/>
+      <c r="AV55" s="22"/>
+      <c r="AW55" s="22"/>
+      <c r="AX55" s="22"/>
+      <c r="AY55" s="22"/>
+      <c r="AZ55" s="22"/>
+      <c r="BA55" s="124"/>
+      <c r="BB55" s="125"/>
+    </row>
+    <row r="56" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A56" s="242" t="s">
         <v>395</v>
       </c>
       <c r="T56" s="242" t="s">
+        <v>395</v>
+      </c>
+      <c r="AL56" s="242" t="s">
         <v>395</v>
       </c>
     </row>
@@ -60562,7 +60951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="U41" sqref="U41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed the door vs. switch issue Made the sewer planks into wood
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="29" activeTab="39"/>
+    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="31" activeTab="41"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -48,6 +48,7 @@
     <sheet name="Mineshafts" sheetId="47" r:id="rId39"/>
     <sheet name="Bunkers" sheetId="48" r:id="rId40"/>
     <sheet name="Sewers2" sheetId="49" r:id="rId41"/>
+    <sheet name="Sheet2" sheetId="50" r:id="rId42"/>
   </sheets>
   <definedNames>
     <definedName name="AbsoluteMaximumFloorsBelow">Sheet3!$C$6</definedName>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="441">
   <si>
     <t>grove</t>
   </si>
@@ -1940,7 +1941,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="412">
+  <cellXfs count="413">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2649,6 +2650,9 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3675,7 +3679,7 @@
       </c>
       <c r="O6">
         <f t="shared" ref="O6:AB15" ca="1" si="8">IF(AND(MOD(O$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3695,7 +3699,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4245,7 +4249,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4265,7 +4269,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4285,7 +4289,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4795,7 +4799,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4815,7 +4819,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4855,7 +4859,7 @@
       </c>
       <c r="Y16">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5345,7 +5349,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5385,7 +5389,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5915,7 +5919,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5935,7 +5939,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5955,7 +5959,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -53195,7 +53199,7 @@
   <dimension ref="A1:CL37"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="AO28" sqref="AO28"/>
+      <selection activeCell="A20" sqref="A20:R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57301,7 +57305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BV56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB19" workbookViewId="0">
+    <sheetView topLeftCell="AB19" workbookViewId="0">
       <selection activeCell="AR26" sqref="AR26"/>
     </sheetView>
   </sheetViews>
@@ -64045,6 +64049,2427 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BB36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A1" s="242"/>
+      <c r="B1" s="70">
+        <v>0</v>
+      </c>
+      <c r="C1" s="70">
+        <f t="shared" ref="C1:Q1" si="0">B1+1</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="70">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E1" s="70">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F1" s="70">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G1" s="70">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H1" s="70">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I1" s="70">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J1" s="70">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K1" s="70">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L1" s="70">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M1" s="70">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="N1" s="70">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O1" s="70">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P1" s="70">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q1" s="70">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="R1" s="242" t="s">
+        <v>394</v>
+      </c>
+      <c r="S1" s="242"/>
+      <c r="T1" s="70">
+        <v>0</v>
+      </c>
+      <c r="U1" s="70">
+        <f t="shared" ref="U1" si="1">T1+1</f>
+        <v>1</v>
+      </c>
+      <c r="V1" s="70">
+        <f t="shared" ref="V1" si="2">U1+1</f>
+        <v>2</v>
+      </c>
+      <c r="W1" s="70">
+        <f t="shared" ref="W1" si="3">V1+1</f>
+        <v>3</v>
+      </c>
+      <c r="X1" s="70">
+        <f t="shared" ref="X1" si="4">W1+1</f>
+        <v>4</v>
+      </c>
+      <c r="Y1" s="70">
+        <f t="shared" ref="Y1" si="5">X1+1</f>
+        <v>5</v>
+      </c>
+      <c r="Z1" s="70">
+        <f t="shared" ref="Z1" si="6">Y1+1</f>
+        <v>6</v>
+      </c>
+      <c r="AA1" s="70">
+        <f t="shared" ref="AA1" si="7">Z1+1</f>
+        <v>7</v>
+      </c>
+      <c r="AB1" s="70">
+        <f t="shared" ref="AB1" si="8">AA1+1</f>
+        <v>8</v>
+      </c>
+      <c r="AC1" s="70">
+        <f t="shared" ref="AC1" si="9">AB1+1</f>
+        <v>9</v>
+      </c>
+      <c r="AD1" s="70">
+        <f t="shared" ref="AD1" si="10">AC1+1</f>
+        <v>10</v>
+      </c>
+      <c r="AE1" s="70">
+        <f t="shared" ref="AE1" si="11">AD1+1</f>
+        <v>11</v>
+      </c>
+      <c r="AF1" s="70">
+        <f t="shared" ref="AF1" si="12">AE1+1</f>
+        <v>12</v>
+      </c>
+      <c r="AG1" s="70">
+        <f t="shared" ref="AG1" si="13">AF1+1</f>
+        <v>13</v>
+      </c>
+      <c r="AH1" s="70">
+        <f t="shared" ref="AH1" si="14">AG1+1</f>
+        <v>14</v>
+      </c>
+      <c r="AI1" s="70">
+        <f t="shared" ref="AI1" si="15">AH1+1</f>
+        <v>15</v>
+      </c>
+      <c r="AJ1" s="242" t="s">
+        <v>394</v>
+      </c>
+      <c r="AK1" s="242"/>
+      <c r="AL1" s="70">
+        <v>0</v>
+      </c>
+      <c r="AM1" s="70">
+        <f t="shared" ref="AM1" si="16">AL1+1</f>
+        <v>1</v>
+      </c>
+      <c r="AN1" s="70">
+        <f t="shared" ref="AN1" si="17">AM1+1</f>
+        <v>2</v>
+      </c>
+      <c r="AO1" s="70">
+        <f t="shared" ref="AO1" si="18">AN1+1</f>
+        <v>3</v>
+      </c>
+      <c r="AP1" s="70">
+        <f t="shared" ref="AP1" si="19">AO1+1</f>
+        <v>4</v>
+      </c>
+      <c r="AQ1" s="70">
+        <f t="shared" ref="AQ1" si="20">AP1+1</f>
+        <v>5</v>
+      </c>
+      <c r="AR1" s="70">
+        <f t="shared" ref="AR1" si="21">AQ1+1</f>
+        <v>6</v>
+      </c>
+      <c r="AS1" s="70">
+        <f t="shared" ref="AS1" si="22">AR1+1</f>
+        <v>7</v>
+      </c>
+      <c r="AT1" s="70">
+        <f t="shared" ref="AT1" si="23">AS1+1</f>
+        <v>8</v>
+      </c>
+      <c r="AU1" s="70">
+        <f t="shared" ref="AU1" si="24">AT1+1</f>
+        <v>9</v>
+      </c>
+      <c r="AV1" s="70">
+        <f t="shared" ref="AV1" si="25">AU1+1</f>
+        <v>10</v>
+      </c>
+      <c r="AW1" s="70">
+        <f t="shared" ref="AW1" si="26">AV1+1</f>
+        <v>11</v>
+      </c>
+      <c r="AX1" s="70">
+        <f t="shared" ref="AX1" si="27">AW1+1</f>
+        <v>12</v>
+      </c>
+      <c r="AY1" s="70">
+        <f t="shared" ref="AY1" si="28">AX1+1</f>
+        <v>13</v>
+      </c>
+      <c r="AZ1" s="70">
+        <f t="shared" ref="AZ1" si="29">AY1+1</f>
+        <v>14</v>
+      </c>
+      <c r="BA1" s="70">
+        <f t="shared" ref="BA1" si="30">AZ1+1</f>
+        <v>15</v>
+      </c>
+      <c r="BB1" s="242" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A2" s="70">
+        <v>0</v>
+      </c>
+      <c r="B2" s="311"/>
+      <c r="C2" s="312"/>
+      <c r="D2" s="312"/>
+      <c r="E2" s="312"/>
+      <c r="F2" s="312"/>
+      <c r="G2" s="312"/>
+      <c r="H2" s="357"/>
+      <c r="I2" s="312"/>
+      <c r="J2" s="312"/>
+      <c r="K2" s="357"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="312"/>
+      <c r="N2" s="312"/>
+      <c r="O2" s="312"/>
+      <c r="P2" s="312"/>
+      <c r="Q2" s="313"/>
+      <c r="S2" s="70">
+        <v>0</v>
+      </c>
+      <c r="T2" s="311"/>
+      <c r="U2" s="312"/>
+      <c r="V2" s="312"/>
+      <c r="W2" s="312"/>
+      <c r="X2" s="312"/>
+      <c r="Y2" s="312"/>
+      <c r="Z2" s="357"/>
+      <c r="AA2" s="312"/>
+      <c r="AB2" s="312"/>
+      <c r="AC2" s="357"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="312"/>
+      <c r="AF2" s="312"/>
+      <c r="AG2" s="312"/>
+      <c r="AH2" s="312"/>
+      <c r="AI2" s="313"/>
+      <c r="AK2" s="70">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="311"/>
+      <c r="AM2" s="312"/>
+      <c r="AN2" s="312"/>
+      <c r="AO2" s="312"/>
+      <c r="AP2" s="312"/>
+      <c r="AQ2" s="312"/>
+      <c r="AR2" s="357"/>
+      <c r="AS2" s="312"/>
+      <c r="AT2" s="312"/>
+      <c r="AU2" s="357"/>
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="312"/>
+      <c r="AX2" s="312"/>
+      <c r="AY2" s="312"/>
+      <c r="AZ2" s="312"/>
+      <c r="BA2" s="313"/>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A3" s="70">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="314"/>
+      <c r="C3" s="244"/>
+      <c r="D3" s="244"/>
+      <c r="E3" s="244"/>
+      <c r="F3" s="244"/>
+      <c r="G3" s="244"/>
+      <c r="H3" s="342"/>
+      <c r="I3" s="244"/>
+      <c r="J3" s="244"/>
+      <c r="K3" s="342"/>
+      <c r="L3" s="244"/>
+      <c r="M3" s="244"/>
+      <c r="N3" s="244"/>
+      <c r="O3" s="244"/>
+      <c r="P3" s="244"/>
+      <c r="Q3" s="315"/>
+      <c r="S3" s="70">
+        <f>S2+1</f>
+        <v>1</v>
+      </c>
+      <c r="T3" s="314"/>
+      <c r="U3" s="244"/>
+      <c r="V3" s="244"/>
+      <c r="W3" s="244"/>
+      <c r="X3" s="244"/>
+      <c r="Y3" s="244"/>
+      <c r="Z3" s="342"/>
+      <c r="AA3" s="244"/>
+      <c r="AB3" s="244"/>
+      <c r="AC3" s="342"/>
+      <c r="AD3" s="244"/>
+      <c r="AE3" s="244"/>
+      <c r="AF3" s="244"/>
+      <c r="AG3" s="244"/>
+      <c r="AH3" s="244"/>
+      <c r="AI3" s="315"/>
+      <c r="AK3" s="70">
+        <f>AK2+1</f>
+        <v>1</v>
+      </c>
+      <c r="AL3" s="314"/>
+      <c r="AM3" s="244"/>
+      <c r="AN3" s="244"/>
+      <c r="AO3" s="244"/>
+      <c r="AP3" s="244"/>
+      <c r="AQ3" s="244"/>
+      <c r="AR3" s="342"/>
+      <c r="AS3" s="244"/>
+      <c r="AT3" s="244"/>
+      <c r="AU3" s="342"/>
+      <c r="AV3" s="244"/>
+      <c r="AW3" s="244"/>
+      <c r="AX3" s="244"/>
+      <c r="AY3" s="244"/>
+      <c r="AZ3" s="244"/>
+      <c r="BA3" s="315"/>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A4" s="70">
+        <f t="shared" ref="A4:A17" si="31">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="314"/>
+      <c r="C4" s="244"/>
+      <c r="D4" s="244"/>
+      <c r="E4" s="244"/>
+      <c r="F4" s="244"/>
+      <c r="G4" s="244"/>
+      <c r="H4" s="342"/>
+      <c r="I4" s="244"/>
+      <c r="J4" s="244"/>
+      <c r="K4" s="342"/>
+      <c r="L4" s="244"/>
+      <c r="M4" s="244"/>
+      <c r="N4" s="244"/>
+      <c r="O4" s="244"/>
+      <c r="P4" s="244"/>
+      <c r="Q4" s="26"/>
+      <c r="S4" s="70">
+        <f t="shared" ref="S4:S17" si="32">S3+1</f>
+        <v>2</v>
+      </c>
+      <c r="T4" s="314"/>
+      <c r="U4" s="244"/>
+      <c r="V4" s="244"/>
+      <c r="W4" s="244"/>
+      <c r="X4" s="244"/>
+      <c r="Y4" s="244"/>
+      <c r="Z4" s="342"/>
+      <c r="AA4" s="244"/>
+      <c r="AB4" s="244"/>
+      <c r="AC4" s="342"/>
+      <c r="AD4" s="244"/>
+      <c r="AE4" s="244"/>
+      <c r="AF4" s="244"/>
+      <c r="AG4" s="244"/>
+      <c r="AH4" s="244"/>
+      <c r="AI4" s="26"/>
+      <c r="AK4" s="70">
+        <f t="shared" ref="AK4:AK17" si="33">AK3+1</f>
+        <v>2</v>
+      </c>
+      <c r="AL4" s="314"/>
+      <c r="AM4" s="244"/>
+      <c r="AN4" s="244"/>
+      <c r="AO4" s="244"/>
+      <c r="AP4" s="244"/>
+      <c r="AQ4" s="244"/>
+      <c r="AR4" s="342"/>
+      <c r="AS4" s="244"/>
+      <c r="AT4" s="244"/>
+      <c r="AU4" s="342"/>
+      <c r="AV4" s="244"/>
+      <c r="AW4" s="244"/>
+      <c r="AX4" s="244"/>
+      <c r="AY4" s="244"/>
+      <c r="AZ4" s="244"/>
+      <c r="BA4" s="26"/>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A5" s="70">
+        <f t="shared" si="31"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="314"/>
+      <c r="C5" s="244"/>
+      <c r="D5" s="244"/>
+      <c r="E5" s="244"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="219"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="219"/>
+      <c r="L5" s="244"/>
+      <c r="M5" s="244"/>
+      <c r="N5" s="244"/>
+      <c r="O5" s="244"/>
+      <c r="P5" s="244"/>
+      <c r="Q5" s="26"/>
+      <c r="S5" s="70">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+      <c r="T5" s="314"/>
+      <c r="U5" s="244"/>
+      <c r="V5" s="244"/>
+      <c r="W5" s="244"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="219"/>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="219"/>
+      <c r="AD5" s="244"/>
+      <c r="AE5" s="244"/>
+      <c r="AF5" s="244"/>
+      <c r="AG5" s="244"/>
+      <c r="AH5" s="244"/>
+      <c r="AI5" s="26"/>
+      <c r="AK5" s="70">
+        <f t="shared" si="33"/>
+        <v>3</v>
+      </c>
+      <c r="AL5" s="314"/>
+      <c r="AM5" s="244"/>
+      <c r="AN5" s="244"/>
+      <c r="AO5" s="244"/>
+      <c r="AP5" s="17"/>
+      <c r="AQ5" s="17"/>
+      <c r="AR5" s="219"/>
+      <c r="AS5" s="17"/>
+      <c r="AT5" s="17"/>
+      <c r="AU5" s="219"/>
+      <c r="AV5" s="244"/>
+      <c r="AW5" s="244"/>
+      <c r="AX5" s="244"/>
+      <c r="AY5" s="244"/>
+      <c r="AZ5" s="244"/>
+      <c r="BA5" s="26"/>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A6" s="70">
+        <f t="shared" si="31"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="314"/>
+      <c r="C6" s="244"/>
+      <c r="D6" s="244"/>
+      <c r="E6" s="244"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="246"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="152"/>
+      <c r="L6" s="244"/>
+      <c r="M6" s="244"/>
+      <c r="N6" s="244"/>
+      <c r="O6" s="244"/>
+      <c r="P6" s="244"/>
+      <c r="Q6" s="26"/>
+      <c r="S6" s="70">
+        <f t="shared" si="32"/>
+        <v>4</v>
+      </c>
+      <c r="T6" s="314"/>
+      <c r="U6" s="244"/>
+      <c r="V6" s="244"/>
+      <c r="W6" s="244"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="244"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="244"/>
+      <c r="AE6" s="244"/>
+      <c r="AF6" s="244"/>
+      <c r="AG6" s="244"/>
+      <c r="AH6" s="244"/>
+      <c r="AI6" s="26"/>
+      <c r="AK6" s="70">
+        <f t="shared" si="33"/>
+        <v>4</v>
+      </c>
+      <c r="AL6" s="314"/>
+      <c r="AM6" s="244"/>
+      <c r="AN6" s="244"/>
+      <c r="AO6" s="244"/>
+      <c r="AP6" s="17"/>
+      <c r="AQ6" s="17"/>
+      <c r="AR6" s="342"/>
+      <c r="AS6" s="17"/>
+      <c r="AT6" s="17"/>
+      <c r="AU6" s="219"/>
+      <c r="AV6" s="244"/>
+      <c r="AW6" s="244"/>
+      <c r="AX6" s="244"/>
+      <c r="AY6" s="244"/>
+      <c r="AZ6" s="244"/>
+      <c r="BA6" s="26"/>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A7" s="70">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="314"/>
+      <c r="C7" s="244"/>
+      <c r="D7" s="244"/>
+      <c r="E7" s="244"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="219"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="219"/>
+      <c r="L7" s="244"/>
+      <c r="M7" s="244"/>
+      <c r="N7" s="244"/>
+      <c r="O7" s="244"/>
+      <c r="P7" s="244"/>
+      <c r="Q7" s="26"/>
+      <c r="S7" s="70">
+        <f t="shared" si="32"/>
+        <v>5</v>
+      </c>
+      <c r="T7" s="314"/>
+      <c r="U7" s="244"/>
+      <c r="V7" s="244"/>
+      <c r="W7" s="244"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17"/>
+      <c r="AA7" s="17"/>
+      <c r="AB7" s="17"/>
+      <c r="AC7" s="17"/>
+      <c r="AD7" s="244"/>
+      <c r="AE7" s="244"/>
+      <c r="AF7" s="244"/>
+      <c r="AG7" s="244"/>
+      <c r="AH7" s="244"/>
+      <c r="AI7" s="26"/>
+      <c r="AK7" s="70">
+        <f t="shared" si="33"/>
+        <v>5</v>
+      </c>
+      <c r="AL7" s="314"/>
+      <c r="AM7" s="244"/>
+      <c r="AN7" s="244"/>
+      <c r="AO7" s="244"/>
+      <c r="AP7" s="17"/>
+      <c r="AQ7" s="17"/>
+      <c r="AR7" s="219"/>
+      <c r="AS7" s="17"/>
+      <c r="AT7" s="17"/>
+      <c r="AU7" s="219"/>
+      <c r="AV7" s="244"/>
+      <c r="AW7" s="244"/>
+      <c r="AX7" s="244"/>
+      <c r="AY7" s="244"/>
+      <c r="AZ7" s="244"/>
+      <c r="BA7" s="26"/>
+    </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A8" s="70">
+        <f t="shared" si="31"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="308"/>
+      <c r="C8" s="219"/>
+      <c r="D8" s="219"/>
+      <c r="E8" s="219"/>
+      <c r="F8" s="152"/>
+      <c r="G8" s="219"/>
+      <c r="H8" s="219"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="219"/>
+      <c r="L8" s="219"/>
+      <c r="M8" s="152"/>
+      <c r="N8" s="219"/>
+      <c r="O8" s="219"/>
+      <c r="P8" s="219"/>
+      <c r="Q8" s="309"/>
+      <c r="S8" s="70">
+        <f t="shared" si="32"/>
+        <v>6</v>
+      </c>
+      <c r="T8" s="308"/>
+      <c r="U8" s="219"/>
+      <c r="V8" s="219"/>
+      <c r="W8" s="219"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="17"/>
+      <c r="AF8" s="219"/>
+      <c r="AG8" s="219"/>
+      <c r="AH8" s="219"/>
+      <c r="AI8" s="309"/>
+      <c r="AK8" s="70">
+        <f t="shared" si="33"/>
+        <v>6</v>
+      </c>
+      <c r="AL8" s="16"/>
+      <c r="AM8" s="17"/>
+      <c r="AN8" s="17"/>
+      <c r="AO8" s="17"/>
+      <c r="AP8" s="17"/>
+      <c r="AQ8" s="17"/>
+      <c r="AR8" s="219"/>
+      <c r="AS8" s="17"/>
+      <c r="AT8" s="17"/>
+      <c r="AU8" s="219"/>
+      <c r="AV8" s="17"/>
+      <c r="AW8" s="17"/>
+      <c r="AX8" s="17"/>
+      <c r="AY8" s="17"/>
+      <c r="AZ8" s="17"/>
+      <c r="BA8" s="26"/>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A9" s="70">
+        <f t="shared" si="31"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="314"/>
+      <c r="C9" s="244"/>
+      <c r="D9" s="244"/>
+      <c r="E9" s="244"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="244"/>
+      <c r="M9" s="244"/>
+      <c r="N9" s="244"/>
+      <c r="O9" s="244"/>
+      <c r="P9" s="244"/>
+      <c r="Q9" s="315"/>
+      <c r="S9" s="70">
+        <f t="shared" si="32"/>
+        <v>7</v>
+      </c>
+      <c r="T9" s="314"/>
+      <c r="U9" s="244"/>
+      <c r="V9" s="244"/>
+      <c r="W9" s="244"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17"/>
+      <c r="AA9" s="17"/>
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="17"/>
+      <c r="AD9" s="244"/>
+      <c r="AE9" s="244"/>
+      <c r="AF9" s="244"/>
+      <c r="AG9" s="244"/>
+      <c r="AH9" s="244"/>
+      <c r="AI9" s="315"/>
+      <c r="AK9" s="70">
+        <f t="shared" si="33"/>
+        <v>7</v>
+      </c>
+      <c r="AL9" s="314"/>
+      <c r="AM9" s="244"/>
+      <c r="AN9" s="244"/>
+      <c r="AO9" s="244"/>
+      <c r="AP9" s="17"/>
+      <c r="AQ9" s="17"/>
+      <c r="AR9" s="17"/>
+      <c r="AS9" s="17"/>
+      <c r="AT9" s="17"/>
+      <c r="AU9" s="17"/>
+      <c r="AV9" s="244"/>
+      <c r="AW9" s="244"/>
+      <c r="AX9" s="244"/>
+      <c r="AY9" s="244"/>
+      <c r="AZ9" s="244"/>
+      <c r="BA9" s="315"/>
+    </row>
+    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A10" s="70">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="314"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="244"/>
+      <c r="P10" s="244"/>
+      <c r="Q10" s="315"/>
+      <c r="S10" s="70">
+        <f t="shared" si="32"/>
+        <v>8</v>
+      </c>
+      <c r="T10" s="314"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
+      <c r="AA10" s="17"/>
+      <c r="AB10" s="17"/>
+      <c r="AC10" s="17"/>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="17"/>
+      <c r="AF10" s="17"/>
+      <c r="AG10" s="244"/>
+      <c r="AH10" s="244"/>
+      <c r="AI10" s="315"/>
+      <c r="AK10" s="70">
+        <f t="shared" si="33"/>
+        <v>8</v>
+      </c>
+      <c r="AL10" s="314"/>
+      <c r="AM10" s="17"/>
+      <c r="AN10" s="17"/>
+      <c r="AO10" s="17"/>
+      <c r="AP10" s="17"/>
+      <c r="AQ10" s="17"/>
+      <c r="AR10" s="17"/>
+      <c r="AS10" s="17"/>
+      <c r="AT10" s="17"/>
+      <c r="AU10" s="17"/>
+      <c r="AV10" s="17"/>
+      <c r="AW10" s="17"/>
+      <c r="AX10" s="17"/>
+      <c r="AY10" s="244"/>
+      <c r="AZ10" s="244"/>
+      <c r="BA10" s="315"/>
+    </row>
+    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A11" s="70">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="383"/>
+      <c r="C11" s="342"/>
+      <c r="D11" s="342"/>
+      <c r="E11" s="342"/>
+      <c r="F11" s="246"/>
+      <c r="G11" s="342"/>
+      <c r="H11" s="342"/>
+      <c r="I11" s="244"/>
+      <c r="J11" s="244"/>
+      <c r="K11" s="342"/>
+      <c r="L11" s="342"/>
+      <c r="M11" s="246"/>
+      <c r="N11" s="342"/>
+      <c r="O11" s="342"/>
+      <c r="P11" s="342"/>
+      <c r="Q11" s="352"/>
+      <c r="S11" s="70">
+        <f t="shared" si="32"/>
+        <v>9</v>
+      </c>
+      <c r="T11" s="383"/>
+      <c r="U11" s="342"/>
+      <c r="V11" s="342"/>
+      <c r="W11" s="342"/>
+      <c r="X11" s="244"/>
+      <c r="Y11" s="244"/>
+      <c r="Z11" s="244"/>
+      <c r="AA11" s="244"/>
+      <c r="AB11" s="244"/>
+      <c r="AC11" s="244"/>
+      <c r="AD11" s="244"/>
+      <c r="AE11" s="244"/>
+      <c r="AF11" s="342"/>
+      <c r="AG11" s="342"/>
+      <c r="AH11" s="342"/>
+      <c r="AI11" s="352"/>
+      <c r="AK11" s="70">
+        <f t="shared" si="33"/>
+        <v>9</v>
+      </c>
+      <c r="AL11" s="314"/>
+      <c r="AM11" s="244"/>
+      <c r="AN11" s="244"/>
+      <c r="AO11" s="244"/>
+      <c r="AP11" s="244"/>
+      <c r="AQ11" s="244"/>
+      <c r="AR11" s="244"/>
+      <c r="AS11" s="244"/>
+      <c r="AT11" s="244"/>
+      <c r="AU11" s="244"/>
+      <c r="AV11" s="244"/>
+      <c r="AW11" s="244"/>
+      <c r="AX11" s="244"/>
+      <c r="AY11" s="244"/>
+      <c r="AZ11" s="244"/>
+      <c r="BA11" s="315"/>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A12" s="70">
+        <f t="shared" si="31"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="244"/>
+      <c r="D12" s="244"/>
+      <c r="E12" s="244"/>
+      <c r="F12" s="244"/>
+      <c r="G12" s="244"/>
+      <c r="H12" s="342"/>
+      <c r="I12" s="244"/>
+      <c r="J12" s="244"/>
+      <c r="K12" s="342"/>
+      <c r="L12" s="244"/>
+      <c r="M12" s="244"/>
+      <c r="N12" s="244"/>
+      <c r="O12" s="244"/>
+      <c r="P12" s="244"/>
+      <c r="Q12" s="26"/>
+      <c r="S12" s="70">
+        <f t="shared" si="32"/>
+        <v>10</v>
+      </c>
+      <c r="T12" s="16"/>
+      <c r="U12" s="244"/>
+      <c r="V12" s="244"/>
+      <c r="W12" s="244"/>
+      <c r="X12" s="244"/>
+      <c r="Y12" s="244"/>
+      <c r="Z12" s="244"/>
+      <c r="AA12" s="244"/>
+      <c r="AB12" s="244"/>
+      <c r="AC12" s="244"/>
+      <c r="AD12" s="244"/>
+      <c r="AE12" s="244"/>
+      <c r="AF12" s="244"/>
+      <c r="AG12" s="244"/>
+      <c r="AH12" s="244"/>
+      <c r="AI12" s="26"/>
+      <c r="AK12" s="70">
+        <f t="shared" si="33"/>
+        <v>10</v>
+      </c>
+      <c r="AL12" s="16"/>
+      <c r="AM12" s="244"/>
+      <c r="AN12" s="244"/>
+      <c r="AO12" s="244"/>
+      <c r="AP12" s="244"/>
+      <c r="AQ12" s="244"/>
+      <c r="AR12" s="342"/>
+      <c r="AS12" s="244"/>
+      <c r="AT12" s="244"/>
+      <c r="AU12" s="342"/>
+      <c r="AV12" s="244"/>
+      <c r="AW12" s="244"/>
+      <c r="AX12" s="244"/>
+      <c r="AY12" s="244"/>
+      <c r="AZ12" s="244"/>
+      <c r="BA12" s="26"/>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A13" s="70">
+        <f t="shared" si="31"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="314"/>
+      <c r="C13" s="244"/>
+      <c r="D13" s="244"/>
+      <c r="E13" s="244"/>
+      <c r="F13" s="244"/>
+      <c r="G13" s="244"/>
+      <c r="H13" s="246"/>
+      <c r="I13" s="244"/>
+      <c r="J13" s="244"/>
+      <c r="K13" s="246"/>
+      <c r="L13" s="244"/>
+      <c r="M13" s="244"/>
+      <c r="N13" s="244"/>
+      <c r="O13" s="244"/>
+      <c r="P13" s="244"/>
+      <c r="Q13" s="26"/>
+      <c r="S13" s="70">
+        <f t="shared" si="32"/>
+        <v>11</v>
+      </c>
+      <c r="T13" s="314"/>
+      <c r="U13" s="244"/>
+      <c r="V13" s="244"/>
+      <c r="W13" s="244"/>
+      <c r="X13" s="244"/>
+      <c r="Y13" s="244"/>
+      <c r="Z13" s="244"/>
+      <c r="AA13" s="244"/>
+      <c r="AB13" s="244"/>
+      <c r="AC13" s="244"/>
+      <c r="AD13" s="244"/>
+      <c r="AE13" s="244"/>
+      <c r="AF13" s="244"/>
+      <c r="AG13" s="244"/>
+      <c r="AH13" s="244"/>
+      <c r="AI13" s="26"/>
+      <c r="AK13" s="70">
+        <f t="shared" si="33"/>
+        <v>11</v>
+      </c>
+      <c r="AL13" s="314"/>
+      <c r="AM13" s="244"/>
+      <c r="AN13" s="244"/>
+      <c r="AO13" s="244"/>
+      <c r="AP13" s="244"/>
+      <c r="AQ13" s="244"/>
+      <c r="AR13" s="342"/>
+      <c r="AS13" s="244"/>
+      <c r="AT13" s="244"/>
+      <c r="AU13" s="342"/>
+      <c r="AV13" s="244"/>
+      <c r="AW13" s="244"/>
+      <c r="AX13" s="244"/>
+      <c r="AY13" s="244"/>
+      <c r="AZ13" s="244"/>
+      <c r="BA13" s="26"/>
+    </row>
+    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A14" s="70">
+        <f t="shared" si="31"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="314"/>
+      <c r="C14" s="244"/>
+      <c r="D14" s="244"/>
+      <c r="E14" s="244"/>
+      <c r="F14" s="244"/>
+      <c r="G14" s="244"/>
+      <c r="H14" s="342"/>
+      <c r="I14" s="244"/>
+      <c r="J14" s="244"/>
+      <c r="K14" s="342"/>
+      <c r="L14" s="244"/>
+      <c r="M14" s="244"/>
+      <c r="N14" s="244"/>
+      <c r="O14" s="244"/>
+      <c r="P14" s="244"/>
+      <c r="Q14" s="26"/>
+      <c r="S14" s="70">
+        <f t="shared" si="32"/>
+        <v>12</v>
+      </c>
+      <c r="T14" s="314"/>
+      <c r="U14" s="244"/>
+      <c r="V14" s="244"/>
+      <c r="W14" s="244"/>
+      <c r="X14" s="244"/>
+      <c r="Y14" s="244"/>
+      <c r="Z14" s="342"/>
+      <c r="AA14" s="244"/>
+      <c r="AB14" s="244"/>
+      <c r="AC14" s="342"/>
+      <c r="AD14" s="244"/>
+      <c r="AE14" s="244"/>
+      <c r="AF14" s="244"/>
+      <c r="AG14" s="244"/>
+      <c r="AH14" s="244"/>
+      <c r="AI14" s="26"/>
+      <c r="AK14" s="70">
+        <f t="shared" si="33"/>
+        <v>12</v>
+      </c>
+      <c r="AL14" s="314"/>
+      <c r="AM14" s="244"/>
+      <c r="AN14" s="244"/>
+      <c r="AO14" s="244"/>
+      <c r="AP14" s="244"/>
+      <c r="AQ14" s="244"/>
+      <c r="AR14" s="342"/>
+      <c r="AS14" s="244"/>
+      <c r="AT14" s="244"/>
+      <c r="AU14" s="342"/>
+      <c r="AV14" s="244"/>
+      <c r="AW14" s="244"/>
+      <c r="AX14" s="244"/>
+      <c r="AY14" s="244"/>
+      <c r="AZ14" s="244"/>
+      <c r="BA14" s="26"/>
+    </row>
+    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A15" s="70">
+        <f t="shared" si="31"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="314"/>
+      <c r="C15" s="244"/>
+      <c r="D15" s="244"/>
+      <c r="E15" s="244"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="219"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="219"/>
+      <c r="L15" s="244"/>
+      <c r="M15" s="244"/>
+      <c r="N15" s="244"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="26"/>
+      <c r="S15" s="70">
+        <f t="shared" si="32"/>
+        <v>13</v>
+      </c>
+      <c r="T15" s="314"/>
+      <c r="U15" s="244"/>
+      <c r="V15" s="244"/>
+      <c r="W15" s="244"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="219"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="219"/>
+      <c r="AD15" s="244"/>
+      <c r="AE15" s="244"/>
+      <c r="AF15" s="244"/>
+      <c r="AG15" s="17"/>
+      <c r="AH15" s="17"/>
+      <c r="AI15" s="26"/>
+      <c r="AK15" s="70">
+        <f t="shared" si="33"/>
+        <v>13</v>
+      </c>
+      <c r="AL15" s="314"/>
+      <c r="AM15" s="244"/>
+      <c r="AN15" s="244"/>
+      <c r="AO15" s="244"/>
+      <c r="AP15" s="17"/>
+      <c r="AQ15" s="17"/>
+      <c r="AR15" s="219"/>
+      <c r="AS15" s="17"/>
+      <c r="AT15" s="17"/>
+      <c r="AU15" s="219"/>
+      <c r="AV15" s="244"/>
+      <c r="AW15" s="244"/>
+      <c r="AX15" s="244"/>
+      <c r="AY15" s="17"/>
+      <c r="AZ15" s="17"/>
+      <c r="BA15" s="26"/>
+    </row>
+    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A16" s="70">
+        <f t="shared" si="31"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="219"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="219"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="26"/>
+      <c r="S16" s="70">
+        <f t="shared" si="32"/>
+        <v>14</v>
+      </c>
+      <c r="T16" s="16"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="219"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="219"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="17"/>
+      <c r="AF16" s="17"/>
+      <c r="AG16" s="17"/>
+      <c r="AH16" s="17"/>
+      <c r="AI16" s="26"/>
+      <c r="AK16" s="70">
+        <f t="shared" si="33"/>
+        <v>14</v>
+      </c>
+      <c r="AL16" s="16"/>
+      <c r="AM16" s="17"/>
+      <c r="AN16" s="17"/>
+      <c r="AO16" s="17"/>
+      <c r="AP16" s="17"/>
+      <c r="AQ16" s="17"/>
+      <c r="AR16" s="219"/>
+      <c r="AS16" s="17"/>
+      <c r="AT16" s="17"/>
+      <c r="AU16" s="219"/>
+      <c r="AV16" s="17"/>
+      <c r="AW16" s="17"/>
+      <c r="AX16" s="17"/>
+      <c r="AY16" s="17"/>
+      <c r="AZ16" s="17"/>
+      <c r="BA16" s="26"/>
+    </row>
+    <row r="17" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A17" s="70">
+        <f t="shared" si="31"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="412"/>
+      <c r="I17" s="317"/>
+      <c r="J17" s="317"/>
+      <c r="K17" s="412"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="33"/>
+      <c r="S17" s="70">
+        <f t="shared" si="32"/>
+        <v>15</v>
+      </c>
+      <c r="T17" s="32"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="412"/>
+      <c r="AA17" s="317"/>
+      <c r="AB17" s="317"/>
+      <c r="AC17" s="412"/>
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+      <c r="AG17" s="22"/>
+      <c r="AH17" s="22"/>
+      <c r="AI17" s="33"/>
+      <c r="AK17" s="70">
+        <f t="shared" si="33"/>
+        <v>15</v>
+      </c>
+      <c r="AL17" s="32"/>
+      <c r="AM17" s="22"/>
+      <c r="AN17" s="22"/>
+      <c r="AO17" s="22"/>
+      <c r="AP17" s="22"/>
+      <c r="AQ17" s="22"/>
+      <c r="AR17" s="412"/>
+      <c r="AS17" s="317"/>
+      <c r="AT17" s="317"/>
+      <c r="AU17" s="412"/>
+      <c r="AV17" s="22"/>
+      <c r="AW17" s="22"/>
+      <c r="AX17" s="22"/>
+      <c r="AY17" s="22"/>
+      <c r="AZ17" s="22"/>
+      <c r="BA17" s="33"/>
+    </row>
+    <row r="18" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A18" s="242" t="s">
+        <v>395</v>
+      </c>
+      <c r="S18" s="242" t="s">
+        <v>395</v>
+      </c>
+      <c r="AK18" s="242" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A19" s="242"/>
+      <c r="B19" s="70">
+        <v>0</v>
+      </c>
+      <c r="C19" s="70">
+        <f t="shared" ref="C19" si="34">B19+1</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="70">
+        <f t="shared" ref="D19" si="35">C19+1</f>
+        <v>2</v>
+      </c>
+      <c r="E19" s="70">
+        <f t="shared" ref="E19" si="36">D19+1</f>
+        <v>3</v>
+      </c>
+      <c r="F19" s="70">
+        <f t="shared" ref="F19" si="37">E19+1</f>
+        <v>4</v>
+      </c>
+      <c r="G19" s="70">
+        <f t="shared" ref="G19" si="38">F19+1</f>
+        <v>5</v>
+      </c>
+      <c r="H19" s="70">
+        <f t="shared" ref="H19" si="39">G19+1</f>
+        <v>6</v>
+      </c>
+      <c r="I19" s="70">
+        <f t="shared" ref="I19" si="40">H19+1</f>
+        <v>7</v>
+      </c>
+      <c r="J19" s="70">
+        <f t="shared" ref="J19" si="41">I19+1</f>
+        <v>8</v>
+      </c>
+      <c r="K19" s="70">
+        <f t="shared" ref="K19" si="42">J19+1</f>
+        <v>9</v>
+      </c>
+      <c r="L19" s="70">
+        <f t="shared" ref="L19" si="43">K19+1</f>
+        <v>10</v>
+      </c>
+      <c r="M19" s="70">
+        <f t="shared" ref="M19" si="44">L19+1</f>
+        <v>11</v>
+      </c>
+      <c r="N19" s="70">
+        <f t="shared" ref="N19" si="45">M19+1</f>
+        <v>12</v>
+      </c>
+      <c r="O19" s="70">
+        <f t="shared" ref="O19" si="46">N19+1</f>
+        <v>13</v>
+      </c>
+      <c r="P19" s="70">
+        <f t="shared" ref="P19" si="47">O19+1</f>
+        <v>14</v>
+      </c>
+      <c r="Q19" s="70">
+        <f t="shared" ref="Q19" si="48">P19+1</f>
+        <v>15</v>
+      </c>
+      <c r="R19" s="242" t="s">
+        <v>394</v>
+      </c>
+      <c r="S19" s="242"/>
+      <c r="T19" s="70">
+        <v>0</v>
+      </c>
+      <c r="U19" s="70">
+        <f t="shared" ref="U19" si="49">T19+1</f>
+        <v>1</v>
+      </c>
+      <c r="V19" s="70">
+        <f t="shared" ref="V19" si="50">U19+1</f>
+        <v>2</v>
+      </c>
+      <c r="W19" s="70">
+        <f t="shared" ref="W19" si="51">V19+1</f>
+        <v>3</v>
+      </c>
+      <c r="X19" s="70">
+        <f t="shared" ref="X19" si="52">W19+1</f>
+        <v>4</v>
+      </c>
+      <c r="Y19" s="70">
+        <f t="shared" ref="Y19" si="53">X19+1</f>
+        <v>5</v>
+      </c>
+      <c r="Z19" s="70">
+        <f t="shared" ref="Z19" si="54">Y19+1</f>
+        <v>6</v>
+      </c>
+      <c r="AA19" s="70">
+        <f t="shared" ref="AA19" si="55">Z19+1</f>
+        <v>7</v>
+      </c>
+      <c r="AB19" s="70">
+        <f t="shared" ref="AB19" si="56">AA19+1</f>
+        <v>8</v>
+      </c>
+      <c r="AC19" s="70">
+        <f t="shared" ref="AC19" si="57">AB19+1</f>
+        <v>9</v>
+      </c>
+      <c r="AD19" s="70">
+        <f t="shared" ref="AD19" si="58">AC19+1</f>
+        <v>10</v>
+      </c>
+      <c r="AE19" s="70">
+        <f t="shared" ref="AE19" si="59">AD19+1</f>
+        <v>11</v>
+      </c>
+      <c r="AF19" s="70">
+        <f t="shared" ref="AF19" si="60">AE19+1</f>
+        <v>12</v>
+      </c>
+      <c r="AG19" s="70">
+        <f t="shared" ref="AG19" si="61">AF19+1</f>
+        <v>13</v>
+      </c>
+      <c r="AH19" s="70">
+        <f t="shared" ref="AH19" si="62">AG19+1</f>
+        <v>14</v>
+      </c>
+      <c r="AI19" s="70">
+        <f t="shared" ref="AI19" si="63">AH19+1</f>
+        <v>15</v>
+      </c>
+      <c r="AJ19" s="242" t="s">
+        <v>394</v>
+      </c>
+      <c r="AK19" s="242"/>
+      <c r="AL19" s="70">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="70">
+        <f t="shared" ref="AM19" si="64">AL19+1</f>
+        <v>1</v>
+      </c>
+      <c r="AN19" s="70">
+        <f t="shared" ref="AN19" si="65">AM19+1</f>
+        <v>2</v>
+      </c>
+      <c r="AO19" s="70">
+        <f t="shared" ref="AO19" si="66">AN19+1</f>
+        <v>3</v>
+      </c>
+      <c r="AP19" s="70">
+        <f t="shared" ref="AP19" si="67">AO19+1</f>
+        <v>4</v>
+      </c>
+      <c r="AQ19" s="70">
+        <f t="shared" ref="AQ19" si="68">AP19+1</f>
+        <v>5</v>
+      </c>
+      <c r="AR19" s="70">
+        <f t="shared" ref="AR19" si="69">AQ19+1</f>
+        <v>6</v>
+      </c>
+      <c r="AS19" s="70">
+        <f t="shared" ref="AS19" si="70">AR19+1</f>
+        <v>7</v>
+      </c>
+      <c r="AT19" s="70">
+        <f t="shared" ref="AT19" si="71">AS19+1</f>
+        <v>8</v>
+      </c>
+      <c r="AU19" s="70">
+        <f t="shared" ref="AU19" si="72">AT19+1</f>
+        <v>9</v>
+      </c>
+      <c r="AV19" s="70">
+        <f t="shared" ref="AV19" si="73">AU19+1</f>
+        <v>10</v>
+      </c>
+      <c r="AW19" s="70">
+        <f t="shared" ref="AW19" si="74">AV19+1</f>
+        <v>11</v>
+      </c>
+      <c r="AX19" s="70">
+        <f t="shared" ref="AX19" si="75">AW19+1</f>
+        <v>12</v>
+      </c>
+      <c r="AY19" s="70">
+        <f t="shared" ref="AY19" si="76">AX19+1</f>
+        <v>13</v>
+      </c>
+      <c r="AZ19" s="70">
+        <f t="shared" ref="AZ19" si="77">AY19+1</f>
+        <v>14</v>
+      </c>
+      <c r="BA19" s="70">
+        <f t="shared" ref="BA19" si="78">AZ19+1</f>
+        <v>15</v>
+      </c>
+      <c r="BB19" s="242" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="20" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A20" s="70">
+        <v>0</v>
+      </c>
+      <c r="B20" s="311"/>
+      <c r="C20" s="312"/>
+      <c r="D20" s="312"/>
+      <c r="E20" s="312"/>
+      <c r="F20" s="312"/>
+      <c r="G20" s="312"/>
+      <c r="H20" s="357"/>
+      <c r="I20" s="312"/>
+      <c r="J20" s="312"/>
+      <c r="K20" s="357"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="312"/>
+      <c r="N20" s="312"/>
+      <c r="O20" s="312"/>
+      <c r="P20" s="312"/>
+      <c r="Q20" s="313"/>
+      <c r="S20" s="70">
+        <v>0</v>
+      </c>
+      <c r="T20" s="311"/>
+      <c r="U20" s="312"/>
+      <c r="V20" s="312"/>
+      <c r="W20" s="312"/>
+      <c r="X20" s="312"/>
+      <c r="Y20" s="312"/>
+      <c r="Z20" s="312"/>
+      <c r="AA20" s="312"/>
+      <c r="AB20" s="312"/>
+      <c r="AC20" s="312"/>
+      <c r="AD20" s="20"/>
+      <c r="AE20" s="312"/>
+      <c r="AF20" s="312"/>
+      <c r="AG20" s="312"/>
+      <c r="AH20" s="312"/>
+      <c r="AI20" s="313"/>
+      <c r="AK20" s="70">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="311"/>
+      <c r="AM20" s="312"/>
+      <c r="AN20" s="312"/>
+      <c r="AO20" s="312"/>
+      <c r="AP20" s="312"/>
+      <c r="AQ20" s="312"/>
+      <c r="AR20" s="312"/>
+      <c r="AS20" s="312"/>
+      <c r="AT20" s="312"/>
+      <c r="AU20" s="312"/>
+      <c r="AV20" s="20"/>
+      <c r="AW20" s="312"/>
+      <c r="AX20" s="312"/>
+      <c r="AY20" s="312"/>
+      <c r="AZ20" s="312"/>
+      <c r="BA20" s="313"/>
+    </row>
+    <row r="21" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A21" s="70">
+        <f>A20+1</f>
+        <v>1</v>
+      </c>
+      <c r="B21" s="314"/>
+      <c r="C21" s="244"/>
+      <c r="D21" s="244"/>
+      <c r="E21" s="244"/>
+      <c r="F21" s="244"/>
+      <c r="G21" s="244"/>
+      <c r="H21" s="342"/>
+      <c r="I21" s="244"/>
+      <c r="J21" s="244"/>
+      <c r="K21" s="342"/>
+      <c r="L21" s="244"/>
+      <c r="M21" s="244"/>
+      <c r="N21" s="244"/>
+      <c r="O21" s="244"/>
+      <c r="P21" s="244"/>
+      <c r="Q21" s="315"/>
+      <c r="S21" s="70">
+        <f>S20+1</f>
+        <v>1</v>
+      </c>
+      <c r="T21" s="314"/>
+      <c r="U21" s="244"/>
+      <c r="V21" s="244"/>
+      <c r="W21" s="244"/>
+      <c r="X21" s="244"/>
+      <c r="Y21" s="244"/>
+      <c r="Z21" s="244"/>
+      <c r="AA21" s="244"/>
+      <c r="AB21" s="244"/>
+      <c r="AC21" s="244"/>
+      <c r="AD21" s="244"/>
+      <c r="AE21" s="244"/>
+      <c r="AF21" s="244"/>
+      <c r="AG21" s="244"/>
+      <c r="AH21" s="244"/>
+      <c r="AI21" s="315"/>
+      <c r="AK21" s="70">
+        <f>AK20+1</f>
+        <v>1</v>
+      </c>
+      <c r="AL21" s="314"/>
+      <c r="AM21" s="244"/>
+      <c r="AN21" s="244"/>
+      <c r="AO21" s="244"/>
+      <c r="AP21" s="244"/>
+      <c r="AQ21" s="244"/>
+      <c r="AR21" s="244"/>
+      <c r="AS21" s="244"/>
+      <c r="AT21" s="244"/>
+      <c r="AU21" s="244"/>
+      <c r="AV21" s="244"/>
+      <c r="AW21" s="244"/>
+      <c r="AX21" s="244"/>
+      <c r="AY21" s="244"/>
+      <c r="AZ21" s="244"/>
+      <c r="BA21" s="315"/>
+    </row>
+    <row r="22" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A22" s="70">
+        <f t="shared" ref="A22:A35" si="79">A21+1</f>
+        <v>2</v>
+      </c>
+      <c r="B22" s="314"/>
+      <c r="C22" s="244"/>
+      <c r="D22" s="244"/>
+      <c r="E22" s="244"/>
+      <c r="F22" s="244"/>
+      <c r="G22" s="244"/>
+      <c r="H22" s="342"/>
+      <c r="I22" s="244"/>
+      <c r="J22" s="244"/>
+      <c r="K22" s="342"/>
+      <c r="L22" s="244"/>
+      <c r="M22" s="244"/>
+      <c r="N22" s="244"/>
+      <c r="O22" s="244"/>
+      <c r="P22" s="244"/>
+      <c r="Q22" s="26"/>
+      <c r="S22" s="70">
+        <f t="shared" ref="S22:S35" si="80">S21+1</f>
+        <v>2</v>
+      </c>
+      <c r="T22" s="314"/>
+      <c r="U22" s="244"/>
+      <c r="V22" s="244"/>
+      <c r="W22" s="244"/>
+      <c r="X22" s="244"/>
+      <c r="Y22" s="244"/>
+      <c r="Z22" s="244"/>
+      <c r="AA22" s="244"/>
+      <c r="AB22" s="244"/>
+      <c r="AC22" s="244"/>
+      <c r="AD22" s="244"/>
+      <c r="AE22" s="244"/>
+      <c r="AF22" s="244"/>
+      <c r="AG22" s="244"/>
+      <c r="AH22" s="244"/>
+      <c r="AI22" s="26"/>
+      <c r="AK22" s="70">
+        <f t="shared" ref="AK22:AK35" si="81">AK21+1</f>
+        <v>2</v>
+      </c>
+      <c r="AL22" s="314"/>
+      <c r="AM22" s="244"/>
+      <c r="AN22" s="244"/>
+      <c r="AO22" s="244"/>
+      <c r="AP22" s="244"/>
+      <c r="AQ22" s="244"/>
+      <c r="AR22" s="244"/>
+      <c r="AS22" s="244"/>
+      <c r="AT22" s="244"/>
+      <c r="AU22" s="244"/>
+      <c r="AV22" s="244"/>
+      <c r="AW22" s="244"/>
+      <c r="AX22" s="244"/>
+      <c r="AY22" s="244"/>
+      <c r="AZ22" s="244"/>
+      <c r="BA22" s="26"/>
+    </row>
+    <row r="23" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A23" s="70">
+        <f t="shared" si="79"/>
+        <v>3</v>
+      </c>
+      <c r="B23" s="314"/>
+      <c r="C23" s="244"/>
+      <c r="D23" s="244"/>
+      <c r="E23" s="244"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="219"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="219"/>
+      <c r="L23" s="244"/>
+      <c r="M23" s="244"/>
+      <c r="N23" s="244"/>
+      <c r="O23" s="244"/>
+      <c r="P23" s="244"/>
+      <c r="Q23" s="26"/>
+      <c r="S23" s="70">
+        <f t="shared" si="80"/>
+        <v>3</v>
+      </c>
+      <c r="T23" s="314"/>
+      <c r="U23" s="244"/>
+      <c r="V23" s="244"/>
+      <c r="W23" s="244"/>
+      <c r="X23" s="17"/>
+      <c r="Y23" s="17"/>
+      <c r="Z23" s="17"/>
+      <c r="AA23" s="17"/>
+      <c r="AB23" s="17"/>
+      <c r="AC23" s="17"/>
+      <c r="AD23" s="244"/>
+      <c r="AE23" s="244"/>
+      <c r="AF23" s="244"/>
+      <c r="AG23" s="244"/>
+      <c r="AH23" s="244"/>
+      <c r="AI23" s="26"/>
+      <c r="AK23" s="70">
+        <f t="shared" si="81"/>
+        <v>3</v>
+      </c>
+      <c r="AL23" s="314"/>
+      <c r="AM23" s="244"/>
+      <c r="AN23" s="244"/>
+      <c r="AO23" s="244"/>
+      <c r="AP23" s="17"/>
+      <c r="AQ23" s="17"/>
+      <c r="AR23" s="17"/>
+      <c r="AS23" s="17"/>
+      <c r="AT23" s="17"/>
+      <c r="AU23" s="17"/>
+      <c r="AV23" s="244"/>
+      <c r="AW23" s="244"/>
+      <c r="AX23" s="244"/>
+      <c r="AY23" s="244"/>
+      <c r="AZ23" s="244"/>
+      <c r="BA23" s="26"/>
+    </row>
+    <row r="24" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A24" s="70">
+        <f t="shared" si="79"/>
+        <v>4</v>
+      </c>
+      <c r="B24" s="314"/>
+      <c r="C24" s="244"/>
+      <c r="D24" s="244"/>
+      <c r="E24" s="244"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="342"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="219"/>
+      <c r="L24" s="244"/>
+      <c r="M24" s="244"/>
+      <c r="N24" s="244"/>
+      <c r="O24" s="244"/>
+      <c r="P24" s="244"/>
+      <c r="Q24" s="26"/>
+      <c r="S24" s="70">
+        <f t="shared" si="80"/>
+        <v>4</v>
+      </c>
+      <c r="T24" s="314"/>
+      <c r="U24" s="244"/>
+      <c r="V24" s="244"/>
+      <c r="W24" s="244"/>
+      <c r="X24" s="17"/>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="244"/>
+      <c r="AA24" s="17"/>
+      <c r="AB24" s="17"/>
+      <c r="AC24" s="17"/>
+      <c r="AD24" s="244"/>
+      <c r="AE24" s="244"/>
+      <c r="AF24" s="244"/>
+      <c r="AG24" s="244"/>
+      <c r="AH24" s="244"/>
+      <c r="AI24" s="26"/>
+      <c r="AK24" s="70">
+        <f t="shared" si="81"/>
+        <v>4</v>
+      </c>
+      <c r="AL24" s="314"/>
+      <c r="AM24" s="244"/>
+      <c r="AN24" s="244"/>
+      <c r="AO24" s="244"/>
+      <c r="AP24" s="17"/>
+      <c r="AQ24" s="17"/>
+      <c r="AR24" s="244"/>
+      <c r="AS24" s="17"/>
+      <c r="AT24" s="17"/>
+      <c r="AU24" s="17"/>
+      <c r="AV24" s="244"/>
+      <c r="AW24" s="244"/>
+      <c r="AX24" s="244"/>
+      <c r="AY24" s="244"/>
+      <c r="AZ24" s="244"/>
+      <c r="BA24" s="26"/>
+    </row>
+    <row r="25" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A25" s="70">
+        <f t="shared" si="79"/>
+        <v>5</v>
+      </c>
+      <c r="B25" s="314"/>
+      <c r="C25" s="244"/>
+      <c r="D25" s="244"/>
+      <c r="E25" s="244"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="219"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="219"/>
+      <c r="L25" s="244"/>
+      <c r="M25" s="244"/>
+      <c r="N25" s="244"/>
+      <c r="O25" s="244"/>
+      <c r="P25" s="244"/>
+      <c r="Q25" s="26"/>
+      <c r="S25" s="70">
+        <f t="shared" si="80"/>
+        <v>5</v>
+      </c>
+      <c r="T25" s="314"/>
+      <c r="U25" s="244"/>
+      <c r="V25" s="244"/>
+      <c r="W25" s="244"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="17"/>
+      <c r="AA25" s="17"/>
+      <c r="AB25" s="17"/>
+      <c r="AC25" s="17"/>
+      <c r="AD25" s="244"/>
+      <c r="AE25" s="244"/>
+      <c r="AF25" s="244"/>
+      <c r="AG25" s="244"/>
+      <c r="AH25" s="244"/>
+      <c r="AI25" s="26"/>
+      <c r="AK25" s="70">
+        <f t="shared" si="81"/>
+        <v>5</v>
+      </c>
+      <c r="AL25" s="314"/>
+      <c r="AM25" s="244"/>
+      <c r="AN25" s="244"/>
+      <c r="AO25" s="244"/>
+      <c r="AP25" s="17"/>
+      <c r="AQ25" s="17"/>
+      <c r="AR25" s="17"/>
+      <c r="AS25" s="17"/>
+      <c r="AT25" s="17"/>
+      <c r="AU25" s="17"/>
+      <c r="AV25" s="244"/>
+      <c r="AW25" s="244"/>
+      <c r="AX25" s="244"/>
+      <c r="AY25" s="244"/>
+      <c r="AZ25" s="244"/>
+      <c r="BA25" s="26"/>
+    </row>
+    <row r="26" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A26" s="70">
+        <f t="shared" si="79"/>
+        <v>6</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="219"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="219"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="26"/>
+      <c r="S26" s="70">
+        <f t="shared" si="80"/>
+        <v>6</v>
+      </c>
+      <c r="T26" s="308"/>
+      <c r="U26" s="219"/>
+      <c r="V26" s="219"/>
+      <c r="W26" s="219"/>
+      <c r="X26" s="219"/>
+      <c r="Y26" s="219"/>
+      <c r="Z26" s="219"/>
+      <c r="AA26" s="17"/>
+      <c r="AB26" s="17"/>
+      <c r="AC26" s="219"/>
+      <c r="AD26" s="219"/>
+      <c r="AE26" s="219"/>
+      <c r="AF26" s="219"/>
+      <c r="AG26" s="219"/>
+      <c r="AH26" s="219"/>
+      <c r="AI26" s="309"/>
+      <c r="AK26" s="70">
+        <f t="shared" si="81"/>
+        <v>6</v>
+      </c>
+      <c r="AL26" s="16"/>
+      <c r="AM26" s="17"/>
+      <c r="AN26" s="17"/>
+      <c r="AO26" s="17"/>
+      <c r="AP26" s="17"/>
+      <c r="AQ26" s="17"/>
+      <c r="AR26" s="17"/>
+      <c r="AS26" s="17"/>
+      <c r="AT26" s="17"/>
+      <c r="AU26" s="17"/>
+      <c r="AV26" s="17"/>
+      <c r="AW26" s="17"/>
+      <c r="AX26" s="17"/>
+      <c r="AY26" s="17"/>
+      <c r="AZ26" s="17"/>
+      <c r="BA26" s="26"/>
+    </row>
+    <row r="27" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A27" s="70">
+        <f t="shared" si="79"/>
+        <v>7</v>
+      </c>
+      <c r="B27" s="314"/>
+      <c r="C27" s="244"/>
+      <c r="D27" s="244"/>
+      <c r="E27" s="244"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="244"/>
+      <c r="M27" s="244"/>
+      <c r="N27" s="244"/>
+      <c r="O27" s="244"/>
+      <c r="P27" s="244"/>
+      <c r="Q27" s="315"/>
+      <c r="S27" s="70">
+        <f t="shared" si="80"/>
+        <v>7</v>
+      </c>
+      <c r="T27" s="314"/>
+      <c r="U27" s="244"/>
+      <c r="V27" s="244"/>
+      <c r="W27" s="244"/>
+      <c r="X27" s="17"/>
+      <c r="Y27" s="17"/>
+      <c r="Z27" s="17"/>
+      <c r="AA27" s="17"/>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="17"/>
+      <c r="AD27" s="244"/>
+      <c r="AE27" s="244"/>
+      <c r="AF27" s="244"/>
+      <c r="AG27" s="244"/>
+      <c r="AH27" s="244"/>
+      <c r="AI27" s="315"/>
+      <c r="AK27" s="70">
+        <f t="shared" si="81"/>
+        <v>7</v>
+      </c>
+      <c r="AL27" s="314"/>
+      <c r="AM27" s="244"/>
+      <c r="AN27" s="244"/>
+      <c r="AO27" s="244"/>
+      <c r="AP27" s="17"/>
+      <c r="AQ27" s="17"/>
+      <c r="AR27" s="17"/>
+      <c r="AS27" s="17"/>
+      <c r="AT27" s="17"/>
+      <c r="AU27" s="17"/>
+      <c r="AV27" s="244"/>
+      <c r="AW27" s="244"/>
+      <c r="AX27" s="244"/>
+      <c r="AY27" s="244"/>
+      <c r="AZ27" s="244"/>
+      <c r="BA27" s="315"/>
+    </row>
+    <row r="28" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A28" s="70">
+        <f t="shared" si="79"/>
+        <v>8</v>
+      </c>
+      <c r="B28" s="314"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="244"/>
+      <c r="P28" s="244"/>
+      <c r="Q28" s="315"/>
+      <c r="S28" s="70">
+        <f t="shared" si="80"/>
+        <v>8</v>
+      </c>
+      <c r="T28" s="314"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="17"/>
+      <c r="AC28" s="17"/>
+      <c r="AD28" s="17"/>
+      <c r="AE28" s="17"/>
+      <c r="AF28" s="17"/>
+      <c r="AG28" s="244"/>
+      <c r="AH28" s="244"/>
+      <c r="AI28" s="315"/>
+      <c r="AK28" s="70">
+        <f t="shared" si="81"/>
+        <v>8</v>
+      </c>
+      <c r="AL28" s="314"/>
+      <c r="AM28" s="17"/>
+      <c r="AN28" s="17"/>
+      <c r="AO28" s="17"/>
+      <c r="AP28" s="17"/>
+      <c r="AQ28" s="17"/>
+      <c r="AR28" s="17"/>
+      <c r="AS28" s="17"/>
+      <c r="AT28" s="17"/>
+      <c r="AU28" s="17"/>
+      <c r="AV28" s="17"/>
+      <c r="AW28" s="17"/>
+      <c r="AX28" s="17"/>
+      <c r="AY28" s="244"/>
+      <c r="AZ28" s="244"/>
+      <c r="BA28" s="315"/>
+    </row>
+    <row r="29" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A29" s="70">
+        <f t="shared" si="79"/>
+        <v>9</v>
+      </c>
+      <c r="B29" s="314"/>
+      <c r="C29" s="244"/>
+      <c r="D29" s="244"/>
+      <c r="E29" s="244"/>
+      <c r="F29" s="244"/>
+      <c r="G29" s="244"/>
+      <c r="H29" s="342"/>
+      <c r="I29" s="244"/>
+      <c r="J29" s="244"/>
+      <c r="K29" s="342"/>
+      <c r="L29" s="244"/>
+      <c r="M29" s="244"/>
+      <c r="N29" s="244"/>
+      <c r="O29" s="244"/>
+      <c r="P29" s="244"/>
+      <c r="Q29" s="315"/>
+      <c r="S29" s="70">
+        <f t="shared" si="80"/>
+        <v>9</v>
+      </c>
+      <c r="T29" s="383"/>
+      <c r="U29" s="342"/>
+      <c r="V29" s="342"/>
+      <c r="W29" s="342"/>
+      <c r="X29" s="342"/>
+      <c r="Y29" s="342"/>
+      <c r="Z29" s="342"/>
+      <c r="AA29" s="244"/>
+      <c r="AB29" s="244"/>
+      <c r="AC29" s="342"/>
+      <c r="AD29" s="342"/>
+      <c r="AE29" s="342"/>
+      <c r="AF29" s="342"/>
+      <c r="AG29" s="342"/>
+      <c r="AH29" s="342"/>
+      <c r="AI29" s="352"/>
+      <c r="AK29" s="70">
+        <f t="shared" si="81"/>
+        <v>9</v>
+      </c>
+      <c r="AL29" s="314"/>
+      <c r="AM29" s="244"/>
+      <c r="AN29" s="244"/>
+      <c r="AO29" s="244"/>
+      <c r="AP29" s="244"/>
+      <c r="AQ29" s="244"/>
+      <c r="AR29" s="244"/>
+      <c r="AS29" s="244"/>
+      <c r="AT29" s="244"/>
+      <c r="AU29" s="244"/>
+      <c r="AV29" s="244"/>
+      <c r="AW29" s="244"/>
+      <c r="AX29" s="244"/>
+      <c r="AY29" s="244"/>
+      <c r="AZ29" s="244"/>
+      <c r="BA29" s="315"/>
+    </row>
+    <row r="30" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A30" s="70">
+        <f t="shared" si="79"/>
+        <v>10</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="244"/>
+      <c r="D30" s="244"/>
+      <c r="E30" s="244"/>
+      <c r="F30" s="244"/>
+      <c r="G30" s="244"/>
+      <c r="H30" s="342"/>
+      <c r="I30" s="244"/>
+      <c r="J30" s="244"/>
+      <c r="K30" s="342"/>
+      <c r="L30" s="244"/>
+      <c r="M30" s="244"/>
+      <c r="N30" s="244"/>
+      <c r="O30" s="244"/>
+      <c r="P30" s="244"/>
+      <c r="Q30" s="26"/>
+      <c r="S30" s="70">
+        <f t="shared" si="80"/>
+        <v>10</v>
+      </c>
+      <c r="T30" s="16"/>
+      <c r="U30" s="244"/>
+      <c r="V30" s="244"/>
+      <c r="W30" s="244"/>
+      <c r="X30" s="244"/>
+      <c r="Y30" s="244"/>
+      <c r="Z30" s="244"/>
+      <c r="AA30" s="244"/>
+      <c r="AB30" s="244"/>
+      <c r="AC30" s="244"/>
+      <c r="AD30" s="244"/>
+      <c r="AE30" s="244"/>
+      <c r="AF30" s="244"/>
+      <c r="AG30" s="244"/>
+      <c r="AH30" s="244"/>
+      <c r="AI30" s="26"/>
+      <c r="AK30" s="70">
+        <f t="shared" si="81"/>
+        <v>10</v>
+      </c>
+      <c r="AL30" s="16"/>
+      <c r="AM30" s="244"/>
+      <c r="AN30" s="244"/>
+      <c r="AO30" s="244"/>
+      <c r="AP30" s="244"/>
+      <c r="AQ30" s="244"/>
+      <c r="AR30" s="244"/>
+      <c r="AS30" s="244"/>
+      <c r="AT30" s="244"/>
+      <c r="AU30" s="244"/>
+      <c r="AV30" s="244"/>
+      <c r="AW30" s="244"/>
+      <c r="AX30" s="244"/>
+      <c r="AY30" s="244"/>
+      <c r="AZ30" s="244"/>
+      <c r="BA30" s="26"/>
+    </row>
+    <row r="31" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A31" s="70">
+        <f t="shared" si="79"/>
+        <v>11</v>
+      </c>
+      <c r="B31" s="314"/>
+      <c r="C31" s="244"/>
+      <c r="D31" s="244"/>
+      <c r="E31" s="244"/>
+      <c r="F31" s="244"/>
+      <c r="G31" s="244"/>
+      <c r="H31" s="342"/>
+      <c r="I31" s="244"/>
+      <c r="J31" s="244"/>
+      <c r="K31" s="342"/>
+      <c r="L31" s="244"/>
+      <c r="M31" s="244"/>
+      <c r="N31" s="244"/>
+      <c r="O31" s="244"/>
+      <c r="P31" s="244"/>
+      <c r="Q31" s="26"/>
+      <c r="S31" s="70">
+        <f t="shared" si="80"/>
+        <v>11</v>
+      </c>
+      <c r="T31" s="314"/>
+      <c r="U31" s="244"/>
+      <c r="V31" s="244"/>
+      <c r="W31" s="244"/>
+      <c r="X31" s="244"/>
+      <c r="Y31" s="244"/>
+      <c r="Z31" s="244"/>
+      <c r="AA31" s="244"/>
+      <c r="AB31" s="244"/>
+      <c r="AC31" s="244"/>
+      <c r="AD31" s="244"/>
+      <c r="AE31" s="244"/>
+      <c r="AF31" s="244"/>
+      <c r="AG31" s="244"/>
+      <c r="AH31" s="244"/>
+      <c r="AI31" s="26"/>
+      <c r="AK31" s="70">
+        <f t="shared" si="81"/>
+        <v>11</v>
+      </c>
+      <c r="AL31" s="314"/>
+      <c r="AM31" s="244"/>
+      <c r="AN31" s="244"/>
+      <c r="AO31" s="244"/>
+      <c r="AP31" s="244"/>
+      <c r="AQ31" s="244"/>
+      <c r="AR31" s="244"/>
+      <c r="AS31" s="244"/>
+      <c r="AT31" s="244"/>
+      <c r="AU31" s="244"/>
+      <c r="AV31" s="244"/>
+      <c r="AW31" s="244"/>
+      <c r="AX31" s="244"/>
+      <c r="AY31" s="244"/>
+      <c r="AZ31" s="244"/>
+      <c r="BA31" s="26"/>
+    </row>
+    <row r="32" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A32" s="70">
+        <f t="shared" si="79"/>
+        <v>12</v>
+      </c>
+      <c r="B32" s="314"/>
+      <c r="C32" s="244"/>
+      <c r="D32" s="244"/>
+      <c r="E32" s="244"/>
+      <c r="F32" s="244"/>
+      <c r="G32" s="244"/>
+      <c r="H32" s="342"/>
+      <c r="I32" s="244"/>
+      <c r="J32" s="244"/>
+      <c r="K32" s="342"/>
+      <c r="L32" s="244"/>
+      <c r="M32" s="244"/>
+      <c r="N32" s="244"/>
+      <c r="O32" s="244"/>
+      <c r="P32" s="244"/>
+      <c r="Q32" s="26"/>
+      <c r="S32" s="70">
+        <f t="shared" si="80"/>
+        <v>12</v>
+      </c>
+      <c r="T32" s="314"/>
+      <c r="U32" s="244"/>
+      <c r="V32" s="244"/>
+      <c r="W32" s="244"/>
+      <c r="X32" s="244"/>
+      <c r="Y32" s="244"/>
+      <c r="Z32" s="244"/>
+      <c r="AA32" s="244"/>
+      <c r="AB32" s="244"/>
+      <c r="AC32" s="244"/>
+      <c r="AD32" s="244"/>
+      <c r="AE32" s="244"/>
+      <c r="AF32" s="244"/>
+      <c r="AG32" s="244"/>
+      <c r="AH32" s="244"/>
+      <c r="AI32" s="26"/>
+      <c r="AK32" s="70">
+        <f t="shared" si="81"/>
+        <v>12</v>
+      </c>
+      <c r="AL32" s="314"/>
+      <c r="AM32" s="244"/>
+      <c r="AN32" s="244"/>
+      <c r="AO32" s="244"/>
+      <c r="AP32" s="244"/>
+      <c r="AQ32" s="244"/>
+      <c r="AR32" s="244"/>
+      <c r="AS32" s="244"/>
+      <c r="AT32" s="244"/>
+      <c r="AU32" s="244"/>
+      <c r="AV32" s="244"/>
+      <c r="AW32" s="244"/>
+      <c r="AX32" s="244"/>
+      <c r="AY32" s="244"/>
+      <c r="AZ32" s="244"/>
+      <c r="BA32" s="26"/>
+    </row>
+    <row r="33" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A33" s="70">
+        <f t="shared" si="79"/>
+        <v>13</v>
+      </c>
+      <c r="B33" s="314"/>
+      <c r="C33" s="244"/>
+      <c r="D33" s="244"/>
+      <c r="E33" s="244"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="219"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="219"/>
+      <c r="L33" s="244"/>
+      <c r="M33" s="244"/>
+      <c r="N33" s="244"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="26"/>
+      <c r="S33" s="70">
+        <f t="shared" si="80"/>
+        <v>13</v>
+      </c>
+      <c r="T33" s="314"/>
+      <c r="U33" s="244"/>
+      <c r="V33" s="244"/>
+      <c r="W33" s="244"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="17"/>
+      <c r="Z33" s="17"/>
+      <c r="AA33" s="17"/>
+      <c r="AB33" s="17"/>
+      <c r="AC33" s="17"/>
+      <c r="AD33" s="244"/>
+      <c r="AE33" s="244"/>
+      <c r="AF33" s="244"/>
+      <c r="AG33" s="17"/>
+      <c r="AH33" s="17"/>
+      <c r="AI33" s="26"/>
+      <c r="AK33" s="70">
+        <f t="shared" si="81"/>
+        <v>13</v>
+      </c>
+      <c r="AL33" s="314"/>
+      <c r="AM33" s="244"/>
+      <c r="AN33" s="244"/>
+      <c r="AO33" s="244"/>
+      <c r="AP33" s="17"/>
+      <c r="AQ33" s="17"/>
+      <c r="AR33" s="17"/>
+      <c r="AS33" s="17"/>
+      <c r="AT33" s="17"/>
+      <c r="AU33" s="17"/>
+      <c r="AV33" s="244"/>
+      <c r="AW33" s="244"/>
+      <c r="AX33" s="244"/>
+      <c r="AY33" s="17"/>
+      <c r="AZ33" s="17"/>
+      <c r="BA33" s="26"/>
+    </row>
+    <row r="34" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A34" s="70">
+        <f t="shared" si="79"/>
+        <v>14</v>
+      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="219"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="219"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="26"/>
+      <c r="S34" s="70">
+        <f t="shared" si="80"/>
+        <v>14</v>
+      </c>
+      <c r="T34" s="16"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="17"/>
+      <c r="Z34" s="17"/>
+      <c r="AA34" s="17"/>
+      <c r="AB34" s="17"/>
+      <c r="AC34" s="17"/>
+      <c r="AD34" s="17"/>
+      <c r="AE34" s="17"/>
+      <c r="AF34" s="17"/>
+      <c r="AG34" s="17"/>
+      <c r="AH34" s="17"/>
+      <c r="AI34" s="26"/>
+      <c r="AK34" s="70">
+        <f t="shared" si="81"/>
+        <v>14</v>
+      </c>
+      <c r="AL34" s="16"/>
+      <c r="AM34" s="17"/>
+      <c r="AN34" s="17"/>
+      <c r="AO34" s="17"/>
+      <c r="AP34" s="17"/>
+      <c r="AQ34" s="17"/>
+      <c r="AR34" s="17"/>
+      <c r="AS34" s="17"/>
+      <c r="AT34" s="17"/>
+      <c r="AU34" s="17"/>
+      <c r="AV34" s="17"/>
+      <c r="AW34" s="17"/>
+      <c r="AX34" s="17"/>
+      <c r="AY34" s="17"/>
+      <c r="AZ34" s="17"/>
+      <c r="BA34" s="26"/>
+    </row>
+    <row r="35" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A35" s="70">
+        <f t="shared" si="79"/>
+        <v>15</v>
+      </c>
+      <c r="B35" s="32"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="412"/>
+      <c r="I35" s="317"/>
+      <c r="J35" s="317"/>
+      <c r="K35" s="412"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="33"/>
+      <c r="S35" s="70">
+        <f t="shared" si="80"/>
+        <v>15</v>
+      </c>
+      <c r="T35" s="32"/>
+      <c r="U35" s="22"/>
+      <c r="V35" s="22"/>
+      <c r="W35" s="22"/>
+      <c r="X35" s="22"/>
+      <c r="Y35" s="22"/>
+      <c r="Z35" s="317"/>
+      <c r="AA35" s="317"/>
+      <c r="AB35" s="317"/>
+      <c r="AC35" s="317"/>
+      <c r="AD35" s="22"/>
+      <c r="AE35" s="22"/>
+      <c r="AF35" s="22"/>
+      <c r="AG35" s="22"/>
+      <c r="AH35" s="22"/>
+      <c r="AI35" s="33"/>
+      <c r="AK35" s="70">
+        <f t="shared" si="81"/>
+        <v>15</v>
+      </c>
+      <c r="AL35" s="32"/>
+      <c r="AM35" s="22"/>
+      <c r="AN35" s="22"/>
+      <c r="AO35" s="22"/>
+      <c r="AP35" s="22"/>
+      <c r="AQ35" s="22"/>
+      <c r="AR35" s="317"/>
+      <c r="AS35" s="317"/>
+      <c r="AT35" s="317"/>
+      <c r="AU35" s="317"/>
+      <c r="AV35" s="22"/>
+      <c r="AW35" s="22"/>
+      <c r="AX35" s="22"/>
+      <c r="AY35" s="22"/>
+      <c r="AZ35" s="22"/>
+      <c r="BA35" s="33"/>
+    </row>
+    <row r="36" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A36" s="242" t="s">
+        <v>395</v>
+      </c>
+      <c r="S36" s="242" t="s">
+        <v>395</v>
+      </c>
+      <c r="AK36" s="242" t="s">
+        <v>395</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed numerous snow and foliage generation issues (above tunnels, bunkers and around radio towers) Now generating ladders up the radio tower bases
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="31" activeTab="41"/>
+    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="21" activeTab="41"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -3639,7 +3639,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:N15" ca="1" si="7">IF(AND(MOD(E$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="Y6">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4229,7 +4229,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4249,7 +4249,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4269,7 +4269,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4289,7 +4289,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4779,7 +4779,7 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:N29" ca="1" si="11">IF(AND(MOD(E$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4799,7 +4799,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4819,7 +4819,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4859,7 +4859,7 @@
       </c>
       <c r="Y16">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5429,7 +5429,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5919,7 +5919,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5979,7 +5979,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>

</xml_diff>

<commit_message>
Renamed a few files to make them clearer as to what they do Added a mine entrance but it is pretty darn rare Added IncludeSeas and IncludeMountains to allow folks to turn them off Fixed a few option permutation issues
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="21" activeTab="41"/>
+    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="21" activeTab="38"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -1451,7 +1451,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="50">
+  <fills count="51">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1746,6 +1746,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -1941,7 +1947,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="413">
+  <cellXfs count="427">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2653,6 +2659,40 @@
     <xf numFmtId="0" fontId="0" fillId="31" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3639,7 +3679,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:N15" ca="1" si="7">IF(AND(MOD(E$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3659,7 +3699,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3679,7 +3719,7 @@
       </c>
       <c r="O6">
         <f t="shared" ref="O6:AB15" ca="1" si="8">IF(AND(MOD(O$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3719,7 +3759,7 @@
       </c>
       <c r="Y6">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4229,7 +4269,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4249,7 +4289,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4269,7 +4309,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4779,7 +4819,7 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:N29" ca="1" si="11">IF(AND(MOD(E$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4839,7 +4879,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5389,7 +5429,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5409,7 +5449,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5429,7 +5469,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5959,7 +5999,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5979,7 +6019,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5999,7 +6039,7 @@
       </c>
       <c r="Y26">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -53196,15 +53236,15 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CL37"/>
+  <dimension ref="A1:BT37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:R37"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:90" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A1" s="242"/>
       <c r="B1" s="70">
         <v>0</v>
@@ -53341,11 +53381,11 @@
         <v>0</v>
       </c>
       <c r="AN1">
-        <f t="shared" ref="AN1:BB1" si="2">AM1+1</f>
+        <f>AM1+1</f>
         <v>1</v>
       </c>
       <c r="AO1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AO1:BB1" si="2">AN1+1</f>
         <v>2</v>
       </c>
       <c r="AP1">
@@ -53463,71 +53503,8 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="BW1">
-        <v>0</v>
-      </c>
-      <c r="BX1">
-        <f>BW1+1</f>
-        <v>1</v>
-      </c>
-      <c r="BY1">
-        <f t="shared" ref="BY1:CL1" si="4">BX1+1</f>
-        <v>2</v>
-      </c>
-      <c r="BZ1">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="CA1">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="CB1">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="CC1">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="CD1">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="CE1">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="CF1">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="CG1">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="CH1">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="CI1">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="CJ1">
-        <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="CK1">
-        <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="CL1">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A2" s="70">
         <v>0</v>
       </c>
@@ -53570,8 +53547,8 @@
         <v>0</v>
       </c>
       <c r="AL2">
-        <f t="shared" ref="AL2:AL31" si="5">AL3+1</f>
-        <v>31</v>
+        <f t="shared" ref="AL2:AL31" si="4">AL3+1</f>
+        <v>47</v>
       </c>
       <c r="AM2" s="1"/>
       <c r="AN2" s="2"/>
@@ -53590,8 +53567,7 @@
       <c r="BA2" s="2"/>
       <c r="BB2" s="5"/>
       <c r="BD2">
-        <f t="shared" ref="BD2:BD31" si="6">BD3+1</f>
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="BE2" s="1"/>
       <c r="BF2" s="2"/>
@@ -53609,33 +53585,14 @@
       <c r="BR2" s="2"/>
       <c r="BS2" s="2"/>
       <c r="BT2" s="5"/>
-      <c r="BV2">
-        <v>0</v>
-      </c>
-      <c r="BW2" s="1"/>
-      <c r="BX2" s="2"/>
-      <c r="BY2" s="2"/>
-      <c r="BZ2" s="2"/>
-      <c r="CA2" s="2"/>
-      <c r="CB2" s="2"/>
-      <c r="CC2" s="20"/>
-      <c r="CD2" s="20"/>
-      <c r="CE2" s="20"/>
-      <c r="CF2" s="20"/>
-      <c r="CG2" s="2"/>
-      <c r="CH2" s="2"/>
-      <c r="CI2" s="2"/>
-      <c r="CJ2" s="2"/>
-      <c r="CK2" s="2"/>
-      <c r="CL2" s="5"/>
-    </row>
-    <row r="3" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A3" s="70">
         <f>A2+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="314"/>
-      <c r="C3" s="244"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="244"/>
       <c r="E3" s="244"/>
       <c r="F3" s="244"/>
@@ -53675,8 +53632,8 @@
         <v>1</v>
       </c>
       <c r="AL3">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="4"/>
+        <v>46</v>
       </c>
       <c r="AM3" s="10"/>
       <c r="AN3" s="6"/>
@@ -53695,8 +53652,8 @@
       <c r="BA3" s="6"/>
       <c r="BB3" s="9"/>
       <c r="BD3">
-        <f t="shared" si="6"/>
-        <v>46</v>
+        <f>BD2+1</f>
+        <v>1</v>
       </c>
       <c r="BE3" s="10"/>
       <c r="BF3" s="6"/>
@@ -53714,34 +53671,14 @@
       <c r="BR3" s="6"/>
       <c r="BS3" s="6"/>
       <c r="BT3" s="9"/>
-      <c r="BV3">
-        <f>BV2+1</f>
-        <v>1</v>
-      </c>
-      <c r="BW3" s="10"/>
-      <c r="BX3" s="6"/>
-      <c r="BY3" s="6"/>
-      <c r="BZ3" s="6"/>
-      <c r="CA3" s="6"/>
-      <c r="CB3" s="6"/>
-      <c r="CC3" s="17"/>
-      <c r="CD3" s="17"/>
-      <c r="CE3" s="17"/>
-      <c r="CF3" s="17"/>
-      <c r="CG3" s="6"/>
-      <c r="CH3" s="6"/>
-      <c r="CI3" s="6"/>
-      <c r="CJ3" s="6"/>
-      <c r="CK3" s="6"/>
-      <c r="CL3" s="9"/>
-    </row>
-    <row r="4" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A4" s="70">
-        <f t="shared" ref="A4:A17" si="7">A3+1</f>
+        <f t="shared" ref="A4:A17" si="5">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="314"/>
-      <c r="C4" s="244"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="244"/>
       <c r="E4" s="244"/>
       <c r="F4" s="244"/>
@@ -53757,7 +53694,7 @@
       <c r="P4" s="244"/>
       <c r="Q4" s="315"/>
       <c r="S4" s="70">
-        <f t="shared" ref="S4:S17" si="8">S3+1</f>
+        <f t="shared" ref="S4:S17" si="6">S3+1</f>
         <v>2</v>
       </c>
       <c r="T4" s="314"/>
@@ -53777,12 +53714,12 @@
       <c r="AH4" s="244"/>
       <c r="AI4" s="9"/>
       <c r="AJ4" s="70">
-        <f t="shared" ref="AJ4:AJ17" si="9">AJ3+1</f>
+        <f t="shared" ref="AJ4:AJ17" si="7">AJ3+1</f>
         <v>2</v>
       </c>
       <c r="AL4">
-        <f t="shared" si="5"/>
-        <v>29</v>
+        <f t="shared" si="4"/>
+        <v>45</v>
       </c>
       <c r="AM4" s="10"/>
       <c r="AN4" s="6"/>
@@ -53801,15 +53738,15 @@
       <c r="BA4" s="6"/>
       <c r="BB4" s="9"/>
       <c r="BD4">
-        <f t="shared" si="6"/>
-        <v>45</v>
+        <f t="shared" ref="BD4:BD17" si="8">BD3+1</f>
+        <v>2</v>
       </c>
       <c r="BE4" s="10"/>
-      <c r="BF4" s="6"/>
-      <c r="BG4" s="6"/>
-      <c r="BH4" s="6"/>
-      <c r="BI4" s="6"/>
-      <c r="BJ4" s="6"/>
+      <c r="BF4" s="17"/>
+      <c r="BG4" s="17"/>
+      <c r="BH4" s="17"/>
+      <c r="BI4" s="17"/>
+      <c r="BJ4" s="17"/>
       <c r="BK4" s="17"/>
       <c r="BL4" s="17"/>
       <c r="BM4" s="17"/>
@@ -53820,34 +53757,14 @@
       <c r="BR4" s="6"/>
       <c r="BS4" s="6"/>
       <c r="BT4" s="9"/>
-      <c r="BV4">
-        <f t="shared" ref="BV4:BV17" si="10">BV3+1</f>
-        <v>2</v>
-      </c>
-      <c r="BW4" s="10"/>
-      <c r="BX4" s="17"/>
-      <c r="BY4" s="17"/>
-      <c r="BZ4" s="17"/>
-      <c r="CA4" s="17"/>
-      <c r="CB4" s="17"/>
-      <c r="CC4" s="17"/>
-      <c r="CD4" s="17"/>
-      <c r="CE4" s="17"/>
-      <c r="CF4" s="17"/>
-      <c r="CG4" s="6"/>
-      <c r="CH4" s="6"/>
-      <c r="CI4" s="6"/>
-      <c r="CJ4" s="6"/>
-      <c r="CK4" s="6"/>
-      <c r="CL4" s="9"/>
-    </row>
-    <row r="5" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A5" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="B5" s="314"/>
-      <c r="C5" s="244"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="244"/>
       <c r="E5" s="244"/>
       <c r="F5" s="244"/>
@@ -53863,7 +53780,7 @@
       <c r="P5" s="244"/>
       <c r="Q5" s="315"/>
       <c r="S5" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="T5" s="314"/>
@@ -53883,12 +53800,12 @@
       <c r="AH5" s="244"/>
       <c r="AI5" s="9"/>
       <c r="AJ5" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="AL5">
-        <f t="shared" si="5"/>
-        <v>28</v>
+        <f t="shared" si="4"/>
+        <v>44</v>
       </c>
       <c r="AM5" s="10"/>
       <c r="AN5" s="6"/>
@@ -53907,15 +53824,15 @@
       <c r="BA5" s="6"/>
       <c r="BB5" s="9"/>
       <c r="BD5">
-        <f t="shared" si="6"/>
-        <v>44</v>
+        <f t="shared" si="8"/>
+        <v>3</v>
       </c>
       <c r="BE5" s="10"/>
-      <c r="BF5" s="6"/>
-      <c r="BG5" s="6"/>
-      <c r="BH5" s="6"/>
-      <c r="BI5" s="6"/>
-      <c r="BJ5" s="6"/>
+      <c r="BF5" s="17"/>
+      <c r="BG5" s="17"/>
+      <c r="BH5" s="17"/>
+      <c r="BI5" s="17"/>
+      <c r="BJ5" s="17"/>
       <c r="BK5" s="17"/>
       <c r="BL5" s="17"/>
       <c r="BM5" s="17"/>
@@ -53926,38 +53843,18 @@
       <c r="BR5" s="6"/>
       <c r="BS5" s="6"/>
       <c r="BT5" s="9"/>
-      <c r="BV5">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="BW5" s="10"/>
-      <c r="BX5" s="17"/>
-      <c r="BY5" s="17"/>
-      <c r="BZ5" s="17"/>
-      <c r="CA5" s="17"/>
-      <c r="CB5" s="17"/>
-      <c r="CC5" s="17"/>
-      <c r="CD5" s="17"/>
-      <c r="CE5" s="17"/>
-      <c r="CF5" s="17"/>
-      <c r="CG5" s="6"/>
-      <c r="CH5" s="6"/>
-      <c r="CI5" s="6"/>
-      <c r="CJ5" s="6"/>
-      <c r="CK5" s="6"/>
-      <c r="CL5" s="9"/>
-    </row>
-    <row r="6" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A6" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="B6" s="314"/>
-      <c r="C6" s="244"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="244"/>
       <c r="E6" s="244"/>
       <c r="F6" s="244"/>
-      <c r="G6" s="17"/>
+      <c r="G6" s="244"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -53969,7 +53866,7 @@
       <c r="P6" s="244"/>
       <c r="Q6" s="315"/>
       <c r="S6" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="T6" s="314"/>
@@ -53989,12 +53886,12 @@
       <c r="AH6" s="244"/>
       <c r="AI6" s="9"/>
       <c r="AJ6" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AL6">
-        <f t="shared" si="5"/>
-        <v>27</v>
+        <f t="shared" si="4"/>
+        <v>43</v>
       </c>
       <c r="AM6" s="10"/>
       <c r="AN6" s="6"/>
@@ -54013,15 +53910,10 @@
       <c r="BA6" s="6"/>
       <c r="BB6" s="9"/>
       <c r="BD6">
-        <f t="shared" si="6"/>
-        <v>43</v>
+        <f t="shared" si="8"/>
+        <v>4</v>
       </c>
       <c r="BE6" s="10"/>
-      <c r="BF6" s="6"/>
-      <c r="BG6" s="6"/>
-      <c r="BH6" s="6"/>
-      <c r="BI6" s="6"/>
-      <c r="BJ6" s="6"/>
       <c r="BK6" s="17"/>
       <c r="BL6" s="17"/>
       <c r="BM6" s="17"/>
@@ -54032,33 +53924,18 @@
       <c r="BR6" s="6"/>
       <c r="BS6" s="6"/>
       <c r="BT6" s="9"/>
-      <c r="BV6">
-        <f t="shared" si="10"/>
-        <v>4</v>
-      </c>
-      <c r="BW6" s="10"/>
-      <c r="CC6" s="17"/>
-      <c r="CD6" s="17"/>
-      <c r="CE6" s="17"/>
-      <c r="CF6" s="17"/>
-      <c r="CG6" s="6"/>
-      <c r="CH6" s="6"/>
-      <c r="CI6" s="6"/>
-      <c r="CJ6" s="6"/>
-      <c r="CK6" s="6"/>
-      <c r="CL6" s="9"/>
-    </row>
-    <row r="7" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A7" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="B7" s="314"/>
-      <c r="C7" s="244"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="244"/>
       <c r="E7" s="244"/>
       <c r="F7" s="244"/>
-      <c r="G7" s="17"/>
+      <c r="G7" s="244"/>
       <c r="H7" s="17"/>
       <c r="I7" s="244"/>
       <c r="J7" s="17"/>
@@ -54070,7 +53947,7 @@
       <c r="P7" s="244"/>
       <c r="Q7" s="315"/>
       <c r="S7" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="T7" s="314"/>
@@ -54090,12 +53967,12 @@
       <c r="AH7" s="372"/>
       <c r="AI7" s="373"/>
       <c r="AJ7" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="AL7">
-        <f t="shared" si="5"/>
-        <v>26</v>
+        <f t="shared" si="4"/>
+        <v>42</v>
       </c>
       <c r="AM7" s="10"/>
       <c r="AN7" s="6"/>
@@ -54114,47 +53991,27 @@
       <c r="BA7" s="6"/>
       <c r="BB7" s="9"/>
       <c r="BD7">
-        <f t="shared" si="6"/>
-        <v>42</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="BE7" s="10"/>
-      <c r="BF7" s="6"/>
-      <c r="BG7" s="6"/>
-      <c r="BH7" s="6"/>
-      <c r="BI7" s="6"/>
-      <c r="BJ7" s="6"/>
-      <c r="BK7" s="17"/>
-      <c r="BL7" s="17"/>
-      <c r="BM7" s="17"/>
-      <c r="BN7" s="17"/>
-      <c r="BO7" s="6"/>
-      <c r="BP7" s="6"/>
-      <c r="BQ7" s="6"/>
+      <c r="BH7" s="326"/>
+      <c r="BI7" s="362"/>
+      <c r="BJ7" s="362"/>
+      <c r="BK7" s="362"/>
+      <c r="BL7" s="362"/>
+      <c r="BM7" s="362"/>
+      <c r="BN7" s="362"/>
+      <c r="BO7" s="362"/>
+      <c r="BP7" s="362"/>
+      <c r="BQ7" s="326"/>
       <c r="BR7" s="6"/>
       <c r="BS7" s="6"/>
       <c r="BT7" s="9"/>
-      <c r="BV7">
-        <f t="shared" si="10"/>
-        <v>5</v>
-      </c>
-      <c r="BW7" s="10"/>
-      <c r="BZ7" s="326"/>
-      <c r="CA7" s="362"/>
-      <c r="CB7" s="362"/>
-      <c r="CC7" s="362"/>
-      <c r="CD7" s="362"/>
-      <c r="CE7" s="362"/>
-      <c r="CF7" s="362"/>
-      <c r="CG7" s="362"/>
-      <c r="CH7" s="362"/>
-      <c r="CI7" s="326"/>
-      <c r="CJ7" s="6"/>
-      <c r="CK7" s="6"/>
-      <c r="CL7" s="9"/>
-    </row>
-    <row r="8" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A8" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="B8" s="314"/>
@@ -54162,7 +54019,7 @@
       <c r="D8" s="244"/>
       <c r="E8" s="244"/>
       <c r="F8" s="244"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
@@ -54174,7 +54031,7 @@
       <c r="P8" s="244"/>
       <c r="Q8" s="315"/>
       <c r="S8" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="T8" s="127"/>
@@ -54194,73 +54051,53 @@
       <c r="AH8" s="128"/>
       <c r="AI8" s="130"/>
       <c r="AJ8" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="AL8">
-        <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="AM8" s="235"/>
-      <c r="AN8" s="342"/>
-      <c r="AO8" s="353"/>
-      <c r="AP8" s="353"/>
-      <c r="AQ8" s="342"/>
-      <c r="AR8" s="353"/>
-      <c r="AS8" s="353"/>
-      <c r="AT8" s="353"/>
-      <c r="AU8" s="353"/>
-      <c r="AV8" s="353"/>
-      <c r="AW8" s="353"/>
-      <c r="AX8" s="342"/>
-      <c r="AY8" s="353"/>
-      <c r="AZ8" s="353"/>
-      <c r="BA8" s="342"/>
-      <c r="BB8" s="233"/>
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="AM8" s="359"/>
+      <c r="AN8" s="219"/>
+      <c r="AO8" s="226"/>
+      <c r="AP8" s="226"/>
+      <c r="AQ8" s="226"/>
+      <c r="AR8" s="219"/>
+      <c r="AS8" s="363"/>
+      <c r="AT8" s="361"/>
+      <c r="AU8" s="361"/>
+      <c r="AV8" s="364"/>
+      <c r="AW8" s="219"/>
+      <c r="AX8" s="226"/>
+      <c r="AY8" s="226"/>
+      <c r="AZ8" s="226"/>
+      <c r="BA8" s="219"/>
+      <c r="BB8" s="360"/>
       <c r="BD8">
-        <f t="shared" si="6"/>
-        <v>41</v>
+        <f t="shared" si="8"/>
+        <v>6</v>
       </c>
       <c r="BE8" s="359"/>
       <c r="BF8" s="219"/>
       <c r="BG8" s="226"/>
-      <c r="BH8" s="226"/>
+      <c r="BH8" s="326"/>
       <c r="BI8" s="226"/>
       <c r="BJ8" s="219"/>
-      <c r="BK8" s="363"/>
-      <c r="BL8" s="361"/>
-      <c r="BM8" s="361"/>
-      <c r="BN8" s="364"/>
+      <c r="BK8" s="226"/>
+      <c r="BL8" s="226"/>
+      <c r="BM8" s="226"/>
+      <c r="BN8" s="226"/>
       <c r="BO8" s="219"/>
       <c r="BP8" s="226"/>
       <c r="BQ8" s="226"/>
       <c r="BR8" s="226"/>
       <c r="BS8" s="219"/>
       <c r="BT8" s="360"/>
-      <c r="BV8">
-        <f t="shared" si="10"/>
-        <v>6</v>
-      </c>
-      <c r="BW8" s="359"/>
-      <c r="BX8" s="219"/>
-      <c r="BY8" s="226"/>
-      <c r="BZ8" s="326"/>
-      <c r="CA8" s="226"/>
-      <c r="CB8" s="219"/>
-      <c r="CC8" s="226"/>
-      <c r="CD8" s="226"/>
-      <c r="CE8" s="226"/>
-      <c r="CF8" s="226"/>
-      <c r="CG8" s="219"/>
-      <c r="CH8" s="226"/>
-      <c r="CI8" s="226"/>
-      <c r="CJ8" s="226"/>
-      <c r="CK8" s="219"/>
-      <c r="CL8" s="360"/>
-    </row>
-    <row r="9" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A9" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="B9" s="16"/>
@@ -54268,7 +54105,7 @@
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
@@ -54280,7 +54117,7 @@
       <c r="P9" s="17"/>
       <c r="Q9" s="26"/>
       <c r="S9" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="T9" s="345"/>
@@ -54300,73 +54137,53 @@
       <c r="AH9" s="342"/>
       <c r="AI9" s="347"/>
       <c r="AJ9" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="AL9">
-        <f t="shared" si="5"/>
-        <v>24</v>
-      </c>
-      <c r="AM9" s="345"/>
-      <c r="AN9" s="342"/>
-      <c r="AO9" s="346"/>
-      <c r="AP9" s="346"/>
-      <c r="AQ9" s="219"/>
-      <c r="AR9" s="353"/>
-      <c r="AS9" s="353"/>
-      <c r="AT9" s="353"/>
-      <c r="AU9" s="353"/>
-      <c r="AV9" s="353"/>
-      <c r="AW9" s="346"/>
-      <c r="AX9" s="342"/>
-      <c r="AY9" s="346"/>
-      <c r="AZ9" s="140"/>
-      <c r="BA9" s="342"/>
-      <c r="BB9" s="347"/>
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="AM9" s="359"/>
+      <c r="AN9" s="219"/>
+      <c r="AO9" s="226"/>
+      <c r="AP9" s="226"/>
+      <c r="AQ9" s="226"/>
+      <c r="AR9" s="219"/>
+      <c r="AS9" s="359"/>
+      <c r="AT9" s="226"/>
+      <c r="AU9" s="226"/>
+      <c r="AV9" s="360"/>
+      <c r="AW9" s="140"/>
+      <c r="AX9" s="226"/>
+      <c r="AY9" s="226"/>
+      <c r="AZ9" s="226"/>
+      <c r="BA9" s="219"/>
+      <c r="BB9" s="360"/>
       <c r="BD9">
-        <f t="shared" si="6"/>
-        <v>40</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
       </c>
       <c r="BE9" s="359"/>
       <c r="BF9" s="219"/>
       <c r="BG9" s="226"/>
-      <c r="BH9" s="226"/>
+      <c r="BH9" s="326"/>
       <c r="BI9" s="226"/>
       <c r="BJ9" s="219"/>
-      <c r="BK9" s="359"/>
+      <c r="BK9" s="226"/>
       <c r="BL9" s="226"/>
       <c r="BM9" s="226"/>
-      <c r="BN9" s="360"/>
-      <c r="BO9" s="140"/>
+      <c r="BN9" s="226"/>
+      <c r="BO9" s="219"/>
       <c r="BP9" s="226"/>
       <c r="BQ9" s="226"/>
       <c r="BR9" s="226"/>
       <c r="BS9" s="219"/>
       <c r="BT9" s="360"/>
-      <c r="BV9">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="BW9" s="359"/>
-      <c r="BX9" s="219"/>
-      <c r="BY9" s="226"/>
-      <c r="BZ9" s="326"/>
-      <c r="CA9" s="226"/>
-      <c r="CB9" s="219"/>
-      <c r="CC9" s="226"/>
-      <c r="CD9" s="226"/>
-      <c r="CE9" s="226"/>
-      <c r="CF9" s="226"/>
-      <c r="CG9" s="219"/>
-      <c r="CH9" s="226"/>
-      <c r="CI9" s="226"/>
-      <c r="CJ9" s="226"/>
-      <c r="CK9" s="219"/>
-      <c r="CL9" s="360"/>
-    </row>
-    <row r="10" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A10" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="B10" s="314"/>
@@ -54374,7 +54191,7 @@
       <c r="D10" s="244"/>
       <c r="E10" s="244"/>
       <c r="F10" s="244"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
@@ -54386,7 +54203,7 @@
       <c r="P10" s="244"/>
       <c r="Q10" s="315"/>
       <c r="S10" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="T10" s="345"/>
@@ -54406,73 +54223,53 @@
       <c r="AH10" s="342"/>
       <c r="AI10" s="347"/>
       <c r="AJ10" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="AL10">
-        <f t="shared" si="5"/>
-        <v>23</v>
-      </c>
-      <c r="AM10" s="345"/>
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="AM10" s="359"/>
       <c r="AN10" s="219"/>
-      <c r="AO10" s="353"/>
-      <c r="AP10" s="353"/>
-      <c r="AQ10" s="219"/>
-      <c r="AR10" s="353"/>
-      <c r="AS10" s="353"/>
-      <c r="AT10" s="353"/>
-      <c r="AU10" s="353"/>
-      <c r="AV10" s="353"/>
-      <c r="AW10" s="353"/>
-      <c r="AX10" s="219"/>
-      <c r="AY10" s="140"/>
-      <c r="AZ10" s="140"/>
-      <c r="BA10" s="342"/>
-      <c r="BB10" s="347"/>
+      <c r="AO10" s="226"/>
+      <c r="AP10" s="226"/>
+      <c r="AQ10" s="226"/>
+      <c r="AR10" s="219"/>
+      <c r="AS10" s="359"/>
+      <c r="AT10" s="226"/>
+      <c r="AU10" s="226"/>
+      <c r="AV10" s="140"/>
+      <c r="AW10" s="140"/>
+      <c r="AX10" s="226"/>
+      <c r="AY10" s="226"/>
+      <c r="AZ10" s="226"/>
+      <c r="BA10" s="219"/>
+      <c r="BB10" s="360"/>
       <c r="BD10">
-        <f t="shared" si="6"/>
-        <v>39</v>
+        <f t="shared" si="8"/>
+        <v>8</v>
       </c>
       <c r="BE10" s="359"/>
       <c r="BF10" s="219"/>
       <c r="BG10" s="226"/>
-      <c r="BH10" s="226"/>
+      <c r="BH10" s="326"/>
       <c r="BI10" s="226"/>
       <c r="BJ10" s="219"/>
-      <c r="BK10" s="359"/>
+      <c r="BK10" s="226"/>
       <c r="BL10" s="226"/>
       <c r="BM10" s="226"/>
-      <c r="BN10" s="140"/>
-      <c r="BO10" s="140"/>
+      <c r="BN10" s="226"/>
+      <c r="BO10" s="219"/>
       <c r="BP10" s="226"/>
       <c r="BQ10" s="226"/>
       <c r="BR10" s="226"/>
       <c r="BS10" s="219"/>
       <c r="BT10" s="360"/>
-      <c r="BV10">
-        <f t="shared" si="10"/>
-        <v>8</v>
-      </c>
-      <c r="BW10" s="359"/>
-      <c r="BX10" s="219"/>
-      <c r="BY10" s="226"/>
-      <c r="BZ10" s="326"/>
-      <c r="CA10" s="226"/>
-      <c r="CB10" s="219"/>
-      <c r="CC10" s="226"/>
-      <c r="CD10" s="226"/>
-      <c r="CE10" s="226"/>
-      <c r="CF10" s="226"/>
-      <c r="CG10" s="219"/>
-      <c r="CH10" s="226"/>
-      <c r="CI10" s="226"/>
-      <c r="CJ10" s="226"/>
-      <c r="CK10" s="219"/>
-      <c r="CL10" s="360"/>
-    </row>
-    <row r="11" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A11" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B11" s="314"/>
@@ -54480,7 +54277,7 @@
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
@@ -54492,7 +54289,7 @@
       <c r="P11" s="244"/>
       <c r="Q11" s="315"/>
       <c r="S11" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="T11" s="343"/>
@@ -54512,77 +54309,57 @@
       <c r="AH11" s="327"/>
       <c r="AI11" s="344"/>
       <c r="AJ11" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="AL11">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="AM11" s="308"/>
+      <c r="AN11" s="219"/>
+      <c r="AO11" s="219"/>
+      <c r="AP11" s="219"/>
+      <c r="AQ11" s="219"/>
+      <c r="AR11" s="219"/>
+      <c r="AS11" s="323"/>
+      <c r="AT11" s="218"/>
+      <c r="AU11" s="140"/>
+      <c r="AV11" s="140"/>
+      <c r="AW11" s="140"/>
+      <c r="AX11" s="365"/>
+      <c r="AY11" s="326"/>
+      <c r="AZ11" s="219"/>
+      <c r="BA11" s="219"/>
+      <c r="BB11" s="309"/>
+      <c r="BD11">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="BE11" s="359"/>
+      <c r="BF11" s="219"/>
+      <c r="BG11" s="226"/>
+      <c r="BH11" s="326"/>
+      <c r="BI11" s="226"/>
+      <c r="BJ11" s="219"/>
+      <c r="BK11" s="226"/>
+      <c r="BL11" s="226"/>
+      <c r="BM11" s="226"/>
+      <c r="BN11" s="226"/>
+      <c r="BO11" s="219"/>
+      <c r="BP11" s="226"/>
+      <c r="BQ11" s="226"/>
+      <c r="BR11" s="226"/>
+      <c r="BS11" s="219"/>
+      <c r="BT11" s="360"/>
+    </row>
+    <row r="12" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A12" s="70">
         <f t="shared" si="5"/>
-        <v>22</v>
-      </c>
-      <c r="AM11" s="343"/>
-      <c r="AN11" s="327"/>
-      <c r="AO11" s="327"/>
-      <c r="AP11" s="327"/>
-      <c r="AQ11" s="327"/>
-      <c r="AR11" s="327"/>
-      <c r="AS11" s="327"/>
-      <c r="AT11" s="327"/>
-      <c r="AU11" s="327"/>
-      <c r="AV11" s="327"/>
-      <c r="AW11" s="327"/>
-      <c r="AX11" s="140"/>
-      <c r="AY11" s="140"/>
-      <c r="AZ11" s="140"/>
-      <c r="BA11" s="365"/>
-      <c r="BB11" s="344"/>
-      <c r="BD11">
-        <f t="shared" si="6"/>
-        <v>38</v>
-      </c>
-      <c r="BE11" s="308"/>
-      <c r="BF11" s="219"/>
-      <c r="BG11" s="219"/>
-      <c r="BH11" s="219"/>
-      <c r="BI11" s="219"/>
-      <c r="BJ11" s="219"/>
-      <c r="BK11" s="323"/>
-      <c r="BL11" s="218"/>
-      <c r="BM11" s="140"/>
-      <c r="BN11" s="140"/>
-      <c r="BO11" s="140"/>
-      <c r="BP11" s="365"/>
-      <c r="BQ11" s="326"/>
-      <c r="BR11" s="219"/>
-      <c r="BS11" s="219"/>
-      <c r="BT11" s="309"/>
-      <c r="BV11">
-        <f t="shared" si="10"/>
-        <v>9</v>
-      </c>
-      <c r="BW11" s="359"/>
-      <c r="BX11" s="219"/>
-      <c r="BY11" s="226"/>
-      <c r="BZ11" s="326"/>
-      <c r="CA11" s="226"/>
-      <c r="CB11" s="219"/>
-      <c r="CC11" s="226"/>
-      <c r="CD11" s="226"/>
-      <c r="CE11" s="226"/>
-      <c r="CF11" s="226"/>
-      <c r="CG11" s="219"/>
-      <c r="CH11" s="226"/>
-      <c r="CI11" s="226"/>
-      <c r="CJ11" s="226"/>
-      <c r="CK11" s="219"/>
-      <c r="CL11" s="360"/>
-    </row>
-    <row r="12" spans="1:90" x14ac:dyDescent="0.3">
-      <c r="A12" s="70">
-        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="B12" s="314"/>
-      <c r="C12" s="244"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="244"/>
       <c r="E12" s="244"/>
       <c r="F12" s="244"/>
@@ -54598,7 +54375,7 @@
       <c r="P12" s="244"/>
       <c r="Q12" s="315"/>
       <c r="S12" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="T12" s="10"/>
@@ -54618,72 +54395,55 @@
       <c r="AH12" s="372"/>
       <c r="AI12" s="373"/>
       <c r="AJ12" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="AL12">
-        <f t="shared" si="5"/>
-        <v>21</v>
+        <f t="shared" si="4"/>
+        <v>37</v>
       </c>
       <c r="AM12" s="10"/>
       <c r="AN12" s="17"/>
       <c r="AO12" s="17"/>
-      <c r="AS12" s="17"/>
-      <c r="AT12" s="17"/>
-      <c r="AU12" s="6"/>
-      <c r="AV12" s="6"/>
-      <c r="AW12" s="140"/>
-      <c r="AX12" s="140"/>
-      <c r="AY12" s="140"/>
-      <c r="AZ12" s="365"/>
+      <c r="AP12" s="17"/>
+      <c r="AQ12" s="17"/>
+      <c r="AR12" s="6"/>
+      <c r="AS12" s="6"/>
+      <c r="AT12" s="140"/>
+      <c r="AU12" s="140"/>
+      <c r="AV12" s="140"/>
+      <c r="AW12" s="365"/>
+      <c r="AX12" s="366"/>
+      <c r="AY12" s="366"/>
+      <c r="AZ12" s="366"/>
       <c r="BA12" s="366"/>
-      <c r="BB12" s="366"/>
+      <c r="BB12" s="9"/>
       <c r="BD12">
-        <f t="shared" si="6"/>
-        <v>37</v>
+        <f t="shared" si="8"/>
+        <v>10</v>
       </c>
       <c r="BE12" s="10"/>
-      <c r="BF12" s="17"/>
-      <c r="BG12" s="17"/>
-      <c r="BH12" s="17"/>
-      <c r="BI12" s="17"/>
-      <c r="BJ12" s="6"/>
-      <c r="BK12" s="6"/>
-      <c r="BL12" s="140"/>
-      <c r="BM12" s="140"/>
-      <c r="BN12" s="140"/>
-      <c r="BO12" s="365"/>
-      <c r="BP12" s="366"/>
-      <c r="BQ12" s="366"/>
-      <c r="BR12" s="366"/>
-      <c r="BS12" s="366"/>
+      <c r="BH12" s="326"/>
+      <c r="BI12" s="362"/>
+      <c r="BJ12" s="362"/>
+      <c r="BK12" s="362"/>
+      <c r="BL12" s="362"/>
+      <c r="BM12" s="362"/>
+      <c r="BN12" s="367"/>
+      <c r="BO12" s="367"/>
+      <c r="BP12" s="367"/>
+      <c r="BQ12" s="326"/>
+      <c r="BR12" s="6"/>
+      <c r="BS12" s="6"/>
       <c r="BT12" s="9"/>
-      <c r="BV12">
-        <f t="shared" si="10"/>
-        <v>10</v>
-      </c>
-      <c r="BW12" s="10"/>
-      <c r="BZ12" s="326"/>
-      <c r="CA12" s="362"/>
-      <c r="CB12" s="362"/>
-      <c r="CC12" s="362"/>
-      <c r="CD12" s="362"/>
-      <c r="CE12" s="362"/>
-      <c r="CF12" s="367"/>
-      <c r="CG12" s="367"/>
-      <c r="CH12" s="367"/>
-      <c r="CI12" s="326"/>
-      <c r="CJ12" s="6"/>
-      <c r="CK12" s="6"/>
-      <c r="CL12" s="9"/>
-    </row>
-    <row r="13" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A13" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="B13" s="314"/>
-      <c r="C13" s="244"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="244"/>
       <c r="E13" s="244"/>
       <c r="F13" s="244"/>
@@ -54699,7 +54459,7 @@
       <c r="P13" s="244"/>
       <c r="Q13" s="315"/>
       <c r="S13" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="T13" s="314"/>
@@ -54719,66 +54479,49 @@
       <c r="AH13" s="244"/>
       <c r="AI13" s="9"/>
       <c r="AJ13" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="AL13">
-        <f t="shared" si="5"/>
-        <v>20</v>
+        <f t="shared" si="4"/>
+        <v>36</v>
       </c>
       <c r="AM13" s="10"/>
       <c r="AN13" s="17"/>
       <c r="AO13" s="17"/>
-      <c r="AS13" s="17"/>
-      <c r="AT13" s="17"/>
-      <c r="AU13" s="6"/>
-      <c r="AV13" s="140"/>
-      <c r="AW13" s="140"/>
-      <c r="AX13" s="140"/>
-      <c r="AY13" s="365"/>
+      <c r="AP13" s="17"/>
+      <c r="AQ13" s="17"/>
+      <c r="AR13" s="6"/>
+      <c r="AS13" s="140"/>
+      <c r="AT13" s="140"/>
+      <c r="AU13" s="140"/>
+      <c r="AV13" s="365"/>
+      <c r="AW13" s="366"/>
+      <c r="AX13" s="366"/>
+      <c r="AY13" s="366"/>
       <c r="AZ13" s="366"/>
       <c r="BA13" s="366"/>
-      <c r="BB13" s="366"/>
+      <c r="BB13" s="9"/>
       <c r="BD13">
-        <f t="shared" si="6"/>
-        <v>36</v>
+        <f t="shared" si="8"/>
+        <v>11</v>
       </c>
       <c r="BE13" s="10"/>
-      <c r="BF13" s="17"/>
-      <c r="BG13" s="17"/>
-      <c r="BH13" s="17"/>
-      <c r="BI13" s="17"/>
-      <c r="BJ13" s="6"/>
-      <c r="BK13" s="140"/>
-      <c r="BL13" s="140"/>
-      <c r="BM13" s="140"/>
-      <c r="BN13" s="365"/>
-      <c r="BO13" s="366"/>
-      <c r="BP13" s="366"/>
-      <c r="BQ13" s="366"/>
-      <c r="BR13" s="366"/>
-      <c r="BS13" s="366"/>
+      <c r="BN13" s="17"/>
+      <c r="BO13" s="6"/>
+      <c r="BP13" s="6"/>
+      <c r="BQ13" s="6"/>
+      <c r="BR13" s="6"/>
+      <c r="BS13" s="6"/>
       <c r="BT13" s="9"/>
-      <c r="BV13">
-        <f t="shared" si="10"/>
-        <v>11</v>
-      </c>
-      <c r="BW13" s="10"/>
-      <c r="CF13" s="17"/>
-      <c r="CG13" s="6"/>
-      <c r="CH13" s="6"/>
-      <c r="CI13" s="6"/>
-      <c r="CJ13" s="6"/>
-      <c r="CK13" s="6"/>
-      <c r="CL13" s="9"/>
-    </row>
-    <row r="14" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A14" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="B14" s="314"/>
-      <c r="C14" s="244"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="244"/>
       <c r="E14" s="244"/>
       <c r="F14" s="244"/>
@@ -54794,7 +54537,7 @@
       <c r="P14" s="244"/>
       <c r="Q14" s="315"/>
       <c r="S14" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="T14" s="314"/>
@@ -54814,74 +54557,57 @@
       <c r="AH14" s="244"/>
       <c r="AI14" s="9"/>
       <c r="AJ14" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="AL14">
-        <f t="shared" si="5"/>
-        <v>19</v>
+        <f t="shared" si="4"/>
+        <v>35</v>
       </c>
       <c r="AM14" s="10"/>
       <c r="AN14" s="17"/>
       <c r="AO14" s="17"/>
-      <c r="AS14" s="17"/>
-      <c r="AT14" s="6"/>
-      <c r="AU14" s="140"/>
-      <c r="AV14" s="140"/>
-      <c r="AW14" s="140"/>
-      <c r="AX14" s="365"/>
-      <c r="AY14" s="17"/>
+      <c r="AP14" s="17"/>
+      <c r="AQ14" s="6"/>
+      <c r="AR14" s="140"/>
+      <c r="AS14" s="140"/>
+      <c r="AT14" s="140"/>
+      <c r="AU14" s="365"/>
+      <c r="AV14" s="17"/>
+      <c r="AW14" s="366"/>
+      <c r="AX14" s="366"/>
+      <c r="AY14" s="366"/>
       <c r="AZ14" s="366"/>
       <c r="BA14" s="366"/>
-      <c r="BB14" s="366"/>
+      <c r="BB14" s="9"/>
       <c r="BD14">
-        <f t="shared" si="6"/>
-        <v>35</v>
+        <f t="shared" si="8"/>
+        <v>12</v>
       </c>
       <c r="BE14" s="10"/>
-      <c r="BF14" s="17"/>
-      <c r="BG14" s="17"/>
-      <c r="BH14" s="17"/>
+      <c r="BF14" s="6"/>
+      <c r="BG14" s="6"/>
+      <c r="BH14" s="6"/>
       <c r="BI14" s="6"/>
-      <c r="BJ14" s="140"/>
-      <c r="BK14" s="140"/>
-      <c r="BL14" s="140"/>
-      <c r="BM14" s="365"/>
+      <c r="BJ14" s="6"/>
+      <c r="BK14" s="17"/>
+      <c r="BL14" s="17"/>
+      <c r="BM14" s="17"/>
       <c r="BN14" s="17"/>
-      <c r="BO14" s="366"/>
-      <c r="BP14" s="366"/>
-      <c r="BQ14" s="366"/>
-      <c r="BR14" s="366"/>
-      <c r="BS14" s="366"/>
+      <c r="BO14" s="6"/>
+      <c r="BP14" s="6"/>
+      <c r="BQ14" s="6"/>
+      <c r="BR14" s="6"/>
+      <c r="BS14" s="6"/>
       <c r="BT14" s="9"/>
-      <c r="BV14">
-        <f t="shared" si="10"/>
-        <v>12</v>
-      </c>
-      <c r="BW14" s="10"/>
-      <c r="BX14" s="6"/>
-      <c r="BY14" s="6"/>
-      <c r="BZ14" s="6"/>
-      <c r="CA14" s="6"/>
-      <c r="CB14" s="6"/>
-      <c r="CC14" s="17"/>
-      <c r="CD14" s="17"/>
-      <c r="CE14" s="17"/>
-      <c r="CF14" s="17"/>
-      <c r="CG14" s="6"/>
-      <c r="CH14" s="6"/>
-      <c r="CI14" s="6"/>
-      <c r="CJ14" s="6"/>
-      <c r="CK14" s="6"/>
-      <c r="CL14" s="9"/>
-    </row>
-    <row r="15" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A15" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="B15" s="314"/>
-      <c r="C15" s="244"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="244"/>
       <c r="E15" s="244"/>
       <c r="F15" s="244"/>
@@ -54897,7 +54623,7 @@
       <c r="P15" s="244"/>
       <c r="Q15" s="315"/>
       <c r="S15" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="T15" s="314"/>
@@ -54917,78 +54643,61 @@
       <c r="AH15" s="17"/>
       <c r="AI15" s="9"/>
       <c r="AJ15" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="AL15">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" si="4"/>
+        <v>34</v>
       </c>
       <c r="AM15" s="10"/>
       <c r="AN15" s="17"/>
       <c r="AO15" s="17"/>
-      <c r="AS15" s="17"/>
-      <c r="AT15" s="140"/>
-      <c r="AU15" s="140"/>
-      <c r="AV15" s="140"/>
-      <c r="AW15" s="365"/>
-      <c r="AX15" s="17"/>
-      <c r="AY15" s="17"/>
+      <c r="AP15" s="17"/>
+      <c r="AQ15" s="140"/>
+      <c r="AR15" s="140"/>
+      <c r="AS15" s="140"/>
+      <c r="AT15" s="365"/>
+      <c r="AU15" s="17"/>
+      <c r="AV15" s="17"/>
+      <c r="AW15" s="366"/>
+      <c r="AX15" s="366"/>
+      <c r="AY15" s="366"/>
       <c r="AZ15" s="366"/>
       <c r="BA15" s="366"/>
-      <c r="BB15" s="366"/>
+      <c r="BB15" s="9"/>
       <c r="BD15">
-        <f t="shared" si="6"/>
-        <v>34</v>
+        <f t="shared" si="8"/>
+        <v>13</v>
       </c>
       <c r="BE15" s="10"/>
-      <c r="BF15" s="17"/>
-      <c r="BG15" s="17"/>
-      <c r="BH15" s="17"/>
-      <c r="BI15" s="140"/>
-      <c r="BJ15" s="140"/>
-      <c r="BK15" s="140"/>
-      <c r="BL15" s="365"/>
+      <c r="BF15" s="6"/>
+      <c r="BG15" s="6"/>
+      <c r="BH15" s="6"/>
+      <c r="BI15" s="6"/>
+      <c r="BJ15" s="6"/>
+      <c r="BK15" s="17"/>
+      <c r="BL15" s="17"/>
       <c r="BM15" s="17"/>
       <c r="BN15" s="17"/>
-      <c r="BO15" s="366"/>
-      <c r="BP15" s="366"/>
-      <c r="BQ15" s="366"/>
-      <c r="BR15" s="366"/>
-      <c r="BS15" s="366"/>
+      <c r="BO15" s="6"/>
+      <c r="BP15" s="6"/>
+      <c r="BQ15" s="6"/>
+      <c r="BR15" s="6"/>
+      <c r="BS15" s="6"/>
       <c r="BT15" s="9"/>
-      <c r="BV15">
-        <f t="shared" si="10"/>
-        <v>13</v>
-      </c>
-      <c r="BW15" s="10"/>
-      <c r="BX15" s="6"/>
-      <c r="BY15" s="6"/>
-      <c r="BZ15" s="6"/>
-      <c r="CA15" s="6"/>
-      <c r="CB15" s="6"/>
-      <c r="CC15" s="17"/>
-      <c r="CD15" s="17"/>
-      <c r="CE15" s="17"/>
-      <c r="CF15" s="17"/>
-      <c r="CG15" s="6"/>
-      <c r="CH15" s="6"/>
-      <c r="CI15" s="6"/>
-      <c r="CJ15" s="6"/>
-      <c r="CK15" s="6"/>
-      <c r="CL15" s="9"/>
-    </row>
-    <row r="16" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A16" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="244"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="244"/>
       <c r="F16" s="244"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="244"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
@@ -55000,7 +54709,7 @@
       <c r="P16" s="17"/>
       <c r="Q16" s="26"/>
       <c r="S16" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="T16" s="16"/>
@@ -55020,70 +54729,53 @@
       <c r="AH16" s="17"/>
       <c r="AI16" s="9"/>
       <c r="AJ16" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="AL16">
-        <f t="shared" si="5"/>
-        <v>17</v>
+        <f t="shared" si="4"/>
+        <v>33</v>
       </c>
       <c r="AM16" s="10"/>
       <c r="AN16" s="17"/>
       <c r="AO16" s="17"/>
-      <c r="AS16" s="140"/>
-      <c r="AT16" s="140"/>
-      <c r="AU16" s="140"/>
-      <c r="AV16" s="365"/>
-      <c r="AW16" s="17"/>
-      <c r="AX16" s="17"/>
-      <c r="AY16" s="17"/>
+      <c r="AP16" s="140"/>
+      <c r="AQ16" s="140"/>
+      <c r="AR16" s="140"/>
+      <c r="AS16" s="365"/>
+      <c r="AT16" s="17"/>
+      <c r="AU16" s="17"/>
+      <c r="AV16" s="17"/>
+      <c r="AW16" s="366"/>
+      <c r="AX16" s="366"/>
+      <c r="AY16" s="366"/>
       <c r="AZ16" s="366"/>
       <c r="BA16" s="366"/>
-      <c r="BB16" s="366"/>
+      <c r="BB16" s="9"/>
       <c r="BD16">
-        <f t="shared" si="6"/>
-        <v>33</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="BE16" s="10"/>
-      <c r="BF16" s="17"/>
-      <c r="BG16" s="17"/>
-      <c r="BH16" s="140"/>
-      <c r="BI16" s="140"/>
-      <c r="BJ16" s="140"/>
-      <c r="BK16" s="365"/>
+      <c r="BF16" s="6"/>
+      <c r="BG16" s="6"/>
+      <c r="BH16" s="6"/>
+      <c r="BI16" s="6"/>
+      <c r="BJ16" s="6"/>
+      <c r="BK16" s="17"/>
       <c r="BL16" s="17"/>
       <c r="BM16" s="17"/>
       <c r="BN16" s="17"/>
-      <c r="BO16" s="366"/>
-      <c r="BP16" s="366"/>
-      <c r="BQ16" s="366"/>
-      <c r="BR16" s="366"/>
-      <c r="BS16" s="366"/>
+      <c r="BO16" s="6"/>
+      <c r="BP16" s="6"/>
+      <c r="BQ16" s="6"/>
+      <c r="BR16" s="6"/>
+      <c r="BS16" s="6"/>
       <c r="BT16" s="9"/>
-      <c r="BV16">
-        <f t="shared" si="10"/>
-        <v>14</v>
-      </c>
-      <c r="BW16" s="10"/>
-      <c r="BX16" s="6"/>
-      <c r="BY16" s="6"/>
-      <c r="BZ16" s="6"/>
-      <c r="CA16" s="6"/>
-      <c r="CB16" s="6"/>
-      <c r="CC16" s="17"/>
-      <c r="CD16" s="17"/>
-      <c r="CE16" s="17"/>
-      <c r="CF16" s="17"/>
-      <c r="CG16" s="6"/>
-      <c r="CH16" s="6"/>
-      <c r="CI16" s="6"/>
-      <c r="CJ16" s="6"/>
-      <c r="CK16" s="6"/>
-      <c r="CL16" s="9"/>
-    </row>
-    <row r="17" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A17" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="B17" s="32"/>
@@ -55103,7 +54795,7 @@
       <c r="P17" s="22"/>
       <c r="Q17" s="33"/>
       <c r="S17" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="T17" s="32"/>
@@ -55123,68 +54815,51 @@
       <c r="AH17" s="14"/>
       <c r="AI17" s="15"/>
       <c r="AJ17" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="AL17">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <f t="shared" si="4"/>
+        <v>32</v>
       </c>
       <c r="AM17" s="13"/>
       <c r="AN17" s="22"/>
       <c r="AO17" s="22"/>
-      <c r="AS17" s="140"/>
-      <c r="AT17" s="140"/>
-      <c r="AU17" s="365"/>
-      <c r="AV17" s="14"/>
-      <c r="AW17" s="22"/>
-      <c r="AX17" s="22"/>
-      <c r="AY17" s="22"/>
+      <c r="AP17" s="140"/>
+      <c r="AQ17" s="140"/>
+      <c r="AR17" s="365"/>
+      <c r="AS17" s="14"/>
+      <c r="AT17" s="22"/>
+      <c r="AU17" s="22"/>
+      <c r="AV17" s="22"/>
+      <c r="AW17" s="368"/>
+      <c r="AX17" s="368"/>
+      <c r="AY17" s="368"/>
       <c r="AZ17" s="368"/>
       <c r="BA17" s="368"/>
-      <c r="BB17" s="368"/>
+      <c r="BB17" s="15"/>
       <c r="BD17">
-        <f t="shared" si="6"/>
-        <v>32</v>
+        <f t="shared" si="8"/>
+        <v>15</v>
       </c>
       <c r="BE17" s="13"/>
-      <c r="BF17" s="22"/>
-      <c r="BG17" s="22"/>
-      <c r="BH17" s="140"/>
-      <c r="BI17" s="140"/>
-      <c r="BJ17" s="365"/>
-      <c r="BK17" s="14"/>
+      <c r="BF17" s="14"/>
+      <c r="BG17" s="14"/>
+      <c r="BH17" s="14"/>
+      <c r="BI17" s="14"/>
+      <c r="BJ17" s="14"/>
+      <c r="BK17" s="22"/>
       <c r="BL17" s="22"/>
       <c r="BM17" s="22"/>
       <c r="BN17" s="22"/>
-      <c r="BO17" s="368"/>
-      <c r="BP17" s="368"/>
-      <c r="BQ17" s="368"/>
-      <c r="BR17" s="368"/>
-      <c r="BS17" s="368"/>
+      <c r="BO17" s="14"/>
+      <c r="BP17" s="14"/>
+      <c r="BQ17" s="14"/>
+      <c r="BR17" s="14"/>
+      <c r="BS17" s="14"/>
       <c r="BT17" s="15"/>
-      <c r="BV17">
-        <f t="shared" si="10"/>
-        <v>15</v>
-      </c>
-      <c r="BW17" s="13"/>
-      <c r="BX17" s="14"/>
-      <c r="BY17" s="14"/>
-      <c r="BZ17" s="14"/>
-      <c r="CA17" s="14"/>
-      <c r="CB17" s="14"/>
-      <c r="CC17" s="22"/>
-      <c r="CD17" s="22"/>
-      <c r="CE17" s="22"/>
-      <c r="CF17" s="22"/>
-      <c r="CG17" s="14"/>
-      <c r="CH17" s="14"/>
-      <c r="CI17" s="14"/>
-      <c r="CJ17" s="14"/>
-      <c r="CK17" s="14"/>
-      <c r="CL17" s="15"/>
-    </row>
-    <row r="18" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A18" s="242" t="s">
         <v>395</v>
       </c>
@@ -55195,350 +54870,299 @@
         <v>395</v>
       </c>
       <c r="AL18">
-        <f t="shared" si="5"/>
-        <v>15</v>
+        <f t="shared" si="4"/>
+        <v>31</v>
       </c>
       <c r="AM18" s="10"/>
       <c r="AN18" s="17"/>
       <c r="AO18" s="17"/>
+      <c r="AP18" s="140"/>
+      <c r="AQ18" s="365"/>
+      <c r="AR18" s="140"/>
       <c r="AS18" s="140"/>
-      <c r="AT18" s="365"/>
-      <c r="AU18" s="140"/>
-      <c r="AV18" s="140"/>
-      <c r="AW18" s="6"/>
-      <c r="AX18" s="17"/>
-      <c r="AY18" s="17"/>
+      <c r="AT18" s="6"/>
+      <c r="AU18" s="17"/>
+      <c r="AV18" s="17"/>
+      <c r="AW18" s="366"/>
+      <c r="AX18" s="366"/>
+      <c r="AY18" s="366"/>
       <c r="AZ18" s="366"/>
       <c r="BA18" s="366"/>
-      <c r="BB18" s="366"/>
-      <c r="BD18">
-        <f t="shared" si="6"/>
-        <v>31</v>
-      </c>
-      <c r="BE18" s="10"/>
-      <c r="BF18" s="17"/>
-      <c r="BG18" s="17"/>
-      <c r="BH18" s="140"/>
-      <c r="BI18" s="365"/>
-      <c r="BJ18" s="140"/>
-      <c r="BK18" s="140"/>
-      <c r="BL18" s="6"/>
-      <c r="BM18" s="17"/>
-      <c r="BN18" s="17"/>
-      <c r="BO18" s="366"/>
-      <c r="BP18" s="366"/>
-      <c r="BQ18" s="366"/>
-      <c r="BR18" s="366"/>
-      <c r="BS18" s="366"/>
-      <c r="BT18" s="9"/>
-    </row>
-    <row r="19" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="BB18" s="9"/>
+    </row>
+    <row r="19" spans="1:72" x14ac:dyDescent="0.3">
       <c r="AL19">
-        <f t="shared" si="5"/>
-        <v>14</v>
+        <f t="shared" si="4"/>
+        <v>30</v>
       </c>
       <c r="AM19" s="10"/>
       <c r="AN19" s="17"/>
       <c r="AO19" s="17"/>
-      <c r="AS19" s="326"/>
-      <c r="AT19" s="369"/>
-      <c r="AU19" s="140"/>
-      <c r="AV19" s="140"/>
-      <c r="AW19" s="140"/>
-      <c r="AX19" s="17"/>
-      <c r="AY19" s="17"/>
+      <c r="AP19" s="326"/>
+      <c r="AQ19" s="369"/>
+      <c r="AR19" s="140"/>
+      <c r="AS19" s="140"/>
+      <c r="AT19" s="140"/>
+      <c r="AU19" s="17"/>
+      <c r="AV19" s="17"/>
+      <c r="AW19" s="366"/>
+      <c r="AX19" s="366"/>
+      <c r="AY19" s="366"/>
       <c r="AZ19" s="366"/>
       <c r="BA19" s="366"/>
-      <c r="BB19" s="366"/>
-      <c r="BD19">
-        <f t="shared" si="6"/>
-        <v>30</v>
-      </c>
-      <c r="BE19" s="10"/>
-      <c r="BF19" s="17"/>
-      <c r="BG19" s="17"/>
-      <c r="BH19" s="326"/>
-      <c r="BI19" s="369"/>
-      <c r="BJ19" s="140"/>
-      <c r="BK19" s="140"/>
-      <c r="BL19" s="140"/>
-      <c r="BM19" s="17"/>
-      <c r="BN19" s="17"/>
-      <c r="BO19" s="366"/>
-      <c r="BP19" s="366"/>
-      <c r="BQ19" s="366"/>
-      <c r="BR19" s="366"/>
-      <c r="BS19" s="366"/>
-      <c r="BT19" s="9"/>
-      <c r="BW19">
-        <v>0</v>
-      </c>
-      <c r="BX19">
-        <f>BW19+1</f>
+      <c r="BB19" s="9"/>
+      <c r="BE19">
+        <v>0</v>
+      </c>
+      <c r="BF19">
+        <f>BE19+1</f>
         <v>1</v>
       </c>
-      <c r="BY19">
-        <f t="shared" ref="BY19:CL19" si="11">BX19+1</f>
+      <c r="BG19">
+        <f t="shared" ref="BG19:BT19" si="9">BF19+1</f>
         <v>2</v>
       </c>
-      <c r="BZ19">
+      <c r="BH19">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="BI19">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="BJ19">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="BK19">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="BL19">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="BM19">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="BN19">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="BO19">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="BP19">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="BQ19">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="BR19">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="BS19">
+        <f t="shared" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="BT19">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A20" s="242"/>
+      <c r="B20" s="70">
+        <v>0</v>
+      </c>
+      <c r="C20" s="70">
+        <f t="shared" ref="C20:Q20" si="10">B20+1</f>
+        <v>1</v>
+      </c>
+      <c r="D20" s="70">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="E20" s="70">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="F20" s="70">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="G20" s="70">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="H20" s="70">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="I20" s="70">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="J20" s="70">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="K20" s="70">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="L20" s="70">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="M20" s="70">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="N20" s="70">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="O20" s="70">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="P20" s="70">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="Q20" s="70">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="R20" s="242" t="s">
+        <v>394</v>
+      </c>
+      <c r="S20" s="242"/>
+      <c r="T20" s="70">
+        <v>0</v>
+      </c>
+      <c r="U20" s="70">
+        <f t="shared" ref="U20:AI20" si="11">T20+1</f>
+        <v>1</v>
+      </c>
+      <c r="V20" s="70">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="W20" s="70">
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="CA19">
+      <c r="X20" s="70">
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="CB19">
+      <c r="Y20" s="70">
         <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="CC19">
+      <c r="Z20" s="70">
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="CD19">
+      <c r="AA20" s="70">
         <f t="shared" si="11"/>
         <v>7</v>
       </c>
-      <c r="CE19">
+      <c r="AB20" s="70">
         <f t="shared" si="11"/>
         <v>8</v>
       </c>
-      <c r="CF19">
+      <c r="AC20" s="70">
         <f t="shared" si="11"/>
         <v>9</v>
       </c>
-      <c r="CG19">
+      <c r="AD20" s="70">
         <f t="shared" si="11"/>
         <v>10</v>
       </c>
-      <c r="CH19">
+      <c r="AE20" s="70">
         <f t="shared" si="11"/>
         <v>11</v>
       </c>
-      <c r="CI19">
+      <c r="AF20" s="70">
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="CJ19">
+      <c r="AG20" s="70">
         <f t="shared" si="11"/>
         <v>13</v>
       </c>
-      <c r="CK19">
+      <c r="AH20" s="70">
         <f t="shared" si="11"/>
         <v>14</v>
       </c>
-      <c r="CL19">
+      <c r="AI20" s="70">
         <f t="shared" si="11"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:90" x14ac:dyDescent="0.3">
-      <c r="A20" s="242"/>
-      <c r="B20" s="70">
-        <v>0</v>
-      </c>
-      <c r="C20" s="70">
-        <f t="shared" ref="C20:Q20" si="12">B20+1</f>
-        <v>1</v>
-      </c>
-      <c r="D20" s="70">
-        <f t="shared" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="E20" s="70">
-        <f t="shared" si="12"/>
-        <v>3</v>
-      </c>
-      <c r="F20" s="70">
-        <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="G20" s="70">
-        <f t="shared" si="12"/>
-        <v>5</v>
-      </c>
-      <c r="H20" s="70">
-        <f t="shared" si="12"/>
-        <v>6</v>
-      </c>
-      <c r="I20" s="70">
-        <f t="shared" si="12"/>
-        <v>7</v>
-      </c>
-      <c r="J20" s="70">
-        <f t="shared" si="12"/>
-        <v>8</v>
-      </c>
-      <c r="K20" s="70">
-        <f t="shared" si="12"/>
-        <v>9</v>
-      </c>
-      <c r="L20" s="70">
-        <f t="shared" si="12"/>
-        <v>10</v>
-      </c>
-      <c r="M20" s="70">
-        <f t="shared" si="12"/>
-        <v>11</v>
-      </c>
-      <c r="N20" s="70">
-        <f t="shared" si="12"/>
-        <v>12</v>
-      </c>
-      <c r="O20" s="70">
-        <f t="shared" si="12"/>
-        <v>13</v>
-      </c>
-      <c r="P20" s="70">
-        <f t="shared" si="12"/>
-        <v>14</v>
-      </c>
-      <c r="Q20" s="70">
-        <f t="shared" si="12"/>
-        <v>15</v>
-      </c>
-      <c r="R20" s="242" t="s">
-        <v>394</v>
-      </c>
-      <c r="S20" s="242"/>
-      <c r="T20" s="70">
-        <v>0</v>
-      </c>
-      <c r="U20" s="70">
-        <f t="shared" ref="U20:AI20" si="13">T20+1</f>
-        <v>1</v>
-      </c>
-      <c r="V20" s="70">
-        <f t="shared" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="W20" s="70">
-        <f t="shared" si="13"/>
-        <v>3</v>
-      </c>
-      <c r="X20" s="70">
-        <f t="shared" si="13"/>
-        <v>4</v>
-      </c>
-      <c r="Y20" s="70">
-        <f t="shared" si="13"/>
-        <v>5</v>
-      </c>
-      <c r="Z20" s="70">
-        <f t="shared" si="13"/>
-        <v>6</v>
-      </c>
-      <c r="AA20" s="70">
-        <f t="shared" si="13"/>
-        <v>7</v>
-      </c>
-      <c r="AB20" s="70">
-        <f t="shared" si="13"/>
-        <v>8</v>
-      </c>
-      <c r="AC20" s="70">
-        <f t="shared" si="13"/>
-        <v>9</v>
-      </c>
-      <c r="AD20" s="70">
-        <f t="shared" si="13"/>
-        <v>10</v>
-      </c>
-      <c r="AE20" s="70">
-        <f t="shared" si="13"/>
-        <v>11</v>
-      </c>
-      <c r="AF20" s="70">
-        <f t="shared" si="13"/>
-        <v>12</v>
-      </c>
-      <c r="AG20" s="70">
-        <f t="shared" si="13"/>
-        <v>13</v>
-      </c>
-      <c r="AH20" s="70">
-        <f t="shared" si="13"/>
-        <v>14</v>
-      </c>
-      <c r="AI20" s="70">
-        <f t="shared" si="13"/>
-        <v>15</v>
-      </c>
       <c r="AJ20" s="242"/>
       <c r="AL20">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <f t="shared" si="4"/>
+        <v>29</v>
       </c>
       <c r="AM20" s="10"/>
       <c r="AN20" s="17"/>
       <c r="AO20" s="17"/>
-      <c r="AS20" s="17"/>
-      <c r="AT20" s="17"/>
-      <c r="AU20" s="369"/>
-      <c r="AV20" s="140"/>
-      <c r="AW20" s="140"/>
-      <c r="AX20" s="140"/>
-      <c r="AY20" s="17"/>
+      <c r="AP20" s="17"/>
+      <c r="AQ20" s="17"/>
+      <c r="AR20" s="369"/>
+      <c r="AS20" s="140"/>
+      <c r="AT20" s="140"/>
+      <c r="AU20" s="140"/>
+      <c r="AV20" s="17"/>
+      <c r="AW20" s="366"/>
+      <c r="AX20" s="366"/>
+      <c r="AY20" s="366"/>
       <c r="AZ20" s="366"/>
       <c r="BA20" s="366"/>
-      <c r="BB20" s="366"/>
+      <c r="BB20" s="9"/>
       <c r="BD20">
-        <f t="shared" si="6"/>
-        <v>29</v>
-      </c>
-      <c r="BE20" s="10"/>
-      <c r="BF20" s="17"/>
-      <c r="BG20" s="17"/>
-      <c r="BH20" s="17"/>
-      <c r="BI20" s="17"/>
-      <c r="BJ20" s="369"/>
-      <c r="BK20" s="140"/>
-      <c r="BL20" s="140"/>
-      <c r="BM20" s="140"/>
-      <c r="BN20" s="17"/>
-      <c r="BO20" s="366"/>
-      <c r="BP20" s="366"/>
-      <c r="BQ20" s="366"/>
-      <c r="BR20" s="366"/>
-      <c r="BS20" s="366"/>
-      <c r="BT20" s="9"/>
-      <c r="BV20">
-        <v>0</v>
-      </c>
-      <c r="BW20" s="1"/>
-      <c r="BX20" s="2"/>
-      <c r="BY20" s="2"/>
-      <c r="BZ20" s="2"/>
-      <c r="CA20" s="2"/>
-      <c r="CB20" s="2"/>
-      <c r="CC20" s="361"/>
-      <c r="CD20" s="361"/>
-      <c r="CE20" s="361"/>
-      <c r="CF20" s="361"/>
-      <c r="CG20" s="2"/>
-      <c r="CH20" s="2"/>
-      <c r="CI20" s="2"/>
-      <c r="CJ20" s="2"/>
-      <c r="CK20" s="2"/>
-      <c r="CL20" s="5"/>
-    </row>
-    <row r="21" spans="1:90" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="BE20" s="1"/>
+      <c r="BF20" s="2"/>
+      <c r="BG20" s="2"/>
+      <c r="BH20" s="2"/>
+      <c r="BI20" s="2"/>
+      <c r="BJ20" s="2"/>
+      <c r="BK20" s="361"/>
+      <c r="BL20" s="361"/>
+      <c r="BM20" s="361"/>
+      <c r="BN20" s="361"/>
+      <c r="BO20" s="2"/>
+      <c r="BP20" s="2"/>
+      <c r="BQ20" s="2"/>
+      <c r="BR20" s="2"/>
+      <c r="BS20" s="2"/>
+      <c r="BT20" s="5"/>
+    </row>
+    <row r="21" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A21" s="70">
         <v>0</v>
       </c>
-      <c r="B21" s="311"/>
-      <c r="C21" s="312"/>
-      <c r="D21" s="312"/>
-      <c r="E21" s="312"/>
+      <c r="B21" s="422"/>
+      <c r="C21" s="425"/>
+      <c r="D21" s="423"/>
+      <c r="E21" s="413"/>
       <c r="F21" s="312"/>
-      <c r="G21" s="312"/>
-      <c r="H21" s="312"/>
-      <c r="I21" s="312"/>
-      <c r="J21" s="312"/>
-      <c r="K21" s="312"/>
-      <c r="L21" s="20"/>
+      <c r="G21" s="415"/>
+      <c r="H21" s="348"/>
+      <c r="I21" s="355"/>
+      <c r="J21" s="355"/>
+      <c r="K21" s="348"/>
+      <c r="L21" s="416"/>
       <c r="M21" s="312"/>
       <c r="N21" s="312"/>
       <c r="O21" s="312"/>
@@ -55567,79 +55191,62 @@
         <v>0</v>
       </c>
       <c r="AL21">
-        <f t="shared" si="5"/>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>28</v>
       </c>
       <c r="AM21" s="10"/>
       <c r="AN21" s="17"/>
       <c r="AO21" s="17"/>
-      <c r="AS21" s="17"/>
-      <c r="AT21" s="17"/>
-      <c r="AU21" s="6"/>
-      <c r="AV21" s="369"/>
-      <c r="AW21" s="140"/>
-      <c r="AX21" s="140"/>
-      <c r="AY21" s="140"/>
+      <c r="AP21" s="17"/>
+      <c r="AQ21" s="17"/>
+      <c r="AR21" s="6"/>
+      <c r="AS21" s="369"/>
+      <c r="AT21" s="140"/>
+      <c r="AU21" s="140"/>
+      <c r="AV21" s="140"/>
+      <c r="AW21" s="366"/>
+      <c r="AX21" s="366"/>
+      <c r="AY21" s="366"/>
       <c r="AZ21" s="366"/>
       <c r="BA21" s="366"/>
-      <c r="BB21" s="366"/>
+      <c r="BB21" s="9"/>
       <c r="BD21">
-        <f t="shared" si="6"/>
-        <v>28</v>
+        <f>BD20+1</f>
+        <v>1</v>
       </c>
       <c r="BE21" s="10"/>
-      <c r="BF21" s="17"/>
-      <c r="BG21" s="17"/>
-      <c r="BH21" s="17"/>
-      <c r="BI21" s="17"/>
+      <c r="BF21" s="6"/>
+      <c r="BG21" s="6"/>
+      <c r="BH21" s="6"/>
+      <c r="BI21" s="6"/>
       <c r="BJ21" s="6"/>
-      <c r="BK21" s="369"/>
-      <c r="BL21" s="140"/>
-      <c r="BM21" s="140"/>
-      <c r="BN21" s="140"/>
-      <c r="BO21" s="366"/>
-      <c r="BP21" s="366"/>
-      <c r="BQ21" s="366"/>
-      <c r="BR21" s="366"/>
-      <c r="BS21" s="366"/>
+      <c r="BK21" s="219"/>
+      <c r="BL21" s="219"/>
+      <c r="BM21" s="219"/>
+      <c r="BN21" s="219"/>
+      <c r="BO21" s="6"/>
+      <c r="BP21" s="6"/>
+      <c r="BQ21" s="6"/>
+      <c r="BR21" s="6"/>
+      <c r="BS21" s="6"/>
       <c r="BT21" s="9"/>
-      <c r="BV21">
-        <f>BV20+1</f>
-        <v>1</v>
-      </c>
-      <c r="BW21" s="10"/>
-      <c r="BX21" s="6"/>
-      <c r="BY21" s="6"/>
-      <c r="BZ21" s="6"/>
-      <c r="CA21" s="6"/>
-      <c r="CB21" s="6"/>
-      <c r="CC21" s="219"/>
-      <c r="CD21" s="219"/>
-      <c r="CE21" s="219"/>
-      <c r="CF21" s="219"/>
-      <c r="CG21" s="6"/>
-      <c r="CH21" s="6"/>
-      <c r="CI21" s="6"/>
-      <c r="CJ21" s="6"/>
-      <c r="CK21" s="6"/>
-      <c r="CL21" s="9"/>
-    </row>
-    <row r="22" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A22" s="70">
         <f>A21+1</f>
         <v>1</v>
       </c>
-      <c r="B22" s="314"/>
-      <c r="C22" s="244"/>
-      <c r="D22" s="244"/>
-      <c r="E22" s="244"/>
+      <c r="B22" s="424"/>
+      <c r="C22" s="372"/>
+      <c r="D22" s="372"/>
+      <c r="E22" s="421"/>
       <c r="F22" s="244"/>
-      <c r="G22" s="244"/>
-      <c r="H22" s="244"/>
-      <c r="I22" s="244"/>
-      <c r="J22" s="244"/>
-      <c r="K22" s="244"/>
-      <c r="L22" s="244"/>
+      <c r="G22" s="408"/>
+      <c r="H22" s="327"/>
+      <c r="I22" s="342"/>
+      <c r="J22" s="342"/>
+      <c r="K22" s="327"/>
+      <c r="L22" s="408"/>
       <c r="M22" s="244"/>
       <c r="N22" s="244"/>
       <c r="O22" s="244"/>
@@ -55670,86 +55277,69 @@
         <v>1</v>
       </c>
       <c r="AL22">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <f t="shared" si="4"/>
+        <v>27</v>
       </c>
       <c r="AM22" s="10"/>
       <c r="AN22" s="17"/>
       <c r="AO22" s="17"/>
+      <c r="AP22" s="17"/>
+      <c r="AQ22" s="6"/>
+      <c r="AR22" s="6"/>
       <c r="AS22" s="17"/>
-      <c r="AT22" s="6"/>
-      <c r="AU22" s="6"/>
-      <c r="AV22" s="17"/>
-      <c r="AW22" s="369"/>
-      <c r="AX22" s="140"/>
-      <c r="AY22" s="140"/>
-      <c r="AZ22" s="140"/>
+      <c r="AT22" s="369"/>
+      <c r="AU22" s="140"/>
+      <c r="AV22" s="140"/>
+      <c r="AW22" s="140"/>
+      <c r="AX22" s="366"/>
+      <c r="AY22" s="366"/>
+      <c r="AZ22" s="366"/>
       <c r="BA22" s="366"/>
-      <c r="BB22" s="366"/>
+      <c r="BB22" s="9"/>
       <c r="BD22">
-        <f t="shared" si="6"/>
-        <v>27</v>
+        <f t="shared" ref="BD22:BD35" si="12">BD21+1</f>
+        <v>2</v>
       </c>
       <c r="BE22" s="10"/>
       <c r="BF22" s="17"/>
       <c r="BG22" s="17"/>
       <c r="BH22" s="17"/>
-      <c r="BI22" s="6"/>
-      <c r="BJ22" s="6"/>
-      <c r="BK22" s="17"/>
-      <c r="BL22" s="369"/>
-      <c r="BM22" s="140"/>
-      <c r="BN22" s="140"/>
-      <c r="BO22" s="140"/>
-      <c r="BP22" s="366"/>
-      <c r="BQ22" s="366"/>
-      <c r="BR22" s="366"/>
-      <c r="BS22" s="366"/>
+      <c r="BI22" s="17"/>
+      <c r="BJ22" s="17"/>
+      <c r="BK22" s="226"/>
+      <c r="BL22" s="226"/>
+      <c r="BM22" s="226"/>
+      <c r="BN22" s="226"/>
+      <c r="BO22" s="6"/>
+      <c r="BP22" s="6"/>
+      <c r="BQ22" s="6"/>
+      <c r="BR22" s="6"/>
+      <c r="BS22" s="6"/>
       <c r="BT22" s="9"/>
-      <c r="BV22">
-        <f t="shared" ref="BV22:BV35" si="14">BV21+1</f>
+    </row>
+    <row r="23" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A23" s="70">
+        <f t="shared" ref="A23:A36" si="13">A22+1</f>
         <v>2</v>
       </c>
-      <c r="BW22" s="10"/>
-      <c r="BX22" s="17"/>
-      <c r="BY22" s="17"/>
-      <c r="BZ22" s="17"/>
-      <c r="CA22" s="17"/>
-      <c r="CB22" s="17"/>
-      <c r="CC22" s="226"/>
-      <c r="CD22" s="226"/>
-      <c r="CE22" s="226"/>
-      <c r="CF22" s="226"/>
-      <c r="CG22" s="6"/>
-      <c r="CH22" s="6"/>
-      <c r="CI22" s="6"/>
-      <c r="CJ22" s="6"/>
-      <c r="CK22" s="6"/>
-      <c r="CL22" s="9"/>
-    </row>
-    <row r="23" spans="1:90" x14ac:dyDescent="0.3">
-      <c r="A23" s="70">
-        <f t="shared" ref="A23:A36" si="15">A22+1</f>
-        <v>2</v>
-      </c>
-      <c r="B23" s="314"/>
-      <c r="C23" s="244"/>
-      <c r="D23" s="244"/>
-      <c r="E23" s="244"/>
+      <c r="B23" s="426"/>
+      <c r="C23" s="372"/>
+      <c r="D23" s="372"/>
+      <c r="E23" s="395"/>
       <c r="F23" s="244"/>
-      <c r="G23" s="244"/>
-      <c r="H23" s="244"/>
-      <c r="I23" s="244"/>
-      <c r="J23" s="244"/>
-      <c r="K23" s="244"/>
-      <c r="L23" s="244"/>
+      <c r="G23" s="408"/>
+      <c r="H23" s="327"/>
+      <c r="I23" s="346"/>
+      <c r="J23" s="346"/>
+      <c r="K23" s="327"/>
+      <c r="L23" s="408"/>
       <c r="M23" s="244"/>
       <c r="N23" s="244"/>
       <c r="O23" s="244"/>
       <c r="P23" s="244"/>
-      <c r="Q23" s="26"/>
+      <c r="Q23" s="9"/>
       <c r="S23" s="70">
-        <f t="shared" ref="S23:S36" si="16">S22+1</f>
+        <f t="shared" ref="S23:S36" si="14">S22+1</f>
         <v>2</v>
       </c>
       <c r="T23" s="314"/>
@@ -55769,90 +55359,73 @@
       <c r="AH23" s="244"/>
       <c r="AI23" s="9"/>
       <c r="AJ23" s="70">
-        <f t="shared" ref="AJ23:AJ36" si="17">AJ22+1</f>
+        <f t="shared" ref="AJ23:AJ36" si="15">AJ22+1</f>
         <v>2</v>
       </c>
       <c r="AL23">
-        <f t="shared" si="5"/>
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="AM23" s="10"/>
       <c r="AN23" s="6"/>
       <c r="AO23" s="6"/>
-      <c r="AS23" s="6"/>
-      <c r="AT23" s="6"/>
-      <c r="AU23" s="6"/>
-      <c r="AV23" s="17"/>
-      <c r="AW23" s="17"/>
-      <c r="AX23" s="369"/>
-      <c r="AY23" s="140"/>
-      <c r="AZ23" s="140"/>
-      <c r="BA23" s="140"/>
-      <c r="BB23" s="366"/>
+      <c r="AP23" s="6"/>
+      <c r="AQ23" s="6"/>
+      <c r="AR23" s="6"/>
+      <c r="AS23" s="17"/>
+      <c r="AT23" s="17"/>
+      <c r="AU23" s="369"/>
+      <c r="AV23" s="140"/>
+      <c r="AW23" s="140"/>
+      <c r="AX23" s="140"/>
+      <c r="AY23" s="366"/>
+      <c r="AZ23" s="366"/>
+      <c r="BA23" s="366"/>
+      <c r="BB23" s="9"/>
       <c r="BD23">
-        <f t="shared" si="6"/>
-        <v>26</v>
+        <f t="shared" si="12"/>
+        <v>3</v>
       </c>
       <c r="BE23" s="10"/>
-      <c r="BF23" s="6"/>
-      <c r="BG23" s="6"/>
-      <c r="BH23" s="6"/>
-      <c r="BI23" s="6"/>
-      <c r="BJ23" s="6"/>
-      <c r="BK23" s="17"/>
-      <c r="BL23" s="17"/>
-      <c r="BM23" s="369"/>
-      <c r="BN23" s="140"/>
-      <c r="BO23" s="140"/>
-      <c r="BP23" s="140"/>
-      <c r="BQ23" s="366"/>
-      <c r="BR23" s="366"/>
-      <c r="BS23" s="366"/>
+      <c r="BF23" s="17"/>
+      <c r="BG23" s="17"/>
+      <c r="BH23" s="17"/>
+      <c r="BI23" s="17"/>
+      <c r="BJ23" s="17"/>
+      <c r="BK23" s="226"/>
+      <c r="BL23" s="226"/>
+      <c r="BM23" s="226"/>
+      <c r="BN23" s="226"/>
+      <c r="BO23" s="6"/>
+      <c r="BP23" s="6"/>
+      <c r="BQ23" s="6"/>
+      <c r="BR23" s="6"/>
+      <c r="BS23" s="6"/>
       <c r="BT23" s="9"/>
-      <c r="BV23">
-        <f t="shared" si="14"/>
+    </row>
+    <row r="24" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A24" s="70">
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
-      <c r="BW23" s="10"/>
-      <c r="BX23" s="17"/>
-      <c r="BY23" s="17"/>
-      <c r="BZ23" s="17"/>
-      <c r="CA23" s="17"/>
-      <c r="CB23" s="17"/>
-      <c r="CC23" s="226"/>
-      <c r="CD23" s="226"/>
-      <c r="CE23" s="226"/>
-      <c r="CF23" s="226"/>
-      <c r="CG23" s="6"/>
-      <c r="CH23" s="6"/>
-      <c r="CI23" s="6"/>
-      <c r="CJ23" s="6"/>
-      <c r="CK23" s="6"/>
-      <c r="CL23" s="9"/>
-    </row>
-    <row r="24" spans="1:90" x14ac:dyDescent="0.3">
-      <c r="A24" s="70">
-        <f t="shared" si="15"/>
-        <v>3</v>
-      </c>
-      <c r="B24" s="314"/>
-      <c r="C24" s="244"/>
-      <c r="D24" s="244"/>
-      <c r="E24" s="244"/>
+      <c r="B24" s="414"/>
+      <c r="C24" s="395"/>
+      <c r="D24" s="421"/>
+      <c r="E24" s="372"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="244"/>
+      <c r="G24" s="326"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="353"/>
+      <c r="J24" s="353"/>
+      <c r="K24" s="128"/>
+      <c r="L24" s="408"/>
       <c r="M24" s="244"/>
       <c r="N24" s="244"/>
       <c r="O24" s="244"/>
       <c r="P24" s="244"/>
-      <c r="Q24" s="26"/>
+      <c r="Q24" s="9"/>
       <c r="S24" s="70">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="T24" s="314"/>
@@ -55872,88 +55445,68 @@
       <c r="AH24" s="244"/>
       <c r="AI24" s="9"/>
       <c r="AJ24" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="AL24">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="AM24" s="235"/>
-      <c r="AN24" s="342"/>
-      <c r="AO24" s="353"/>
-      <c r="AP24" s="353"/>
-      <c r="AQ24" s="342"/>
-      <c r="AR24" s="353"/>
-      <c r="AS24" s="353"/>
-      <c r="AT24" s="353"/>
-      <c r="AU24" s="353"/>
-      <c r="AV24" s="353"/>
-      <c r="AW24" s="353"/>
-      <c r="AX24" s="342"/>
-      <c r="AY24" s="369"/>
-      <c r="AZ24" s="353"/>
-      <c r="BA24" s="342"/>
-      <c r="BB24" s="233"/>
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="AM24" s="359"/>
+      <c r="AN24" s="219"/>
+      <c r="AO24" s="226"/>
+      <c r="AP24" s="226"/>
+      <c r="AQ24" s="226"/>
+      <c r="AR24" s="219"/>
+      <c r="AS24" s="363"/>
+      <c r="AT24" s="361"/>
+      <c r="AU24" s="361"/>
+      <c r="AV24" s="370"/>
+      <c r="AW24" s="219"/>
+      <c r="AX24" s="140"/>
+      <c r="AY24" s="140"/>
+      <c r="AZ24" s="226"/>
+      <c r="BA24" s="219"/>
+      <c r="BB24" s="360"/>
       <c r="BD24">
-        <f t="shared" si="6"/>
-        <v>25</v>
-      </c>
-      <c r="BE24" s="359"/>
-      <c r="BF24" s="219"/>
-      <c r="BG24" s="226"/>
-      <c r="BH24" s="226"/>
-      <c r="BI24" s="226"/>
-      <c r="BJ24" s="219"/>
-      <c r="BK24" s="363"/>
-      <c r="BL24" s="361"/>
-      <c r="BM24" s="361"/>
-      <c r="BN24" s="370"/>
-      <c r="BO24" s="219"/>
-      <c r="BP24" s="140"/>
-      <c r="BQ24" s="140"/>
-      <c r="BR24" s="226"/>
-      <c r="BS24" s="219"/>
-      <c r="BT24" s="360"/>
-      <c r="BV24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="BW24" s="10"/>
-      <c r="CC24" s="226"/>
-      <c r="CD24" s="226"/>
-      <c r="CE24" s="226"/>
-      <c r="CF24" s="226"/>
-      <c r="CG24" s="6"/>
-      <c r="CH24" s="6"/>
-      <c r="CI24" s="6"/>
-      <c r="CJ24" s="6"/>
-      <c r="CK24" s="6"/>
-      <c r="CL24" s="9"/>
-    </row>
-    <row r="25" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="BE24" s="10"/>
+      <c r="BK24" s="226"/>
+      <c r="BL24" s="226"/>
+      <c r="BM24" s="226"/>
+      <c r="BN24" s="226"/>
+      <c r="BO24" s="6"/>
+      <c r="BP24" s="6"/>
+      <c r="BQ24" s="6"/>
+      <c r="BR24" s="6"/>
+      <c r="BS24" s="6"/>
+      <c r="BT24" s="9"/>
+    </row>
+    <row r="25" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A25" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="B25" s="314"/>
       <c r="C25" s="244"/>
-      <c r="D25" s="244"/>
-      <c r="E25" s="244"/>
+      <c r="D25" s="372"/>
+      <c r="E25" s="372"/>
       <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="244"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="244"/>
+      <c r="G25" s="326"/>
+      <c r="H25" s="327"/>
+      <c r="I25" s="219"/>
+      <c r="J25" s="219"/>
+      <c r="K25" s="128"/>
+      <c r="L25" s="408"/>
       <c r="M25" s="244"/>
       <c r="N25" s="244"/>
       <c r="O25" s="244"/>
       <c r="P25" s="244"/>
-      <c r="Q25" s="26"/>
+      <c r="Q25" s="9"/>
       <c r="S25" s="70">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="T25" s="314"/>
@@ -55973,88 +55526,68 @@
       <c r="AH25" s="244"/>
       <c r="AI25" s="9"/>
       <c r="AJ25" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="AL25">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="AM25" s="345"/>
-      <c r="AN25" s="342"/>
-      <c r="AO25" s="346"/>
-      <c r="AP25" s="346"/>
-      <c r="AQ25" s="219"/>
-      <c r="AR25" s="353"/>
-      <c r="AS25" s="353"/>
-      <c r="AT25" s="353"/>
-      <c r="AU25" s="353"/>
-      <c r="AV25" s="353"/>
-      <c r="AW25" s="346"/>
-      <c r="AX25" s="342"/>
-      <c r="AY25" s="346"/>
-      <c r="AZ25" s="369"/>
-      <c r="BA25" s="342"/>
-      <c r="BB25" s="347"/>
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="AM25" s="359"/>
+      <c r="AN25" s="219"/>
+      <c r="AO25" s="226"/>
+      <c r="AP25" s="226"/>
+      <c r="AQ25" s="226"/>
+      <c r="AR25" s="219"/>
+      <c r="AS25" s="359"/>
+      <c r="AT25" s="226"/>
+      <c r="AU25" s="226"/>
+      <c r="AV25" s="360"/>
+      <c r="AW25" s="308"/>
+      <c r="AX25" s="140"/>
+      <c r="AY25" s="140"/>
+      <c r="AZ25" s="226"/>
+      <c r="BA25" s="219"/>
+      <c r="BB25" s="360"/>
       <c r="BD25">
-        <f t="shared" si="6"/>
-        <v>24</v>
-      </c>
-      <c r="BE25" s="359"/>
-      <c r="BF25" s="219"/>
-      <c r="BG25" s="226"/>
-      <c r="BH25" s="226"/>
-      <c r="BI25" s="226"/>
-      <c r="BJ25" s="219"/>
-      <c r="BK25" s="359"/>
-      <c r="BL25" s="226"/>
-      <c r="BM25" s="226"/>
-      <c r="BN25" s="360"/>
-      <c r="BO25" s="308"/>
-      <c r="BP25" s="140"/>
-      <c r="BQ25" s="140"/>
-      <c r="BR25" s="226"/>
-      <c r="BS25" s="219"/>
-      <c r="BT25" s="360"/>
-      <c r="BV25">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="BE25" s="10"/>
+      <c r="BK25" s="219"/>
+      <c r="BL25" s="219"/>
+      <c r="BM25" s="219"/>
+      <c r="BN25" s="219"/>
+      <c r="BO25" s="6"/>
+      <c r="BP25" s="6"/>
+      <c r="BQ25" s="6"/>
+      <c r="BR25" s="6"/>
+      <c r="BS25" s="6"/>
+      <c r="BT25" s="9"/>
+    </row>
+    <row r="26" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A26" s="70">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="B26" s="420"/>
+      <c r="C26" s="408"/>
+      <c r="D26" s="372"/>
+      <c r="E26" s="372"/>
+      <c r="F26" s="326"/>
+      <c r="G26" s="326"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="353"/>
+      <c r="J26" s="353"/>
+      <c r="K26" s="128"/>
+      <c r="L26" s="408"/>
+      <c r="M26" s="408"/>
+      <c r="N26" s="408"/>
+      <c r="O26" s="408"/>
+      <c r="P26" s="408"/>
+      <c r="Q26" s="417"/>
+      <c r="S26" s="70">
         <f t="shared" si="14"/>
-        <v>5</v>
-      </c>
-      <c r="BW25" s="10"/>
-      <c r="CC25" s="219"/>
-      <c r="CD25" s="219"/>
-      <c r="CE25" s="219"/>
-      <c r="CF25" s="219"/>
-      <c r="CG25" s="6"/>
-      <c r="CH25" s="6"/>
-      <c r="CI25" s="6"/>
-      <c r="CJ25" s="6"/>
-      <c r="CK25" s="6"/>
-      <c r="CL25" s="9"/>
-    </row>
-    <row r="26" spans="1:90" x14ac:dyDescent="0.3">
-      <c r="A26" s="70">
-        <f t="shared" si="15"/>
-        <v>5</v>
-      </c>
-      <c r="B26" s="314"/>
-      <c r="C26" s="244"/>
-      <c r="D26" s="244"/>
-      <c r="E26" s="244"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="244"/>
-      <c r="M26" s="244"/>
-      <c r="N26" s="244"/>
-      <c r="O26" s="244"/>
-      <c r="P26" s="244"/>
-      <c r="Q26" s="26"/>
-      <c r="S26" s="70">
-        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="T26" s="314"/>
@@ -56074,93 +55607,73 @@
       <c r="AH26" s="244"/>
       <c r="AI26" s="9"/>
       <c r="AJ26" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="AL26">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="AM26" s="345"/>
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="AM26" s="359"/>
       <c r="AN26" s="219"/>
-      <c r="AO26" s="353"/>
-      <c r="AP26" s="353"/>
-      <c r="AQ26" s="219"/>
-      <c r="AR26" s="353"/>
-      <c r="AS26" s="353"/>
-      <c r="AT26" s="353"/>
-      <c r="AU26" s="353"/>
-      <c r="AV26" s="353"/>
-      <c r="AW26" s="353"/>
-      <c r="AX26" s="219"/>
-      <c r="AY26" s="353"/>
-      <c r="AZ26" s="346"/>
-      <c r="BA26" s="369"/>
-      <c r="BB26" s="347"/>
+      <c r="AO26" s="226"/>
+      <c r="AP26" s="226"/>
+      <c r="AQ26" s="226"/>
+      <c r="AR26" s="219"/>
+      <c r="AS26" s="359"/>
+      <c r="AT26" s="226"/>
+      <c r="AU26" s="226"/>
+      <c r="AV26" s="360"/>
+      <c r="AW26" s="219"/>
+      <c r="AX26" s="371"/>
+      <c r="AY26" s="140"/>
+      <c r="AZ26" s="226"/>
+      <c r="BA26" s="219"/>
+      <c r="BB26" s="360"/>
       <c r="BD26">
-        <f t="shared" si="6"/>
-        <v>23</v>
-      </c>
-      <c r="BE26" s="359"/>
-      <c r="BF26" s="219"/>
-      <c r="BG26" s="226"/>
-      <c r="BH26" s="226"/>
-      <c r="BI26" s="226"/>
-      <c r="BJ26" s="219"/>
-      <c r="BK26" s="359"/>
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="BE26" s="16"/>
+      <c r="BF26" s="17"/>
+      <c r="BG26" s="17"/>
+      <c r="BH26" s="17"/>
+      <c r="BI26" s="17"/>
+      <c r="BJ26" s="17"/>
+      <c r="BK26" s="226"/>
       <c r="BL26" s="226"/>
       <c r="BM26" s="226"/>
-      <c r="BN26" s="360"/>
-      <c r="BO26" s="219"/>
-      <c r="BP26" s="371"/>
-      <c r="BQ26" s="140"/>
-      <c r="BR26" s="226"/>
-      <c r="BS26" s="219"/>
-      <c r="BT26" s="360"/>
-      <c r="BV26">
+      <c r="BN26" s="226"/>
+      <c r="BO26" s="17"/>
+      <c r="BP26" s="17"/>
+      <c r="BQ26" s="17"/>
+      <c r="BR26" s="17"/>
+      <c r="BS26" s="17"/>
+      <c r="BT26" s="26"/>
+    </row>
+    <row r="27" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A27" s="70">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="B27" s="127"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="128"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="128"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="353"/>
+      <c r="J27" s="353"/>
+      <c r="K27" s="128"/>
+      <c r="L27" s="128"/>
+      <c r="M27" s="128"/>
+      <c r="N27" s="128"/>
+      <c r="O27" s="128"/>
+      <c r="P27" s="128"/>
+      <c r="Q27" s="130"/>
+      <c r="S27" s="70">
         <f t="shared" si="14"/>
-        <v>6</v>
-      </c>
-      <c r="BW26" s="16"/>
-      <c r="BX26" s="17"/>
-      <c r="BY26" s="17"/>
-      <c r="BZ26" s="17"/>
-      <c r="CA26" s="17"/>
-      <c r="CB26" s="17"/>
-      <c r="CC26" s="226"/>
-      <c r="CD26" s="226"/>
-      <c r="CE26" s="226"/>
-      <c r="CF26" s="226"/>
-      <c r="CG26" s="17"/>
-      <c r="CH26" s="17"/>
-      <c r="CI26" s="17"/>
-      <c r="CJ26" s="17"/>
-      <c r="CK26" s="17"/>
-      <c r="CL26" s="26"/>
-    </row>
-    <row r="27" spans="1:90" x14ac:dyDescent="0.3">
-      <c r="A27" s="70">
-        <f t="shared" si="15"/>
-        <v>6</v>
-      </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="26"/>
-      <c r="S27" s="70">
-        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="T27" s="127"/>
@@ -56180,93 +55693,73 @@
       <c r="AH27" s="128"/>
       <c r="AI27" s="130"/>
       <c r="AJ27" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="AL27">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="AM27" s="343"/>
-      <c r="AN27" s="327"/>
-      <c r="AO27" s="327"/>
-      <c r="AP27" s="327"/>
-      <c r="AQ27" s="327"/>
-      <c r="AR27" s="327"/>
-      <c r="AS27" s="327"/>
-      <c r="AT27" s="327"/>
-      <c r="AU27" s="327"/>
-      <c r="AV27" s="327"/>
-      <c r="AW27" s="327"/>
-      <c r="AX27" s="327"/>
-      <c r="AY27" s="327"/>
-      <c r="AZ27" s="327"/>
-      <c r="BA27" s="327"/>
-      <c r="BB27" s="344"/>
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="AM27" s="308"/>
+      <c r="AN27" s="219"/>
+      <c r="AO27" s="219"/>
+      <c r="AP27" s="219"/>
+      <c r="AQ27" s="219"/>
+      <c r="AR27" s="219"/>
+      <c r="AS27" s="323"/>
+      <c r="AT27" s="218"/>
+      <c r="AU27" s="218"/>
+      <c r="AV27" s="325"/>
+      <c r="AW27" s="219"/>
+      <c r="AX27" s="219"/>
+      <c r="AY27" s="326"/>
+      <c r="AZ27" s="219"/>
+      <c r="BA27" s="219"/>
+      <c r="BB27" s="309"/>
       <c r="BD27">
-        <f t="shared" si="6"/>
-        <v>22</v>
-      </c>
-      <c r="BE27" s="308"/>
-      <c r="BF27" s="219"/>
-      <c r="BG27" s="219"/>
-      <c r="BH27" s="219"/>
-      <c r="BI27" s="219"/>
-      <c r="BJ27" s="219"/>
-      <c r="BK27" s="323"/>
-      <c r="BL27" s="218"/>
-      <c r="BM27" s="218"/>
-      <c r="BN27" s="325"/>
-      <c r="BO27" s="219"/>
-      <c r="BP27" s="219"/>
-      <c r="BQ27" s="326"/>
-      <c r="BR27" s="219"/>
-      <c r="BS27" s="219"/>
-      <c r="BT27" s="309"/>
-      <c r="BV27">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="BE27" s="16"/>
+      <c r="BF27" s="17"/>
+      <c r="BG27" s="17"/>
+      <c r="BH27" s="17"/>
+      <c r="BI27" s="17"/>
+      <c r="BJ27" s="17"/>
+      <c r="BK27" s="226"/>
+      <c r="BL27" s="226"/>
+      <c r="BM27" s="226"/>
+      <c r="BN27" s="226"/>
+      <c r="BO27" s="17"/>
+      <c r="BP27" s="17"/>
+      <c r="BQ27" s="17"/>
+      <c r="BR27" s="17"/>
+      <c r="BS27" s="17"/>
+      <c r="BT27" s="26"/>
+    </row>
+    <row r="28" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A28" s="70">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B28" s="345"/>
+      <c r="C28" s="342"/>
+      <c r="D28" s="346"/>
+      <c r="E28" s="346"/>
+      <c r="F28" s="219"/>
+      <c r="G28" s="353"/>
+      <c r="H28" s="353"/>
+      <c r="I28" s="353"/>
+      <c r="J28" s="353"/>
+      <c r="K28" s="353"/>
+      <c r="L28" s="346"/>
+      <c r="M28" s="342"/>
+      <c r="N28" s="346"/>
+      <c r="O28" s="346"/>
+      <c r="P28" s="342"/>
+      <c r="Q28" s="347"/>
+      <c r="S28" s="70">
         <f t="shared" si="14"/>
-        <v>7</v>
-      </c>
-      <c r="BW27" s="16"/>
-      <c r="BX27" s="17"/>
-      <c r="BY27" s="17"/>
-      <c r="BZ27" s="17"/>
-      <c r="CA27" s="17"/>
-      <c r="CB27" s="17"/>
-      <c r="CC27" s="226"/>
-      <c r="CD27" s="226"/>
-      <c r="CE27" s="226"/>
-      <c r="CF27" s="226"/>
-      <c r="CG27" s="17"/>
-      <c r="CH27" s="17"/>
-      <c r="CI27" s="17"/>
-      <c r="CJ27" s="17"/>
-      <c r="CK27" s="17"/>
-      <c r="CL27" s="26"/>
-    </row>
-    <row r="28" spans="1:90" x14ac:dyDescent="0.3">
-      <c r="A28" s="70">
-        <f t="shared" si="15"/>
-        <v>7</v>
-      </c>
-      <c r="B28" s="314"/>
-      <c r="C28" s="244"/>
-      <c r="D28" s="244"/>
-      <c r="E28" s="244"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="244"/>
-      <c r="M28" s="244"/>
-      <c r="N28" s="244"/>
-      <c r="O28" s="244"/>
-      <c r="P28" s="244"/>
-      <c r="Q28" s="315"/>
-      <c r="S28" s="70">
-        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="T28" s="345"/>
@@ -56286,12 +55779,12 @@
       <c r="AH28" s="342"/>
       <c r="AI28" s="347"/>
       <c r="AJ28" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="AL28">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>21</v>
       </c>
       <c r="AM28" s="10"/>
       <c r="AN28" s="6"/>
@@ -56310,69 +55803,49 @@
       <c r="BA28" s="6"/>
       <c r="BB28" s="9"/>
       <c r="BD28">
-        <f t="shared" si="6"/>
-        <v>21</v>
-      </c>
-      <c r="BE28" s="10"/>
-      <c r="BF28" s="6"/>
-      <c r="BG28" s="6"/>
-      <c r="BH28" s="6"/>
-      <c r="BI28" s="6"/>
-      <c r="BJ28" s="6"/>
-      <c r="BK28" s="17"/>
-      <c r="BL28" s="17"/>
-      <c r="BM28" s="17"/>
-      <c r="BN28" s="17"/>
-      <c r="BO28" s="6"/>
-      <c r="BP28" s="6"/>
-      <c r="BQ28" s="6"/>
-      <c r="BR28" s="6"/>
-      <c r="BS28" s="6"/>
-      <c r="BT28" s="9"/>
-      <c r="BV28">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="BE28" s="16"/>
+      <c r="BF28" s="17"/>
+      <c r="BG28" s="17"/>
+      <c r="BH28" s="17"/>
+      <c r="BI28" s="17"/>
+      <c r="BJ28" s="17"/>
+      <c r="BK28" s="226"/>
+      <c r="BL28" s="226"/>
+      <c r="BM28" s="226"/>
+      <c r="BN28" s="226"/>
+      <c r="BO28" s="17"/>
+      <c r="BP28" s="17"/>
+      <c r="BQ28" s="17"/>
+      <c r="BR28" s="17"/>
+      <c r="BS28" s="17"/>
+      <c r="BT28" s="26"/>
+    </row>
+    <row r="29" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A29" s="70">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="B29" s="345"/>
+      <c r="C29" s="219"/>
+      <c r="D29" s="353"/>
+      <c r="E29" s="353"/>
+      <c r="F29" s="219"/>
+      <c r="G29" s="353"/>
+      <c r="H29" s="353"/>
+      <c r="I29" s="353"/>
+      <c r="J29" s="353"/>
+      <c r="K29" s="353"/>
+      <c r="L29" s="353"/>
+      <c r="M29" s="219"/>
+      <c r="N29" s="353"/>
+      <c r="O29" s="346"/>
+      <c r="P29" s="342"/>
+      <c r="Q29" s="347"/>
+      <c r="S29" s="70">
         <f t="shared" si="14"/>
-        <v>8</v>
-      </c>
-      <c r="BW28" s="16"/>
-      <c r="BX28" s="17"/>
-      <c r="BY28" s="17"/>
-      <c r="BZ28" s="17"/>
-      <c r="CA28" s="17"/>
-      <c r="CB28" s="17"/>
-      <c r="CC28" s="226"/>
-      <c r="CD28" s="226"/>
-      <c r="CE28" s="226"/>
-      <c r="CF28" s="226"/>
-      <c r="CG28" s="17"/>
-      <c r="CH28" s="17"/>
-      <c r="CI28" s="17"/>
-      <c r="CJ28" s="17"/>
-      <c r="CK28" s="17"/>
-      <c r="CL28" s="26"/>
-    </row>
-    <row r="29" spans="1:90" x14ac:dyDescent="0.3">
-      <c r="A29" s="70">
-        <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
-      <c r="B29" s="314"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="244"/>
-      <c r="P29" s="244"/>
-      <c r="Q29" s="315"/>
-      <c r="S29" s="70">
-        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="T29" s="345"/>
@@ -56392,12 +55865,12 @@
       <c r="AH29" s="342"/>
       <c r="AI29" s="347"/>
       <c r="AJ29" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="AL29">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="AM29" s="10"/>
       <c r="AN29" s="6"/>
@@ -56416,69 +55889,49 @@
       <c r="BA29" s="6"/>
       <c r="BB29" s="9"/>
       <c r="BD29">
-        <f t="shared" si="6"/>
-        <v>20</v>
-      </c>
-      <c r="BE29" s="10"/>
-      <c r="BF29" s="6"/>
-      <c r="BG29" s="6"/>
-      <c r="BH29" s="6"/>
-      <c r="BI29" s="6"/>
-      <c r="BJ29" s="6"/>
-      <c r="BK29" s="17"/>
-      <c r="BL29" s="17"/>
-      <c r="BM29" s="17"/>
-      <c r="BN29" s="17"/>
-      <c r="BO29" s="6"/>
-      <c r="BP29" s="6"/>
-      <c r="BQ29" s="6"/>
-      <c r="BR29" s="6"/>
-      <c r="BS29" s="6"/>
-      <c r="BT29" s="9"/>
-      <c r="BV29">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="BE29" s="16"/>
+      <c r="BF29" s="17"/>
+      <c r="BG29" s="17"/>
+      <c r="BH29" s="17"/>
+      <c r="BI29" s="17"/>
+      <c r="BJ29" s="17"/>
+      <c r="BK29" s="226"/>
+      <c r="BL29" s="226"/>
+      <c r="BM29" s="226"/>
+      <c r="BN29" s="226"/>
+      <c r="BO29" s="17"/>
+      <c r="BP29" s="17"/>
+      <c r="BQ29" s="17"/>
+      <c r="BR29" s="17"/>
+      <c r="BS29" s="17"/>
+      <c r="BT29" s="26"/>
+    </row>
+    <row r="30" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A30" s="70">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="B30" s="343"/>
+      <c r="C30" s="327"/>
+      <c r="D30" s="327"/>
+      <c r="E30" s="327"/>
+      <c r="F30" s="327"/>
+      <c r="G30" s="327"/>
+      <c r="H30" s="327"/>
+      <c r="I30" s="346"/>
+      <c r="J30" s="346"/>
+      <c r="K30" s="327"/>
+      <c r="L30" s="327"/>
+      <c r="M30" s="327"/>
+      <c r="N30" s="327"/>
+      <c r="O30" s="327"/>
+      <c r="P30" s="327"/>
+      <c r="Q30" s="344"/>
+      <c r="S30" s="70">
         <f t="shared" si="14"/>
-        <v>9</v>
-      </c>
-      <c r="BW29" s="16"/>
-      <c r="BX29" s="17"/>
-      <c r="BY29" s="17"/>
-      <c r="BZ29" s="17"/>
-      <c r="CA29" s="17"/>
-      <c r="CB29" s="17"/>
-      <c r="CC29" s="226"/>
-      <c r="CD29" s="226"/>
-      <c r="CE29" s="226"/>
-      <c r="CF29" s="226"/>
-      <c r="CG29" s="17"/>
-      <c r="CH29" s="17"/>
-      <c r="CI29" s="17"/>
-      <c r="CJ29" s="17"/>
-      <c r="CK29" s="17"/>
-      <c r="CL29" s="26"/>
-    </row>
-    <row r="30" spans="1:90" x14ac:dyDescent="0.3">
-      <c r="A30" s="70">
-        <f t="shared" si="15"/>
-        <v>9</v>
-      </c>
-      <c r="B30" s="314"/>
-      <c r="C30" s="244"/>
-      <c r="D30" s="244"/>
-      <c r="E30" s="244"/>
-      <c r="F30" s="244"/>
-      <c r="G30" s="244"/>
-      <c r="H30" s="244"/>
-      <c r="I30" s="244"/>
-      <c r="J30" s="244"/>
-      <c r="K30" s="244"/>
-      <c r="L30" s="244"/>
-      <c r="M30" s="244"/>
-      <c r="N30" s="244"/>
-      <c r="O30" s="244"/>
-      <c r="P30" s="244"/>
-      <c r="Q30" s="315"/>
-      <c r="S30" s="70">
-        <f t="shared" si="16"/>
         <v>9</v>
       </c>
       <c r="T30" s="343"/>
@@ -56498,12 +55951,12 @@
       <c r="AH30" s="327"/>
       <c r="AI30" s="344"/>
       <c r="AJ30" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>9</v>
       </c>
       <c r="AL30">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>19</v>
       </c>
       <c r="AM30" s="10"/>
       <c r="AN30" s="6"/>
@@ -56522,67 +55975,47 @@
       <c r="BA30" s="6"/>
       <c r="BB30" s="9"/>
       <c r="BD30">
-        <f t="shared" si="6"/>
-        <v>19</v>
+        <f t="shared" si="12"/>
+        <v>10</v>
       </c>
       <c r="BE30" s="10"/>
-      <c r="BF30" s="6"/>
-      <c r="BG30" s="6"/>
-      <c r="BH30" s="6"/>
-      <c r="BI30" s="6"/>
-      <c r="BJ30" s="6"/>
-      <c r="BK30" s="17"/>
-      <c r="BL30" s="17"/>
-      <c r="BM30" s="17"/>
-      <c r="BN30" s="17"/>
+      <c r="BH30" s="34"/>
+      <c r="BI30" s="34"/>
+      <c r="BJ30" s="34"/>
+      <c r="BK30" s="219"/>
+      <c r="BL30" s="219"/>
+      <c r="BM30" s="219"/>
+      <c r="BN30" s="219"/>
       <c r="BO30" s="6"/>
       <c r="BP30" s="6"/>
       <c r="BQ30" s="6"/>
       <c r="BR30" s="6"/>
       <c r="BS30" s="6"/>
       <c r="BT30" s="9"/>
-      <c r="BV30">
+    </row>
+    <row r="31" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A31" s="70">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B31" s="419"/>
+      <c r="C31" s="408"/>
+      <c r="D31" s="408"/>
+      <c r="E31" s="408"/>
+      <c r="F31" s="408"/>
+      <c r="G31" s="408"/>
+      <c r="H31" s="327"/>
+      <c r="I31" s="346"/>
+      <c r="J31" s="346"/>
+      <c r="K31" s="327"/>
+      <c r="L31" s="408"/>
+      <c r="M31" s="408"/>
+      <c r="N31" s="408"/>
+      <c r="O31" s="408"/>
+      <c r="P31" s="408"/>
+      <c r="Q31" s="417"/>
+      <c r="S31" s="70">
         <f t="shared" si="14"/>
-        <v>10</v>
-      </c>
-      <c r="BW30" s="10"/>
-      <c r="BZ30" s="34"/>
-      <c r="CA30" s="34"/>
-      <c r="CB30" s="34"/>
-      <c r="CC30" s="219"/>
-      <c r="CD30" s="219"/>
-      <c r="CE30" s="219"/>
-      <c r="CF30" s="219"/>
-      <c r="CG30" s="6"/>
-      <c r="CH30" s="6"/>
-      <c r="CI30" s="6"/>
-      <c r="CJ30" s="6"/>
-      <c r="CK30" s="6"/>
-      <c r="CL30" s="9"/>
-    </row>
-    <row r="31" spans="1:90" x14ac:dyDescent="0.3">
-      <c r="A31" s="70">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="244"/>
-      <c r="D31" s="244"/>
-      <c r="E31" s="244"/>
-      <c r="F31" s="244"/>
-      <c r="G31" s="244"/>
-      <c r="H31" s="244"/>
-      <c r="I31" s="244"/>
-      <c r="J31" s="244"/>
-      <c r="K31" s="244"/>
-      <c r="L31" s="244"/>
-      <c r="M31" s="244"/>
-      <c r="N31" s="244"/>
-      <c r="O31" s="244"/>
-      <c r="P31" s="244"/>
-      <c r="Q31" s="26"/>
-      <c r="S31" s="70">
-        <f t="shared" si="16"/>
         <v>10</v>
       </c>
       <c r="T31" s="10"/>
@@ -56602,12 +56035,12 @@
       <c r="AH31" s="244"/>
       <c r="AI31" s="9"/>
       <c r="AJ31" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>10</v>
       </c>
       <c r="AL31">
-        <f t="shared" si="5"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>18</v>
       </c>
       <c r="AM31" s="10"/>
       <c r="AN31" s="6"/>
@@ -56626,47 +56059,27 @@
       <c r="BA31" s="6"/>
       <c r="BB31" s="9"/>
       <c r="BD31">
-        <f t="shared" si="6"/>
-        <v>18</v>
+        <f t="shared" si="12"/>
+        <v>11</v>
       </c>
       <c r="BE31" s="10"/>
-      <c r="BF31" s="6"/>
-      <c r="BG31" s="6"/>
-      <c r="BH31" s="6"/>
-      <c r="BI31" s="6"/>
-      <c r="BJ31" s="6"/>
-      <c r="BK31" s="17"/>
-      <c r="BL31" s="17"/>
-      <c r="BM31" s="17"/>
-      <c r="BN31" s="17"/>
+      <c r="BH31" s="34"/>
+      <c r="BI31" s="34"/>
+      <c r="BJ31" s="34"/>
+      <c r="BK31" s="226"/>
+      <c r="BL31" s="226"/>
+      <c r="BM31" s="226"/>
+      <c r="BN31" s="226"/>
       <c r="BO31" s="6"/>
       <c r="BP31" s="6"/>
       <c r="BQ31" s="6"/>
       <c r="BR31" s="6"/>
       <c r="BS31" s="6"/>
       <c r="BT31" s="9"/>
-      <c r="BV31">
-        <f t="shared" si="14"/>
-        <v>11</v>
-      </c>
-      <c r="BW31" s="10"/>
-      <c r="BZ31" s="34"/>
-      <c r="CA31" s="34"/>
-      <c r="CB31" s="34"/>
-      <c r="CC31" s="226"/>
-      <c r="CD31" s="226"/>
-      <c r="CE31" s="226"/>
-      <c r="CF31" s="226"/>
-      <c r="CG31" s="6"/>
-      <c r="CH31" s="6"/>
-      <c r="CI31" s="6"/>
-      <c r="CJ31" s="6"/>
-      <c r="CK31" s="6"/>
-      <c r="CL31" s="9"/>
-    </row>
-    <row r="32" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A32" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="B32" s="314"/>
@@ -56674,19 +56087,19 @@
       <c r="D32" s="244"/>
       <c r="E32" s="244"/>
       <c r="F32" s="244"/>
-      <c r="G32" s="244"/>
-      <c r="H32" s="244"/>
-      <c r="I32" s="244"/>
-      <c r="J32" s="244"/>
-      <c r="K32" s="244"/>
-      <c r="L32" s="244"/>
+      <c r="G32" s="408"/>
+      <c r="H32" s="327"/>
+      <c r="I32" s="342"/>
+      <c r="J32" s="342"/>
+      <c r="K32" s="327"/>
+      <c r="L32" s="408"/>
       <c r="M32" s="244"/>
       <c r="N32" s="244"/>
       <c r="O32" s="244"/>
       <c r="P32" s="244"/>
-      <c r="Q32" s="26"/>
+      <c r="Q32" s="9"/>
       <c r="S32" s="70">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>11</v>
       </c>
       <c r="T32" s="314"/>
@@ -56706,12 +56119,12 @@
       <c r="AH32" s="244"/>
       <c r="AI32" s="9"/>
       <c r="AJ32" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>11</v>
       </c>
       <c r="AL32">
         <f>AL33+1</f>
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="AM32" s="10"/>
       <c r="AN32" s="6"/>
@@ -56730,8 +56143,8 @@
       <c r="BA32" s="6"/>
       <c r="BB32" s="9"/>
       <c r="BD32">
-        <f>BD33+1</f>
-        <v>17</v>
+        <f t="shared" si="12"/>
+        <v>12</v>
       </c>
       <c r="BE32" s="10"/>
       <c r="BF32" s="6"/>
@@ -56739,40 +56152,20 @@
       <c r="BH32" s="6"/>
       <c r="BI32" s="6"/>
       <c r="BJ32" s="6"/>
-      <c r="BK32" s="17"/>
-      <c r="BL32" s="17"/>
-      <c r="BM32" s="17"/>
-      <c r="BN32" s="17"/>
+      <c r="BK32" s="226"/>
+      <c r="BL32" s="226"/>
+      <c r="BM32" s="226"/>
+      <c r="BN32" s="226"/>
       <c r="BO32" s="6"/>
       <c r="BP32" s="6"/>
       <c r="BQ32" s="6"/>
       <c r="BR32" s="6"/>
       <c r="BS32" s="6"/>
       <c r="BT32" s="9"/>
-      <c r="BV32">
-        <f t="shared" si="14"/>
-        <v>12</v>
-      </c>
-      <c r="BW32" s="10"/>
-      <c r="BX32" s="6"/>
-      <c r="BY32" s="6"/>
-      <c r="BZ32" s="6"/>
-      <c r="CA32" s="6"/>
-      <c r="CB32" s="6"/>
-      <c r="CC32" s="226"/>
-      <c r="CD32" s="226"/>
-      <c r="CE32" s="226"/>
-      <c r="CF32" s="226"/>
-      <c r="CG32" s="6"/>
-      <c r="CH32" s="6"/>
-      <c r="CI32" s="6"/>
-      <c r="CJ32" s="6"/>
-      <c r="CK32" s="6"/>
-      <c r="CL32" s="9"/>
-    </row>
-    <row r="33" spans="1:90" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A33" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>12</v>
       </c>
       <c r="B33" s="314"/>
@@ -56780,19 +56173,19 @@
       <c r="D33" s="244"/>
       <c r="E33" s="244"/>
       <c r="F33" s="244"/>
-      <c r="G33" s="244"/>
-      <c r="H33" s="244"/>
-      <c r="I33" s="244"/>
-      <c r="J33" s="244"/>
-      <c r="K33" s="244"/>
-      <c r="L33" s="244"/>
+      <c r="G33" s="408"/>
+      <c r="H33" s="327"/>
+      <c r="I33" s="346"/>
+      <c r="J33" s="346"/>
+      <c r="K33" s="327"/>
+      <c r="L33" s="408"/>
       <c r="M33" s="244"/>
       <c r="N33" s="244"/>
       <c r="O33" s="244"/>
       <c r="P33" s="244"/>
-      <c r="Q33" s="26"/>
+      <c r="Q33" s="9"/>
       <c r="S33" s="70">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>12</v>
       </c>
       <c r="T33" s="314"/>
@@ -56812,11 +56205,11 @@
       <c r="AH33" s="244"/>
       <c r="AI33" s="9"/>
       <c r="AJ33" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="AL33">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AM33" s="13"/>
       <c r="AN33" s="14"/>
@@ -56835,48 +56228,29 @@
       <c r="BA33" s="14"/>
       <c r="BB33" s="15"/>
       <c r="BD33">
-        <v>16</v>
-      </c>
-      <c r="BE33" s="13"/>
-      <c r="BF33" s="14"/>
-      <c r="BG33" s="14"/>
-      <c r="BH33" s="14"/>
-      <c r="BI33" s="14"/>
-      <c r="BJ33" s="14"/>
-      <c r="BK33" s="22"/>
-      <c r="BL33" s="22"/>
-      <c r="BM33" s="22"/>
-      <c r="BN33" s="22"/>
-      <c r="BO33" s="14"/>
-      <c r="BP33" s="14"/>
-      <c r="BQ33" s="14"/>
-      <c r="BR33" s="14"/>
-      <c r="BS33" s="14"/>
-      <c r="BT33" s="15"/>
-      <c r="BV33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
-      <c r="BW33" s="10"/>
-      <c r="BX33" s="6"/>
-      <c r="BY33" s="6"/>
-      <c r="BZ33" s="6"/>
-      <c r="CA33" s="6"/>
-      <c r="CB33" s="6"/>
-      <c r="CC33" s="226"/>
-      <c r="CD33" s="226"/>
-      <c r="CE33" s="226"/>
-      <c r="CF33" s="226"/>
-      <c r="CG33" s="6"/>
-      <c r="CH33" s="6"/>
-      <c r="CI33" s="6"/>
-      <c r="CJ33" s="6"/>
-      <c r="CK33" s="6"/>
-      <c r="CL33" s="9"/>
-    </row>
-    <row r="34" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="BE33" s="10"/>
+      <c r="BF33" s="6"/>
+      <c r="BG33" s="6"/>
+      <c r="BH33" s="6"/>
+      <c r="BI33" s="6"/>
+      <c r="BJ33" s="6"/>
+      <c r="BK33" s="226"/>
+      <c r="BL33" s="226"/>
+      <c r="BM33" s="226"/>
+      <c r="BN33" s="226"/>
+      <c r="BO33" s="6"/>
+      <c r="BP33" s="6"/>
+      <c r="BQ33" s="6"/>
+      <c r="BR33" s="6"/>
+      <c r="BS33" s="6"/>
+      <c r="BT33" s="9"/>
+    </row>
+    <row r="34" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A34" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>13</v>
       </c>
       <c r="B34" s="314"/>
@@ -56884,19 +56258,19 @@
       <c r="D34" s="244"/>
       <c r="E34" s="244"/>
       <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="244"/>
+      <c r="G34" s="326"/>
+      <c r="H34" s="128"/>
+      <c r="I34" s="353"/>
+      <c r="J34" s="353"/>
+      <c r="K34" s="128"/>
+      <c r="L34" s="408"/>
       <c r="M34" s="244"/>
       <c r="N34" s="244"/>
       <c r="O34" s="17"/>
       <c r="P34" s="17"/>
-      <c r="Q34" s="26"/>
+      <c r="Q34" s="9"/>
       <c r="S34" s="70">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>13</v>
       </c>
       <c r="T34" s="314"/>
@@ -56916,33 +56290,33 @@
       <c r="AH34" s="17"/>
       <c r="AI34" s="9"/>
       <c r="AJ34" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>13</v>
       </c>
-      <c r="BV34">
-        <f t="shared" si="14"/>
+      <c r="BD34">
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
-      <c r="BW34" s="10"/>
-      <c r="BX34" s="6"/>
-      <c r="BY34" s="6"/>
-      <c r="BZ34" s="6"/>
-      <c r="CA34" s="6"/>
-      <c r="CB34" s="6"/>
-      <c r="CC34" s="219"/>
-      <c r="CD34" s="219"/>
-      <c r="CE34" s="219"/>
-      <c r="CF34" s="219"/>
-      <c r="CG34" s="6"/>
-      <c r="CH34" s="6"/>
-      <c r="CI34" s="6"/>
-      <c r="CJ34" s="6"/>
-      <c r="CK34" s="6"/>
-      <c r="CL34" s="9"/>
-    </row>
-    <row r="35" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="BE34" s="10"/>
+      <c r="BF34" s="6"/>
+      <c r="BG34" s="6"/>
+      <c r="BH34" s="6"/>
+      <c r="BI34" s="6"/>
+      <c r="BJ34" s="6"/>
+      <c r="BK34" s="219"/>
+      <c r="BL34" s="219"/>
+      <c r="BM34" s="219"/>
+      <c r="BN34" s="219"/>
+      <c r="BO34" s="6"/>
+      <c r="BP34" s="6"/>
+      <c r="BQ34" s="6"/>
+      <c r="BR34" s="6"/>
+      <c r="BS34" s="6"/>
+      <c r="BT34" s="9"/>
+    </row>
+    <row r="35" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A35" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
       <c r="B35" s="16"/>
@@ -56950,19 +56324,19 @@
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
+      <c r="G35" s="326"/>
+      <c r="H35" s="128"/>
+      <c r="I35" s="219"/>
+      <c r="J35" s="219"/>
+      <c r="K35" s="128"/>
+      <c r="L35" s="326"/>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
       <c r="O35" s="17"/>
       <c r="P35" s="17"/>
-      <c r="Q35" s="26"/>
+      <c r="Q35" s="9"/>
       <c r="S35" s="70">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="T35" s="16"/>
@@ -56982,53 +56356,53 @@
       <c r="AH35" s="17"/>
       <c r="AI35" s="9"/>
       <c r="AJ35" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>14</v>
       </c>
-      <c r="BV35">
-        <f t="shared" si="14"/>
+      <c r="BD35">
+        <f t="shared" si="12"/>
         <v>15</v>
       </c>
-      <c r="BW35" s="13"/>
-      <c r="BX35" s="14"/>
-      <c r="BY35" s="14"/>
-      <c r="BZ35" s="14"/>
-      <c r="CA35" s="14"/>
-      <c r="CB35" s="14"/>
-      <c r="CC35" s="358"/>
-      <c r="CD35" s="358"/>
-      <c r="CE35" s="358"/>
-      <c r="CF35" s="358"/>
-      <c r="CG35" s="14"/>
-      <c r="CH35" s="14"/>
-      <c r="CI35" s="14"/>
-      <c r="CJ35" s="14"/>
-      <c r="CK35" s="14"/>
-      <c r="CL35" s="15"/>
-    </row>
-    <row r="36" spans="1:90" x14ac:dyDescent="0.3">
+      <c r="BE35" s="13"/>
+      <c r="BF35" s="14"/>
+      <c r="BG35" s="14"/>
+      <c r="BH35" s="14"/>
+      <c r="BI35" s="14"/>
+      <c r="BJ35" s="14"/>
+      <c r="BK35" s="358"/>
+      <c r="BL35" s="358"/>
+      <c r="BM35" s="358"/>
+      <c r="BN35" s="358"/>
+      <c r="BO35" s="14"/>
+      <c r="BP35" s="14"/>
+      <c r="BQ35" s="14"/>
+      <c r="BR35" s="14"/>
+      <c r="BS35" s="14"/>
+      <c r="BT35" s="15"/>
+    </row>
+    <row r="36" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A36" s="70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
       <c r="B36" s="32"/>
       <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="317"/>
-      <c r="I36" s="317"/>
-      <c r="J36" s="317"/>
-      <c r="K36" s="317"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="22"/>
-      <c r="Q36" s="33"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="418"/>
+      <c r="H36" s="350"/>
+      <c r="I36" s="354"/>
+      <c r="J36" s="354"/>
+      <c r="K36" s="350"/>
+      <c r="L36" s="418"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="15"/>
       <c r="S36" s="70">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="T36" s="32"/>
@@ -57048,11 +56422,11 @@
       <c r="AH36" s="14"/>
       <c r="AI36" s="15"/>
       <c r="AJ36" s="70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:90" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A37" s="242" t="s">
         <v>395</v>
       </c>
@@ -64056,7 +63430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Reworked the ore system... still needs to be optimized but it will do Fluids are a bit safer
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -3679,7 +3679,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:N15" ca="1" si="7">IF(AND(MOD(E$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="Y6">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4249,7 +4249,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4269,7 +4269,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4289,7 +4289,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4329,7 +4329,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4819,7 +4819,7 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:N29" ca="1" si="11">IF(AND(MOD(E$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4839,7 +4839,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4859,7 +4859,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4879,7 +4879,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4899,7 +4899,7 @@
       </c>
       <c r="Y16">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5449,7 +5449,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5959,7 +5959,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5979,7 +5979,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -53239,7 +53239,7 @@
   <dimension ref="A1:BT37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="N33" sqref="N33:P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Reworked the Ore populator for the last time... dammit! Fixed a block before chunk populator issue Roads have black wool instead of stone... good idea or not? Bumped the version to 1.02 I think I made CityWorld work with 1.6 again... maybe
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="7" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="36" activeTab="42"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="455">
   <si>
     <t>grove</t>
   </si>
@@ -1389,11 +1389,57 @@
   <si>
     <t>Street names</t>
   </si>
+  <si>
+    <t>BlocksPY</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>BlocksPR</t>
+  </si>
+  <si>
+    <t>Grav</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Lapis</t>
+  </si>
+  <si>
+    <t>Redstone</t>
+  </si>
+  <si>
+    <t>Diamond</t>
+  </si>
+  <si>
+    <t>ore_maxY</t>
+  </si>
+  <si>
+    <t>ore_minY</t>
+  </si>
+  <si>
+    <t>ore_amount</t>
+  </si>
+  <si>
+    <t>ore_iterations</t>
+  </si>
+  <si>
+    <t>BlocksPS</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="0.0000%"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1948,7 +1994,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="427">
+  <cellXfs count="436">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2657,9 +2703,6 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
@@ -2693,6 +2736,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="50" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3690,7 +3763,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:N15" ca="1" si="7">IF(AND(MOD(E$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3710,7 +3783,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3730,7 +3803,7 @@
       </c>
       <c r="O6">
         <f t="shared" ref="O6:AB15" ca="1" si="8">IF(AND(MOD(O$5,block)=0,MOD($D6,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3750,7 +3823,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -3770,7 +3843,7 @@
       </c>
       <c r="Y6">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4260,7 +4333,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4280,7 +4353,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4320,7 +4393,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4340,7 +4413,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4850,7 +4923,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4870,7 +4943,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5400,7 +5473,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5460,7 +5533,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5480,7 +5553,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5970,7 +6043,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5990,7 +6063,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -6010,7 +6083,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -15490,7 +15563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
@@ -19013,11 +19086,11 @@
         <v>0</v>
       </c>
       <c r="G131">
-        <f t="shared" ref="G131:G180" si="10">COUNTIF(F$1:F$1000, F131)</f>
+        <f t="shared" ref="G131:G149" si="10">COUNTIF(F$1:F$1000, F131)</f>
         <v>0</v>
       </c>
       <c r="I131">
-        <f t="shared" ref="I131:I180" si="11">COUNTIF(H$1:H$1000, H131)</f>
+        <f t="shared" ref="I131:I149" si="11">COUNTIF(H$1:H$1000, H131)</f>
         <v>0</v>
       </c>
       <c r="L131">
@@ -59357,17 +59430,17 @@
       <c r="A21" s="70">
         <v>0</v>
       </c>
-      <c r="B21" s="422"/>
-      <c r="C21" s="425"/>
-      <c r="D21" s="423"/>
-      <c r="E21" s="413"/>
+      <c r="B21" s="421"/>
+      <c r="C21" s="424"/>
+      <c r="D21" s="422"/>
+      <c r="E21" s="412"/>
       <c r="F21" s="312"/>
-      <c r="G21" s="415"/>
+      <c r="G21" s="414"/>
       <c r="H21" s="348"/>
       <c r="I21" s="355"/>
       <c r="J21" s="355"/>
       <c r="K21" s="348"/>
-      <c r="L21" s="416"/>
+      <c r="L21" s="415"/>
       <c r="M21" s="312"/>
       <c r="N21" s="312"/>
       <c r="O21" s="312"/>
@@ -59441,10 +59514,10 @@
         <f>A21+1</f>
         <v>1</v>
       </c>
-      <c r="B22" s="424"/>
+      <c r="B22" s="423"/>
       <c r="C22" s="372"/>
       <c r="D22" s="372"/>
-      <c r="E22" s="421"/>
+      <c r="E22" s="420"/>
       <c r="F22" s="244"/>
       <c r="G22" s="408"/>
       <c r="H22" s="327"/>
@@ -59527,7 +59600,7 @@
         <f t="shared" ref="A23:A36" si="13">A22+1</f>
         <v>2</v>
       </c>
-      <c r="B23" s="426"/>
+      <c r="B23" s="425"/>
       <c r="C23" s="372"/>
       <c r="D23" s="372"/>
       <c r="E23" s="395"/>
@@ -59613,9 +59686,9 @@
         <f t="shared" si="13"/>
         <v>3</v>
       </c>
-      <c r="B24" s="414"/>
+      <c r="B24" s="413"/>
       <c r="C24" s="395"/>
-      <c r="D24" s="421"/>
+      <c r="D24" s="420"/>
       <c r="E24" s="372"/>
       <c r="F24" s="17"/>
       <c r="G24" s="326"/>
@@ -59775,7 +59848,7 @@
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
-      <c r="B26" s="420"/>
+      <c r="B26" s="419"/>
       <c r="C26" s="408"/>
       <c r="D26" s="372"/>
       <c r="E26" s="372"/>
@@ -59790,7 +59863,7 @@
       <c r="N26" s="408"/>
       <c r="O26" s="408"/>
       <c r="P26" s="408"/>
-      <c r="Q26" s="417"/>
+      <c r="Q26" s="416"/>
       <c r="S26" s="70">
         <f t="shared" si="14"/>
         <v>5</v>
@@ -60203,7 +60276,7 @@
         <f t="shared" si="13"/>
         <v>10</v>
       </c>
-      <c r="B31" s="419"/>
+      <c r="B31" s="418"/>
       <c r="C31" s="408"/>
       <c r="D31" s="408"/>
       <c r="E31" s="408"/>
@@ -60218,7 +60291,7 @@
       <c r="N31" s="408"/>
       <c r="O31" s="408"/>
       <c r="P31" s="408"/>
-      <c r="Q31" s="417"/>
+      <c r="Q31" s="416"/>
       <c r="S31" s="70">
         <f t="shared" si="14"/>
         <v>10</v>
@@ -60595,12 +60668,12 @@
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
-      <c r="G36" s="418"/>
+      <c r="G36" s="417"/>
       <c r="H36" s="350"/>
       <c r="I36" s="354"/>
       <c r="J36" s="354"/>
       <c r="K36" s="350"/>
-      <c r="L36" s="418"/>
+      <c r="L36" s="417"/>
       <c r="M36" s="14"/>
       <c r="N36" s="14"/>
       <c r="O36" s="14"/>
@@ -67400,2422 +67473,1422 @@
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB36"/>
+  <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2328" topLeftCell="O1" activePane="topRight"/>
+      <selection activeCell="P30" sqref="P30"/>
+      <selection pane="topRight" activeCell="AB23" sqref="AB23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="426"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A1" s="242"/>
-      <c r="B1" s="70">
-        <v>0</v>
-      </c>
-      <c r="C1" s="70">
-        <f t="shared" ref="C1:Q1" si="0">B1+1</f>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B1" s="305"/>
+      <c r="C1" s="305"/>
+      <c r="D1" s="305"/>
+      <c r="E1" s="305"/>
+      <c r="F1" s="305"/>
+      <c r="G1" s="305"/>
+      <c r="H1" s="305"/>
+      <c r="I1" s="305"/>
+      <c r="J1" s="305"/>
+      <c r="K1" s="305"/>
+      <c r="L1" s="305"/>
+      <c r="M1" s="305"/>
+      <c r="N1" s="305"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B2" s="305"/>
+      <c r="C2" s="305"/>
+      <c r="D2" s="305"/>
+      <c r="E2" s="305"/>
+      <c r="F2" s="305"/>
+      <c r="G2" s="305"/>
+      <c r="H2" s="305"/>
+      <c r="I2" s="305"/>
+      <c r="J2" s="305"/>
+      <c r="K2" s="305"/>
+      <c r="L2" s="305"/>
+      <c r="M2" s="305"/>
+      <c r="N2" s="305"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="305"/>
+      <c r="C3" s="305">
+        <v>16</v>
+      </c>
+      <c r="D3" s="305"/>
+      <c r="E3" s="305"/>
+      <c r="F3" s="305"/>
+      <c r="G3" s="305"/>
+      <c r="H3" s="305"/>
+      <c r="I3" s="305"/>
+      <c r="J3" s="305"/>
+      <c r="K3" s="305"/>
+      <c r="L3" s="305"/>
+      <c r="M3" s="305"/>
+      <c r="N3" s="305"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="305"/>
+      <c r="B4" s="305"/>
+      <c r="C4" s="305">
+        <v>16</v>
+      </c>
+      <c r="D4" s="305"/>
+      <c r="E4" s="305"/>
+      <c r="F4" s="305"/>
+      <c r="G4" s="305"/>
+      <c r="H4" s="305"/>
+      <c r="I4" s="305"/>
+      <c r="J4" s="305"/>
+      <c r="K4" s="305"/>
+      <c r="L4" s="305"/>
+      <c r="M4" s="305"/>
+      <c r="N4" s="305"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="305"/>
+      <c r="B5" s="305"/>
+      <c r="C5" s="305">
+        <v>16</v>
+      </c>
+      <c r="D5" s="305"/>
+      <c r="E5" s="305"/>
+      <c r="F5" s="305"/>
+      <c r="G5" s="305"/>
+      <c r="H5" s="305"/>
+      <c r="I5" s="305"/>
+      <c r="J5" s="305"/>
+      <c r="K5" s="305"/>
+      <c r="L5" s="305"/>
+      <c r="M5" s="305"/>
+      <c r="N5" s="305"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="305"/>
+      <c r="B6" s="305"/>
+      <c r="C6" s="305">
+        <f>C4*C5</f>
+        <v>256</v>
+      </c>
+      <c r="D6" s="305"/>
+      <c r="E6" s="305"/>
+      <c r="F6" s="305"/>
+      <c r="G6" s="305"/>
+      <c r="H6" s="305"/>
+      <c r="I6" s="305"/>
+      <c r="J6" s="305"/>
+      <c r="K6" s="305"/>
+      <c r="L6" s="305"/>
+      <c r="M6" s="305"/>
+      <c r="N6" s="305"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="305"/>
+      <c r="B7" s="305"/>
+      <c r="C7" s="305"/>
+      <c r="D7" s="305"/>
+      <c r="H7" s="305"/>
+      <c r="I7" s="305"/>
+      <c r="J7" s="305"/>
+      <c r="K7" s="305"/>
+      <c r="L7" s="305"/>
+      <c r="M7" s="305"/>
+      <c r="N7" s="305"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="305"/>
+      <c r="B8" s="305" t="s">
+        <v>342</v>
+      </c>
+      <c r="C8" s="305" t="s">
+        <v>441</v>
+      </c>
+      <c r="D8" s="426" t="s">
+        <v>453</v>
+      </c>
+      <c r="I8" s="427" t="s">
+        <v>449</v>
+      </c>
+      <c r="J8" s="427" t="s">
+        <v>450</v>
+      </c>
+      <c r="K8" s="305" t="s">
+        <v>442</v>
+      </c>
+      <c r="L8" s="305" t="s">
+        <v>443</v>
+      </c>
+      <c r="M8" s="427" t="s">
+        <v>451</v>
+      </c>
+      <c r="N8" s="427" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="305" t="s">
+        <v>444</v>
+      </c>
+      <c r="B9" s="428">
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="429">
+        <f t="shared" ref="C9:C17" si="0">$C$6*B9</f>
+        <v>2.56</v>
+      </c>
+      <c r="D9" s="430">
+        <f>C9*$C$3</f>
+        <v>40.96</v>
+      </c>
+      <c r="H9" s="430"/>
+      <c r="I9" s="305">
+        <v>96</v>
+      </c>
+      <c r="J9" s="305">
+        <v>40</v>
+      </c>
+      <c r="K9" s="431">
+        <f>I9-J9</f>
+        <v>56</v>
+      </c>
+      <c r="L9" s="305">
+        <f>K9*C9</f>
+        <v>143.36000000000001</v>
+      </c>
+      <c r="M9" s="431">
+        <f>L9/N9</f>
+        <v>8.4329411764705888</v>
+      </c>
+      <c r="N9" s="435">
+        <v>17</v>
+      </c>
+      <c r="O9" s="426">
+        <v>40</v>
+      </c>
+      <c r="P9" s="430">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="426">
+        <f>O9*P9</f>
+        <v>320</v>
+      </c>
+      <c r="R9" s="434">
+        <f>Q9/K9</f>
+        <v>5.7142857142857144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="305" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="428">
+        <v>0.01</v>
+      </c>
+      <c r="C10" s="429">
+        <f t="shared" si="0"/>
+        <v>2.56</v>
+      </c>
+      <c r="D10" s="430">
+        <f t="shared" ref="D10:D17" si="1">C10*$C$3</f>
+        <v>40.96</v>
+      </c>
+      <c r="H10" s="430"/>
+      <c r="I10" s="305">
+        <v>64</v>
+      </c>
+      <c r="J10" s="305">
+        <v>40</v>
+      </c>
+      <c r="K10" s="431">
+        <f t="shared" ref="K10" si="2">I10-J10</f>
+        <v>24</v>
+      </c>
+      <c r="L10" s="305">
+        <f>K10*C10</f>
+        <v>61.44</v>
+      </c>
+      <c r="M10" s="431">
+        <f t="shared" ref="M10" si="3">L10/N10</f>
+        <v>7.68</v>
+      </c>
+      <c r="N10" s="435">
+        <v>8</v>
+      </c>
+      <c r="O10" s="426">
+        <v>8</v>
+      </c>
+      <c r="P10" s="430">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="426">
+        <f t="shared" ref="Q10:Q17" si="4">O10*P10</f>
+        <v>64</v>
+      </c>
+      <c r="R10" s="434">
+        <f>Q10/K10</f>
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="305" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="428">
+        <v>0.01</v>
+      </c>
+      <c r="C11" s="429">
+        <f t="shared" si="0"/>
+        <v>2.56</v>
+      </c>
+      <c r="D11" s="430">
+        <f t="shared" si="1"/>
+        <v>40.96</v>
+      </c>
+      <c r="H11" s="430"/>
+      <c r="I11" s="305">
+        <v>80</v>
+      </c>
+      <c r="J11" s="305">
+        <v>48</v>
+      </c>
+      <c r="K11" s="431">
+        <f>I11-J11</f>
+        <v>32</v>
+      </c>
+      <c r="L11" s="305">
+        <f>K11*C11</f>
+        <v>81.92</v>
+      </c>
+      <c r="M11" s="431">
+        <f>L11/N11</f>
+        <v>8.1920000000000002</v>
+      </c>
+      <c r="N11" s="435">
+        <v>10</v>
+      </c>
+      <c r="O11" s="426">
+        <v>10</v>
+      </c>
+      <c r="P11" s="430">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="426">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="R11" s="434">
+        <f>Q11/K11</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="305" t="s">
+        <v>445</v>
+      </c>
+      <c r="B12" s="428">
+        <v>0.01</v>
+      </c>
+      <c r="C12" s="429">
+        <f t="shared" si="0"/>
+        <v>2.56</v>
+      </c>
+      <c r="D12" s="430">
+        <f t="shared" si="1"/>
+        <v>40.96</v>
+      </c>
+      <c r="H12" s="430"/>
+      <c r="I12" s="305">
+        <v>128</v>
+      </c>
+      <c r="J12" s="305">
+        <v>16</v>
+      </c>
+      <c r="K12" s="431">
+        <f>I12-J12</f>
+        <v>112</v>
+      </c>
+      <c r="L12" s="305">
+        <f>K12*C12</f>
+        <v>286.72000000000003</v>
+      </c>
+      <c r="M12" s="431">
+        <f t="shared" ref="M12:M17" si="5">L12/N12</f>
+        <v>8.1920000000000002</v>
+      </c>
+      <c r="N12" s="435">
+        <v>35</v>
+      </c>
+      <c r="O12" s="426">
+        <v>35</v>
+      </c>
+      <c r="P12" s="430">
+        <v>8</v>
+      </c>
+      <c r="Q12" s="426">
+        <f t="shared" si="4"/>
+        <v>280</v>
+      </c>
+      <c r="R12" s="434">
+        <f>Q12/K12</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="305" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="428">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C13" s="429">
+        <f t="shared" si="0"/>
+        <v>1.536</v>
+      </c>
+      <c r="D13" s="430">
+        <f t="shared" si="1"/>
+        <v>24.576000000000001</v>
+      </c>
+      <c r="H13" s="430"/>
+      <c r="I13" s="305">
+        <v>68</v>
+      </c>
+      <c r="J13" s="305">
+        <v>16</v>
+      </c>
+      <c r="K13" s="431">
+        <f t="shared" ref="K13:K17" si="6">I13-J13</f>
+        <v>52</v>
+      </c>
+      <c r="L13" s="305">
+        <f>K13*C13</f>
+        <v>79.872</v>
+      </c>
+      <c r="M13" s="431">
+        <f t="shared" si="5"/>
+        <v>7.9871999999999996</v>
+      </c>
+      <c r="N13" s="435">
+        <v>10</v>
+      </c>
+      <c r="O13" s="426">
+        <v>12</v>
+      </c>
+      <c r="P13" s="430">
+        <v>8</v>
+      </c>
+      <c r="Q13" s="426">
+        <f t="shared" si="4"/>
+        <v>96</v>
+      </c>
+      <c r="R13" s="434">
+        <f>Q13/K13</f>
+        <v>1.8461538461538463</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="305" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="428">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C14" s="429">
+        <f t="shared" si="0"/>
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="D14" s="430">
+        <f t="shared" si="1"/>
+        <v>6.1440000000000001</v>
+      </c>
+      <c r="H14" s="430"/>
+      <c r="I14" s="305">
+        <v>34</v>
+      </c>
+      <c r="J14" s="305">
+        <v>5</v>
+      </c>
+      <c r="K14" s="431">
+        <f t="shared" si="6"/>
+        <v>29</v>
+      </c>
+      <c r="L14" s="305">
+        <f>K14*C14</f>
+        <v>11.136000000000001</v>
+      </c>
+      <c r="M14" s="431">
+        <f t="shared" si="5"/>
+        <v>3.7120000000000002</v>
+      </c>
+      <c r="N14" s="435">
+        <v>3</v>
+      </c>
+      <c r="O14" s="426">
+        <v>4</v>
+      </c>
+      <c r="P14" s="430">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="426">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="R14" s="434">
+        <f>Q14/K14</f>
+        <v>0.41379310344827586</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="305" t="s">
+        <v>446</v>
+      </c>
+      <c r="B15" s="428">
+        <v>1.4E-3</v>
+      </c>
+      <c r="C15" s="429">
+        <f t="shared" si="0"/>
+        <v>0.3584</v>
+      </c>
+      <c r="D15" s="430">
+        <f t="shared" si="1"/>
+        <v>5.7343999999999999</v>
+      </c>
+      <c r="H15" s="430"/>
+      <c r="I15" s="305">
+        <v>30</v>
+      </c>
+      <c r="J15" s="305">
+        <v>5</v>
+      </c>
+      <c r="K15" s="431">
+        <f>I15-J15</f>
+        <v>25</v>
+      </c>
+      <c r="L15" s="305">
+        <f>K15*C15</f>
+        <v>8.9599999999999991</v>
+      </c>
+      <c r="M15" s="431">
+        <f>L15/N15</f>
+        <v>4.4799999999999995</v>
+      </c>
+      <c r="N15" s="435">
+        <v>2</v>
+      </c>
+      <c r="O15" s="426">
+        <v>3</v>
+      </c>
+      <c r="P15" s="430">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="426">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="R15" s="434">
+        <f>Q15/K15</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="305" t="s">
+        <v>447</v>
+      </c>
+      <c r="B16" s="428">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C16" s="429">
+        <f t="shared" si="0"/>
+        <v>2.048</v>
+      </c>
+      <c r="D16" s="430">
+        <f t="shared" si="1"/>
+        <v>32.768000000000001</v>
+      </c>
+      <c r="H16" s="430"/>
+      <c r="I16" s="305">
+        <v>17</v>
+      </c>
+      <c r="J16" s="305">
+        <v>8</v>
+      </c>
+      <c r="K16" s="431">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="L16" s="305">
+        <f>K16*C16</f>
+        <v>18.432000000000002</v>
+      </c>
+      <c r="M16" s="431">
+        <f t="shared" si="5"/>
+        <v>3.6864000000000003</v>
+      </c>
+      <c r="N16" s="435">
+        <v>5</v>
+      </c>
+      <c r="O16" s="426">
+        <v>6</v>
+      </c>
+      <c r="P16" s="430">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="426">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="R16" s="434">
+        <f>Q16/K16</f>
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A17" s="305" t="s">
+        <v>448</v>
+      </c>
+      <c r="B17" s="428">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C17" s="429">
+        <f t="shared" si="0"/>
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="D17" s="430">
+        <f t="shared" si="1"/>
+        <v>6.1440000000000001</v>
+      </c>
+      <c r="H17" s="430"/>
+      <c r="I17" s="305">
+        <v>16</v>
+      </c>
+      <c r="J17" s="305">
         <v>1</v>
       </c>
-      <c r="D1" s="70">
-        <f t="shared" si="0"/>
+      <c r="K17" s="431">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="L17" s="305">
+        <f>K17*C17</f>
+        <v>5.76</v>
+      </c>
+      <c r="M17" s="431">
+        <f t="shared" si="5"/>
+        <v>2.88</v>
+      </c>
+      <c r="N17" s="435">
         <v>2</v>
       </c>
-      <c r="E1" s="70">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F1" s="70">
-        <f t="shared" si="0"/>
+      <c r="O17" s="426">
+        <v>2</v>
+      </c>
+      <c r="P17" s="430">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="426">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="G1" s="70">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H1" s="70">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I1" s="70">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="J1" s="70">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K1" s="70">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="L1" s="70">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="M1" s="70">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="N1" s="70">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="O1" s="70">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="P1" s="70">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="Q1" s="70">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="R1" s="242" t="s">
-        <v>394</v>
-      </c>
-      <c r="S1" s="242"/>
-      <c r="T1" s="70">
-        <v>0</v>
-      </c>
-      <c r="U1" s="70">
-        <f t="shared" ref="U1" si="1">T1+1</f>
-        <v>1</v>
-      </c>
-      <c r="V1" s="70">
-        <f t="shared" ref="V1" si="2">U1+1</f>
-        <v>2</v>
-      </c>
-      <c r="W1" s="70">
-        <f t="shared" ref="W1" si="3">V1+1</f>
-        <v>3</v>
-      </c>
-      <c r="X1" s="70">
-        <f t="shared" ref="X1" si="4">W1+1</f>
-        <v>4</v>
-      </c>
-      <c r="Y1" s="70">
-        <f t="shared" ref="Y1" si="5">X1+1</f>
-        <v>5</v>
-      </c>
-      <c r="Z1" s="70">
-        <f t="shared" ref="Z1" si="6">Y1+1</f>
-        <v>6</v>
-      </c>
-      <c r="AA1" s="70">
-        <f t="shared" ref="AA1" si="7">Z1+1</f>
-        <v>7</v>
-      </c>
-      <c r="AB1" s="70">
-        <f t="shared" ref="AB1" si="8">AA1+1</f>
-        <v>8</v>
-      </c>
-      <c r="AC1" s="70">
-        <f t="shared" ref="AC1" si="9">AB1+1</f>
-        <v>9</v>
-      </c>
-      <c r="AD1" s="70">
-        <f t="shared" ref="AD1" si="10">AC1+1</f>
-        <v>10</v>
-      </c>
-      <c r="AE1" s="70">
-        <f t="shared" ref="AE1" si="11">AD1+1</f>
-        <v>11</v>
-      </c>
-      <c r="AF1" s="70">
-        <f t="shared" ref="AF1" si="12">AE1+1</f>
-        <v>12</v>
-      </c>
-      <c r="AG1" s="70">
-        <f t="shared" ref="AG1" si="13">AF1+1</f>
-        <v>13</v>
-      </c>
-      <c r="AH1" s="70">
-        <f t="shared" ref="AH1" si="14">AG1+1</f>
-        <v>14</v>
-      </c>
-      <c r="AI1" s="70">
-        <f t="shared" ref="AI1" si="15">AH1+1</f>
-        <v>15</v>
-      </c>
-      <c r="AJ1" s="242" t="s">
-        <v>394</v>
-      </c>
-      <c r="AK1" s="242"/>
-      <c r="AL1" s="70">
-        <v>0</v>
-      </c>
-      <c r="AM1" s="70">
-        <f t="shared" ref="AM1" si="16">AL1+1</f>
-        <v>1</v>
-      </c>
-      <c r="AN1" s="70">
-        <f t="shared" ref="AN1" si="17">AM1+1</f>
-        <v>2</v>
-      </c>
-      <c r="AO1" s="70">
-        <f t="shared" ref="AO1" si="18">AN1+1</f>
-        <v>3</v>
-      </c>
-      <c r="AP1" s="70">
-        <f t="shared" ref="AP1" si="19">AO1+1</f>
-        <v>4</v>
-      </c>
-      <c r="AQ1" s="70">
-        <f t="shared" ref="AQ1" si="20">AP1+1</f>
-        <v>5</v>
-      </c>
-      <c r="AR1" s="70">
-        <f t="shared" ref="AR1" si="21">AQ1+1</f>
-        <v>6</v>
-      </c>
-      <c r="AS1" s="70">
-        <f t="shared" ref="AS1" si="22">AR1+1</f>
-        <v>7</v>
-      </c>
-      <c r="AT1" s="70">
-        <f t="shared" ref="AT1" si="23">AS1+1</f>
-        <v>8</v>
-      </c>
-      <c r="AU1" s="70">
-        <f t="shared" ref="AU1" si="24">AT1+1</f>
-        <v>9</v>
-      </c>
-      <c r="AV1" s="70">
-        <f t="shared" ref="AV1" si="25">AU1+1</f>
-        <v>10</v>
-      </c>
-      <c r="AW1" s="70">
-        <f t="shared" ref="AW1" si="26">AV1+1</f>
-        <v>11</v>
-      </c>
-      <c r="AX1" s="70">
-        <f t="shared" ref="AX1" si="27">AW1+1</f>
-        <v>12</v>
-      </c>
-      <c r="AY1" s="70">
-        <f t="shared" ref="AY1" si="28">AX1+1</f>
-        <v>13</v>
-      </c>
-      <c r="AZ1" s="70">
-        <f t="shared" ref="AZ1" si="29">AY1+1</f>
-        <v>14</v>
-      </c>
-      <c r="BA1" s="70">
-        <f t="shared" ref="BA1" si="30">AZ1+1</f>
-        <v>15</v>
-      </c>
-      <c r="BB1" s="242" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A2" s="70">
-        <v>0</v>
-      </c>
-      <c r="B2" s="311"/>
-      <c r="C2" s="312"/>
-      <c r="D2" s="312"/>
-      <c r="E2" s="312"/>
-      <c r="F2" s="312"/>
-      <c r="G2" s="312"/>
-      <c r="H2" s="357"/>
-      <c r="I2" s="312"/>
-      <c r="J2" s="312"/>
-      <c r="K2" s="357"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="312"/>
-      <c r="N2" s="312"/>
-      <c r="O2" s="312"/>
-      <c r="P2" s="312"/>
-      <c r="Q2" s="313"/>
-      <c r="S2" s="70">
-        <v>0</v>
-      </c>
-      <c r="T2" s="311"/>
-      <c r="U2" s="312"/>
-      <c r="V2" s="312"/>
-      <c r="W2" s="312"/>
-      <c r="X2" s="312"/>
-      <c r="Y2" s="312"/>
-      <c r="Z2" s="357"/>
-      <c r="AA2" s="312"/>
-      <c r="AB2" s="312"/>
-      <c r="AC2" s="357"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="312"/>
-      <c r="AF2" s="312"/>
-      <c r="AG2" s="312"/>
-      <c r="AH2" s="312"/>
-      <c r="AI2" s="313"/>
-      <c r="AK2" s="70">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="311"/>
-      <c r="AM2" s="312"/>
-      <c r="AN2" s="312"/>
-      <c r="AO2" s="312"/>
-      <c r="AP2" s="312"/>
-      <c r="AQ2" s="312"/>
-      <c r="AR2" s="357"/>
-      <c r="AS2" s="312"/>
-      <c r="AT2" s="312"/>
-      <c r="AU2" s="357"/>
-      <c r="AV2" s="20"/>
-      <c r="AW2" s="312"/>
-      <c r="AX2" s="312"/>
-      <c r="AY2" s="312"/>
-      <c r="AZ2" s="312"/>
-      <c r="BA2" s="313"/>
-    </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A3" s="70">
-        <f>A2+1</f>
-        <v>1</v>
-      </c>
-      <c r="B3" s="314"/>
-      <c r="C3" s="244"/>
-      <c r="D3" s="244"/>
-      <c r="E3" s="244"/>
-      <c r="F3" s="244"/>
-      <c r="G3" s="244"/>
-      <c r="H3" s="342"/>
-      <c r="I3" s="244"/>
-      <c r="J3" s="244"/>
-      <c r="K3" s="342"/>
-      <c r="L3" s="244"/>
-      <c r="M3" s="244"/>
-      <c r="N3" s="244"/>
-      <c r="O3" s="244"/>
-      <c r="P3" s="244"/>
-      <c r="Q3" s="315"/>
-      <c r="S3" s="70">
-        <f>S2+1</f>
-        <v>1</v>
-      </c>
-      <c r="T3" s="314"/>
-      <c r="U3" s="244"/>
-      <c r="V3" s="244"/>
-      <c r="W3" s="244"/>
-      <c r="X3" s="244"/>
-      <c r="Y3" s="244"/>
-      <c r="Z3" s="342"/>
-      <c r="AA3" s="244"/>
-      <c r="AB3" s="244"/>
-      <c r="AC3" s="342"/>
-      <c r="AD3" s="244"/>
-      <c r="AE3" s="244"/>
-      <c r="AF3" s="244"/>
-      <c r="AG3" s="244"/>
-      <c r="AH3" s="244"/>
-      <c r="AI3" s="315"/>
-      <c r="AK3" s="70">
-        <f>AK2+1</f>
-        <v>1</v>
-      </c>
-      <c r="AL3" s="314"/>
-      <c r="AM3" s="244"/>
-      <c r="AN3" s="244"/>
-      <c r="AO3" s="244"/>
-      <c r="AP3" s="244"/>
-      <c r="AQ3" s="244"/>
-      <c r="AR3" s="342"/>
-      <c r="AS3" s="244"/>
-      <c r="AT3" s="244"/>
-      <c r="AU3" s="342"/>
-      <c r="AV3" s="244"/>
-      <c r="AW3" s="244"/>
-      <c r="AX3" s="244"/>
-      <c r="AY3" s="244"/>
-      <c r="AZ3" s="244"/>
-      <c r="BA3" s="315"/>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A4" s="70">
-        <f t="shared" ref="A4:A17" si="31">A3+1</f>
-        <v>2</v>
-      </c>
-      <c r="B4" s="314"/>
-      <c r="C4" s="244"/>
-      <c r="D4" s="244"/>
-      <c r="E4" s="244"/>
-      <c r="F4" s="244"/>
-      <c r="G4" s="244"/>
-      <c r="H4" s="342"/>
-      <c r="I4" s="244"/>
-      <c r="J4" s="244"/>
-      <c r="K4" s="342"/>
-      <c r="L4" s="244"/>
-      <c r="M4" s="244"/>
-      <c r="N4" s="244"/>
-      <c r="O4" s="244"/>
-      <c r="P4" s="244"/>
-      <c r="Q4" s="26"/>
-      <c r="S4" s="70">
-        <f t="shared" ref="S4:S17" si="32">S3+1</f>
-        <v>2</v>
-      </c>
-      <c r="T4" s="314"/>
-      <c r="U4" s="244"/>
-      <c r="V4" s="244"/>
-      <c r="W4" s="244"/>
-      <c r="X4" s="244"/>
-      <c r="Y4" s="244"/>
-      <c r="Z4" s="342"/>
-      <c r="AA4" s="244"/>
-      <c r="AB4" s="244"/>
-      <c r="AC4" s="342"/>
-      <c r="AD4" s="244"/>
-      <c r="AE4" s="244"/>
-      <c r="AF4" s="244"/>
-      <c r="AG4" s="244"/>
-      <c r="AH4" s="244"/>
-      <c r="AI4" s="26"/>
-      <c r="AK4" s="70">
-        <f t="shared" ref="AK4:AK17" si="33">AK3+1</f>
-        <v>2</v>
-      </c>
-      <c r="AL4" s="314"/>
-      <c r="AM4" s="244"/>
-      <c r="AN4" s="244"/>
-      <c r="AO4" s="244"/>
-      <c r="AP4" s="244"/>
-      <c r="AQ4" s="244"/>
-      <c r="AR4" s="342"/>
-      <c r="AS4" s="244"/>
-      <c r="AT4" s="244"/>
-      <c r="AU4" s="342"/>
-      <c r="AV4" s="244"/>
-      <c r="AW4" s="244"/>
-      <c r="AX4" s="244"/>
-      <c r="AY4" s="244"/>
-      <c r="AZ4" s="244"/>
-      <c r="BA4" s="26"/>
-    </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A5" s="70">
-        <f t="shared" si="31"/>
-        <v>3</v>
-      </c>
-      <c r="B5" s="314"/>
-      <c r="C5" s="244"/>
-      <c r="D5" s="244"/>
-      <c r="E5" s="244"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="219"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="219"/>
-      <c r="L5" s="244"/>
-      <c r="M5" s="244"/>
-      <c r="N5" s="244"/>
-      <c r="O5" s="244"/>
-      <c r="P5" s="244"/>
-      <c r="Q5" s="26"/>
-      <c r="S5" s="70">
-        <f t="shared" si="32"/>
-        <v>3</v>
-      </c>
-      <c r="T5" s="314"/>
-      <c r="U5" s="244"/>
-      <c r="V5" s="244"/>
-      <c r="W5" s="244"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="219"/>
-      <c r="AA5" s="17"/>
-      <c r="AB5" s="17"/>
-      <c r="AC5" s="219"/>
-      <c r="AD5" s="244"/>
-      <c r="AE5" s="244"/>
-      <c r="AF5" s="244"/>
-      <c r="AG5" s="244"/>
-      <c r="AH5" s="244"/>
-      <c r="AI5" s="26"/>
-      <c r="AK5" s="70">
-        <f t="shared" si="33"/>
-        <v>3</v>
-      </c>
-      <c r="AL5" s="314"/>
-      <c r="AM5" s="244"/>
-      <c r="AN5" s="244"/>
-      <c r="AO5" s="244"/>
-      <c r="AP5" s="17"/>
-      <c r="AQ5" s="17"/>
-      <c r="AR5" s="219"/>
-      <c r="AS5" s="17"/>
-      <c r="AT5" s="17"/>
-      <c r="AU5" s="219"/>
-      <c r="AV5" s="244"/>
-      <c r="AW5" s="244"/>
-      <c r="AX5" s="244"/>
-      <c r="AY5" s="244"/>
-      <c r="AZ5" s="244"/>
-      <c r="BA5" s="26"/>
-    </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A6" s="70">
-        <f t="shared" si="31"/>
-        <v>4</v>
-      </c>
-      <c r="B6" s="314"/>
-      <c r="C6" s="244"/>
-      <c r="D6" s="244"/>
-      <c r="E6" s="244"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="246"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="152"/>
-      <c r="L6" s="244"/>
-      <c r="M6" s="244"/>
-      <c r="N6" s="244"/>
-      <c r="O6" s="244"/>
-      <c r="P6" s="244"/>
-      <c r="Q6" s="26"/>
-      <c r="S6" s="70">
-        <f t="shared" si="32"/>
-        <v>4</v>
-      </c>
-      <c r="T6" s="314"/>
-      <c r="U6" s="244"/>
-      <c r="V6" s="244"/>
-      <c r="W6" s="244"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="244"/>
-      <c r="AA6" s="17"/>
-      <c r="AB6" s="17"/>
-      <c r="AC6" s="17"/>
-      <c r="AD6" s="244"/>
-      <c r="AE6" s="244"/>
-      <c r="AF6" s="244"/>
-      <c r="AG6" s="244"/>
-      <c r="AH6" s="244"/>
-      <c r="AI6" s="26"/>
-      <c r="AK6" s="70">
-        <f t="shared" si="33"/>
-        <v>4</v>
-      </c>
-      <c r="AL6" s="314"/>
-      <c r="AM6" s="244"/>
-      <c r="AN6" s="244"/>
-      <c r="AO6" s="244"/>
-      <c r="AP6" s="17"/>
-      <c r="AQ6" s="17"/>
-      <c r="AR6" s="342"/>
-      <c r="AS6" s="17"/>
-      <c r="AT6" s="17"/>
-      <c r="AU6" s="219"/>
-      <c r="AV6" s="244"/>
-      <c r="AW6" s="244"/>
-      <c r="AX6" s="244"/>
-      <c r="AY6" s="244"/>
-      <c r="AZ6" s="244"/>
-      <c r="BA6" s="26"/>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A7" s="70">
-        <f t="shared" si="31"/>
-        <v>5</v>
-      </c>
-      <c r="B7" s="314"/>
-      <c r="C7" s="244"/>
-      <c r="D7" s="244"/>
-      <c r="E7" s="244"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="219"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="219"/>
-      <c r="L7" s="244"/>
-      <c r="M7" s="244"/>
-      <c r="N7" s="244"/>
-      <c r="O7" s="244"/>
-      <c r="P7" s="244"/>
-      <c r="Q7" s="26"/>
-      <c r="S7" s="70">
-        <f t="shared" si="32"/>
-        <v>5</v>
-      </c>
-      <c r="T7" s="314"/>
-      <c r="U7" s="244"/>
-      <c r="V7" s="244"/>
-      <c r="W7" s="244"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="17"/>
-      <c r="AA7" s="17"/>
-      <c r="AB7" s="17"/>
-      <c r="AC7" s="17"/>
-      <c r="AD7" s="244"/>
-      <c r="AE7" s="244"/>
-      <c r="AF7" s="244"/>
-      <c r="AG7" s="244"/>
-      <c r="AH7" s="244"/>
-      <c r="AI7" s="26"/>
-      <c r="AK7" s="70">
-        <f t="shared" si="33"/>
-        <v>5</v>
-      </c>
-      <c r="AL7" s="314"/>
-      <c r="AM7" s="244"/>
-      <c r="AN7" s="244"/>
-      <c r="AO7" s="244"/>
-      <c r="AP7" s="17"/>
-      <c r="AQ7" s="17"/>
-      <c r="AR7" s="219"/>
-      <c r="AS7" s="17"/>
-      <c r="AT7" s="17"/>
-      <c r="AU7" s="219"/>
-      <c r="AV7" s="244"/>
-      <c r="AW7" s="244"/>
-      <c r="AX7" s="244"/>
-      <c r="AY7" s="244"/>
-      <c r="AZ7" s="244"/>
-      <c r="BA7" s="26"/>
-    </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A8" s="70">
-        <f t="shared" si="31"/>
-        <v>6</v>
-      </c>
-      <c r="B8" s="308"/>
-      <c r="C8" s="219"/>
-      <c r="D8" s="219"/>
-      <c r="E8" s="219"/>
-      <c r="F8" s="152"/>
-      <c r="G8" s="219"/>
-      <c r="H8" s="219"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="219"/>
-      <c r="L8" s="219"/>
-      <c r="M8" s="152"/>
-      <c r="N8" s="219"/>
-      <c r="O8" s="219"/>
-      <c r="P8" s="219"/>
-      <c r="Q8" s="309"/>
-      <c r="S8" s="70">
-        <f t="shared" si="32"/>
-        <v>6</v>
-      </c>
-      <c r="T8" s="308"/>
-      <c r="U8" s="219"/>
-      <c r="V8" s="219"/>
-      <c r="W8" s="219"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="17"/>
-      <c r="AA8" s="17"/>
-      <c r="AB8" s="17"/>
-      <c r="AC8" s="17"/>
-      <c r="AD8" s="17"/>
-      <c r="AE8" s="17"/>
-      <c r="AF8" s="219"/>
-      <c r="AG8" s="219"/>
-      <c r="AH8" s="219"/>
-      <c r="AI8" s="309"/>
-      <c r="AK8" s="70">
-        <f t="shared" si="33"/>
-        <v>6</v>
-      </c>
-      <c r="AL8" s="16"/>
-      <c r="AM8" s="17"/>
-      <c r="AN8" s="17"/>
-      <c r="AO8" s="17"/>
-      <c r="AP8" s="17"/>
-      <c r="AQ8" s="17"/>
-      <c r="AR8" s="219"/>
-      <c r="AS8" s="17"/>
-      <c r="AT8" s="17"/>
-      <c r="AU8" s="219"/>
-      <c r="AV8" s="17"/>
-      <c r="AW8" s="17"/>
-      <c r="AX8" s="17"/>
-      <c r="AY8" s="17"/>
-      <c r="AZ8" s="17"/>
-      <c r="BA8" s="26"/>
-    </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A9" s="70">
-        <f t="shared" si="31"/>
-        <v>7</v>
-      </c>
-      <c r="B9" s="314"/>
-      <c r="C9" s="244"/>
-      <c r="D9" s="244"/>
-      <c r="E9" s="244"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="244"/>
-      <c r="M9" s="244"/>
-      <c r="N9" s="244"/>
-      <c r="O9" s="244"/>
-      <c r="P9" s="244"/>
-      <c r="Q9" s="315"/>
-      <c r="S9" s="70">
-        <f t="shared" si="32"/>
-        <v>7</v>
-      </c>
-      <c r="T9" s="314"/>
-      <c r="U9" s="244"/>
-      <c r="V9" s="244"/>
-      <c r="W9" s="244"/>
-      <c r="X9" s="17"/>
-      <c r="Y9" s="17"/>
-      <c r="Z9" s="17"/>
-      <c r="AA9" s="17"/>
-      <c r="AB9" s="17"/>
-      <c r="AC9" s="17"/>
-      <c r="AD9" s="244"/>
-      <c r="AE9" s="244"/>
-      <c r="AF9" s="244"/>
-      <c r="AG9" s="244"/>
-      <c r="AH9" s="244"/>
-      <c r="AI9" s="315"/>
-      <c r="AK9" s="70">
-        <f t="shared" si="33"/>
-        <v>7</v>
-      </c>
-      <c r="AL9" s="314"/>
-      <c r="AM9" s="244"/>
-      <c r="AN9" s="244"/>
-      <c r="AO9" s="244"/>
-      <c r="AP9" s="17"/>
-      <c r="AQ9" s="17"/>
-      <c r="AR9" s="17"/>
-      <c r="AS9" s="17"/>
-      <c r="AT9" s="17"/>
-      <c r="AU9" s="17"/>
-      <c r="AV9" s="244"/>
-      <c r="AW9" s="244"/>
-      <c r="AX9" s="244"/>
-      <c r="AY9" s="244"/>
-      <c r="AZ9" s="244"/>
-      <c r="BA9" s="315"/>
-    </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A10" s="70">
-        <f t="shared" si="31"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="314"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="244"/>
-      <c r="P10" s="244"/>
-      <c r="Q10" s="315"/>
-      <c r="S10" s="70">
-        <f t="shared" si="32"/>
-        <v>8</v>
-      </c>
-      <c r="T10" s="314"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17"/>
-      <c r="W10" s="17"/>
-      <c r="X10" s="17"/>
-      <c r="Y10" s="17"/>
-      <c r="Z10" s="17"/>
-      <c r="AA10" s="17"/>
-      <c r="AB10" s="17"/>
-      <c r="AC10" s="17"/>
-      <c r="AD10" s="17"/>
-      <c r="AE10" s="17"/>
-      <c r="AF10" s="17"/>
-      <c r="AG10" s="244"/>
-      <c r="AH10" s="244"/>
-      <c r="AI10" s="315"/>
-      <c r="AK10" s="70">
-        <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="AL10" s="314"/>
-      <c r="AM10" s="17"/>
-      <c r="AN10" s="17"/>
-      <c r="AO10" s="17"/>
-      <c r="AP10" s="17"/>
-      <c r="AQ10" s="17"/>
-      <c r="AR10" s="17"/>
-      <c r="AS10" s="17"/>
-      <c r="AT10" s="17"/>
-      <c r="AU10" s="17"/>
-      <c r="AV10" s="17"/>
-      <c r="AW10" s="17"/>
-      <c r="AX10" s="17"/>
-      <c r="AY10" s="244"/>
-      <c r="AZ10" s="244"/>
-      <c r="BA10" s="315"/>
-    </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A11" s="70">
-        <f t="shared" si="31"/>
-        <v>9</v>
-      </c>
-      <c r="B11" s="383"/>
-      <c r="C11" s="342"/>
-      <c r="D11" s="342"/>
-      <c r="E11" s="342"/>
-      <c r="F11" s="246"/>
-      <c r="G11" s="342"/>
-      <c r="H11" s="342"/>
-      <c r="I11" s="244"/>
-      <c r="J11" s="244"/>
-      <c r="K11" s="342"/>
-      <c r="L11" s="342"/>
-      <c r="M11" s="246"/>
-      <c r="N11" s="342"/>
-      <c r="O11" s="342"/>
-      <c r="P11" s="342"/>
-      <c r="Q11" s="352"/>
-      <c r="S11" s="70">
-        <f t="shared" si="32"/>
-        <v>9</v>
-      </c>
-      <c r="T11" s="383"/>
-      <c r="U11" s="342"/>
-      <c r="V11" s="342"/>
-      <c r="W11" s="342"/>
-      <c r="X11" s="244"/>
-      <c r="Y11" s="244"/>
-      <c r="Z11" s="244"/>
-      <c r="AA11" s="244"/>
-      <c r="AB11" s="244"/>
-      <c r="AC11" s="244"/>
-      <c r="AD11" s="244"/>
-      <c r="AE11" s="244"/>
-      <c r="AF11" s="342"/>
-      <c r="AG11" s="342"/>
-      <c r="AH11" s="342"/>
-      <c r="AI11" s="352"/>
-      <c r="AK11" s="70">
-        <f t="shared" si="33"/>
-        <v>9</v>
-      </c>
-      <c r="AL11" s="314"/>
-      <c r="AM11" s="244"/>
-      <c r="AN11" s="244"/>
-      <c r="AO11" s="244"/>
-      <c r="AP11" s="244"/>
-      <c r="AQ11" s="244"/>
-      <c r="AR11" s="244"/>
-      <c r="AS11" s="244"/>
-      <c r="AT11" s="244"/>
-      <c r="AU11" s="244"/>
-      <c r="AV11" s="244"/>
-      <c r="AW11" s="244"/>
-      <c r="AX11" s="244"/>
-      <c r="AY11" s="244"/>
-      <c r="AZ11" s="244"/>
-      <c r="BA11" s="315"/>
-    </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A12" s="70">
-        <f t="shared" si="31"/>
-        <v>10</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="244"/>
-      <c r="D12" s="244"/>
-      <c r="E12" s="244"/>
-      <c r="F12" s="244"/>
-      <c r="G12" s="244"/>
-      <c r="H12" s="342"/>
-      <c r="I12" s="244"/>
-      <c r="J12" s="244"/>
-      <c r="K12" s="342"/>
-      <c r="L12" s="244"/>
-      <c r="M12" s="244"/>
-      <c r="N12" s="244"/>
-      <c r="O12" s="244"/>
-      <c r="P12" s="244"/>
-      <c r="Q12" s="26"/>
-      <c r="S12" s="70">
-        <f t="shared" si="32"/>
-        <v>10</v>
-      </c>
-      <c r="T12" s="16"/>
-      <c r="U12" s="244"/>
-      <c r="V12" s="244"/>
-      <c r="W12" s="244"/>
-      <c r="X12" s="244"/>
-      <c r="Y12" s="244"/>
-      <c r="Z12" s="244"/>
-      <c r="AA12" s="244"/>
-      <c r="AB12" s="244"/>
-      <c r="AC12" s="244"/>
-      <c r="AD12" s="244"/>
-      <c r="AE12" s="244"/>
-      <c r="AF12" s="244"/>
-      <c r="AG12" s="244"/>
-      <c r="AH12" s="244"/>
-      <c r="AI12" s="26"/>
-      <c r="AK12" s="70">
-        <f t="shared" si="33"/>
-        <v>10</v>
-      </c>
-      <c r="AL12" s="16"/>
-      <c r="AM12" s="244"/>
-      <c r="AN12" s="244"/>
-      <c r="AO12" s="244"/>
-      <c r="AP12" s="244"/>
-      <c r="AQ12" s="244"/>
-      <c r="AR12" s="342"/>
-      <c r="AS12" s="244"/>
-      <c r="AT12" s="244"/>
-      <c r="AU12" s="342"/>
-      <c r="AV12" s="244"/>
-      <c r="AW12" s="244"/>
-      <c r="AX12" s="244"/>
-      <c r="AY12" s="244"/>
-      <c r="AZ12" s="244"/>
-      <c r="BA12" s="26"/>
-    </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A13" s="70">
-        <f t="shared" si="31"/>
-        <v>11</v>
-      </c>
-      <c r="B13" s="314"/>
-      <c r="C13" s="244"/>
-      <c r="D13" s="244"/>
-      <c r="E13" s="244"/>
-      <c r="F13" s="244"/>
-      <c r="G13" s="244"/>
-      <c r="H13" s="246"/>
-      <c r="I13" s="244"/>
-      <c r="J13" s="244"/>
-      <c r="K13" s="246"/>
-      <c r="L13" s="244"/>
-      <c r="M13" s="244"/>
-      <c r="N13" s="244"/>
-      <c r="O13" s="244"/>
-      <c r="P13" s="244"/>
-      <c r="Q13" s="26"/>
-      <c r="S13" s="70">
-        <f t="shared" si="32"/>
-        <v>11</v>
-      </c>
-      <c r="T13" s="314"/>
-      <c r="U13" s="244"/>
-      <c r="V13" s="244"/>
-      <c r="W13" s="244"/>
-      <c r="X13" s="244"/>
-      <c r="Y13" s="244"/>
-      <c r="Z13" s="244"/>
-      <c r="AA13" s="244"/>
-      <c r="AB13" s="244"/>
-      <c r="AC13" s="244"/>
-      <c r="AD13" s="244"/>
-      <c r="AE13" s="244"/>
-      <c r="AF13" s="244"/>
-      <c r="AG13" s="244"/>
-      <c r="AH13" s="244"/>
-      <c r="AI13" s="26"/>
-      <c r="AK13" s="70">
-        <f t="shared" si="33"/>
-        <v>11</v>
-      </c>
-      <c r="AL13" s="314"/>
-      <c r="AM13" s="244"/>
-      <c r="AN13" s="244"/>
-      <c r="AO13" s="244"/>
-      <c r="AP13" s="244"/>
-      <c r="AQ13" s="244"/>
-      <c r="AR13" s="342"/>
-      <c r="AS13" s="244"/>
-      <c r="AT13" s="244"/>
-      <c r="AU13" s="342"/>
-      <c r="AV13" s="244"/>
-      <c r="AW13" s="244"/>
-      <c r="AX13" s="244"/>
-      <c r="AY13" s="244"/>
-      <c r="AZ13" s="244"/>
-      <c r="BA13" s="26"/>
-    </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A14" s="70">
-        <f t="shared" si="31"/>
-        <v>12</v>
-      </c>
-      <c r="B14" s="314"/>
-      <c r="C14" s="244"/>
-      <c r="D14" s="244"/>
-      <c r="E14" s="244"/>
-      <c r="F14" s="244"/>
-      <c r="G14" s="244"/>
-      <c r="H14" s="342"/>
-      <c r="I14" s="244"/>
-      <c r="J14" s="244"/>
-      <c r="K14" s="342"/>
-      <c r="L14" s="244"/>
-      <c r="M14" s="244"/>
-      <c r="N14" s="244"/>
-      <c r="O14" s="244"/>
-      <c r="P14" s="244"/>
-      <c r="Q14" s="26"/>
-      <c r="S14" s="70">
-        <f t="shared" si="32"/>
-        <v>12</v>
-      </c>
-      <c r="T14" s="314"/>
-      <c r="U14" s="244"/>
-      <c r="V14" s="244"/>
-      <c r="W14" s="244"/>
-      <c r="X14" s="244"/>
-      <c r="Y14" s="244"/>
-      <c r="Z14" s="342"/>
-      <c r="AA14" s="244"/>
-      <c r="AB14" s="244"/>
-      <c r="AC14" s="342"/>
-      <c r="AD14" s="244"/>
-      <c r="AE14" s="244"/>
-      <c r="AF14" s="244"/>
-      <c r="AG14" s="244"/>
-      <c r="AH14" s="244"/>
-      <c r="AI14" s="26"/>
-      <c r="AK14" s="70">
-        <f t="shared" si="33"/>
-        <v>12</v>
-      </c>
-      <c r="AL14" s="314"/>
-      <c r="AM14" s="244"/>
-      <c r="AN14" s="244"/>
-      <c r="AO14" s="244"/>
-      <c r="AP14" s="244"/>
-      <c r="AQ14" s="244"/>
-      <c r="AR14" s="342"/>
-      <c r="AS14" s="244"/>
-      <c r="AT14" s="244"/>
-      <c r="AU14" s="342"/>
-      <c r="AV14" s="244"/>
-      <c r="AW14" s="244"/>
-      <c r="AX14" s="244"/>
-      <c r="AY14" s="244"/>
-      <c r="AZ14" s="244"/>
-      <c r="BA14" s="26"/>
-    </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A15" s="70">
-        <f t="shared" si="31"/>
-        <v>13</v>
-      </c>
-      <c r="B15" s="314"/>
-      <c r="C15" s="244"/>
-      <c r="D15" s="244"/>
-      <c r="E15" s="244"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="219"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="219"/>
-      <c r="L15" s="244"/>
-      <c r="M15" s="244"/>
-      <c r="N15" s="244"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="26"/>
-      <c r="S15" s="70">
-        <f t="shared" si="32"/>
-        <v>13</v>
-      </c>
-      <c r="T15" s="314"/>
-      <c r="U15" s="244"/>
-      <c r="V15" s="244"/>
-      <c r="W15" s="244"/>
-      <c r="X15" s="17"/>
-      <c r="Y15" s="17"/>
-      <c r="Z15" s="219"/>
-      <c r="AA15" s="17"/>
-      <c r="AB15" s="17"/>
-      <c r="AC15" s="219"/>
-      <c r="AD15" s="244"/>
-      <c r="AE15" s="244"/>
-      <c r="AF15" s="244"/>
-      <c r="AG15" s="17"/>
-      <c r="AH15" s="17"/>
-      <c r="AI15" s="26"/>
-      <c r="AK15" s="70">
-        <f t="shared" si="33"/>
-        <v>13</v>
-      </c>
-      <c r="AL15" s="314"/>
-      <c r="AM15" s="244"/>
-      <c r="AN15" s="244"/>
-      <c r="AO15" s="244"/>
-      <c r="AP15" s="17"/>
-      <c r="AQ15" s="17"/>
-      <c r="AR15" s="219"/>
-      <c r="AS15" s="17"/>
-      <c r="AT15" s="17"/>
-      <c r="AU15" s="219"/>
-      <c r="AV15" s="244"/>
-      <c r="AW15" s="244"/>
-      <c r="AX15" s="244"/>
-      <c r="AY15" s="17"/>
-      <c r="AZ15" s="17"/>
-      <c r="BA15" s="26"/>
-    </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A16" s="70">
-        <f t="shared" si="31"/>
-        <v>14</v>
-      </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="219"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="219"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="26"/>
-      <c r="S16" s="70">
-        <f t="shared" si="32"/>
-        <v>14</v>
-      </c>
-      <c r="T16" s="16"/>
-      <c r="U16" s="17"/>
-      <c r="V16" s="17"/>
-      <c r="W16" s="17"/>
-      <c r="X16" s="17"/>
-      <c r="Y16" s="17"/>
-      <c r="Z16" s="219"/>
-      <c r="AA16" s="17"/>
-      <c r="AB16" s="17"/>
-      <c r="AC16" s="219"/>
-      <c r="AD16" s="17"/>
-      <c r="AE16" s="17"/>
-      <c r="AF16" s="17"/>
-      <c r="AG16" s="17"/>
-      <c r="AH16" s="17"/>
-      <c r="AI16" s="26"/>
-      <c r="AK16" s="70">
-        <f t="shared" si="33"/>
-        <v>14</v>
-      </c>
-      <c r="AL16" s="16"/>
-      <c r="AM16" s="17"/>
-      <c r="AN16" s="17"/>
-      <c r="AO16" s="17"/>
-      <c r="AP16" s="17"/>
-      <c r="AQ16" s="17"/>
-      <c r="AR16" s="219"/>
-      <c r="AS16" s="17"/>
-      <c r="AT16" s="17"/>
-      <c r="AU16" s="219"/>
-      <c r="AV16" s="17"/>
-      <c r="AW16" s="17"/>
-      <c r="AX16" s="17"/>
-      <c r="AY16" s="17"/>
-      <c r="AZ16" s="17"/>
-      <c r="BA16" s="26"/>
-    </row>
-    <row r="17" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A17" s="70">
-        <f t="shared" si="31"/>
-        <v>15</v>
-      </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="412"/>
-      <c r="I17" s="317"/>
-      <c r="J17" s="317"/>
-      <c r="K17" s="412"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="33"/>
-      <c r="S17" s="70">
-        <f t="shared" si="32"/>
-        <v>15</v>
-      </c>
-      <c r="T17" s="32"/>
-      <c r="U17" s="22"/>
-      <c r="V17" s="22"/>
-      <c r="W17" s="22"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="22"/>
-      <c r="Z17" s="412"/>
-      <c r="AA17" s="317"/>
-      <c r="AB17" s="317"/>
-      <c r="AC17" s="412"/>
-      <c r="AD17" s="22"/>
-      <c r="AE17" s="22"/>
-      <c r="AF17" s="22"/>
-      <c r="AG17" s="22"/>
-      <c r="AH17" s="22"/>
-      <c r="AI17" s="33"/>
-      <c r="AK17" s="70">
-        <f t="shared" si="33"/>
-        <v>15</v>
-      </c>
-      <c r="AL17" s="32"/>
-      <c r="AM17" s="22"/>
-      <c r="AN17" s="22"/>
-      <c r="AO17" s="22"/>
-      <c r="AP17" s="22"/>
-      <c r="AQ17" s="22"/>
-      <c r="AR17" s="412"/>
-      <c r="AS17" s="317"/>
-      <c r="AT17" s="317"/>
-      <c r="AU17" s="412"/>
-      <c r="AV17" s="22"/>
-      <c r="AW17" s="22"/>
-      <c r="AX17" s="22"/>
-      <c r="AY17" s="22"/>
-      <c r="AZ17" s="22"/>
-      <c r="BA17" s="33"/>
-    </row>
-    <row r="18" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A18" s="242" t="s">
-        <v>395</v>
-      </c>
-      <c r="S18" s="242" t="s">
-        <v>395</v>
-      </c>
-      <c r="AK18" s="242" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="19" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A19" s="242"/>
-      <c r="B19" s="70">
-        <v>0</v>
-      </c>
-      <c r="C19" s="70">
-        <f t="shared" ref="C19" si="34">B19+1</f>
-        <v>1</v>
-      </c>
-      <c r="D19" s="70">
-        <f t="shared" ref="D19" si="35">C19+1</f>
-        <v>2</v>
-      </c>
-      <c r="E19" s="70">
-        <f t="shared" ref="E19" si="36">D19+1</f>
-        <v>3</v>
-      </c>
-      <c r="F19" s="70">
-        <f t="shared" ref="F19" si="37">E19+1</f>
-        <v>4</v>
-      </c>
-      <c r="G19" s="70">
-        <f t="shared" ref="G19" si="38">F19+1</f>
-        <v>5</v>
-      </c>
-      <c r="H19" s="70">
-        <f t="shared" ref="H19" si="39">G19+1</f>
-        <v>6</v>
-      </c>
-      <c r="I19" s="70">
-        <f t="shared" ref="I19" si="40">H19+1</f>
-        <v>7</v>
-      </c>
-      <c r="J19" s="70">
-        <f t="shared" ref="J19" si="41">I19+1</f>
-        <v>8</v>
-      </c>
-      <c r="K19" s="70">
-        <f t="shared" ref="K19" si="42">J19+1</f>
-        <v>9</v>
-      </c>
-      <c r="L19" s="70">
-        <f t="shared" ref="L19" si="43">K19+1</f>
-        <v>10</v>
-      </c>
-      <c r="M19" s="70">
-        <f t="shared" ref="M19" si="44">L19+1</f>
-        <v>11</v>
-      </c>
-      <c r="N19" s="70">
-        <f t="shared" ref="N19" si="45">M19+1</f>
-        <v>12</v>
-      </c>
-      <c r="O19" s="70">
-        <f t="shared" ref="O19" si="46">N19+1</f>
-        <v>13</v>
-      </c>
-      <c r="P19" s="70">
-        <f t="shared" ref="P19" si="47">O19+1</f>
-        <v>14</v>
-      </c>
-      <c r="Q19" s="70">
-        <f t="shared" ref="Q19" si="48">P19+1</f>
-        <v>15</v>
-      </c>
-      <c r="R19" s="242" t="s">
-        <v>394</v>
-      </c>
-      <c r="S19" s="242"/>
-      <c r="T19" s="70">
-        <v>0</v>
-      </c>
-      <c r="U19" s="70">
-        <f t="shared" ref="U19" si="49">T19+1</f>
-        <v>1</v>
-      </c>
-      <c r="V19" s="70">
-        <f t="shared" ref="V19" si="50">U19+1</f>
-        <v>2</v>
-      </c>
-      <c r="W19" s="70">
-        <f t="shared" ref="W19" si="51">V19+1</f>
-        <v>3</v>
-      </c>
-      <c r="X19" s="70">
-        <f t="shared" ref="X19" si="52">W19+1</f>
-        <v>4</v>
-      </c>
-      <c r="Y19" s="70">
-        <f t="shared" ref="Y19" si="53">X19+1</f>
-        <v>5</v>
-      </c>
-      <c r="Z19" s="70">
-        <f t="shared" ref="Z19" si="54">Y19+1</f>
-        <v>6</v>
-      </c>
-      <c r="AA19" s="70">
-        <f t="shared" ref="AA19" si="55">Z19+1</f>
-        <v>7</v>
-      </c>
-      <c r="AB19" s="70">
-        <f t="shared" ref="AB19" si="56">AA19+1</f>
-        <v>8</v>
-      </c>
-      <c r="AC19" s="70">
-        <f t="shared" ref="AC19" si="57">AB19+1</f>
-        <v>9</v>
-      </c>
-      <c r="AD19" s="70">
-        <f t="shared" ref="AD19" si="58">AC19+1</f>
-        <v>10</v>
-      </c>
-      <c r="AE19" s="70">
-        <f t="shared" ref="AE19" si="59">AD19+1</f>
-        <v>11</v>
-      </c>
-      <c r="AF19" s="70">
-        <f t="shared" ref="AF19" si="60">AE19+1</f>
-        <v>12</v>
-      </c>
-      <c r="AG19" s="70">
-        <f t="shared" ref="AG19" si="61">AF19+1</f>
-        <v>13</v>
-      </c>
-      <c r="AH19" s="70">
-        <f t="shared" ref="AH19" si="62">AG19+1</f>
-        <v>14</v>
-      </c>
-      <c r="AI19" s="70">
-        <f t="shared" ref="AI19" si="63">AH19+1</f>
-        <v>15</v>
-      </c>
-      <c r="AJ19" s="242" t="s">
-        <v>394</v>
-      </c>
-      <c r="AK19" s="242"/>
-      <c r="AL19" s="70">
-        <v>0</v>
-      </c>
-      <c r="AM19" s="70">
-        <f t="shared" ref="AM19" si="64">AL19+1</f>
-        <v>1</v>
-      </c>
-      <c r="AN19" s="70">
-        <f t="shared" ref="AN19" si="65">AM19+1</f>
-        <v>2</v>
-      </c>
-      <c r="AO19" s="70">
-        <f t="shared" ref="AO19" si="66">AN19+1</f>
-        <v>3</v>
-      </c>
-      <c r="AP19" s="70">
-        <f t="shared" ref="AP19" si="67">AO19+1</f>
-        <v>4</v>
-      </c>
-      <c r="AQ19" s="70">
-        <f t="shared" ref="AQ19" si="68">AP19+1</f>
-        <v>5</v>
-      </c>
-      <c r="AR19" s="70">
-        <f t="shared" ref="AR19" si="69">AQ19+1</f>
-        <v>6</v>
-      </c>
-      <c r="AS19" s="70">
-        <f t="shared" ref="AS19" si="70">AR19+1</f>
-        <v>7</v>
-      </c>
-      <c r="AT19" s="70">
-        <f t="shared" ref="AT19" si="71">AS19+1</f>
-        <v>8</v>
-      </c>
-      <c r="AU19" s="70">
-        <f t="shared" ref="AU19" si="72">AT19+1</f>
-        <v>9</v>
-      </c>
-      <c r="AV19" s="70">
-        <f t="shared" ref="AV19" si="73">AU19+1</f>
-        <v>10</v>
-      </c>
-      <c r="AW19" s="70">
-        <f t="shared" ref="AW19" si="74">AV19+1</f>
-        <v>11</v>
-      </c>
-      <c r="AX19" s="70">
-        <f t="shared" ref="AX19" si="75">AW19+1</f>
-        <v>12</v>
-      </c>
-      <c r="AY19" s="70">
-        <f t="shared" ref="AY19" si="76">AX19+1</f>
-        <v>13</v>
-      </c>
-      <c r="AZ19" s="70">
-        <f t="shared" ref="AZ19" si="77">AY19+1</f>
-        <v>14</v>
-      </c>
-      <c r="BA19" s="70">
-        <f t="shared" ref="BA19" si="78">AZ19+1</f>
-        <v>15</v>
-      </c>
-      <c r="BB19" s="242" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="20" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A20" s="70">
-        <v>0</v>
-      </c>
-      <c r="B20" s="311"/>
-      <c r="C20" s="312"/>
-      <c r="D20" s="312"/>
-      <c r="E20" s="312"/>
-      <c r="F20" s="312"/>
-      <c r="G20" s="312"/>
-      <c r="H20" s="357"/>
-      <c r="I20" s="312"/>
-      <c r="J20" s="312"/>
-      <c r="K20" s="357"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="312"/>
-      <c r="N20" s="312"/>
-      <c r="O20" s="312"/>
-      <c r="P20" s="312"/>
-      <c r="Q20" s="313"/>
-      <c r="S20" s="70">
-        <v>0</v>
-      </c>
-      <c r="T20" s="311"/>
-      <c r="U20" s="312"/>
-      <c r="V20" s="312"/>
-      <c r="W20" s="312"/>
-      <c r="X20" s="312"/>
-      <c r="Y20" s="312"/>
-      <c r="Z20" s="312"/>
-      <c r="AA20" s="312"/>
-      <c r="AB20" s="312"/>
-      <c r="AC20" s="312"/>
-      <c r="AD20" s="20"/>
-      <c r="AE20" s="312"/>
-      <c r="AF20" s="312"/>
-      <c r="AG20" s="312"/>
-      <c r="AH20" s="312"/>
-      <c r="AI20" s="313"/>
-      <c r="AK20" s="70">
-        <v>0</v>
-      </c>
-      <c r="AL20" s="311"/>
-      <c r="AM20" s="312"/>
-      <c r="AN20" s="312"/>
-      <c r="AO20" s="312"/>
-      <c r="AP20" s="312"/>
-      <c r="AQ20" s="312"/>
-      <c r="AR20" s="312"/>
-      <c r="AS20" s="312"/>
-      <c r="AT20" s="312"/>
-      <c r="AU20" s="312"/>
-      <c r="AV20" s="20"/>
-      <c r="AW20" s="312"/>
-      <c r="AX20" s="312"/>
-      <c r="AY20" s="312"/>
-      <c r="AZ20" s="312"/>
-      <c r="BA20" s="313"/>
-    </row>
-    <row r="21" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A21" s="70">
-        <f>A20+1</f>
-        <v>1</v>
-      </c>
-      <c r="B21" s="314"/>
-      <c r="C21" s="244"/>
-      <c r="D21" s="244"/>
-      <c r="E21" s="244"/>
-      <c r="F21" s="244"/>
-      <c r="G21" s="244"/>
-      <c r="H21" s="342"/>
-      <c r="I21" s="244"/>
-      <c r="J21" s="244"/>
-      <c r="K21" s="342"/>
-      <c r="L21" s="244"/>
-      <c r="M21" s="244"/>
-      <c r="N21" s="244"/>
-      <c r="O21" s="244"/>
-      <c r="P21" s="244"/>
-      <c r="Q21" s="315"/>
-      <c r="S21" s="70">
-        <f>S20+1</f>
-        <v>1</v>
-      </c>
-      <c r="T21" s="314"/>
-      <c r="U21" s="244"/>
-      <c r="V21" s="244"/>
-      <c r="W21" s="244"/>
-      <c r="X21" s="244"/>
-      <c r="Y21" s="244"/>
-      <c r="Z21" s="244"/>
-      <c r="AA21" s="244"/>
-      <c r="AB21" s="244"/>
-      <c r="AC21" s="244"/>
-      <c r="AD21" s="244"/>
-      <c r="AE21" s="244"/>
-      <c r="AF21" s="244"/>
-      <c r="AG21" s="244"/>
-      <c r="AH21" s="244"/>
-      <c r="AI21" s="315"/>
-      <c r="AK21" s="70">
-        <f>AK20+1</f>
-        <v>1</v>
-      </c>
-      <c r="AL21" s="314"/>
-      <c r="AM21" s="244"/>
-      <c r="AN21" s="244"/>
-      <c r="AO21" s="244"/>
-      <c r="AP21" s="244"/>
-      <c r="AQ21" s="244"/>
-      <c r="AR21" s="244"/>
-      <c r="AS21" s="244"/>
-      <c r="AT21" s="244"/>
-      <c r="AU21" s="244"/>
-      <c r="AV21" s="244"/>
-      <c r="AW21" s="244"/>
-      <c r="AX21" s="244"/>
-      <c r="AY21" s="244"/>
-      <c r="AZ21" s="244"/>
-      <c r="BA21" s="315"/>
-    </row>
-    <row r="22" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A22" s="70">
-        <f t="shared" ref="A22:A35" si="79">A21+1</f>
-        <v>2</v>
-      </c>
-      <c r="B22" s="314"/>
-      <c r="C22" s="244"/>
-      <c r="D22" s="244"/>
-      <c r="E22" s="244"/>
-      <c r="F22" s="244"/>
-      <c r="G22" s="244"/>
-      <c r="H22" s="342"/>
-      <c r="I22" s="244"/>
-      <c r="J22" s="244"/>
-      <c r="K22" s="342"/>
-      <c r="L22" s="244"/>
-      <c r="M22" s="244"/>
-      <c r="N22" s="244"/>
-      <c r="O22" s="244"/>
-      <c r="P22" s="244"/>
-      <c r="Q22" s="26"/>
-      <c r="S22" s="70">
-        <f t="shared" ref="S22:S35" si="80">S21+1</f>
-        <v>2</v>
-      </c>
-      <c r="T22" s="314"/>
-      <c r="U22" s="244"/>
-      <c r="V22" s="244"/>
-      <c r="W22" s="244"/>
-      <c r="X22" s="244"/>
-      <c r="Y22" s="244"/>
-      <c r="Z22" s="244"/>
-      <c r="AA22" s="244"/>
-      <c r="AB22" s="244"/>
-      <c r="AC22" s="244"/>
-      <c r="AD22" s="244"/>
-      <c r="AE22" s="244"/>
-      <c r="AF22" s="244"/>
-      <c r="AG22" s="244"/>
-      <c r="AH22" s="244"/>
-      <c r="AI22" s="26"/>
-      <c r="AK22" s="70">
-        <f t="shared" ref="AK22:AK35" si="81">AK21+1</f>
-        <v>2</v>
-      </c>
-      <c r="AL22" s="314"/>
-      <c r="AM22" s="244"/>
-      <c r="AN22" s="244"/>
-      <c r="AO22" s="244"/>
-      <c r="AP22" s="244"/>
-      <c r="AQ22" s="244"/>
-      <c r="AR22" s="244"/>
-      <c r="AS22" s="244"/>
-      <c r="AT22" s="244"/>
-      <c r="AU22" s="244"/>
-      <c r="AV22" s="244"/>
-      <c r="AW22" s="244"/>
-      <c r="AX22" s="244"/>
-      <c r="AY22" s="244"/>
-      <c r="AZ22" s="244"/>
-      <c r="BA22" s="26"/>
-    </row>
-    <row r="23" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A23" s="70">
-        <f t="shared" si="79"/>
-        <v>3</v>
-      </c>
-      <c r="B23" s="314"/>
-      <c r="C23" s="244"/>
-      <c r="D23" s="244"/>
-      <c r="E23" s="244"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="219"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="219"/>
-      <c r="L23" s="244"/>
-      <c r="M23" s="244"/>
-      <c r="N23" s="244"/>
-      <c r="O23" s="244"/>
-      <c r="P23" s="244"/>
-      <c r="Q23" s="26"/>
-      <c r="S23" s="70">
-        <f t="shared" si="80"/>
-        <v>3</v>
-      </c>
-      <c r="T23" s="314"/>
-      <c r="U23" s="244"/>
-      <c r="V23" s="244"/>
-      <c r="W23" s="244"/>
-      <c r="X23" s="17"/>
-      <c r="Y23" s="17"/>
-      <c r="Z23" s="17"/>
-      <c r="AA23" s="17"/>
-      <c r="AB23" s="17"/>
-      <c r="AC23" s="17"/>
-      <c r="AD23" s="244"/>
-      <c r="AE23" s="244"/>
-      <c r="AF23" s="244"/>
-      <c r="AG23" s="244"/>
-      <c r="AH23" s="244"/>
-      <c r="AI23" s="26"/>
-      <c r="AK23" s="70">
-        <f t="shared" si="81"/>
-        <v>3</v>
-      </c>
-      <c r="AL23" s="314"/>
-      <c r="AM23" s="244"/>
-      <c r="AN23" s="244"/>
-      <c r="AO23" s="244"/>
-      <c r="AP23" s="17"/>
-      <c r="AQ23" s="17"/>
-      <c r="AR23" s="17"/>
-      <c r="AS23" s="17"/>
-      <c r="AT23" s="17"/>
-      <c r="AU23" s="17"/>
-      <c r="AV23" s="244"/>
-      <c r="AW23" s="244"/>
-      <c r="AX23" s="244"/>
-      <c r="AY23" s="244"/>
-      <c r="AZ23" s="244"/>
-      <c r="BA23" s="26"/>
-    </row>
-    <row r="24" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A24" s="70">
-        <f t="shared" si="79"/>
-        <v>4</v>
-      </c>
-      <c r="B24" s="314"/>
-      <c r="C24" s="244"/>
-      <c r="D24" s="244"/>
-      <c r="E24" s="244"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="342"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="219"/>
-      <c r="L24" s="244"/>
-      <c r="M24" s="244"/>
-      <c r="N24" s="244"/>
-      <c r="O24" s="244"/>
-      <c r="P24" s="244"/>
-      <c r="Q24" s="26"/>
-      <c r="S24" s="70">
-        <f t="shared" si="80"/>
-        <v>4</v>
-      </c>
-      <c r="T24" s="314"/>
-      <c r="U24" s="244"/>
-      <c r="V24" s="244"/>
-      <c r="W24" s="244"/>
-      <c r="X24" s="17"/>
-      <c r="Y24" s="17"/>
-      <c r="Z24" s="244"/>
-      <c r="AA24" s="17"/>
-      <c r="AB24" s="17"/>
-      <c r="AC24" s="17"/>
-      <c r="AD24" s="244"/>
-      <c r="AE24" s="244"/>
-      <c r="AF24" s="244"/>
-      <c r="AG24" s="244"/>
-      <c r="AH24" s="244"/>
-      <c r="AI24" s="26"/>
-      <c r="AK24" s="70">
-        <f t="shared" si="81"/>
-        <v>4</v>
-      </c>
-      <c r="AL24" s="314"/>
-      <c r="AM24" s="244"/>
-      <c r="AN24" s="244"/>
-      <c r="AO24" s="244"/>
-      <c r="AP24" s="17"/>
-      <c r="AQ24" s="17"/>
-      <c r="AR24" s="244"/>
-      <c r="AS24" s="17"/>
-      <c r="AT24" s="17"/>
-      <c r="AU24" s="17"/>
-      <c r="AV24" s="244"/>
-      <c r="AW24" s="244"/>
-      <c r="AX24" s="244"/>
-      <c r="AY24" s="244"/>
-      <c r="AZ24" s="244"/>
-      <c r="BA24" s="26"/>
-    </row>
-    <row r="25" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A25" s="70">
-        <f t="shared" si="79"/>
-        <v>5</v>
-      </c>
-      <c r="B25" s="314"/>
-      <c r="C25" s="244"/>
-      <c r="D25" s="244"/>
-      <c r="E25" s="244"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="219"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="219"/>
-      <c r="L25" s="244"/>
-      <c r="M25" s="244"/>
-      <c r="N25" s="244"/>
-      <c r="O25" s="244"/>
-      <c r="P25" s="244"/>
-      <c r="Q25" s="26"/>
-      <c r="S25" s="70">
-        <f t="shared" si="80"/>
-        <v>5</v>
-      </c>
-      <c r="T25" s="314"/>
-      <c r="U25" s="244"/>
-      <c r="V25" s="244"/>
-      <c r="W25" s="244"/>
-      <c r="X25" s="17"/>
-      <c r="Y25" s="17"/>
-      <c r="Z25" s="17"/>
-      <c r="AA25" s="17"/>
-      <c r="AB25" s="17"/>
-      <c r="AC25" s="17"/>
-      <c r="AD25" s="244"/>
-      <c r="AE25" s="244"/>
-      <c r="AF25" s="244"/>
-      <c r="AG25" s="244"/>
-      <c r="AH25" s="244"/>
-      <c r="AI25" s="26"/>
-      <c r="AK25" s="70">
-        <f t="shared" si="81"/>
-        <v>5</v>
-      </c>
-      <c r="AL25" s="314"/>
-      <c r="AM25" s="244"/>
-      <c r="AN25" s="244"/>
-      <c r="AO25" s="244"/>
-      <c r="AP25" s="17"/>
-      <c r="AQ25" s="17"/>
-      <c r="AR25" s="17"/>
-      <c r="AS25" s="17"/>
-      <c r="AT25" s="17"/>
-      <c r="AU25" s="17"/>
-      <c r="AV25" s="244"/>
-      <c r="AW25" s="244"/>
-      <c r="AX25" s="244"/>
-      <c r="AY25" s="244"/>
-      <c r="AZ25" s="244"/>
-      <c r="BA25" s="26"/>
-    </row>
-    <row r="26" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A26" s="70">
-        <f t="shared" si="79"/>
-        <v>6</v>
-      </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="219"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="219"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="26"/>
-      <c r="S26" s="70">
-        <f t="shared" si="80"/>
-        <v>6</v>
-      </c>
-      <c r="T26" s="308"/>
-      <c r="U26" s="219"/>
-      <c r="V26" s="219"/>
-      <c r="W26" s="219"/>
-      <c r="X26" s="219"/>
-      <c r="Y26" s="219"/>
-      <c r="Z26" s="219"/>
-      <c r="AA26" s="17"/>
-      <c r="AB26" s="17"/>
-      <c r="AC26" s="219"/>
-      <c r="AD26" s="219"/>
-      <c r="AE26" s="219"/>
-      <c r="AF26" s="219"/>
-      <c r="AG26" s="219"/>
-      <c r="AH26" s="219"/>
-      <c r="AI26" s="309"/>
-      <c r="AK26" s="70">
-        <f t="shared" si="81"/>
-        <v>6</v>
-      </c>
-      <c r="AL26" s="16"/>
-      <c r="AM26" s="17"/>
-      <c r="AN26" s="17"/>
-      <c r="AO26" s="17"/>
-      <c r="AP26" s="17"/>
-      <c r="AQ26" s="17"/>
-      <c r="AR26" s="17"/>
-      <c r="AS26" s="17"/>
-      <c r="AT26" s="17"/>
-      <c r="AU26" s="17"/>
-      <c r="AV26" s="17"/>
-      <c r="AW26" s="17"/>
-      <c r="AX26" s="17"/>
-      <c r="AY26" s="17"/>
-      <c r="AZ26" s="17"/>
-      <c r="BA26" s="26"/>
-    </row>
-    <row r="27" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A27" s="70">
-        <f t="shared" si="79"/>
-        <v>7</v>
-      </c>
-      <c r="B27" s="314"/>
-      <c r="C27" s="244"/>
-      <c r="D27" s="244"/>
-      <c r="E27" s="244"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="244"/>
-      <c r="M27" s="244"/>
-      <c r="N27" s="244"/>
-      <c r="O27" s="244"/>
-      <c r="P27" s="244"/>
-      <c r="Q27" s="315"/>
-      <c r="S27" s="70">
-        <f t="shared" si="80"/>
-        <v>7</v>
-      </c>
-      <c r="T27" s="314"/>
-      <c r="U27" s="244"/>
-      <c r="V27" s="244"/>
-      <c r="W27" s="244"/>
-      <c r="X27" s="17"/>
-      <c r="Y27" s="17"/>
-      <c r="Z27" s="17"/>
-      <c r="AA27" s="17"/>
-      <c r="AB27" s="17"/>
-      <c r="AC27" s="17"/>
-      <c r="AD27" s="244"/>
-      <c r="AE27" s="244"/>
-      <c r="AF27" s="244"/>
-      <c r="AG27" s="244"/>
-      <c r="AH27" s="244"/>
-      <c r="AI27" s="315"/>
-      <c r="AK27" s="70">
-        <f t="shared" si="81"/>
-        <v>7</v>
-      </c>
-      <c r="AL27" s="314"/>
-      <c r="AM27" s="244"/>
-      <c r="AN27" s="244"/>
-      <c r="AO27" s="244"/>
-      <c r="AP27" s="17"/>
-      <c r="AQ27" s="17"/>
-      <c r="AR27" s="17"/>
-      <c r="AS27" s="17"/>
-      <c r="AT27" s="17"/>
-      <c r="AU27" s="17"/>
-      <c r="AV27" s="244"/>
-      <c r="AW27" s="244"/>
-      <c r="AX27" s="244"/>
-      <c r="AY27" s="244"/>
-      <c r="AZ27" s="244"/>
-      <c r="BA27" s="315"/>
-    </row>
-    <row r="28" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A28" s="70">
-        <f t="shared" si="79"/>
-        <v>8</v>
-      </c>
-      <c r="B28" s="314"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="244"/>
-      <c r="P28" s="244"/>
-      <c r="Q28" s="315"/>
-      <c r="S28" s="70">
-        <f t="shared" si="80"/>
-        <v>8</v>
-      </c>
-      <c r="T28" s="314"/>
-      <c r="U28" s="17"/>
-      <c r="V28" s="17"/>
-      <c r="W28" s="17"/>
-      <c r="X28" s="17"/>
-      <c r="Y28" s="17"/>
-      <c r="Z28" s="17"/>
-      <c r="AA28" s="17"/>
-      <c r="AB28" s="17"/>
-      <c r="AC28" s="17"/>
-      <c r="AD28" s="17"/>
-      <c r="AE28" s="17"/>
-      <c r="AF28" s="17"/>
-      <c r="AG28" s="244"/>
-      <c r="AH28" s="244"/>
-      <c r="AI28" s="315"/>
-      <c r="AK28" s="70">
-        <f t="shared" si="81"/>
-        <v>8</v>
-      </c>
-      <c r="AL28" s="314"/>
-      <c r="AM28" s="17"/>
-      <c r="AN28" s="17"/>
-      <c r="AO28" s="17"/>
-      <c r="AP28" s="17"/>
-      <c r="AQ28" s="17"/>
-      <c r="AR28" s="17"/>
-      <c r="AS28" s="17"/>
-      <c r="AT28" s="17"/>
-      <c r="AU28" s="17"/>
-      <c r="AV28" s="17"/>
-      <c r="AW28" s="17"/>
-      <c r="AX28" s="17"/>
-      <c r="AY28" s="244"/>
-      <c r="AZ28" s="244"/>
-      <c r="BA28" s="315"/>
-    </row>
-    <row r="29" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A29" s="70">
-        <f t="shared" si="79"/>
-        <v>9</v>
-      </c>
-      <c r="B29" s="314"/>
-      <c r="C29" s="244"/>
-      <c r="D29" s="244"/>
-      <c r="E29" s="244"/>
-      <c r="F29" s="244"/>
-      <c r="G29" s="244"/>
-      <c r="H29" s="342"/>
-      <c r="I29" s="244"/>
-      <c r="J29" s="244"/>
-      <c r="K29" s="342"/>
-      <c r="L29" s="244"/>
-      <c r="M29" s="244"/>
-      <c r="N29" s="244"/>
-      <c r="O29" s="244"/>
-      <c r="P29" s="244"/>
-      <c r="Q29" s="315"/>
-      <c r="S29" s="70">
-        <f t="shared" si="80"/>
-        <v>9</v>
-      </c>
-      <c r="T29" s="383"/>
-      <c r="U29" s="342"/>
-      <c r="V29" s="342"/>
-      <c r="W29" s="342"/>
-      <c r="X29" s="342"/>
-      <c r="Y29" s="342"/>
-      <c r="Z29" s="342"/>
-      <c r="AA29" s="244"/>
-      <c r="AB29" s="244"/>
-      <c r="AC29" s="342"/>
-      <c r="AD29" s="342"/>
-      <c r="AE29" s="342"/>
-      <c r="AF29" s="342"/>
-      <c r="AG29" s="342"/>
-      <c r="AH29" s="342"/>
-      <c r="AI29" s="352"/>
-      <c r="AK29" s="70">
-        <f t="shared" si="81"/>
-        <v>9</v>
-      </c>
-      <c r="AL29" s="314"/>
-      <c r="AM29" s="244"/>
-      <c r="AN29" s="244"/>
-      <c r="AO29" s="244"/>
-      <c r="AP29" s="244"/>
-      <c r="AQ29" s="244"/>
-      <c r="AR29" s="244"/>
-      <c r="AS29" s="244"/>
-      <c r="AT29" s="244"/>
-      <c r="AU29" s="244"/>
-      <c r="AV29" s="244"/>
-      <c r="AW29" s="244"/>
-      <c r="AX29" s="244"/>
-      <c r="AY29" s="244"/>
-      <c r="AZ29" s="244"/>
-      <c r="BA29" s="315"/>
-    </row>
-    <row r="30" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A30" s="70">
-        <f t="shared" si="79"/>
-        <v>10</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="244"/>
-      <c r="D30" s="244"/>
-      <c r="E30" s="244"/>
-      <c r="F30" s="244"/>
-      <c r="G30" s="244"/>
-      <c r="H30" s="342"/>
-      <c r="I30" s="244"/>
-      <c r="J30" s="244"/>
-      <c r="K30" s="342"/>
-      <c r="L30" s="244"/>
-      <c r="M30" s="244"/>
-      <c r="N30" s="244"/>
-      <c r="O30" s="244"/>
-      <c r="P30" s="244"/>
-      <c r="Q30" s="26"/>
-      <c r="S30" s="70">
-        <f t="shared" si="80"/>
-        <v>10</v>
-      </c>
-      <c r="T30" s="16"/>
-      <c r="U30" s="244"/>
-      <c r="V30" s="244"/>
-      <c r="W30" s="244"/>
-      <c r="X30" s="244"/>
-      <c r="Y30" s="244"/>
-      <c r="Z30" s="244"/>
-      <c r="AA30" s="244"/>
-      <c r="AB30" s="244"/>
-      <c r="AC30" s="244"/>
-      <c r="AD30" s="244"/>
-      <c r="AE30" s="244"/>
-      <c r="AF30" s="244"/>
-      <c r="AG30" s="244"/>
-      <c r="AH30" s="244"/>
-      <c r="AI30" s="26"/>
-      <c r="AK30" s="70">
-        <f t="shared" si="81"/>
-        <v>10</v>
-      </c>
-      <c r="AL30" s="16"/>
-      <c r="AM30" s="244"/>
-      <c r="AN30" s="244"/>
-      <c r="AO30" s="244"/>
-      <c r="AP30" s="244"/>
-      <c r="AQ30" s="244"/>
-      <c r="AR30" s="244"/>
-      <c r="AS30" s="244"/>
-      <c r="AT30" s="244"/>
-      <c r="AU30" s="244"/>
-      <c r="AV30" s="244"/>
-      <c r="AW30" s="244"/>
-      <c r="AX30" s="244"/>
-      <c r="AY30" s="244"/>
-      <c r="AZ30" s="244"/>
-      <c r="BA30" s="26"/>
-    </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A31" s="70">
-        <f t="shared" si="79"/>
-        <v>11</v>
-      </c>
-      <c r="B31" s="314"/>
-      <c r="C31" s="244"/>
-      <c r="D31" s="244"/>
-      <c r="E31" s="244"/>
-      <c r="F31" s="244"/>
-      <c r="G31" s="244"/>
-      <c r="H31" s="342"/>
-      <c r="I31" s="244"/>
-      <c r="J31" s="244"/>
-      <c r="K31" s="342"/>
-      <c r="L31" s="244"/>
-      <c r="M31" s="244"/>
-      <c r="N31" s="244"/>
-      <c r="O31" s="244"/>
-      <c r="P31" s="244"/>
-      <c r="Q31" s="26"/>
-      <c r="S31" s="70">
-        <f t="shared" si="80"/>
-        <v>11</v>
-      </c>
-      <c r="T31" s="314"/>
-      <c r="U31" s="244"/>
-      <c r="V31" s="244"/>
-      <c r="W31" s="244"/>
-      <c r="X31" s="244"/>
-      <c r="Y31" s="244"/>
-      <c r="Z31" s="244"/>
-      <c r="AA31" s="244"/>
-      <c r="AB31" s="244"/>
-      <c r="AC31" s="244"/>
-      <c r="AD31" s="244"/>
-      <c r="AE31" s="244"/>
-      <c r="AF31" s="244"/>
-      <c r="AG31" s="244"/>
-      <c r="AH31" s="244"/>
-      <c r="AI31" s="26"/>
-      <c r="AK31" s="70">
-        <f t="shared" si="81"/>
-        <v>11</v>
-      </c>
-      <c r="AL31" s="314"/>
-      <c r="AM31" s="244"/>
-      <c r="AN31" s="244"/>
-      <c r="AO31" s="244"/>
-      <c r="AP31" s="244"/>
-      <c r="AQ31" s="244"/>
-      <c r="AR31" s="244"/>
-      <c r="AS31" s="244"/>
-      <c r="AT31" s="244"/>
-      <c r="AU31" s="244"/>
-      <c r="AV31" s="244"/>
-      <c r="AW31" s="244"/>
-      <c r="AX31" s="244"/>
-      <c r="AY31" s="244"/>
-      <c r="AZ31" s="244"/>
-      <c r="BA31" s="26"/>
-    </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A32" s="70">
-        <f t="shared" si="79"/>
-        <v>12</v>
-      </c>
-      <c r="B32" s="314"/>
-      <c r="C32" s="244"/>
-      <c r="D32" s="244"/>
-      <c r="E32" s="244"/>
-      <c r="F32" s="244"/>
-      <c r="G32" s="244"/>
-      <c r="H32" s="342"/>
-      <c r="I32" s="244"/>
-      <c r="J32" s="244"/>
-      <c r="K32" s="342"/>
-      <c r="L32" s="244"/>
-      <c r="M32" s="244"/>
-      <c r="N32" s="244"/>
-      <c r="O32" s="244"/>
-      <c r="P32" s="244"/>
-      <c r="Q32" s="26"/>
-      <c r="S32" s="70">
-        <f t="shared" si="80"/>
-        <v>12</v>
-      </c>
-      <c r="T32" s="314"/>
-      <c r="U32" s="244"/>
-      <c r="V32" s="244"/>
-      <c r="W32" s="244"/>
-      <c r="X32" s="244"/>
-      <c r="Y32" s="244"/>
-      <c r="Z32" s="244"/>
-      <c r="AA32" s="244"/>
-      <c r="AB32" s="244"/>
-      <c r="AC32" s="244"/>
-      <c r="AD32" s="244"/>
-      <c r="AE32" s="244"/>
-      <c r="AF32" s="244"/>
-      <c r="AG32" s="244"/>
-      <c r="AH32" s="244"/>
-      <c r="AI32" s="26"/>
-      <c r="AK32" s="70">
-        <f t="shared" si="81"/>
-        <v>12</v>
-      </c>
-      <c r="AL32" s="314"/>
-      <c r="AM32" s="244"/>
-      <c r="AN32" s="244"/>
-      <c r="AO32" s="244"/>
-      <c r="AP32" s="244"/>
-      <c r="AQ32" s="244"/>
-      <c r="AR32" s="244"/>
-      <c r="AS32" s="244"/>
-      <c r="AT32" s="244"/>
-      <c r="AU32" s="244"/>
-      <c r="AV32" s="244"/>
-      <c r="AW32" s="244"/>
-      <c r="AX32" s="244"/>
-      <c r="AY32" s="244"/>
-      <c r="AZ32" s="244"/>
-      <c r="BA32" s="26"/>
-    </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A33" s="70">
-        <f t="shared" si="79"/>
-        <v>13</v>
-      </c>
-      <c r="B33" s="314"/>
-      <c r="C33" s="244"/>
-      <c r="D33" s="244"/>
-      <c r="E33" s="244"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="219"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="219"/>
-      <c r="L33" s="244"/>
-      <c r="M33" s="244"/>
-      <c r="N33" s="244"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17"/>
-      <c r="Q33" s="26"/>
-      <c r="S33" s="70">
-        <f t="shared" si="80"/>
-        <v>13</v>
-      </c>
-      <c r="T33" s="314"/>
-      <c r="U33" s="244"/>
-      <c r="V33" s="244"/>
-      <c r="W33" s="244"/>
-      <c r="X33" s="17"/>
-      <c r="Y33" s="17"/>
-      <c r="Z33" s="17"/>
-      <c r="AA33" s="17"/>
-      <c r="AB33" s="17"/>
-      <c r="AC33" s="17"/>
-      <c r="AD33" s="244"/>
-      <c r="AE33" s="244"/>
-      <c r="AF33" s="244"/>
-      <c r="AG33" s="17"/>
-      <c r="AH33" s="17"/>
-      <c r="AI33" s="26"/>
-      <c r="AK33" s="70">
-        <f t="shared" si="81"/>
-        <v>13</v>
-      </c>
-      <c r="AL33" s="314"/>
-      <c r="AM33" s="244"/>
-      <c r="AN33" s="244"/>
-      <c r="AO33" s="244"/>
-      <c r="AP33" s="17"/>
-      <c r="AQ33" s="17"/>
-      <c r="AR33" s="17"/>
-      <c r="AS33" s="17"/>
-      <c r="AT33" s="17"/>
-      <c r="AU33" s="17"/>
-      <c r="AV33" s="244"/>
-      <c r="AW33" s="244"/>
-      <c r="AX33" s="244"/>
-      <c r="AY33" s="17"/>
-      <c r="AZ33" s="17"/>
-      <c r="BA33" s="26"/>
-    </row>
-    <row r="34" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A34" s="70">
-        <f t="shared" si="79"/>
-        <v>14</v>
-      </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="219"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="219"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17"/>
-      <c r="Q34" s="26"/>
-      <c r="S34" s="70">
-        <f t="shared" si="80"/>
-        <v>14</v>
-      </c>
-      <c r="T34" s="16"/>
-      <c r="U34" s="17"/>
-      <c r="V34" s="17"/>
-      <c r="W34" s="17"/>
-      <c r="X34" s="17"/>
-      <c r="Y34" s="17"/>
-      <c r="Z34" s="17"/>
-      <c r="AA34" s="17"/>
-      <c r="AB34" s="17"/>
-      <c r="AC34" s="17"/>
-      <c r="AD34" s="17"/>
-      <c r="AE34" s="17"/>
-      <c r="AF34" s="17"/>
-      <c r="AG34" s="17"/>
-      <c r="AH34" s="17"/>
-      <c r="AI34" s="26"/>
-      <c r="AK34" s="70">
-        <f t="shared" si="81"/>
-        <v>14</v>
-      </c>
-      <c r="AL34" s="16"/>
-      <c r="AM34" s="17"/>
-      <c r="AN34" s="17"/>
-      <c r="AO34" s="17"/>
-      <c r="AP34" s="17"/>
-      <c r="AQ34" s="17"/>
-      <c r="AR34" s="17"/>
-      <c r="AS34" s="17"/>
-      <c r="AT34" s="17"/>
-      <c r="AU34" s="17"/>
-      <c r="AV34" s="17"/>
-      <c r="AW34" s="17"/>
-      <c r="AX34" s="17"/>
-      <c r="AY34" s="17"/>
-      <c r="AZ34" s="17"/>
-      <c r="BA34" s="26"/>
-    </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A35" s="70">
-        <f t="shared" si="79"/>
-        <v>15</v>
-      </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="412"/>
-      <c r="I35" s="317"/>
-      <c r="J35" s="317"/>
-      <c r="K35" s="412"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="33"/>
-      <c r="S35" s="70">
-        <f t="shared" si="80"/>
-        <v>15</v>
-      </c>
-      <c r="T35" s="32"/>
-      <c r="U35" s="22"/>
-      <c r="V35" s="22"/>
-      <c r="W35" s="22"/>
-      <c r="X35" s="22"/>
-      <c r="Y35" s="22"/>
-      <c r="Z35" s="317"/>
-      <c r="AA35" s="317"/>
-      <c r="AB35" s="317"/>
-      <c r="AC35" s="317"/>
-      <c r="AD35" s="22"/>
-      <c r="AE35" s="22"/>
-      <c r="AF35" s="22"/>
-      <c r="AG35" s="22"/>
-      <c r="AH35" s="22"/>
-      <c r="AI35" s="33"/>
-      <c r="AK35" s="70">
-        <f t="shared" si="81"/>
-        <v>15</v>
-      </c>
-      <c r="AL35" s="32"/>
-      <c r="AM35" s="22"/>
-      <c r="AN35" s="22"/>
-      <c r="AO35" s="22"/>
-      <c r="AP35" s="22"/>
-      <c r="AQ35" s="22"/>
-      <c r="AR35" s="317"/>
-      <c r="AS35" s="317"/>
-      <c r="AT35" s="317"/>
-      <c r="AU35" s="317"/>
-      <c r="AV35" s="22"/>
-      <c r="AW35" s="22"/>
-      <c r="AX35" s="22"/>
-      <c r="AY35" s="22"/>
-      <c r="AZ35" s="22"/>
-      <c r="BA35" s="33"/>
-    </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A36" s="242" t="s">
-        <v>395</v>
-      </c>
-      <c r="S36" s="242" t="s">
-        <v>395</v>
-      </c>
-      <c r="AK36" s="242" t="s">
-        <v>395</v>
+      <c r="R17" s="434">
+        <f>Q17/K17</f>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A18" s="305"/>
+      <c r="B18" s="305"/>
+      <c r="C18" s="305"/>
+      <c r="D18" s="305"/>
+      <c r="E18" s="305"/>
+      <c r="F18" s="305"/>
+      <c r="G18" s="305"/>
+      <c r="H18" s="305"/>
+      <c r="I18" s="305"/>
+      <c r="J18" s="305"/>
+      <c r="K18" s="305"/>
+      <c r="L18" s="305"/>
+      <c r="M18" s="305"/>
+      <c r="N18" s="305"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A19" s="305"/>
+      <c r="B19" s="428"/>
+      <c r="C19" s="429"/>
+      <c r="D19" s="305"/>
+      <c r="E19" s="305"/>
+      <c r="F19" s="305"/>
+      <c r="G19" s="305"/>
+      <c r="K19" s="305">
+        <v>450432</v>
+      </c>
+      <c r="O19" s="305">
+        <v>331968</v>
+      </c>
+      <c r="R19" s="305"/>
+      <c r="S19" s="305">
+        <v>2315040</v>
+      </c>
+      <c r="W19" s="305">
+        <v>2152800</v>
+      </c>
+      <c r="Z19" s="305">
+        <v>2541000</v>
+      </c>
+      <c r="AB19" s="305">
+        <v>2994448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A20" s="305"/>
+      <c r="B20" s="428"/>
+      <c r="C20" s="429"/>
+      <c r="D20" s="305">
+        <v>59823</v>
+      </c>
+      <c r="E20" s="305"/>
+      <c r="G20" s="305"/>
+      <c r="K20" s="305">
+        <f>K19/128</f>
+        <v>3519</v>
+      </c>
+      <c r="O20" s="305">
+        <f>O19/112</f>
+        <v>2964</v>
+      </c>
+      <c r="R20" s="305"/>
+      <c r="S20" s="305">
+        <f>S19/78</f>
+        <v>29680</v>
+      </c>
+      <c r="W20" s="305">
+        <f>W19/115</f>
+        <v>18720</v>
+      </c>
+      <c r="Z20" s="305">
+        <f>Z19/100</f>
+        <v>25410</v>
+      </c>
+      <c r="AB20" s="305">
+        <f>AB19/109</f>
+        <v>27472</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A21" s="305"/>
+      <c r="B21" s="305"/>
+      <c r="C21" s="305"/>
+      <c r="D21" s="426" t="s">
+        <v>454</v>
+      </c>
+      <c r="F21" s="426" t="s">
+        <v>454</v>
+      </c>
+      <c r="G21" s="305"/>
+      <c r="K21" s="305">
+        <f>K20/(16*16)</f>
+        <v>13.74609375</v>
+      </c>
+      <c r="O21" s="305">
+        <f>O20/(16*16)</f>
+        <v>11.578125</v>
+      </c>
+      <c r="R21" s="305"/>
+      <c r="S21" s="305">
+        <f>S20/(16*16)</f>
+        <v>115.9375</v>
+      </c>
+      <c r="W21" s="305">
+        <f>W20/(16*16)</f>
+        <v>73.125</v>
+      </c>
+      <c r="Z21" s="305">
+        <f>Z20/(16*16)</f>
+        <v>99.2578125</v>
+      </c>
+      <c r="AB21" s="305">
+        <f>AB20/(16*16)</f>
+        <v>107.3125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A22" s="305"/>
+      <c r="B22" s="305"/>
+      <c r="C22" s="305"/>
+      <c r="D22" s="430">
+        <f>B9*$D$20</f>
+        <v>598.23</v>
+      </c>
+      <c r="E22" s="430"/>
+      <c r="F22" s="430">
+        <f>K9*C9</f>
+        <v>143.36000000000001</v>
+      </c>
+      <c r="G22" s="431">
+        <f>F22*$K$21</f>
+        <v>1970.64</v>
+      </c>
+      <c r="H22" s="433">
+        <f>G22/K$19</f>
+        <v>4.3750000000000004E-3</v>
+      </c>
+      <c r="I22" s="430">
+        <f>Q9*$K$21</f>
+        <v>4398.75</v>
+      </c>
+      <c r="J22" s="433">
+        <f>I22/K$19</f>
+        <v>9.765625E-3</v>
+      </c>
+      <c r="K22" s="432"/>
+      <c r="L22" s="433">
+        <f>K22/K$19</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="433"/>
+      <c r="N22" s="305">
+        <f>F22*$O$21</f>
+        <v>1659.8400000000001</v>
+      </c>
+      <c r="O22" s="305">
+        <v>6511</v>
+      </c>
+      <c r="P22" s="433">
+        <f>O22/O$19</f>
+        <v>1.9613336225178329E-2</v>
+      </c>
+      <c r="R22" s="305">
+        <f>F22*$S$21</f>
+        <v>16620.800000000003</v>
+      </c>
+      <c r="S22" s="305">
+        <v>50813</v>
+      </c>
+      <c r="T22" s="433">
+        <f>S22/S$19</f>
+        <v>2.1949080793420415E-2</v>
+      </c>
+      <c r="W22" s="305">
+        <v>18509</v>
+      </c>
+      <c r="X22" s="433">
+        <f>W22/W$19</f>
+        <v>8.5976402824228908E-3</v>
+      </c>
+      <c r="Z22" s="305">
+        <v>21511</v>
+      </c>
+      <c r="AA22" s="433">
+        <f>Z22/Z$19</f>
+        <v>8.4655647382920109E-3</v>
+      </c>
+      <c r="AB22" s="305">
+        <v>20101</v>
+      </c>
+      <c r="AC22" s="433">
+        <f>AB22/AB$19</f>
+        <v>6.7127564078588104E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D23" s="430">
+        <f>B10*$D$20</f>
+        <v>598.23</v>
+      </c>
+      <c r="E23" s="430"/>
+      <c r="F23" s="430">
+        <f t="shared" ref="F23:F30" si="7">K10*C10</f>
+        <v>61.44</v>
+      </c>
+      <c r="G23" s="431">
+        <f>F23*$K$21</f>
+        <v>844.56</v>
+      </c>
+      <c r="H23" s="433">
+        <f t="shared" ref="H23:H30" si="8">G23/K$19</f>
+        <v>1.8749999999999999E-3</v>
+      </c>
+      <c r="I23" s="430">
+        <f>Q10*$K$21</f>
+        <v>879.75</v>
+      </c>
+      <c r="J23" s="433">
+        <f t="shared" ref="J23:J30" si="9">I23/K$19</f>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="K23" s="432"/>
+      <c r="L23" s="433">
+        <f>K23/K$19</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="305">
+        <f>F23*$O$21</f>
+        <v>711.36</v>
+      </c>
+      <c r="P23" s="433">
+        <f>O23/O$19</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="305">
+        <f>F23*$S$21</f>
+        <v>7123.2</v>
+      </c>
+      <c r="T23" s="433">
+        <f>S23/S$19</f>
+        <v>0</v>
+      </c>
+      <c r="X23" s="433">
+        <f>W23/W$19</f>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="433">
+        <f>Z23/Z$19</f>
+        <v>0</v>
+      </c>
+      <c r="AC23" s="433">
+        <f>AB23/AB$19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D24" s="430">
+        <f>B11*$D$20</f>
+        <v>598.23</v>
+      </c>
+      <c r="E24" s="430"/>
+      <c r="F24" s="430">
+        <f t="shared" si="7"/>
+        <v>81.92</v>
+      </c>
+      <c r="G24" s="431">
+        <f>F24*$K$21</f>
+        <v>1126.08</v>
+      </c>
+      <c r="H24" s="433">
+        <f t="shared" si="8"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="I24" s="430">
+        <f>Q11*$K$21</f>
+        <v>1099.6875</v>
+      </c>
+      <c r="J24" s="433">
+        <f t="shared" si="9"/>
+        <v>2.44140625E-3</v>
+      </c>
+      <c r="K24" s="432">
+        <v>939</v>
+      </c>
+      <c r="L24" s="433">
+        <f>K24/K$19</f>
+        <v>2.0846653878942882E-3</v>
+      </c>
+      <c r="N24" s="305">
+        <f>F24*$O$21</f>
+        <v>948.48</v>
+      </c>
+      <c r="P24" s="433">
+        <f>O24/O$19</f>
+        <v>0</v>
+      </c>
+      <c r="R24" s="305">
+        <f>F24*$S$21</f>
+        <v>9497.6</v>
+      </c>
+      <c r="T24" s="433">
+        <f>S24/S$19</f>
+        <v>0</v>
+      </c>
+      <c r="X24" s="433">
+        <f>W24/W$19</f>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="433">
+        <f>Z24/Z$19</f>
+        <v>0</v>
+      </c>
+      <c r="AC24" s="433">
+        <f>AB24/AB$19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D25" s="430">
+        <f>B12*$D$20</f>
+        <v>598.23</v>
+      </c>
+      <c r="E25" s="430"/>
+      <c r="F25" s="430">
+        <f t="shared" si="7"/>
+        <v>286.72000000000003</v>
+      </c>
+      <c r="G25" s="431">
+        <f>F25*$K$21</f>
+        <v>3941.28</v>
+      </c>
+      <c r="H25" s="433">
+        <f t="shared" si="8"/>
+        <v>8.7500000000000008E-3</v>
+      </c>
+      <c r="I25" s="430">
+        <f>Q12*$K$21</f>
+        <v>3848.90625</v>
+      </c>
+      <c r="J25" s="433">
+        <f t="shared" si="9"/>
+        <v>8.544921875E-3</v>
+      </c>
+      <c r="K25" s="432">
+        <v>2749</v>
+      </c>
+      <c r="L25" s="433">
+        <f>K25/K$19</f>
+        <v>6.1030299801079855E-3</v>
+      </c>
+      <c r="N25" s="305">
+        <f>F25*$O$21</f>
+        <v>3319.6800000000003</v>
+      </c>
+      <c r="O25" s="426">
+        <v>2699</v>
+      </c>
+      <c r="P25" s="433">
+        <f>O25/O$19</f>
+        <v>8.1303017158280318E-3</v>
+      </c>
+      <c r="R25" s="305">
+        <f>F25*$S$21</f>
+        <v>33241.600000000006</v>
+      </c>
+      <c r="S25" s="426">
+        <v>19441</v>
+      </c>
+      <c r="T25" s="433">
+        <f>S25/S$19</f>
+        <v>8.3976950722233733E-3</v>
+      </c>
+      <c r="W25" s="426">
+        <v>13749</v>
+      </c>
+      <c r="X25" s="433">
+        <f>W25/W$19</f>
+        <v>6.3865663322185059E-3</v>
+      </c>
+      <c r="Z25" s="426">
+        <v>15221</v>
+      </c>
+      <c r="AA25" s="433">
+        <f>Z25/Z$19</f>
+        <v>5.9901613537977176E-3</v>
+      </c>
+      <c r="AB25" s="426">
+        <v>14406</v>
+      </c>
+      <c r="AC25" s="433">
+        <f>AB25/AB$19</f>
+        <v>4.8109033785191796E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D26" s="430">
+        <f>B13*$D$20</f>
+        <v>358.93799999999999</v>
+      </c>
+      <c r="E26" s="430"/>
+      <c r="F26" s="430">
+        <f t="shared" si="7"/>
+        <v>79.872</v>
+      </c>
+      <c r="G26" s="431">
+        <f>F26*$K$21</f>
+        <v>1097.9280000000001</v>
+      </c>
+      <c r="H26" s="433">
+        <f t="shared" si="8"/>
+        <v>2.4375000000000004E-3</v>
+      </c>
+      <c r="I26" s="430">
+        <f>Q13*$K$21</f>
+        <v>1319.625</v>
+      </c>
+      <c r="J26" s="433">
+        <f t="shared" si="9"/>
+        <v>2.9296875E-3</v>
+      </c>
+      <c r="K26" s="432">
+        <v>1118</v>
+      </c>
+      <c r="L26" s="433">
+        <f>K26/K$19</f>
+        <v>2.4820616652458083E-3</v>
+      </c>
+      <c r="N26" s="305">
+        <f>F26*$O$21</f>
+        <v>924.76800000000003</v>
+      </c>
+      <c r="O26" s="426">
+        <v>1142</v>
+      </c>
+      <c r="P26" s="433">
+        <f>O26/O$19</f>
+        <v>3.4400906111432426E-3</v>
+      </c>
+      <c r="R26" s="305">
+        <f>F26*$S$21</f>
+        <v>9260.16</v>
+      </c>
+      <c r="S26" s="426">
+        <v>10442</v>
+      </c>
+      <c r="T26" s="433">
+        <f>S26/S$19</f>
+        <v>4.5105052180523875E-3</v>
+      </c>
+      <c r="W26" s="426">
+        <v>7146</v>
+      </c>
+      <c r="X26" s="433">
+        <f>W26/W$19</f>
+        <v>3.3193979933110367E-3</v>
+      </c>
+      <c r="Z26" s="426">
+        <v>8389</v>
+      </c>
+      <c r="AA26" s="433">
+        <f>Z26/Z$19</f>
+        <v>3.3014561196379379E-3</v>
+      </c>
+      <c r="AB26" s="426">
+        <v>6983</v>
+      </c>
+      <c r="AC26" s="433">
+        <f>AB26/AB$19</f>
+        <v>2.3319823887407629E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D27" s="430">
+        <f>B14*$D$20</f>
+        <v>89.734499999999997</v>
+      </c>
+      <c r="E27" s="430">
+        <v>61</v>
+      </c>
+      <c r="F27" s="430">
+        <f t="shared" si="7"/>
+        <v>11.136000000000001</v>
+      </c>
+      <c r="G27" s="431">
+        <f>F27*$K$21</f>
+        <v>153.07650000000001</v>
+      </c>
+      <c r="H27" s="433">
+        <f t="shared" si="8"/>
+        <v>3.3984375000000003E-4</v>
+      </c>
+      <c r="I27" s="430">
+        <f>Q14*$K$21</f>
+        <v>164.953125</v>
+      </c>
+      <c r="J27" s="433">
+        <f t="shared" si="9"/>
+        <v>3.662109375E-4</v>
+      </c>
+      <c r="K27" s="432">
+        <v>175</v>
+      </c>
+      <c r="L27" s="433">
+        <f>K27/K$19</f>
+        <v>3.8851591361182153E-4</v>
+      </c>
+      <c r="N27" s="305">
+        <f>F27*$O$21</f>
+        <v>128.934</v>
+      </c>
+      <c r="O27" s="426">
+        <v>74</v>
+      </c>
+      <c r="P27" s="433">
+        <f>O27/O$19</f>
+        <v>2.2291305186042029E-4</v>
+      </c>
+      <c r="R27" s="305">
+        <f>F27*$S$21</f>
+        <v>1291.0800000000002</v>
+      </c>
+      <c r="S27" s="426">
+        <v>993</v>
+      </c>
+      <c r="T27" s="433">
+        <f>S27/S$19</f>
+        <v>4.2893427327389593E-4</v>
+      </c>
+      <c r="W27" s="426">
+        <v>1031</v>
+      </c>
+      <c r="X27" s="433">
+        <f>W27/W$19</f>
+        <v>4.7891118543292455E-4</v>
+      </c>
+      <c r="Z27" s="426">
+        <v>1089</v>
+      </c>
+      <c r="AA27" s="433">
+        <f>Z27/Z$19</f>
+        <v>4.2857142857142855E-4</v>
+      </c>
+      <c r="AB27" s="426">
+        <v>615</v>
+      </c>
+      <c r="AC27" s="433">
+        <f>AB27/AB$19</f>
+        <v>2.0538009008672049E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D28" s="430">
+        <f>B15*$D$20</f>
+        <v>83.752200000000002</v>
+      </c>
+      <c r="E28" s="430">
+        <v>57</v>
+      </c>
+      <c r="F28" s="430">
+        <f t="shared" si="7"/>
+        <v>8.9599999999999991</v>
+      </c>
+      <c r="G28" s="431">
+        <f>F28*$K$21</f>
+        <v>123.16499999999999</v>
+      </c>
+      <c r="H28" s="433">
+        <f t="shared" si="8"/>
+        <v>2.7343749999999997E-4</v>
+      </c>
+      <c r="I28" s="430">
+        <f>Q15*$K$21</f>
+        <v>82.4765625</v>
+      </c>
+      <c r="J28" s="433">
+        <f t="shared" si="9"/>
+        <v>1.8310546875E-4</v>
+      </c>
+      <c r="K28" s="432">
+        <v>111</v>
+      </c>
+      <c r="L28" s="433">
+        <f>K28/K$19</f>
+        <v>2.4643009377664109E-4</v>
+      </c>
+      <c r="N28" s="305">
+        <f>F28*$O$21</f>
+        <v>103.74</v>
+      </c>
+      <c r="O28" s="426">
+        <v>52</v>
+      </c>
+      <c r="P28" s="433">
+        <f>O28/O$19</f>
+        <v>1.5664160401002505E-4</v>
+      </c>
+      <c r="R28" s="305">
+        <f>F28*$S$21</f>
+        <v>1038.8</v>
+      </c>
+      <c r="S28" s="426">
+        <v>418</v>
+      </c>
+      <c r="T28" s="433">
+        <f>S28/S$19</f>
+        <v>1.8055843527541642E-4</v>
+      </c>
+      <c r="W28" s="426">
+        <v>680</v>
+      </c>
+      <c r="X28" s="433">
+        <f>W28/W$19</f>
+        <v>3.1586770717205502E-4</v>
+      </c>
+      <c r="Z28" s="426">
+        <v>537</v>
+      </c>
+      <c r="AA28" s="433">
+        <f>Z28/Z$19</f>
+        <v>2.1133412042502952E-4</v>
+      </c>
+      <c r="AB28" s="426">
+        <v>349</v>
+      </c>
+      <c r="AC28" s="433">
+        <f>AB28/AB$19</f>
+        <v>1.1654902673213895E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D29" s="430">
+        <f>B16*$D$20</f>
+        <v>478.584</v>
+      </c>
+      <c r="E29" s="430">
+        <v>322</v>
+      </c>
+      <c r="F29" s="430">
+        <f t="shared" si="7"/>
+        <v>18.432000000000002</v>
+      </c>
+      <c r="G29" s="431">
+        <f>F29*$K$21</f>
+        <v>253.36800000000002</v>
+      </c>
+      <c r="H29" s="433">
+        <f t="shared" si="8"/>
+        <v>5.6250000000000007E-4</v>
+      </c>
+      <c r="I29" s="430">
+        <f>Q16*$K$21</f>
+        <v>329.90625</v>
+      </c>
+      <c r="J29" s="433">
+        <f t="shared" si="9"/>
+        <v>7.32421875E-4</v>
+      </c>
+      <c r="K29" s="432">
+        <v>322</v>
+      </c>
+      <c r="L29" s="433">
+        <f>K29/K$19</f>
+        <v>7.1486928104575159E-4</v>
+      </c>
+      <c r="N29" s="305">
+        <f>F29*$O$21</f>
+        <v>213.40800000000002</v>
+      </c>
+      <c r="O29" s="426">
+        <v>296</v>
+      </c>
+      <c r="P29" s="433">
+        <f>O29/O$19</f>
+        <v>8.9165220744168118E-4</v>
+      </c>
+      <c r="R29" s="305">
+        <f>F29*$S$21</f>
+        <v>2136.96</v>
+      </c>
+      <c r="S29" s="426">
+        <v>3067</v>
+      </c>
+      <c r="T29" s="433">
+        <f>S29/S$19</f>
+        <v>1.3248151219849332E-3</v>
+      </c>
+      <c r="W29" s="426">
+        <v>2023</v>
+      </c>
+      <c r="X29" s="433">
+        <f>W29/W$19</f>
+        <v>9.3970642883686359E-4</v>
+      </c>
+      <c r="Z29" s="426">
+        <v>2242</v>
+      </c>
+      <c r="AA29" s="433">
+        <f>Z29/Z$19</f>
+        <v>8.8232979142070051E-4</v>
+      </c>
+      <c r="AB29" s="426">
+        <v>1664</v>
+      </c>
+      <c r="AC29" s="433">
+        <f>AB29/AB$19</f>
+        <v>5.5569507301512664E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D30" s="430">
+        <f>B17*$D$20</f>
+        <v>89.734499999999997</v>
+      </c>
+      <c r="E30" s="430">
+        <v>96</v>
+      </c>
+      <c r="F30" s="430">
+        <f t="shared" si="7"/>
+        <v>5.76</v>
+      </c>
+      <c r="G30" s="431">
+        <f>F30*$K$21</f>
+        <v>79.177499999999995</v>
+      </c>
+      <c r="H30" s="433">
+        <f t="shared" si="8"/>
+        <v>1.7578124999999999E-4</v>
+      </c>
+      <c r="I30" s="430">
+        <f>Q17*$K$21</f>
+        <v>54.984375</v>
+      </c>
+      <c r="J30" s="433">
+        <f t="shared" si="9"/>
+        <v>1.220703125E-4</v>
+      </c>
+      <c r="K30" s="432">
+        <v>96</v>
+      </c>
+      <c r="L30" s="433">
+        <f>K30/K$19</f>
+        <v>2.1312872975277067E-4</v>
+      </c>
+      <c r="N30" s="305">
+        <f>F30*$O$21</f>
+        <v>66.69</v>
+      </c>
+      <c r="O30" s="426">
+        <v>45</v>
+      </c>
+      <c r="P30" s="433">
+        <f>O30/O$19</f>
+        <v>1.3555523423944477E-4</v>
+      </c>
+      <c r="R30" s="305">
+        <f>F30*$S$21</f>
+        <v>667.8</v>
+      </c>
+      <c r="S30" s="426">
+        <v>404</v>
+      </c>
+      <c r="T30" s="433">
+        <f>S30/S$19</f>
+        <v>1.7451102356762734E-4</v>
+      </c>
+      <c r="W30" s="426">
+        <v>470</v>
+      </c>
+      <c r="X30" s="433">
+        <f>W30/W$19</f>
+        <v>2.1832032701597919E-4</v>
+      </c>
+      <c r="Z30" s="426">
+        <v>365</v>
+      </c>
+      <c r="AA30" s="433">
+        <f>Z30/Z$19</f>
+        <v>1.4364423455332547E-4</v>
+      </c>
+      <c r="AB30" s="426">
+        <v>254</v>
+      </c>
+      <c r="AC30" s="433">
+        <f>AB30/AB$19</f>
+        <v>8.4823646962645536E-5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
* Removed the silverfish from the sewers and mineshafts * Oops, sometimes the vertical mineshafts go down beyond the bedrock * Fixed bunker plots clearing out too much rock * Fixed bunker plots not generating caves correctly * Incorporated support for Tekkit material types above base on initial work by gunre
</commit_message>
<xml_diff>
--- a/notes/PlatMaps.xlsx
+++ b/notes/PlatMaps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="168" windowWidth="16260" windowHeight="8880" tabRatio="740" firstSheet="36" activeTab="42"/>
+    <workbookView xWindow="0" yWindow="228" windowWidth="16260" windowHeight="8820" tabRatio="740" firstSheet="36" activeTab="43"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,8 @@
     <sheet name="Mineshafts" sheetId="47" r:id="rId40"/>
     <sheet name="Bunkers" sheetId="48" r:id="rId41"/>
     <sheet name="Sewers2" sheetId="49" r:id="rId42"/>
-    <sheet name="Sheet2" sheetId="50" r:id="rId43"/>
+    <sheet name="Ore Distribution" sheetId="50" r:id="rId43"/>
+    <sheet name="Tekkit Ores" sheetId="52" r:id="rId44"/>
   </sheets>
   <definedNames>
     <definedName name="AbsoluteMaximumFloorsBelow">Sheet3!$C$6</definedName>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="553">
   <si>
     <t>grove</t>
   </si>
@@ -1431,6 +1432,300 @@
   <si>
     <t>Region</t>
   </si>
+  <si>
+    <t>Unused</t>
+  </si>
+  <si>
+    <t>Tile</t>
+  </si>
+  <si>
+    <t>prefixed stripped</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>dotted</t>
+  </si>
+  <si>
+    <t>Id value</t>
+  </si>
+  <si>
+    <t>Block. Name: eloraam.base.BlockAppliance. ID: 137</t>
+  </si>
+  <si>
+    <t>Block. Name: eloraam.logic.BlockLogic. ID: 138</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.indigo. ID: 139</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.rpores. ID: 140</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.rpleaves. ID: 141</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.rpstone. ID: 142</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.rplog. ID: 143</t>
+  </si>
+  <si>
+    <t>Block. Name: eloraam.world.BlockCustomCrops. ID: 144</t>
+  </si>
+  <si>
+    <t>Block. Name: eloraam.world.BlockStorage. ID: 145</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.rplampon. ID: 146</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.rplampoff. ID: 147</t>
+  </si>
+  <si>
+    <t>Block. Name: eloraam.core.BlockMultipart. ID: 148</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.craftingtableiii. ID: 149</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.rpmachine. ID: 150</t>
+  </si>
+  <si>
+    <t>Block. Name: eloraam.machine.BlockMachinePanel. ID: 151</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.rpframe. ID: 152</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.machineBlock. ID: 153</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.markerBlock. ID: 154</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.fillerBlock. ID: 155</t>
+  </si>
+  <si>
+    <t>Block. Name: buildcraft.transport.LegacyBlock. ID: 156</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.builderBlock. ID: 157</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.templateBlock. ID: 158</t>
+  </si>
+  <si>
+    <t>Block. Name: buildcraft.transport.LegacyBlock. ID: 159</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.frameBlock. ID: 160</t>
+  </si>
+  <si>
+    <t>Block. Name: buildcraft.energy.BlockEngine. ID: 161</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.oilMoving. ID: 162</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.oilStill. ID: 163</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.pumpBlock. ID: 164</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.tankBlock. ID: 165</t>
+  </si>
+  <si>
+    <t>Block. Name: buildcraft.transport.BlockGenericPipe. ID: 166</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.refineryBlock. ID: 167</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.autoWorkbenchBlock. ID: 169</t>
+  </si>
+  <si>
+    <t>Block. Name: buildcraft.transport.LegacyBlock. ID: 170</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.plainPipeBlock. ID: 171</t>
+  </si>
+  <si>
+    <t>Block. Name: buildcraft.transport.LegacyBlock. ID: 172</t>
+  </si>
+  <si>
+    <t>Block. Name: buildcraft.transport.LegacyBlock. ID: 173</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.miningWellBlock. ID: 174</t>
+  </si>
+  <si>
+    <t>Block. Name: buildcraft.transport.LegacyBlock. ID: 175</t>
+  </si>
+  <si>
+    <t>Block. Name: buildcraft.transport.LegacyBlock. ID: 176</t>
+  </si>
+  <si>
+    <t>Block. Name: eloraam.logic.BlockLogic. ID: 177</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.enderchest. ID: 178</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.Teleport Tether. ID: 179</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.IronChest. ID: 181</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.CompactSolar. ID: 183</t>
+  </si>
+  <si>
+    <t>Block. Name: BlockChargingBench. ID: 187</t>
+  </si>
+  <si>
+    <t>Block. Name: ic2.advancedmachines.BlockAdvancedMachines. ID: 188</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.powerConverter. ID: 190</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockThermalMonitor. ID: 192</t>
+  </si>
+  <si>
+    <t>Block. Name: immibis.tubestuff.BlockTubestuff. ID: 194</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.railcraftTrack. ID: 206</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.computer. ID: 207</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.diskdrive. ID: 208</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.structureBlock. ID: 209</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.cartDetector. ID: 211</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.elevatorRail. ID: 212</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockUtility. ID: 213</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockRailcraftCube. ID: 214</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.turtle. ID: 216</t>
+  </si>
+  <si>
+    <t>Block. Name: ic2.common.BlockBarrel. ID: 217</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockCrop. ID: 218</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockLuminatorD. ID: 219</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockScaffold. ID: 220</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockWall. ID: 221</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockFoam. ID: 222</t>
+  </si>
+  <si>
+    <t>Block. Name: ic2.common.BlockMachine2. ID: 223</t>
+  </si>
+  <si>
+    <t>Block. Name: ic2.common.BlockMetal. ID: 224</t>
+  </si>
+  <si>
+    <t>Block. Name: ic2.common.BlockPersonal. ID: 225</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockLuminator. ID: 226</t>
+  </si>
+  <si>
+    <t>Block. Name: ic2.common.BlockElectric. ID: 227</t>
+  </si>
+  <si>
+    <t>Block. Name: ic2.common.BlockCable. ID: 228</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockDoorAlloy. ID: 229</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockAlloyGlass. ID: 230</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockAlloy. ID: 231</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockFenceIron. ID: 232</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockReactorChamber. ID: 233</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockRubber. ID: 234</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockIronScaffold. ID: 235</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockDynamite. ID: 236</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockNuke. ID: 237</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockDynamiteRemote. ID: 238</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockITNT. ID: 239</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockHarz. ID: 240</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockRubSapling. ID: 241</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.leaves. ID: 242</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockRubWood. ID: 243</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockMiningTip. ID: 244</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockMiningPipe. ID: 245</t>
+  </si>
+  <si>
+    <t>Block. Name: ic2.common.BlockGenerator. ID: 246</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockOreUran. ID: 247</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockOreTin. ID: 248</t>
+  </si>
+  <si>
+    <t>Block. Name: tile.blockOreCopper. ID: 249</t>
+  </si>
+  <si>
+    <t>Block. Name: ic2.common.BlockMachine. ID: 250</t>
+  </si>
 </sst>
 </file>
 
@@ -1438,7 +1733,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -2758,7 +3053,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2772,7 +3067,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3783,7 +4098,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3823,7 +4138,7 @@
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4393,7 +4708,7 @@
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4413,7 +4728,7 @@
       </c>
       <c r="Y11">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4923,7 +5238,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -4943,7 +5258,7 @@
       </c>
       <c r="O16">
         <f t="shared" ref="O16:AB29" ca="1" si="12">IF(AND(MOD(O$5,block)=0,MOD($D16,block)=0),RANDBETWEEN(0,2), ".")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -4963,7 +5278,7 @@
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5473,7 +5788,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5493,7 +5808,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -5513,7 +5828,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5533,7 +5848,7 @@
       </c>
       <c r="T21">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -5553,7 +5868,7 @@
       </c>
       <c r="Y21">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -6043,7 +6358,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -6063,7 +6378,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -6083,7 +6398,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -6103,7 +6418,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -10556,7 +10871,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576 E1:E1048576 G1:G1048576 I1:I1048576 L1:L1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19496,7 +19811,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576 E1:E1048576 G1:G1048576 I1:I1048576 L1:L1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67475,10 +67790,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2328" topLeftCell="O1" activePane="topRight"/>
-      <selection activeCell="P30" sqref="P30"/>
-      <selection pane="topRight" activeCell="AB23" sqref="AB23"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="11928" topLeftCell="O1"/>
+      <selection activeCell="AB23" sqref="AB23"/>
+      <selection pane="topRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67658,7 +67973,7 @@
         <v>56</v>
       </c>
       <c r="L9" s="305">
-        <f>K9*C9</f>
+        <f t="shared" ref="L9:L17" si="1">K9*C9</f>
         <v>143.36000000000001</v>
       </c>
       <c r="M9" s="431">
@@ -67679,7 +67994,7 @@
         <v>320</v>
       </c>
       <c r="R9" s="434">
-        <f>Q9/K9</f>
+        <f t="shared" ref="R9:R17" si="2">Q9/K9</f>
         <v>5.7142857142857144</v>
       </c>
     </row>
@@ -67695,7 +68010,7 @@
         <v>2.56</v>
       </c>
       <c r="D10" s="430">
-        <f t="shared" ref="D10:D17" si="1">C10*$C$3</f>
+        <f t="shared" ref="D10:D17" si="3">C10*$C$3</f>
         <v>40.96</v>
       </c>
       <c r="H10" s="430"/>
@@ -67706,15 +68021,15 @@
         <v>40</v>
       </c>
       <c r="K10" s="431">
-        <f t="shared" ref="K10" si="2">I10-J10</f>
+        <f t="shared" ref="K10" si="4">I10-J10</f>
         <v>24</v>
       </c>
       <c r="L10" s="305">
-        <f>K10*C10</f>
+        <f t="shared" si="1"/>
         <v>61.44</v>
       </c>
       <c r="M10" s="431">
-        <f t="shared" ref="M10" si="3">L10/N10</f>
+        <f t="shared" ref="M10" si="5">L10/N10</f>
         <v>7.68</v>
       </c>
       <c r="N10" s="435">
@@ -67727,11 +68042,11 @@
         <v>8</v>
       </c>
       <c r="Q10" s="426">
-        <f t="shared" ref="Q10:Q17" si="4">O10*P10</f>
+        <f t="shared" ref="Q10:Q17" si="6">O10*P10</f>
         <v>64</v>
       </c>
       <c r="R10" s="434">
-        <f>Q10/K10</f>
+        <f t="shared" si="2"/>
         <v>2.6666666666666665</v>
       </c>
     </row>
@@ -67747,7 +68062,7 @@
         <v>2.56</v>
       </c>
       <c r="D11" s="430">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>40.96</v>
       </c>
       <c r="H11" s="430"/>
@@ -67762,7 +68077,7 @@
         <v>32</v>
       </c>
       <c r="L11" s="305">
-        <f>K11*C11</f>
+        <f t="shared" si="1"/>
         <v>81.92</v>
       </c>
       <c r="M11" s="431">
@@ -67779,11 +68094,11 @@
         <v>8</v>
       </c>
       <c r="Q11" s="426">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
       <c r="R11" s="434">
-        <f>Q11/K11</f>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -67799,7 +68114,7 @@
         <v>2.56</v>
       </c>
       <c r="D12" s="430">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>40.96</v>
       </c>
       <c r="H12" s="430"/>
@@ -67814,11 +68129,11 @@
         <v>112</v>
       </c>
       <c r="L12" s="305">
-        <f>K12*C12</f>
+        <f t="shared" si="1"/>
         <v>286.72000000000003</v>
       </c>
       <c r="M12" s="431">
-        <f t="shared" ref="M12:M17" si="5">L12/N12</f>
+        <f t="shared" ref="M12:M17" si="7">L12/N12</f>
         <v>8.1920000000000002</v>
       </c>
       <c r="N12" s="435">
@@ -67831,11 +68146,11 @@
         <v>8</v>
       </c>
       <c r="Q12" s="426">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>280</v>
       </c>
       <c r="R12" s="434">
-        <f>Q12/K12</f>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -67851,7 +68166,7 @@
         <v>1.536</v>
       </c>
       <c r="D13" s="430">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>24.576000000000001</v>
       </c>
       <c r="H13" s="430"/>
@@ -67862,15 +68177,15 @@
         <v>16</v>
       </c>
       <c r="K13" s="431">
-        <f t="shared" ref="K13:K17" si="6">I13-J13</f>
+        <f t="shared" ref="K13:K17" si="8">I13-J13</f>
         <v>52</v>
       </c>
       <c r="L13" s="305">
-        <f>K13*C13</f>
+        <f t="shared" si="1"/>
         <v>79.872</v>
       </c>
       <c r="M13" s="431">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.9871999999999996</v>
       </c>
       <c r="N13" s="435">
@@ -67883,11 +68198,11 @@
         <v>8</v>
       </c>
       <c r="Q13" s="426">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>96</v>
       </c>
       <c r="R13" s="434">
-        <f>Q13/K13</f>
+        <f t="shared" si="2"/>
         <v>1.8461538461538463</v>
       </c>
     </row>
@@ -67903,7 +68218,7 @@
         <v>0.38400000000000001</v>
       </c>
       <c r="D14" s="430">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.1440000000000001</v>
       </c>
       <c r="H14" s="430"/>
@@ -67914,15 +68229,15 @@
         <v>5</v>
       </c>
       <c r="K14" s="431">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
       <c r="L14" s="305">
-        <f>K14*C14</f>
+        <f t="shared" si="1"/>
         <v>11.136000000000001</v>
       </c>
       <c r="M14" s="431">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.7120000000000002</v>
       </c>
       <c r="N14" s="435">
@@ -67935,11 +68250,11 @@
         <v>3</v>
       </c>
       <c r="Q14" s="426">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="R14" s="434">
-        <f>Q14/K14</f>
+        <f t="shared" si="2"/>
         <v>0.41379310344827586</v>
       </c>
     </row>
@@ -67955,7 +68270,7 @@
         <v>0.3584</v>
       </c>
       <c r="D15" s="430">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.7343999999999999</v>
       </c>
       <c r="H15" s="430"/>
@@ -67970,7 +68285,7 @@
         <v>25</v>
       </c>
       <c r="L15" s="305">
-        <f>K15*C15</f>
+        <f t="shared" si="1"/>
         <v>8.9599999999999991</v>
       </c>
       <c r="M15" s="431">
@@ -67987,11 +68302,11 @@
         <v>2</v>
       </c>
       <c r="Q15" s="426">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="R15" s="434">
-        <f>Q15/K15</f>
+        <f t="shared" si="2"/>
         <v>0.24</v>
       </c>
     </row>
@@ -68007,7 +68322,7 @@
         <v>2.048</v>
       </c>
       <c r="D16" s="430">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>32.768000000000001</v>
       </c>
       <c r="H16" s="430"/>
@@ -68018,15 +68333,15 @@
         <v>8</v>
       </c>
       <c r="K16" s="431">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="L16" s="305">
-        <f>K16*C16</f>
+        <f t="shared" si="1"/>
         <v>18.432000000000002</v>
       </c>
       <c r="M16" s="431">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.6864000000000003</v>
       </c>
       <c r="N16" s="435">
@@ -68039,11 +68354,11 @@
         <v>4</v>
       </c>
       <c r="Q16" s="426">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="R16" s="434">
-        <f>Q16/K16</f>
+        <f t="shared" si="2"/>
         <v>2.6666666666666665</v>
       </c>
     </row>
@@ -68059,7 +68374,7 @@
         <v>0.38400000000000001</v>
       </c>
       <c r="D17" s="430">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.1440000000000001</v>
       </c>
       <c r="H17" s="430"/>
@@ -68070,15 +68385,15 @@
         <v>1</v>
       </c>
       <c r="K17" s="431">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="L17" s="305">
-        <f>K17*C17</f>
+        <f t="shared" si="1"/>
         <v>5.76</v>
       </c>
       <c r="M17" s="431">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.88</v>
       </c>
       <c r="N17" s="435">
@@ -68091,11 +68406,11 @@
         <v>2</v>
       </c>
       <c r="Q17" s="426">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="R17" s="434">
-        <f>Q17/K17</f>
+        <f t="shared" si="2"/>
         <v>0.26666666666666666</v>
       </c>
     </row>
@@ -68220,7 +68535,7 @@
       <c r="B22" s="305"/>
       <c r="C22" s="305"/>
       <c r="D22" s="430">
-        <f>B9*$D$20</f>
+        <f t="shared" ref="D22:D30" si="9">B9*$D$20</f>
         <v>598.23</v>
       </c>
       <c r="E22" s="430"/>
@@ -68229,7 +68544,7 @@
         <v>143.36000000000001</v>
       </c>
       <c r="G22" s="431">
-        <f>F22*$K$21</f>
+        <f t="shared" ref="G22:G30" si="10">F22*$K$21</f>
         <v>1970.64</v>
       </c>
       <c r="H22" s="433">
@@ -68237,7 +68552,7 @@
         <v>4.3750000000000004E-3</v>
       </c>
       <c r="I22" s="430">
-        <f>Q9*$K$21</f>
+        <f t="shared" ref="I22:I30" si="11">Q9*$K$21</f>
         <v>4398.75</v>
       </c>
       <c r="J22" s="433">
@@ -68246,649 +68561,3734 @@
       </c>
       <c r="K22" s="432"/>
       <c r="L22" s="433">
-        <f>K22/K$19</f>
+        <f t="shared" ref="L22:L30" si="12">K22/K$19</f>
         <v>0</v>
       </c>
       <c r="M22" s="433"/>
       <c r="N22" s="305">
-        <f>F22*$O$21</f>
+        <f t="shared" ref="N22:N30" si="13">F22*$O$21</f>
         <v>1659.8400000000001</v>
       </c>
       <c r="O22" s="305">
         <v>6511</v>
       </c>
       <c r="P22" s="433">
-        <f>O22/O$19</f>
+        <f t="shared" ref="P22:P30" si="14">O22/O$19</f>
         <v>1.9613336225178329E-2</v>
       </c>
       <c r="R22" s="305">
-        <f>F22*$S$21</f>
+        <f t="shared" ref="R22:R30" si="15">F22*$S$21</f>
         <v>16620.800000000003</v>
       </c>
       <c r="S22" s="305">
         <v>50813</v>
       </c>
       <c r="T22" s="433">
-        <f>S22/S$19</f>
+        <f t="shared" ref="T22:T30" si="16">S22/S$19</f>
         <v>2.1949080793420415E-2</v>
       </c>
       <c r="W22" s="305">
         <v>18509</v>
       </c>
       <c r="X22" s="433">
-        <f>W22/W$19</f>
+        <f t="shared" ref="X22:X30" si="17">W22/W$19</f>
         <v>8.5976402824228908E-3</v>
       </c>
       <c r="Z22" s="305">
         <v>21511</v>
       </c>
       <c r="AA22" s="433">
-        <f>Z22/Z$19</f>
+        <f t="shared" ref="AA22:AA30" si="18">Z22/Z$19</f>
         <v>8.4655647382920109E-3</v>
       </c>
       <c r="AB22" s="305">
         <v>20101</v>
       </c>
       <c r="AC22" s="433">
-        <f>AB22/AB$19</f>
+        <f t="shared" ref="AC22:AC30" si="19">AB22/AB$19</f>
         <v>6.7127564078588104E-3</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D23" s="430">
-        <f>B10*$D$20</f>
+        <f t="shared" si="9"/>
         <v>598.23</v>
       </c>
       <c r="E23" s="430"/>
       <c r="F23" s="430">
-        <f t="shared" ref="F23:F30" si="7">K10*C10</f>
+        <f t="shared" ref="F23:F30" si="20">K10*C10</f>
         <v>61.44</v>
       </c>
       <c r="G23" s="431">
-        <f>F23*$K$21</f>
+        <f t="shared" si="10"/>
         <v>844.56</v>
       </c>
       <c r="H23" s="433">
-        <f t="shared" ref="H23:H30" si="8">G23/K$19</f>
+        <f t="shared" ref="H23:H30" si="21">G23/K$19</f>
         <v>1.8749999999999999E-3</v>
       </c>
       <c r="I23" s="430">
-        <f>Q10*$K$21</f>
+        <f t="shared" si="11"/>
         <v>879.75</v>
       </c>
       <c r="J23" s="433">
-        <f t="shared" ref="J23:J30" si="9">I23/K$19</f>
+        <f t="shared" ref="J23:J30" si="22">I23/K$19</f>
         <v>1.953125E-3</v>
       </c>
       <c r="K23" s="432"/>
       <c r="L23" s="433">
-        <f>K23/K$19</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N23" s="305">
-        <f>F23*$O$21</f>
+        <f t="shared" si="13"/>
         <v>711.36</v>
       </c>
       <c r="P23" s="433">
-        <f>O23/O$19</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="R23" s="305">
-        <f>F23*$S$21</f>
+        <f t="shared" si="15"/>
         <v>7123.2</v>
       </c>
       <c r="T23" s="433">
-        <f>S23/S$19</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X23" s="433">
-        <f>W23/W$19</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AA23" s="433">
-        <f>Z23/Z$19</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AC23" s="433">
-        <f>AB23/AB$19</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D24" s="430">
-        <f>B11*$D$20</f>
+        <f t="shared" si="9"/>
         <v>598.23</v>
       </c>
       <c r="E24" s="430"/>
       <c r="F24" s="430">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>81.92</v>
       </c>
       <c r="G24" s="431">
-        <f>F24*$K$21</f>
+        <f t="shared" si="10"/>
         <v>1126.08</v>
       </c>
       <c r="H24" s="433">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="I24" s="430">
-        <f>Q11*$K$21</f>
+        <f t="shared" si="11"/>
         <v>1099.6875</v>
       </c>
       <c r="J24" s="433">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>2.44140625E-3</v>
       </c>
       <c r="K24" s="432">
         <v>939</v>
       </c>
       <c r="L24" s="433">
-        <f>K24/K$19</f>
+        <f t="shared" si="12"/>
         <v>2.0846653878942882E-3</v>
       </c>
       <c r="N24" s="305">
-        <f>F24*$O$21</f>
+        <f t="shared" si="13"/>
         <v>948.48</v>
       </c>
       <c r="P24" s="433">
-        <f>O24/O$19</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="R24" s="305">
-        <f>F24*$S$21</f>
+        <f t="shared" si="15"/>
         <v>9497.6</v>
       </c>
       <c r="T24" s="433">
-        <f>S24/S$19</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X24" s="433">
-        <f>W24/W$19</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AA24" s="433">
-        <f>Z24/Z$19</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AC24" s="433">
-        <f>AB24/AB$19</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D25" s="430">
-        <f>B12*$D$20</f>
+        <f t="shared" si="9"/>
         <v>598.23</v>
       </c>
       <c r="E25" s="430"/>
       <c r="F25" s="430">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>286.72000000000003</v>
       </c>
       <c r="G25" s="431">
-        <f>F25*$K$21</f>
+        <f t="shared" si="10"/>
         <v>3941.28</v>
       </c>
       <c r="H25" s="433">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>8.7500000000000008E-3</v>
       </c>
       <c r="I25" s="430">
-        <f>Q12*$K$21</f>
+        <f t="shared" si="11"/>
         <v>3848.90625</v>
       </c>
       <c r="J25" s="433">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>8.544921875E-3</v>
       </c>
       <c r="K25" s="432">
         <v>2749</v>
       </c>
       <c r="L25" s="433">
-        <f>K25/K$19</f>
+        <f t="shared" si="12"/>
         <v>6.1030299801079855E-3</v>
       </c>
       <c r="N25" s="305">
-        <f>F25*$O$21</f>
+        <f t="shared" si="13"/>
         <v>3319.6800000000003</v>
       </c>
       <c r="O25" s="426">
         <v>2699</v>
       </c>
       <c r="P25" s="433">
-        <f>O25/O$19</f>
+        <f t="shared" si="14"/>
         <v>8.1303017158280318E-3</v>
       </c>
       <c r="R25" s="305">
-        <f>F25*$S$21</f>
+        <f t="shared" si="15"/>
         <v>33241.600000000006</v>
       </c>
       <c r="S25" s="426">
         <v>19441</v>
       </c>
       <c r="T25" s="433">
-        <f>S25/S$19</f>
+        <f t="shared" si="16"/>
         <v>8.3976950722233733E-3</v>
       </c>
       <c r="W25" s="426">
         <v>13749</v>
       </c>
       <c r="X25" s="433">
-        <f>W25/W$19</f>
+        <f t="shared" si="17"/>
         <v>6.3865663322185059E-3</v>
       </c>
       <c r="Z25" s="426">
         <v>15221</v>
       </c>
       <c r="AA25" s="433">
-        <f>Z25/Z$19</f>
+        <f t="shared" si="18"/>
         <v>5.9901613537977176E-3</v>
       </c>
       <c r="AB25" s="426">
         <v>14406</v>
       </c>
       <c r="AC25" s="433">
-        <f>AB25/AB$19</f>
+        <f t="shared" si="19"/>
         <v>4.8109033785191796E-3</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D26" s="430">
-        <f>B13*$D$20</f>
+        <f t="shared" si="9"/>
         <v>358.93799999999999</v>
       </c>
       <c r="E26" s="430"/>
       <c r="F26" s="430">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>79.872</v>
       </c>
       <c r="G26" s="431">
-        <f>F26*$K$21</f>
+        <f t="shared" si="10"/>
         <v>1097.9280000000001</v>
       </c>
       <c r="H26" s="433">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>2.4375000000000004E-3</v>
       </c>
       <c r="I26" s="430">
-        <f>Q13*$K$21</f>
+        <f t="shared" si="11"/>
         <v>1319.625</v>
       </c>
       <c r="J26" s="433">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>2.9296875E-3</v>
       </c>
       <c r="K26" s="432">
         <v>1118</v>
       </c>
       <c r="L26" s="433">
-        <f>K26/K$19</f>
+        <f t="shared" si="12"/>
         <v>2.4820616652458083E-3</v>
       </c>
       <c r="N26" s="305">
-        <f>F26*$O$21</f>
+        <f t="shared" si="13"/>
         <v>924.76800000000003</v>
       </c>
       <c r="O26" s="426">
         <v>1142</v>
       </c>
       <c r="P26" s="433">
-        <f>O26/O$19</f>
+        <f t="shared" si="14"/>
         <v>3.4400906111432426E-3</v>
       </c>
       <c r="R26" s="305">
-        <f>F26*$S$21</f>
+        <f t="shared" si="15"/>
         <v>9260.16</v>
       </c>
       <c r="S26" s="426">
         <v>10442</v>
       </c>
       <c r="T26" s="433">
-        <f>S26/S$19</f>
+        <f t="shared" si="16"/>
         <v>4.5105052180523875E-3</v>
       </c>
       <c r="W26" s="426">
         <v>7146</v>
       </c>
       <c r="X26" s="433">
-        <f>W26/W$19</f>
+        <f t="shared" si="17"/>
         <v>3.3193979933110367E-3</v>
       </c>
       <c r="Z26" s="426">
         <v>8389</v>
       </c>
       <c r="AA26" s="433">
-        <f>Z26/Z$19</f>
+        <f t="shared" si="18"/>
         <v>3.3014561196379379E-3</v>
       </c>
       <c r="AB26" s="426">
         <v>6983</v>
       </c>
       <c r="AC26" s="433">
-        <f>AB26/AB$19</f>
+        <f t="shared" si="19"/>
         <v>2.3319823887407629E-3</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D27" s="430">
-        <f>B14*$D$20</f>
+        <f t="shared" si="9"/>
         <v>89.734499999999997</v>
       </c>
       <c r="E27" s="430">
         <v>61</v>
       </c>
       <c r="F27" s="430">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>11.136000000000001</v>
       </c>
       <c r="G27" s="431">
-        <f>F27*$K$21</f>
+        <f t="shared" si="10"/>
         <v>153.07650000000001</v>
       </c>
       <c r="H27" s="433">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>3.3984375000000003E-4</v>
       </c>
       <c r="I27" s="430">
-        <f>Q14*$K$21</f>
+        <f t="shared" si="11"/>
         <v>164.953125</v>
       </c>
       <c r="J27" s="433">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>3.662109375E-4</v>
       </c>
       <c r="K27" s="432">
         <v>175</v>
       </c>
       <c r="L27" s="433">
-        <f>K27/K$19</f>
+        <f t="shared" si="12"/>
         <v>3.8851591361182153E-4</v>
       </c>
       <c r="N27" s="305">
-        <f>F27*$O$21</f>
+        <f t="shared" si="13"/>
         <v>128.934</v>
       </c>
       <c r="O27" s="426">
         <v>74</v>
       </c>
       <c r="P27" s="433">
-        <f>O27/O$19</f>
+        <f t="shared" si="14"/>
         <v>2.2291305186042029E-4</v>
       </c>
       <c r="R27" s="305">
-        <f>F27*$S$21</f>
+        <f t="shared" si="15"/>
         <v>1291.0800000000002</v>
       </c>
       <c r="S27" s="426">
         <v>993</v>
       </c>
       <c r="T27" s="433">
-        <f>S27/S$19</f>
+        <f t="shared" si="16"/>
         <v>4.2893427327389593E-4</v>
       </c>
       <c r="W27" s="426">
         <v>1031</v>
       </c>
       <c r="X27" s="433">
-        <f>W27/W$19</f>
+        <f t="shared" si="17"/>
         <v>4.7891118543292455E-4</v>
       </c>
       <c r="Z27" s="426">
         <v>1089</v>
       </c>
       <c r="AA27" s="433">
-        <f>Z27/Z$19</f>
+        <f t="shared" si="18"/>
         <v>4.2857142857142855E-4</v>
       </c>
       <c r="AB27" s="426">
         <v>615</v>
       </c>
       <c r="AC27" s="433">
-        <f>AB27/AB$19</f>
+        <f t="shared" si="19"/>
         <v>2.0538009008672049E-4</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D28" s="430">
-        <f>B15*$D$20</f>
+        <f t="shared" si="9"/>
         <v>83.752200000000002</v>
       </c>
       <c r="E28" s="430">
         <v>57</v>
       </c>
       <c r="F28" s="430">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>8.9599999999999991</v>
       </c>
       <c r="G28" s="431">
-        <f>F28*$K$21</f>
+        <f t="shared" si="10"/>
         <v>123.16499999999999</v>
       </c>
       <c r="H28" s="433">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>2.7343749999999997E-4</v>
       </c>
       <c r="I28" s="430">
-        <f>Q15*$K$21</f>
+        <f t="shared" si="11"/>
         <v>82.4765625</v>
       </c>
       <c r="J28" s="433">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>1.8310546875E-4</v>
       </c>
       <c r="K28" s="432">
         <v>111</v>
       </c>
       <c r="L28" s="433">
-        <f>K28/K$19</f>
+        <f t="shared" si="12"/>
         <v>2.4643009377664109E-4</v>
       </c>
       <c r="N28" s="305">
-        <f>F28*$O$21</f>
+        <f t="shared" si="13"/>
         <v>103.74</v>
       </c>
       <c r="O28" s="426">
         <v>52</v>
       </c>
       <c r="P28" s="433">
-        <f>O28/O$19</f>
+        <f t="shared" si="14"/>
         <v>1.5664160401002505E-4</v>
       </c>
       <c r="R28" s="305">
-        <f>F28*$S$21</f>
+        <f t="shared" si="15"/>
         <v>1038.8</v>
       </c>
       <c r="S28" s="426">
         <v>418</v>
       </c>
       <c r="T28" s="433">
-        <f>S28/S$19</f>
+        <f t="shared" si="16"/>
         <v>1.8055843527541642E-4</v>
       </c>
       <c r="W28" s="426">
         <v>680</v>
       </c>
       <c r="X28" s="433">
-        <f>W28/W$19</f>
+        <f t="shared" si="17"/>
         <v>3.1586770717205502E-4</v>
       </c>
       <c r="Z28" s="426">
         <v>537</v>
       </c>
       <c r="AA28" s="433">
-        <f>Z28/Z$19</f>
+        <f t="shared" si="18"/>
         <v>2.1133412042502952E-4</v>
       </c>
       <c r="AB28" s="426">
         <v>349</v>
       </c>
       <c r="AC28" s="433">
-        <f>AB28/AB$19</f>
+        <f t="shared" si="19"/>
         <v>1.1654902673213895E-4</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D29" s="430">
-        <f>B16*$D$20</f>
+        <f t="shared" si="9"/>
         <v>478.584</v>
       </c>
       <c r="E29" s="430">
         <v>322</v>
       </c>
       <c r="F29" s="430">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>18.432000000000002</v>
       </c>
       <c r="G29" s="431">
-        <f>F29*$K$21</f>
+        <f t="shared" si="10"/>
         <v>253.36800000000002</v>
       </c>
       <c r="H29" s="433">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>5.6250000000000007E-4</v>
       </c>
       <c r="I29" s="430">
-        <f>Q16*$K$21</f>
+        <f t="shared" si="11"/>
         <v>329.90625</v>
       </c>
       <c r="J29" s="433">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>7.32421875E-4</v>
       </c>
       <c r="K29" s="432">
         <v>322</v>
       </c>
       <c r="L29" s="433">
-        <f>K29/K$19</f>
+        <f t="shared" si="12"/>
         <v>7.1486928104575159E-4</v>
       </c>
       <c r="N29" s="305">
-        <f>F29*$O$21</f>
+        <f t="shared" si="13"/>
         <v>213.40800000000002</v>
       </c>
       <c r="O29" s="426">
         <v>296</v>
       </c>
       <c r="P29" s="433">
-        <f>O29/O$19</f>
+        <f t="shared" si="14"/>
         <v>8.9165220744168118E-4</v>
       </c>
       <c r="R29" s="305">
-        <f>F29*$S$21</f>
+        <f t="shared" si="15"/>
         <v>2136.96</v>
       </c>
       <c r="S29" s="426">
         <v>3067</v>
       </c>
       <c r="T29" s="433">
-        <f>S29/S$19</f>
+        <f t="shared" si="16"/>
         <v>1.3248151219849332E-3</v>
       </c>
       <c r="W29" s="426">
         <v>2023</v>
       </c>
       <c r="X29" s="433">
-        <f>W29/W$19</f>
+        <f t="shared" si="17"/>
         <v>9.3970642883686359E-4</v>
       </c>
       <c r="Z29" s="426">
         <v>2242</v>
       </c>
       <c r="AA29" s="433">
-        <f>Z29/Z$19</f>
+        <f t="shared" si="18"/>
         <v>8.8232979142070051E-4</v>
       </c>
       <c r="AB29" s="426">
         <v>1664</v>
       </c>
       <c r="AC29" s="433">
-        <f>AB29/AB$19</f>
+        <f t="shared" si="19"/>
         <v>5.5569507301512664E-4</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D30" s="430">
-        <f>B17*$D$20</f>
+        <f t="shared" si="9"/>
         <v>89.734499999999997</v>
       </c>
       <c r="E30" s="430">
         <v>96</v>
       </c>
       <c r="F30" s="430">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>5.76</v>
       </c>
       <c r="G30" s="431">
-        <f>F30*$K$21</f>
+        <f t="shared" si="10"/>
         <v>79.177499999999995</v>
       </c>
       <c r="H30" s="433">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>1.7578124999999999E-4</v>
       </c>
       <c r="I30" s="430">
-        <f>Q17*$K$21</f>
+        <f t="shared" si="11"/>
         <v>54.984375</v>
       </c>
       <c r="J30" s="433">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>1.220703125E-4</v>
       </c>
       <c r="K30" s="432">
         <v>96</v>
       </c>
       <c r="L30" s="433">
-        <f>K30/K$19</f>
+        <f t="shared" si="12"/>
         <v>2.1312872975277067E-4</v>
       </c>
       <c r="N30" s="305">
-        <f>F30*$O$21</f>
+        <f t="shared" si="13"/>
         <v>66.69</v>
       </c>
       <c r="O30" s="426">
         <v>45</v>
       </c>
       <c r="P30" s="433">
-        <f>O30/O$19</f>
+        <f t="shared" si="14"/>
         <v>1.3555523423944477E-4</v>
       </c>
       <c r="R30" s="305">
-        <f>F30*$S$21</f>
+        <f t="shared" si="15"/>
         <v>667.8</v>
       </c>
       <c r="S30" s="426">
         <v>404</v>
       </c>
       <c r="T30" s="433">
-        <f>S30/S$19</f>
+        <f t="shared" si="16"/>
         <v>1.7451102356762734E-4</v>
       </c>
       <c r="W30" s="426">
         <v>470</v>
       </c>
       <c r="X30" s="433">
-        <f>W30/W$19</f>
+        <f t="shared" si="17"/>
         <v>2.1832032701597919E-4</v>
       </c>
       <c r="Z30" s="426">
         <v>365</v>
       </c>
       <c r="AA30" s="433">
-        <f>Z30/Z$19</f>
+        <f t="shared" si="18"/>
         <v>1.4364423455332547E-4</v>
       </c>
       <c r="AB30" s="426">
         <v>254</v>
       </c>
       <c r="AC30" s="433">
-        <f>AB30/AB$19</f>
+        <f t="shared" si="19"/>
         <v>8.4823646962645536E-5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="59.44140625" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="5" width="40.88671875" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E1" t="s">
+        <v>458</v>
+      </c>
+      <c r="F1" t="s">
+        <v>459</v>
+      </c>
+      <c r="G1" t="s">
+        <v>460</v>
+      </c>
+      <c r="H1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2" t="b">
+        <f t="shared" ref="B2:B65" si="0">IFERROR(SEARCH("unused", A2)&gt;0,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <f t="shared" ref="C2:C65" si="1">IFERROR(SEARCH("tile", A2) &gt; 0, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D65" si="2">IF(C2,RIGHT(A2,LEN(A2)-18),RIGHT(A2,LEN(A2)-13))</f>
+        <v>eloraam.base.BlockAppliance. ID: 137</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E65" si="3">LEFT(D2,SEARCH(". ID",D2) - 1)</f>
+        <v>eloraam.base.BlockAppliance</v>
+      </c>
+      <c r="F2" t="b">
+        <f t="shared" ref="F2:F65" si="4">IFERROR(SEARCH(".", E2)&gt;0,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>RIGHT(D2,LEN(D2) - SEARCH("ID: ",D2) - 3)</f>
+        <v>137</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(F2,"",CONCATENATE(UPPER(E2),"(",G2,"),"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>462</v>
+      </c>
+      <c r="B3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="2"/>
+        <v>eloraam.logic.BlockLogic. ID: 138</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="3"/>
+        <v>eloraam.logic.BlockLogic</v>
+      </c>
+      <c r="F3" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>RIGHT(D3,LEN(D3) - SEARCH("ID: ",D3) - 3)</f>
+        <v>138</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H66" si="5">IF(F3,"",CONCATENATE(UPPER(E3),"(",G3,"),"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B4" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="2"/>
+        <v>indigo. ID: 139</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="3"/>
+        <v>indigo</v>
+      </c>
+      <c r="F4" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G4" t="str">
+        <f>RIGHT(D4,LEN(D4) - SEARCH("ID: ",D4) - 3)</f>
+        <v>139</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="5"/>
+        <v>INDIGO(139),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>464</v>
+      </c>
+      <c r="B5" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="2"/>
+        <v>rpores. ID: 140</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="3"/>
+        <v>rpores</v>
+      </c>
+      <c r="F5" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G5" t="str">
+        <f>RIGHT(D5,LEN(D5) - SEARCH("ID: ",D5) - 3)</f>
+        <v>140</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="5"/>
+        <v>RPORES(140),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>465</v>
+      </c>
+      <c r="B6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C6" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="2"/>
+        <v>rpleaves. ID: 141</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="3"/>
+        <v>rpleaves</v>
+      </c>
+      <c r="F6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G6" t="str">
+        <f>RIGHT(D6,LEN(D6) - SEARCH("ID: ",D6) - 3)</f>
+        <v>141</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="5"/>
+        <v>RPLEAVES(141),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>466</v>
+      </c>
+      <c r="B7" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C7" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="2"/>
+        <v>rpstone. ID: 142</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="3"/>
+        <v>rpstone</v>
+      </c>
+      <c r="F7" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G7" t="str">
+        <f>RIGHT(D7,LEN(D7) - SEARCH("ID: ",D7) - 3)</f>
+        <v>142</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="5"/>
+        <v>RPSTONE(142),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C8" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="2"/>
+        <v>rplog. ID: 143</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="3"/>
+        <v>rplog</v>
+      </c>
+      <c r="F8" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G8" t="str">
+        <f>RIGHT(D8,LEN(D8) - SEARCH("ID: ",D8) - 3)</f>
+        <v>143</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="5"/>
+        <v>RPLOG(143),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>468</v>
+      </c>
+      <c r="B9" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C9" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>eloraam.world.BlockCustomCrops. ID: 144</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="3"/>
+        <v>eloraam.world.BlockCustomCrops</v>
+      </c>
+      <c r="F9" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G9" t="str">
+        <f>RIGHT(D9,LEN(D9) - SEARCH("ID: ",D9) - 3)</f>
+        <v>144</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>469</v>
+      </c>
+      <c r="B10" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C10" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>eloraam.world.BlockStorage. ID: 145</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="3"/>
+        <v>eloraam.world.BlockStorage</v>
+      </c>
+      <c r="F10" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G10" t="str">
+        <f>RIGHT(D10,LEN(D10) - SEARCH("ID: ",D10) - 3)</f>
+        <v>145</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>470</v>
+      </c>
+      <c r="B11" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C11" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="2"/>
+        <v>rplampon. ID: 146</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="3"/>
+        <v>rplampon</v>
+      </c>
+      <c r="F11" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G11" t="str">
+        <f>RIGHT(D11,LEN(D11) - SEARCH("ID: ",D11) - 3)</f>
+        <v>146</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="5"/>
+        <v>RPLAMPON(146),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>471</v>
+      </c>
+      <c r="B12" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C12" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="2"/>
+        <v>rplampoff. ID: 147</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="3"/>
+        <v>rplampoff</v>
+      </c>
+      <c r="F12" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G12" t="str">
+        <f>RIGHT(D12,LEN(D12) - SEARCH("ID: ",D12) - 3)</f>
+        <v>147</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="5"/>
+        <v>RPLAMPOFF(147),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>472</v>
+      </c>
+      <c r="B13" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C13" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="2"/>
+        <v>eloraam.core.BlockMultipart. ID: 148</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="3"/>
+        <v>eloraam.core.BlockMultipart</v>
+      </c>
+      <c r="F13" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G13" t="str">
+        <f>RIGHT(D13,LEN(D13) - SEARCH("ID: ",D13) - 3)</f>
+        <v>148</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>473</v>
+      </c>
+      <c r="B14" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C14" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>craftingtableiii. ID: 149</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="3"/>
+        <v>craftingtableiii</v>
+      </c>
+      <c r="F14" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G14" t="str">
+        <f>RIGHT(D14,LEN(D14) - SEARCH("ID: ",D14) - 3)</f>
+        <v>149</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="5"/>
+        <v>CRAFTINGTABLEIII(149),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>474</v>
+      </c>
+      <c r="B15" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>rpmachine. ID: 150</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="3"/>
+        <v>rpmachine</v>
+      </c>
+      <c r="F15" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G15" t="str">
+        <f>RIGHT(D15,LEN(D15) - SEARCH("ID: ",D15) - 3)</f>
+        <v>150</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="5"/>
+        <v>RPMACHINE(150),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>475</v>
+      </c>
+      <c r="B16" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C16" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>eloraam.machine.BlockMachinePanel. ID: 151</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="3"/>
+        <v>eloraam.machine.BlockMachinePanel</v>
+      </c>
+      <c r="F16" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G16" t="str">
+        <f>RIGHT(D16,LEN(D16) - SEARCH("ID: ",D16) - 3)</f>
+        <v>151</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>476</v>
+      </c>
+      <c r="B17" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C17" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>rpframe. ID: 152</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="3"/>
+        <v>rpframe</v>
+      </c>
+      <c r="F17" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G17" t="str">
+        <f>RIGHT(D17,LEN(D17) - SEARCH("ID: ",D17) - 3)</f>
+        <v>152</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="5"/>
+        <v>RPFRAME(152),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>477</v>
+      </c>
+      <c r="B18" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C18" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>machineBlock. ID: 153</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="3"/>
+        <v>machineBlock</v>
+      </c>
+      <c r="F18" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G18" t="str">
+        <f>RIGHT(D18,LEN(D18) - SEARCH("ID: ",D18) - 3)</f>
+        <v>153</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="5"/>
+        <v>MACHINEBLOCK(153),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>478</v>
+      </c>
+      <c r="B19" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C19" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="2"/>
+        <v>markerBlock. ID: 154</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="3"/>
+        <v>markerBlock</v>
+      </c>
+      <c r="F19" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G19" t="str">
+        <f>RIGHT(D19,LEN(D19) - SEARCH("ID: ",D19) - 3)</f>
+        <v>154</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="5"/>
+        <v>MARKERBLOCK(154),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>479</v>
+      </c>
+      <c r="B20" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C20" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="2"/>
+        <v>fillerBlock. ID: 155</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="3"/>
+        <v>fillerBlock</v>
+      </c>
+      <c r="F20" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G20" t="str">
+        <f>RIGHT(D20,LEN(D20) - SEARCH("ID: ",D20) - 3)</f>
+        <v>155</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="5"/>
+        <v>FILLERBLOCK(155),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>480</v>
+      </c>
+      <c r="B21" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C21" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="2"/>
+        <v>buildcraft.transport.LegacyBlock. ID: 156</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="3"/>
+        <v>buildcraft.transport.LegacyBlock</v>
+      </c>
+      <c r="F21" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G21" t="str">
+        <f>RIGHT(D21,LEN(D21) - SEARCH("ID: ",D21) - 3)</f>
+        <v>156</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>481</v>
+      </c>
+      <c r="B22" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C22" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="2"/>
+        <v>builderBlock. ID: 157</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="3"/>
+        <v>builderBlock</v>
+      </c>
+      <c r="F22" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G22" t="str">
+        <f>RIGHT(D22,LEN(D22) - SEARCH("ID: ",D22) - 3)</f>
+        <v>157</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="5"/>
+        <v>BUILDERBLOCK(157),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>482</v>
+      </c>
+      <c r="B23" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C23" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="2"/>
+        <v>templateBlock. ID: 158</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="3"/>
+        <v>templateBlock</v>
+      </c>
+      <c r="F23" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G23" t="str">
+        <f>RIGHT(D23,LEN(D23) - SEARCH("ID: ",D23) - 3)</f>
+        <v>158</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="5"/>
+        <v>TEMPLATEBLOCK(158),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>483</v>
+      </c>
+      <c r="B24" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C24" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="2"/>
+        <v>buildcraft.transport.LegacyBlock. ID: 159</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="3"/>
+        <v>buildcraft.transport.LegacyBlock</v>
+      </c>
+      <c r="F24" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G24" t="str">
+        <f>RIGHT(D24,LEN(D24) - SEARCH("ID: ",D24) - 3)</f>
+        <v>159</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>484</v>
+      </c>
+      <c r="B25" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C25" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="2"/>
+        <v>frameBlock. ID: 160</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="3"/>
+        <v>frameBlock</v>
+      </c>
+      <c r="F25" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G25" t="str">
+        <f>RIGHT(D25,LEN(D25) - SEARCH("ID: ",D25) - 3)</f>
+        <v>160</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="5"/>
+        <v>FRAMEBLOCK(160),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>485</v>
+      </c>
+      <c r="B26" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="2"/>
+        <v>buildcraft.energy.BlockEngine. ID: 161</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="3"/>
+        <v>buildcraft.energy.BlockEngine</v>
+      </c>
+      <c r="F26" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G26" t="str">
+        <f>RIGHT(D26,LEN(D26) - SEARCH("ID: ",D26) - 3)</f>
+        <v>161</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>486</v>
+      </c>
+      <c r="B27" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C27" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="2"/>
+        <v>oilMoving. ID: 162</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="3"/>
+        <v>oilMoving</v>
+      </c>
+      <c r="F27" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G27" t="str">
+        <f>RIGHT(D27,LEN(D27) - SEARCH("ID: ",D27) - 3)</f>
+        <v>162</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="5"/>
+        <v>OILMOVING(162),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>487</v>
+      </c>
+      <c r="B28" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C28" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="2"/>
+        <v>oilStill. ID: 163</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="3"/>
+        <v>oilStill</v>
+      </c>
+      <c r="F28" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G28" t="str">
+        <f>RIGHT(D28,LEN(D28) - SEARCH("ID: ",D28) - 3)</f>
+        <v>163</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="5"/>
+        <v>OILSTILL(163),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>488</v>
+      </c>
+      <c r="B29" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C29" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="2"/>
+        <v>pumpBlock. ID: 164</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="3"/>
+        <v>pumpBlock</v>
+      </c>
+      <c r="F29" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G29" t="str">
+        <f>RIGHT(D29,LEN(D29) - SEARCH("ID: ",D29) - 3)</f>
+        <v>164</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="5"/>
+        <v>PUMPBLOCK(164),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>489</v>
+      </c>
+      <c r="B30" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C30" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="2"/>
+        <v>tankBlock. ID: 165</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="3"/>
+        <v>tankBlock</v>
+      </c>
+      <c r="F30" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G30" t="str">
+        <f>RIGHT(D30,LEN(D30) - SEARCH("ID: ",D30) - 3)</f>
+        <v>165</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="5"/>
+        <v>TANKBLOCK(165),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>490</v>
+      </c>
+      <c r="B31" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C31" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="2"/>
+        <v>buildcraft.transport.BlockGenericPipe. ID: 166</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="3"/>
+        <v>buildcraft.transport.BlockGenericPipe</v>
+      </c>
+      <c r="F31" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G31" t="str">
+        <f>RIGHT(D31,LEN(D31) - SEARCH("ID: ",D31) - 3)</f>
+        <v>166</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>491</v>
+      </c>
+      <c r="B32" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C32" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="2"/>
+        <v>refineryBlock. ID: 167</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="3"/>
+        <v>refineryBlock</v>
+      </c>
+      <c r="F32" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G32" t="str">
+        <f>RIGHT(D32,LEN(D32) - SEARCH("ID: ",D32) - 3)</f>
+        <v>167</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="5"/>
+        <v>REFINERYBLOCK(167),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>492</v>
+      </c>
+      <c r="B33" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C33" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="2"/>
+        <v>autoWorkbenchBlock. ID: 169</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="3"/>
+        <v>autoWorkbenchBlock</v>
+      </c>
+      <c r="F33" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G33" t="str">
+        <f>RIGHT(D33,LEN(D33) - SEARCH("ID: ",D33) - 3)</f>
+        <v>169</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="5"/>
+        <v>AUTOWORKBENCHBLOCK(169),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B34" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C34" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="2"/>
+        <v>buildcraft.transport.LegacyBlock. ID: 170</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="3"/>
+        <v>buildcraft.transport.LegacyBlock</v>
+      </c>
+      <c r="F34" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G34" t="str">
+        <f>RIGHT(D34,LEN(D34) - SEARCH("ID: ",D34) - 3)</f>
+        <v>170</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>494</v>
+      </c>
+      <c r="B35" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C35" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="2"/>
+        <v>plainPipeBlock. ID: 171</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="3"/>
+        <v>plainPipeBlock</v>
+      </c>
+      <c r="F35" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G35" t="str">
+        <f>RIGHT(D35,LEN(D35) - SEARCH("ID: ",D35) - 3)</f>
+        <v>171</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="5"/>
+        <v>PLAINPIPEBLOCK(171),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>495</v>
+      </c>
+      <c r="B36" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C36" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="2"/>
+        <v>buildcraft.transport.LegacyBlock. ID: 172</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="3"/>
+        <v>buildcraft.transport.LegacyBlock</v>
+      </c>
+      <c r="F36" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G36" t="str">
+        <f>RIGHT(D36,LEN(D36) - SEARCH("ID: ",D36) - 3)</f>
+        <v>172</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>496</v>
+      </c>
+      <c r="B37" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C37" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="2"/>
+        <v>buildcraft.transport.LegacyBlock. ID: 173</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="3"/>
+        <v>buildcraft.transport.LegacyBlock</v>
+      </c>
+      <c r="F37" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G37" t="str">
+        <f>RIGHT(D37,LEN(D37) - SEARCH("ID: ",D37) - 3)</f>
+        <v>173</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>497</v>
+      </c>
+      <c r="B38" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C38" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="2"/>
+        <v>miningWellBlock. ID: 174</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="3"/>
+        <v>miningWellBlock</v>
+      </c>
+      <c r="F38" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G38" t="str">
+        <f>RIGHT(D38,LEN(D38) - SEARCH("ID: ",D38) - 3)</f>
+        <v>174</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="5"/>
+        <v>MININGWELLBLOCK(174),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>498</v>
+      </c>
+      <c r="B39" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C39" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="2"/>
+        <v>buildcraft.transport.LegacyBlock. ID: 175</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="3"/>
+        <v>buildcraft.transport.LegacyBlock</v>
+      </c>
+      <c r="F39" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G39" t="str">
+        <f>RIGHT(D39,LEN(D39) - SEARCH("ID: ",D39) - 3)</f>
+        <v>175</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>499</v>
+      </c>
+      <c r="B40" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C40" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="2"/>
+        <v>buildcraft.transport.LegacyBlock. ID: 176</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="3"/>
+        <v>buildcraft.transport.LegacyBlock</v>
+      </c>
+      <c r="F40" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G40" t="str">
+        <f>RIGHT(D40,LEN(D40) - SEARCH("ID: ",D40) - 3)</f>
+        <v>176</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>500</v>
+      </c>
+      <c r="B41" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C41" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="2"/>
+        <v>eloraam.logic.BlockLogic. ID: 177</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="3"/>
+        <v>eloraam.logic.BlockLogic</v>
+      </c>
+      <c r="F41" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G41" t="str">
+        <f>RIGHT(D41,LEN(D41) - SEARCH("ID: ",D41) - 3)</f>
+        <v>177</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>501</v>
+      </c>
+      <c r="B42" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C42" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="2"/>
+        <v>enderchest. ID: 178</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="3"/>
+        <v>enderchest</v>
+      </c>
+      <c r="F42" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G42" t="str">
+        <f>RIGHT(D42,LEN(D42) - SEARCH("ID: ",D42) - 3)</f>
+        <v>178</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="5"/>
+        <v>ENDERCHEST(178),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>502</v>
+      </c>
+      <c r="B43" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C43" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="2"/>
+        <v>Teleport Tether. ID: 179</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="3"/>
+        <v>Teleport Tether</v>
+      </c>
+      <c r="F43" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G43" t="str">
+        <f>RIGHT(D43,LEN(D43) - SEARCH("ID: ",D43) - 3)</f>
+        <v>179</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="5"/>
+        <v>TELEPORT TETHER(179),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>503</v>
+      </c>
+      <c r="B44" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C44" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="2"/>
+        <v>IronChest. ID: 181</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="3"/>
+        <v>IronChest</v>
+      </c>
+      <c r="F44" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G44" t="str">
+        <f>RIGHT(D44,LEN(D44) - SEARCH("ID: ",D44) - 3)</f>
+        <v>181</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="5"/>
+        <v>IRONCHEST(181),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>504</v>
+      </c>
+      <c r="B45" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C45" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="2"/>
+        <v>CompactSolar. ID: 183</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="3"/>
+        <v>CompactSolar</v>
+      </c>
+      <c r="F45" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G45" t="str">
+        <f>RIGHT(D45,LEN(D45) - SEARCH("ID: ",D45) - 3)</f>
+        <v>183</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="5"/>
+        <v>COMPACTSOLAR(183),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>505</v>
+      </c>
+      <c r="B46" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C46" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="2"/>
+        <v>BlockChargingBench. ID: 187</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="3"/>
+        <v>BlockChargingBench</v>
+      </c>
+      <c r="F46" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G46" t="str">
+        <f>RIGHT(D46,LEN(D46) - SEARCH("ID: ",D46) - 3)</f>
+        <v>187</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="5"/>
+        <v>BLOCKCHARGINGBENCH(187),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>506</v>
+      </c>
+      <c r="B47" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C47" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="2"/>
+        <v>ic2.advancedmachines.BlockAdvancedMachines. ID: 188</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="3"/>
+        <v>ic2.advancedmachines.BlockAdvancedMachines</v>
+      </c>
+      <c r="F47" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G47" t="str">
+        <f>RIGHT(D47,LEN(D47) - SEARCH("ID: ",D47) - 3)</f>
+        <v>188</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>507</v>
+      </c>
+      <c r="B48" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C48" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="2"/>
+        <v>powerConverter. ID: 190</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="3"/>
+        <v>powerConverter</v>
+      </c>
+      <c r="F48" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G48" t="str">
+        <f>RIGHT(D48,LEN(D48) - SEARCH("ID: ",D48) - 3)</f>
+        <v>190</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="5"/>
+        <v>POWERCONVERTER(190),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>508</v>
+      </c>
+      <c r="B49" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C49" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="2"/>
+        <v>blockThermalMonitor. ID: 192</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="3"/>
+        <v>blockThermalMonitor</v>
+      </c>
+      <c r="F49" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G49" t="str">
+        <f>RIGHT(D49,LEN(D49) - SEARCH("ID: ",D49) - 3)</f>
+        <v>192</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="5"/>
+        <v>BLOCKTHERMALMONITOR(192),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>509</v>
+      </c>
+      <c r="B50" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C50" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="2"/>
+        <v>immibis.tubestuff.BlockTubestuff. ID: 194</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="3"/>
+        <v>immibis.tubestuff.BlockTubestuff</v>
+      </c>
+      <c r="F50" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G50" t="str">
+        <f>RIGHT(D50,LEN(D50) - SEARCH("ID: ",D50) - 3)</f>
+        <v>194</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>510</v>
+      </c>
+      <c r="B51" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C51" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="2"/>
+        <v>railcraftTrack. ID: 206</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="3"/>
+        <v>railcraftTrack</v>
+      </c>
+      <c r="F51" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G51" t="str">
+        <f>RIGHT(D51,LEN(D51) - SEARCH("ID: ",D51) - 3)</f>
+        <v>206</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="5"/>
+        <v>RAILCRAFTTRACK(206),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>511</v>
+      </c>
+      <c r="B52" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C52" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="2"/>
+        <v>computer. ID: 207</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="3"/>
+        <v>computer</v>
+      </c>
+      <c r="F52" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G52" t="str">
+        <f>RIGHT(D52,LEN(D52) - SEARCH("ID: ",D52) - 3)</f>
+        <v>207</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="5"/>
+        <v>COMPUTER(207),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>512</v>
+      </c>
+      <c r="B53" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C53" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="2"/>
+        <v>diskdrive. ID: 208</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="3"/>
+        <v>diskdrive</v>
+      </c>
+      <c r="F53" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G53" t="str">
+        <f>RIGHT(D53,LEN(D53) - SEARCH("ID: ",D53) - 3)</f>
+        <v>208</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="5"/>
+        <v>DISKDRIVE(208),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>513</v>
+      </c>
+      <c r="B54" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C54" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="2"/>
+        <v>structureBlock. ID: 209</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="3"/>
+        <v>structureBlock</v>
+      </c>
+      <c r="F54" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G54" t="str">
+        <f>RIGHT(D54,LEN(D54) - SEARCH("ID: ",D54) - 3)</f>
+        <v>209</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="5"/>
+        <v>STRUCTUREBLOCK(209),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>514</v>
+      </c>
+      <c r="B55" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C55" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="2"/>
+        <v>cartDetector. ID: 211</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="3"/>
+        <v>cartDetector</v>
+      </c>
+      <c r="F55" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G55" t="str">
+        <f>RIGHT(D55,LEN(D55) - SEARCH("ID: ",D55) - 3)</f>
+        <v>211</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="5"/>
+        <v>CARTDETECTOR(211),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>515</v>
+      </c>
+      <c r="B56" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C56" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="2"/>
+        <v>elevatorRail. ID: 212</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="3"/>
+        <v>elevatorRail</v>
+      </c>
+      <c r="F56" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G56" t="str">
+        <f>RIGHT(D56,LEN(D56) - SEARCH("ID: ",D56) - 3)</f>
+        <v>212</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="5"/>
+        <v>ELEVATORRAIL(212),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>516</v>
+      </c>
+      <c r="B57" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C57" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="2"/>
+        <v>blockUtility. ID: 213</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="3"/>
+        <v>blockUtility</v>
+      </c>
+      <c r="F57" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G57" t="str">
+        <f>RIGHT(D57,LEN(D57) - SEARCH("ID: ",D57) - 3)</f>
+        <v>213</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="5"/>
+        <v>BLOCKUTILITY(213),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>517</v>
+      </c>
+      <c r="B58" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C58" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="2"/>
+        <v>blockRailcraftCube. ID: 214</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="3"/>
+        <v>blockRailcraftCube</v>
+      </c>
+      <c r="F58" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G58" t="str">
+        <f>RIGHT(D58,LEN(D58) - SEARCH("ID: ",D58) - 3)</f>
+        <v>214</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="5"/>
+        <v>BLOCKRAILCRAFTCUBE(214),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>518</v>
+      </c>
+      <c r="B59" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C59" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="2"/>
+        <v>turtle. ID: 216</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="3"/>
+        <v>turtle</v>
+      </c>
+      <c r="F59" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G59" t="str">
+        <f>RIGHT(D59,LEN(D59) - SEARCH("ID: ",D59) - 3)</f>
+        <v>216</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="5"/>
+        <v>TURTLE(216),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>519</v>
+      </c>
+      <c r="B60" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C60" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="2"/>
+        <v>ic2.common.BlockBarrel. ID: 217</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="3"/>
+        <v>ic2.common.BlockBarrel</v>
+      </c>
+      <c r="F60" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G60" t="str">
+        <f>RIGHT(D60,LEN(D60) - SEARCH("ID: ",D60) - 3)</f>
+        <v>217</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>520</v>
+      </c>
+      <c r="B61" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C61" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="2"/>
+        <v>blockCrop. ID: 218</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="3"/>
+        <v>blockCrop</v>
+      </c>
+      <c r="F61" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G61" t="str">
+        <f>RIGHT(D61,LEN(D61) - SEARCH("ID: ",D61) - 3)</f>
+        <v>218</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="5"/>
+        <v>BLOCKCROP(218),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>521</v>
+      </c>
+      <c r="B62" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C62" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="2"/>
+        <v>blockLuminatorD. ID: 219</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="3"/>
+        <v>blockLuminatorD</v>
+      </c>
+      <c r="F62" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G62" t="str">
+        <f>RIGHT(D62,LEN(D62) - SEARCH("ID: ",D62) - 3)</f>
+        <v>219</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="5"/>
+        <v>BLOCKLUMINATORD(219),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>522</v>
+      </c>
+      <c r="B63" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C63" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="2"/>
+        <v>blockScaffold. ID: 220</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="3"/>
+        <v>blockScaffold</v>
+      </c>
+      <c r="F63" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" ref="G63:G93" si="6">RIGHT(D63,LEN(D63) - SEARCH("ID: ",D63) - 3)</f>
+        <v>220</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="5"/>
+        <v>BLOCKSCAFFOLD(220),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>523</v>
+      </c>
+      <c r="B64" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C64" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="2"/>
+        <v>blockWall. ID: 221</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="3"/>
+        <v>blockWall</v>
+      </c>
+      <c r="F64" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="6"/>
+        <v>221</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="5"/>
+        <v>BLOCKWALL(221),</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>524</v>
+      </c>
+      <c r="B65" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C65" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="2"/>
+        <v>blockFoam. ID: 222</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="3"/>
+        <v>blockFoam</v>
+      </c>
+      <c r="F65" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="6"/>
+        <v>222</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="5"/>
+        <v>BLOCKFOAM(222),</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>525</v>
+      </c>
+      <c r="B66" t="b">
+        <f t="shared" ref="B66:B93" si="7">IFERROR(SEARCH("unused", A66)&gt;0,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="C66" t="b">
+        <f t="shared" ref="C66:C96" si="8">IFERROR(SEARCH("tile", A66) &gt; 0, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" ref="D66:D93" si="9">IF(C66,RIGHT(A66,LEN(A66)-18),RIGHT(A66,LEN(A66)-13))</f>
+        <v>ic2.common.BlockMachine2. ID: 223</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" ref="E66:E93" si="10">LEFT(D66,SEARCH(". ID",D66) - 1)</f>
+        <v>ic2.common.BlockMachine2</v>
+      </c>
+      <c r="F66" t="b">
+        <f t="shared" ref="F66:F93" si="11">IFERROR(SEARCH(".", E66)&gt;0,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="6"/>
+        <v>223</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>526</v>
+      </c>
+      <c r="B67" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C67" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="9"/>
+        <v>ic2.common.BlockMetal. ID: 224</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" si="10"/>
+        <v>ic2.common.BlockMetal</v>
+      </c>
+      <c r="F67" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" si="6"/>
+        <v>224</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" ref="H67:H93" si="12">IF(F67,"",CONCATENATE(UPPER(E67),"(",G67,"),"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>527</v>
+      </c>
+      <c r="B68" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C68" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="9"/>
+        <v>ic2.common.BlockPersonal. ID: 225</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="10"/>
+        <v>ic2.common.BlockPersonal</v>
+      </c>
+      <c r="F68" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="6"/>
+        <v>225</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>528</v>
+      </c>
+      <c r="B69" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C69" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="9"/>
+        <v>blockLuminator. ID: 226</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="10"/>
+        <v>blockLuminator</v>
+      </c>
+      <c r="F69" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="6"/>
+        <v>226</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKLUMINATOR(226),</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>529</v>
+      </c>
+      <c r="B70" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C70" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="9"/>
+        <v>ic2.common.BlockElectric. ID: 227</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="10"/>
+        <v>ic2.common.BlockElectric</v>
+      </c>
+      <c r="F70" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="6"/>
+        <v>227</v>
+      </c>
+      <c r="H70" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>530</v>
+      </c>
+      <c r="B71" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C71" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="9"/>
+        <v>ic2.common.BlockCable. ID: 228</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="10"/>
+        <v>ic2.common.BlockCable</v>
+      </c>
+      <c r="F71" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="6"/>
+        <v>228</v>
+      </c>
+      <c r="H71" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>531</v>
+      </c>
+      <c r="B72" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C72" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="9"/>
+        <v>blockDoorAlloy. ID: 229</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="10"/>
+        <v>blockDoorAlloy</v>
+      </c>
+      <c r="F72" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="6"/>
+        <v>229</v>
+      </c>
+      <c r="H72" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKDOORALLOY(229),</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>532</v>
+      </c>
+      <c r="B73" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C73" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="9"/>
+        <v>blockAlloyGlass. ID: 230</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="10"/>
+        <v>blockAlloyGlass</v>
+      </c>
+      <c r="F73" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="6"/>
+        <v>230</v>
+      </c>
+      <c r="H73" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKALLOYGLASS(230),</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>533</v>
+      </c>
+      <c r="B74" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C74" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="9"/>
+        <v>blockAlloy. ID: 231</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="10"/>
+        <v>blockAlloy</v>
+      </c>
+      <c r="F74" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="6"/>
+        <v>231</v>
+      </c>
+      <c r="H74" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKALLOY(231),</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>534</v>
+      </c>
+      <c r="B75" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C75" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="9"/>
+        <v>blockFenceIron. ID: 232</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="10"/>
+        <v>blockFenceIron</v>
+      </c>
+      <c r="F75" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="6"/>
+        <v>232</v>
+      </c>
+      <c r="H75" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKFENCEIRON(232),</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>535</v>
+      </c>
+      <c r="B76" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C76" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="9"/>
+        <v>blockReactorChamber. ID: 233</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="10"/>
+        <v>blockReactorChamber</v>
+      </c>
+      <c r="F76" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" si="6"/>
+        <v>233</v>
+      </c>
+      <c r="H76" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKREACTORCHAMBER(233),</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>536</v>
+      </c>
+      <c r="B77" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C77" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="9"/>
+        <v>blockRubber. ID: 234</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="10"/>
+        <v>blockRubber</v>
+      </c>
+      <c r="F77" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" si="6"/>
+        <v>234</v>
+      </c>
+      <c r="H77" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKRUBBER(234),</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>537</v>
+      </c>
+      <c r="B78" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C78" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="9"/>
+        <v>blockIronScaffold. ID: 235</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="10"/>
+        <v>blockIronScaffold</v>
+      </c>
+      <c r="F78" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G78" t="str">
+        <f t="shared" si="6"/>
+        <v>235</v>
+      </c>
+      <c r="H78" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKIRONSCAFFOLD(235),</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>538</v>
+      </c>
+      <c r="B79" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C79" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="9"/>
+        <v>blockDynamite. ID: 236</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="10"/>
+        <v>blockDynamite</v>
+      </c>
+      <c r="F79" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G79" t="str">
+        <f t="shared" si="6"/>
+        <v>236</v>
+      </c>
+      <c r="H79" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKDYNAMITE(236),</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>539</v>
+      </c>
+      <c r="B80" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C80" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="9"/>
+        <v>blockNuke. ID: 237</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="10"/>
+        <v>blockNuke</v>
+      </c>
+      <c r="F80" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G80" t="str">
+        <f t="shared" si="6"/>
+        <v>237</v>
+      </c>
+      <c r="H80" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKNUKE(237),</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>540</v>
+      </c>
+      <c r="B81" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C81" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="9"/>
+        <v>blockDynamiteRemote. ID: 238</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="10"/>
+        <v>blockDynamiteRemote</v>
+      </c>
+      <c r="F81" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G81" t="str">
+        <f t="shared" si="6"/>
+        <v>238</v>
+      </c>
+      <c r="H81" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKDYNAMITEREMOTE(238),</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>541</v>
+      </c>
+      <c r="B82" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C82" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="9"/>
+        <v>blockITNT. ID: 239</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="10"/>
+        <v>blockITNT</v>
+      </c>
+      <c r="F82" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G82" t="str">
+        <f t="shared" si="6"/>
+        <v>239</v>
+      </c>
+      <c r="H82" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKITNT(239),</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>542</v>
+      </c>
+      <c r="B83" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C83" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="9"/>
+        <v>blockHarz. ID: 240</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="10"/>
+        <v>blockHarz</v>
+      </c>
+      <c r="F83" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G83" t="str">
+        <f t="shared" si="6"/>
+        <v>240</v>
+      </c>
+      <c r="H83" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKHARZ(240),</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>543</v>
+      </c>
+      <c r="B84" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C84" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="9"/>
+        <v>blockRubSapling. ID: 241</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="10"/>
+        <v>blockRubSapling</v>
+      </c>
+      <c r="F84" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G84" t="str">
+        <f t="shared" si="6"/>
+        <v>241</v>
+      </c>
+      <c r="H84" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKRUBSAPLING(241),</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>544</v>
+      </c>
+      <c r="B85" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C85" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="9"/>
+        <v>leaves. ID: 242</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="10"/>
+        <v>leaves</v>
+      </c>
+      <c r="F85" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G85" t="str">
+        <f t="shared" si="6"/>
+        <v>242</v>
+      </c>
+      <c r="H85" t="str">
+        <f t="shared" si="12"/>
+        <v>LEAVES(242),</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>545</v>
+      </c>
+      <c r="B86" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C86" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="9"/>
+        <v>blockRubWood. ID: 243</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="10"/>
+        <v>blockRubWood</v>
+      </c>
+      <c r="F86" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G86" t="str">
+        <f t="shared" si="6"/>
+        <v>243</v>
+      </c>
+      <c r="H86" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKRUBWOOD(243),</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>546</v>
+      </c>
+      <c r="B87" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C87" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="9"/>
+        <v>blockMiningTip. ID: 244</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="10"/>
+        <v>blockMiningTip</v>
+      </c>
+      <c r="F87" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G87" t="str">
+        <f t="shared" si="6"/>
+        <v>244</v>
+      </c>
+      <c r="H87" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKMININGTIP(244),</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>547</v>
+      </c>
+      <c r="B88" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C88" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="9"/>
+        <v>blockMiningPipe. ID: 245</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="10"/>
+        <v>blockMiningPipe</v>
+      </c>
+      <c r="F88" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G88" t="str">
+        <f t="shared" si="6"/>
+        <v>245</v>
+      </c>
+      <c r="H88" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKMININGPIPE(245),</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>548</v>
+      </c>
+      <c r="B89" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C89" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="9"/>
+        <v>ic2.common.BlockGenerator. ID: 246</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="10"/>
+        <v>ic2.common.BlockGenerator</v>
+      </c>
+      <c r="F89" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="G89" t="str">
+        <f t="shared" si="6"/>
+        <v>246</v>
+      </c>
+      <c r="H89" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>549</v>
+      </c>
+      <c r="B90" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C90" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="9"/>
+        <v>blockOreUran. ID: 247</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="10"/>
+        <v>blockOreUran</v>
+      </c>
+      <c r="F90" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G90" t="str">
+        <f t="shared" si="6"/>
+        <v>247</v>
+      </c>
+      <c r="H90" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKOREURAN(247),</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>550</v>
+      </c>
+      <c r="B91" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C91" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="9"/>
+        <v>blockOreTin. ID: 248</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="10"/>
+        <v>blockOreTin</v>
+      </c>
+      <c r="F91" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G91" t="str">
+        <f t="shared" si="6"/>
+        <v>248</v>
+      </c>
+      <c r="H91" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKORETIN(248),</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>551</v>
+      </c>
+      <c r="B92" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C92" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="9"/>
+        <v>blockOreCopper. ID: 249</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="10"/>
+        <v>blockOreCopper</v>
+      </c>
+      <c r="F92" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G92" t="str">
+        <f t="shared" si="6"/>
+        <v>249</v>
+      </c>
+      <c r="H92" t="str">
+        <f t="shared" si="12"/>
+        <v>BLOCKORECOPPER(249),</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>552</v>
+      </c>
+      <c r="B93" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C93" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="9"/>
+        <v>ic2.common.BlockMachine. ID: 250</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="10"/>
+        <v>ic2.common.BlockMachine</v>
+      </c>
+      <c r="F93" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="G93" t="str">
+        <f t="shared" si="6"/>
+        <v>250</v>
+      </c>
+      <c r="H93" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>